<commit_message>
added effectivenessFP to spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="80" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="17" activeTab="18"/>
+    <workbookView xWindow="2600" yWindow="80" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="16" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E37" authorId="2">
+    <comment ref="E46" authorId="2">
       <text>
         <r>
           <rPr>
@@ -660,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="2">
+    <comment ref="F46" authorId="2">
       <text>
         <r>
           <rPr>
@@ -684,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G37" authorId="2">
+    <comment ref="G46" authorId="2">
       <text>
         <r>
           <rPr>
@@ -708,7 +708,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H37" authorId="2">
+    <comment ref="H46" authorId="2">
       <text>
         <r>
           <rPr>
@@ -732,7 +732,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="2">
+    <comment ref="I46" authorId="2">
       <text>
         <r>
           <rPr>
@@ -756,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E38" authorId="2">
+    <comment ref="E47" authorId="2">
       <text>
         <r>
           <rPr>
@@ -780,7 +780,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="2">
+    <comment ref="F47" authorId="2">
       <text>
         <r>
           <rPr>
@@ -804,7 +804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G38" authorId="2">
+    <comment ref="G47" authorId="2">
       <text>
         <r>
           <rPr>
@@ -828,7 +828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H38" authorId="2">
+    <comment ref="H47" authorId="2">
       <text>
         <r>
           <rPr>
@@ -852,7 +852,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="2">
+    <comment ref="I47" authorId="2">
       <text>
         <r>
           <rPr>
@@ -876,7 +876,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E39" authorId="2">
+    <comment ref="E48" authorId="2">
       <text>
         <r>
           <rPr>
@@ -900,7 +900,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="2">
+    <comment ref="F48" authorId="2">
       <text>
         <r>
           <rPr>
@@ -924,7 +924,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G39" authorId="2">
+    <comment ref="G48" authorId="2">
       <text>
         <r>
           <rPr>
@@ -948,7 +948,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H39" authorId="2">
+    <comment ref="H48" authorId="2">
       <text>
         <r>
           <rPr>
@@ -972,7 +972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I39" authorId="2">
+    <comment ref="I48" authorId="2">
       <text>
         <r>
           <rPr>
@@ -996,7 +996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C41" authorId="2">
+    <comment ref="C50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1020,7 +1020,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="2">
+    <comment ref="D50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1044,7 +1044,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E41" authorId="2">
+    <comment ref="E50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1068,7 +1068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="2">
+    <comment ref="F50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1092,7 +1092,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G41" authorId="2">
+    <comment ref="G50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1116,7 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H41" authorId="2">
+    <comment ref="H50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I41" authorId="2">
+    <comment ref="I50" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1164,7 +1164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E42" authorId="2">
+    <comment ref="E51" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="2">
+    <comment ref="F51" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1212,7 +1212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G42" authorId="2">
+    <comment ref="G51" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1236,7 +1236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H42" authorId="2">
+    <comment ref="H51" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1260,7 +1260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I42" authorId="2">
+    <comment ref="I51" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1284,7 +1284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="2">
+    <comment ref="E52" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1308,7 +1308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="2">
+    <comment ref="F52" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1332,7 +1332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G43" authorId="2">
+    <comment ref="G52" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H43" authorId="2">
+    <comment ref="H52" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1380,7 +1380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I43" authorId="2">
+    <comment ref="I52" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E44" authorId="2">
+    <comment ref="E53" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1428,7 +1428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="2">
+    <comment ref="F53" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1452,7 +1452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G44" authorId="2">
+    <comment ref="G53" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1476,7 +1476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H44" authorId="2">
+    <comment ref="H53" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I44" authorId="2">
+    <comment ref="I53" authorId="2">
       <text>
         <r>
           <rPr>
@@ -3620,7 +3620,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="217">
   <si>
     <t>year</t>
   </si>
@@ -4285,7 +4285,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4409,6 +4409,11 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -4503,7 +4508,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="555">
+  <cellStyleXfs count="565">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5059,8 +5064,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5199,9 +5214,10 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="555">
+  <cellStyles count="565">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5479,6 +5495,11 @@
     <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5755,6 +5776,11 @@
     <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -8142,10 +8168,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -9051,262 +9077,495 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="88" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="59">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A37" s="10" t="s">
+      <c r="B37" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B38" s="88" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B39" s="88" t="s">
+        <v>211</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B40" s="88" t="s">
+        <v>212</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B41" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B42" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B43" s="88" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B44" s="88" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A46" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="35">
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="35">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F37" s="35">
+      <c r="F46" s="35">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G37" s="35">
+      <c r="G46" s="35">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H37" s="35">
+      <c r="H46" s="35">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I37" s="35">
+      <c r="I46" s="35">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B38" s="4" t="s">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="3">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0</v>
-      </c>
-      <c r="E38" s="3">
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F47" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G47" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H47" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I47" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B39" s="4" t="s">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B48" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="3">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0</v>
-      </c>
-      <c r="E39" s="3">
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F48" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G48" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H48" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I48" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B40" s="4" t="s">
+    <row r="49" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B49" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="3">
-        <v>0</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0</v>
-      </c>
-      <c r="E40" s="35">
-        <v>1</v>
-      </c>
-      <c r="F40" s="35">
-        <v>1</v>
-      </c>
-      <c r="G40" s="35">
-        <v>1</v>
-      </c>
-      <c r="H40" s="35">
-        <v>1</v>
-      </c>
-      <c r="I40" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B41" s="4" t="s">
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="35">
+        <v>1</v>
+      </c>
+      <c r="F49" s="35">
+        <v>1</v>
+      </c>
+      <c r="G49" s="35">
+        <v>1</v>
+      </c>
+      <c r="H49" s="35">
+        <v>1</v>
+      </c>
+      <c r="I49" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="35">
+      <c r="C50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D41" s="35">
+      <c r="D50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E41" s="35">
+      <c r="E50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F41" s="35">
+      <c r="F50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G41" s="35">
+      <c r="G50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H41" s="35">
+      <c r="H50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I41" s="35">
+      <c r="I50" s="35">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B42" s="12" t="s">
+    <row r="51" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B51" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="3">
-        <v>0</v>
-      </c>
-      <c r="D42" s="3">
-        <v>0</v>
-      </c>
-      <c r="E42" s="71">
+      <c r="C51" s="3">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="E51" s="71">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F42" s="71">
+      <c r="F51" s="71">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G42" s="71">
+      <c r="G51" s="71">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H42" s="71">
+      <c r="H51" s="71">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I42" s="71">
+      <c r="I51" s="71">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B43" s="12" t="s">
+    <row r="52" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B52" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="3">
-        <v>0</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0</v>
-      </c>
-      <c r="E43" s="69">
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="69">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F43" s="69">
+      <c r="F52" s="69">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G43" s="69">
+      <c r="G52" s="69">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H43" s="69">
+      <c r="H52" s="69">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I43" s="69">
+      <c r="I52" s="69">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B44" s="12" t="s">
+    <row r="53" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B53" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0</v>
-      </c>
-      <c r="E44" s="69">
+      <c r="C53" s="3">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" s="69">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F44" s="69">
+      <c r="F53" s="69">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G44" s="69">
+      <c r="G53" s="69">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H44" s="69">
+      <c r="H53" s="69">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I44" s="69">
+      <c r="I53" s="69">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B48" s="4"/>
-    </row>
-    <row r="49" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B49" s="4"/>
+    <row r="57" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B57" s="4"/>
+    </row>
+    <row r="58" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B58" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11776,8 +12035,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -11795,74 +12054,74 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="13">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="88" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="88">
+      <c r="B2" s="89">
         <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="88">
+      <c r="B3" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="88">
+      <c r="B4" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="88" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="88">
+      <c r="B5" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="13">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="B6" s="88">
+      <c r="B6" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="88">
+      <c r="B7" s="89">
         <v>0.93</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="89">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="13">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="88">
+      <c r="B9" s="89">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="89">
         <v>0.98</v>
       </c>
     </row>
@@ -11881,7 +12140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reversed changes form wasting run
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Nov/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="80" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="17" activeTab="18"/>
+    <workbookView xWindow="2600" yWindow="460" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="6" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -27,13 +32,13 @@
     <sheet name="Interventions family planning" sheetId="34" r:id="rId18"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -4402,12 +4407,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -5192,14 +5199,14 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="555">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7062,13 +7069,13 @@
       <selection activeCell="C26" sqref="C26:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>114</v>
       </c>
@@ -7079,7 +7086,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -7090,7 +7097,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -7098,7 +7105,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="33" t="s">
         <v>135</v>
       </c>
@@ -7106,7 +7113,7 @@
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -7115,7 +7122,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="33" t="s">
         <v>72</v>
       </c>
@@ -7123,7 +7130,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
@@ -7131,7 +7138,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="33" t="s">
         <v>73</v>
       </c>
@@ -7139,14 +7146,14 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="33"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
         <v>141</v>
       </c>
@@ -7157,7 +7164,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>136</v>
       </c>
@@ -7165,7 +7172,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>137</v>
       </c>
@@ -7173,7 +7180,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>138</v>
       </c>
@@ -7181,7 +7188,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>139</v>
       </c>
@@ -7189,7 +7196,7 @@
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>140</v>
       </c>
@@ -7197,11 +7204,11 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="10"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10" t="s">
         <v>75</v>
       </c>
@@ -7212,7 +7219,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="33" t="s">
         <v>106</v>
       </c>
@@ -7220,7 +7227,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="33" t="s">
         <v>107</v>
       </c>
@@ -7228,7 +7235,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="33" t="s">
         <v>108</v>
       </c>
@@ -7236,7 +7243,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="33" t="s">
         <v>76</v>
       </c>
@@ -7244,10 +7251,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="33"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>134</v>
       </c>
@@ -7258,7 +7265,7 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="51" t="s">
         <v>128</v>
       </c>
@@ -7266,7 +7273,7 @@
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="51" t="s">
         <v>129</v>
       </c>
@@ -7274,7 +7281,7 @@
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="51" t="s">
         <v>130</v>
       </c>
@@ -7282,11 +7289,11 @@
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="51"/>
       <c r="C30" s="53"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>125</v>
       </c>
@@ -7297,7 +7304,7 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="50" t="s">
         <v>128</v>
       </c>
@@ -7305,7 +7312,7 @@
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="50" t="s">
         <v>129</v>
       </c>
@@ -7313,7 +7320,7 @@
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="50" t="s">
         <v>130</v>
       </c>
@@ -7325,11 +7332,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7341,14 +7343,14 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>196</v>
       </c>
@@ -7374,11 +7376,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="88" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -7400,8 +7402,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="83"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B3" s="88"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -7422,8 +7424,8 @@
       </c>
       <c r="J3" s="73"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="B4" s="83" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B4" s="88" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
@@ -7445,8 +7447,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="B5" s="83"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B5" s="88"/>
       <c r="C5" t="s">
         <v>194</v>
       </c>
@@ -7466,8 +7468,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="83" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B6" s="88" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -7489,8 +7491,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="83"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B7" s="88"/>
       <c r="C7" t="s">
         <v>194</v>
       </c>
@@ -7510,8 +7512,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="83" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B8" s="88" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
@@ -7533,8 +7535,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="83"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B9" s="88"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -7554,8 +7556,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="83" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B10" s="88" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -7577,8 +7579,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="83"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B11" s="88"/>
       <c r="C11" t="s">
         <v>194</v>
       </c>
@@ -7598,7 +7600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B12" s="79" t="s">
         <v>112</v>
       </c>
@@ -7621,18 +7623,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="D13" s="75"/>
       <c r="E13" s="75"/>
       <c r="F13" s="75"/>
       <c r="G13" s="75"/>
       <c r="H13" s="75"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="88" t="s">
         <v>81</v>
       </c>
       <c r="C14" t="s">
@@ -7654,8 +7656,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="83"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="88"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -7675,8 +7677,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="83" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="88" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
@@ -7698,8 +7700,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="83"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="88"/>
       <c r="C17" t="s">
         <v>194</v>
       </c>
@@ -7719,8 +7721,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="83" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B18" s="88" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
@@ -7742,8 +7744,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="83"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B19" s="88"/>
       <c r="C19" t="s">
         <v>194</v>
       </c>
@@ -7763,8 +7765,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="83" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="88" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
@@ -7786,8 +7788,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="83"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="88"/>
       <c r="C21" t="s">
         <v>194</v>
       </c>
@@ -7807,8 +7809,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="83" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="88" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
@@ -7830,8 +7832,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="83"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="88"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -7851,7 +7853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="80" t="s">
         <v>112</v>
       </c>
@@ -7876,24 +7878,19 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7905,14 +7902,14 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>200</v>
       </c>
@@ -7929,7 +7926,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>201</v>
       </c>
@@ -7938,25 +7935,25 @@
       </c>
       <c r="E2" s="82"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="82"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="82"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="82"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -7965,7 +7962,7 @@
       </c>
       <c r="E6" s="82"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>112</v>
       </c>
@@ -7975,7 +7972,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>202</v>
       </c>
@@ -7984,38 +7981,38 @@
       </c>
       <c r="E9" s="82"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="82"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="82"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="82"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="82"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="82"/>
       <c r="D14" s="82"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
         <v>203</v>
       </c>
@@ -8024,31 +8021,31 @@
       </c>
       <c r="E16" s="82"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="82"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="82"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="82"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="82"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>112</v>
       </c>
@@ -8058,11 +8055,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8077,12 +8069,12 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -8099,7 +8091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
@@ -8116,14 +8108,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -8132,11 +8124,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8148,7 +8135,7 @@
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="54.83203125" customWidth="1"/>
@@ -8159,7 +8146,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>85</v>
       </c>
@@ -8189,7 +8176,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>80</v>
       </c>
@@ -8218,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>176</v>
@@ -8245,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>50</v>
       </c>
@@ -8271,7 +8258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="76" t="s">
         <v>57</v>
       </c>
@@ -8297,7 +8284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>161</v>
       </c>
@@ -8325,7 +8312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>84</v>
       </c>
@@ -8354,7 +8341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>172</v>
       </c>
@@ -8382,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>83</v>
       </c>
@@ -8411,7 +8398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>173</v>
       </c>
@@ -8440,7 +8427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>179</v>
       </c>
@@ -8466,7 +8453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>189</v>
       </c>
@@ -8492,7 +8479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="4" t="s">
         <v>190</v>
       </c>
@@ -8518,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>81</v>
       </c>
@@ -8548,7 +8535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>171</v>
@@ -8575,7 +8562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>174</v>
       </c>
@@ -8602,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="4" t="s">
         <v>86</v>
       </c>
@@ -8628,7 +8615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
         <v>175</v>
       </c>
@@ -8655,7 +8642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>151</v>
       </c>
@@ -8682,7 +8669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
         <v>93</v>
       </c>
@@ -8711,7 +8698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>155</v>
       </c>
@@ -8737,7 +8724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>156</v>
       </c>
@@ -8763,7 +8750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>157</v>
       </c>
@@ -8789,7 +8776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>158</v>
       </c>
@@ -8815,7 +8802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>159</v>
       </c>
@@ -8841,7 +8828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>160</v>
       </c>
@@ -8867,7 +8854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" t="s">
         <v>164</v>
@@ -8894,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>165</v>
       </c>
@@ -8920,7 +8907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>166</v>
       </c>
@@ -8946,7 +8933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>167</v>
       </c>
@@ -8972,7 +8959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>168</v>
       </c>
@@ -8998,7 +8985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>169</v>
       </c>
@@ -9024,7 +9011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>170</v>
       </c>
@@ -9050,11 +9037,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="10" t="s">
         <v>88</v>
       </c>
@@ -9088,7 +9075,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="4" t="s">
         <v>90</v>
       </c>
@@ -9119,7 +9106,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="4" t="s">
         <v>91</v>
       </c>
@@ -9150,7 +9137,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="4" t="s">
         <v>109</v>
       </c>
@@ -9176,7 +9163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="4" t="s">
         <v>87</v>
       </c>
@@ -9209,7 +9196,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="12" t="s">
         <v>180</v>
       </c>
@@ -9240,7 +9227,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="12" t="s">
         <v>181</v>
       </c>
@@ -9271,7 +9258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="12" t="s">
         <v>182</v>
       </c>
@@ -9302,21 +9289,16 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="2:2" ht="15.75" customHeight="1">
+    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9331,14 +9313,14 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -9358,7 +9340,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -9378,7 +9360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>54</v>
       </c>
@@ -9395,7 +9377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -9415,7 +9397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>54</v>
       </c>
@@ -9432,7 +9414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -9452,7 +9434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>54</v>
       </c>
@@ -9469,7 +9451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -9489,7 +9471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -9508,7 +9490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -9528,7 +9510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>54</v>
       </c>
@@ -9551,11 +9533,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9570,7 +9547,7 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="56.5" customWidth="1"/>
@@ -9579,7 +9556,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14" customHeight="1">
+    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
@@ -9626,7 +9603,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>152</v>
       </c>
@@ -9673,7 +9650,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
         <v>175</v>
       </c>
@@ -9717,7 +9694,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>171</v>
       </c>
@@ -9761,7 +9738,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>174</v>
       </c>
@@ -9805,7 +9782,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>151</v>
       </c>
@@ -9849,7 +9826,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>154</v>
       </c>
@@ -9893,7 +9870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>155</v>
       </c>
@@ -9937,7 +9914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>156</v>
       </c>
@@ -9981,7 +9958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>157</v>
       </c>
@@ -10025,7 +10002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>158</v>
       </c>
@@ -10069,7 +10046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>159</v>
       </c>
@@ -10113,7 +10090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -10157,7 +10134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>164</v>
       </c>
@@ -10201,7 +10178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>165</v>
       </c>
@@ -10245,7 +10222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>166</v>
       </c>
@@ -10289,7 +10266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>167</v>
       </c>
@@ -10333,7 +10310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>168</v>
       </c>
@@ -10377,7 +10354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>169</v>
       </c>
@@ -10421,7 +10398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>170</v>
       </c>
@@ -10465,7 +10442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B21" s="4" t="s">
         <v>84</v>
       </c>
@@ -10509,7 +10486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14" customHeight="1">
+    <row r="22" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="4" t="s">
         <v>172</v>
       </c>
@@ -10553,7 +10530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B23" s="60" t="s">
         <v>83</v>
       </c>
@@ -10597,7 +10574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B24" s="60" t="s">
         <v>173</v>
       </c>
@@ -10641,7 +10618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B25" s="60" t="s">
         <v>87</v>
       </c>
@@ -10685,7 +10662,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>153</v>
       </c>
@@ -10732,7 +10709,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B28" s="4" t="s">
         <v>90</v>
       </c>
@@ -10776,7 +10753,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B29" s="4" t="s">
         <v>91</v>
       </c>
@@ -10820,7 +10797,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B30" s="4" t="s">
         <v>109</v>
       </c>
@@ -10864,7 +10841,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B31" s="61" t="s">
         <v>180</v>
       </c>
@@ -10908,7 +10885,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B32" s="61" t="s">
         <v>181</v>
       </c>
@@ -10952,7 +10929,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="33" spans="2:15">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B33" s="61" t="s">
         <v>182</v>
       </c>
@@ -10996,27 +10973,22 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B43" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11031,13 +11003,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="32.83203125" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
@@ -11060,7 +11032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>191</v>
       </c>
@@ -11083,7 +11055,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>192</v>
       </c>
@@ -11108,11 +11080,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11127,7 +11094,7 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="39.1640625" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
@@ -11138,7 +11105,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -11164,7 +11131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
@@ -11190,7 +11157,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>68</v>
       </c>
@@ -11210,7 +11177,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -11232,7 +11199,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="60" t="s">
         <v>163</v>
@@ -11256,7 +11223,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>161</v>
       </c>
@@ -11282,7 +11249,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>69</v>
       </c>
@@ -11302,7 +11269,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>183</v>
       </c>
@@ -11325,7 +11292,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>69</v>
       </c>
@@ -11345,7 +11312,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>84</v>
       </c>
@@ -11371,7 +11338,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>69</v>
       </c>
@@ -11391,7 +11358,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>183</v>
       </c>
@@ -11414,7 +11381,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>69</v>
       </c>
@@ -11434,7 +11401,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>172</v>
       </c>
@@ -11460,7 +11427,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>69</v>
       </c>
@@ -11480,7 +11447,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>183</v>
       </c>
@@ -11503,7 +11470,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>69</v>
       </c>
@@ -11523,7 +11490,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -11549,7 +11516,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>69</v>
       </c>
@@ -11570,7 +11537,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>183</v>
       </c>
@@ -11594,7 +11561,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>69</v>
       </c>
@@ -11615,7 +11582,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>180</v>
       </c>
@@ -11642,7 +11609,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="12"/>
       <c r="C23" t="s">
         <v>68</v>
@@ -11664,7 +11631,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>181</v>
       </c>
@@ -11690,7 +11657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="12"/>
       <c r="C25" t="s">
         <v>68</v>
@@ -11711,7 +11678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>182</v>
       </c>
@@ -11737,7 +11704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" t="s">
         <v>68</v>
       </c>
@@ -11761,11 +11728,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11780,13 +11742,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>215</v>
       </c>
@@ -11794,86 +11756,81 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13">
-      <c r="A2" s="84" t="s">
+    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="83" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="88">
+      <c r="B2" s="87">
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13">
-      <c r="A3" s="84" t="s">
+    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="83" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13">
-      <c r="A4" s="84" t="s">
+      <c r="B3" s="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="83" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13">
-      <c r="A5" s="84" t="s">
+      <c r="B4" s="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="83" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="13">
-      <c r="A6" s="84" t="s">
+      <c r="B5" s="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="83" t="s">
         <v>212</v>
       </c>
-      <c r="B6" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13">
-      <c r="A7" s="84" t="s">
+      <c r="B6" s="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="83" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="88">
+      <c r="B7" s="87">
         <v>0.93</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13">
-      <c r="A8" s="84" t="s">
+    <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="87">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13">
-      <c r="A9" s="84" t="s">
+    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="88">
+      <c r="B9" s="87">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13">
-      <c r="A10" s="84" t="s">
+    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="83" t="s">
         <v>214</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="87">
         <v>0.98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11881,11 +11838,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -11893,7 +11850,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -11907,7 +11864,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
@@ -11921,7 +11878,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>176</v>
       </c>
@@ -11935,7 +11892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -11949,7 +11906,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>57</v>
       </c>
@@ -11963,7 +11920,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>161</v>
       </c>
@@ -11977,7 +11934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>84</v>
       </c>
@@ -11991,7 +11948,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>172</v>
       </c>
@@ -12005,7 +11962,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
@@ -12019,7 +11976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>173</v>
       </c>
@@ -12033,7 +11990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -12047,7 +12004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -12061,7 +12018,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -12075,7 +12032,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>86</v>
       </c>
@@ -12089,7 +12046,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>175</v>
       </c>
@@ -12103,7 +12060,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>151</v>
       </c>
@@ -12117,7 +12074,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -12131,7 +12088,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -12145,7 +12102,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -12159,7 +12116,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -12173,7 +12130,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>158</v>
       </c>
@@ -12187,7 +12144,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -12201,7 +12158,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>160</v>
       </c>
@@ -12215,7 +12172,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -12229,7 +12186,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>165</v>
       </c>
@@ -12243,7 +12200,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -12257,7 +12214,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>167</v>
       </c>
@@ -12271,7 +12228,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -12285,7 +12242,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -12299,7 +12256,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -12313,7 +12270,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>89</v>
       </c>
@@ -12327,7 +12284,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>90</v>
       </c>
@@ -12341,7 +12298,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>91</v>
       </c>
@@ -12355,7 +12312,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>109</v>
       </c>
@@ -12369,7 +12326,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
         <v>180</v>
       </c>
@@ -12383,7 +12340,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
         <v>181</v>
       </c>
@@ -12397,7 +12354,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
         <v>182</v>
       </c>
@@ -12411,7 +12368,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -12425,7 +12382,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>179</v>
       </c>
@@ -12440,7 +12397,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>189</v>
       </c>
@@ -12455,7 +12412,7 @@
         <v>10.046400000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>190</v>
       </c>
@@ -12470,144 +12427,139 @@
         <v>19.933477200000002</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A42" s="84" t="s">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="83" t="s">
         <v>206</v>
       </c>
-      <c r="B42" s="86">
+      <c r="B42" s="85">
         <v>0.09</v>
       </c>
       <c r="C42" s="14">
         <v>0.85</v>
       </c>
-      <c r="D42" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A43" s="84" t="s">
+      <c r="D42" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="83" t="s">
         <v>207</v>
       </c>
-      <c r="B43" s="86">
+      <c r="B43" s="85">
         <v>0.02</v>
       </c>
       <c r="C43" s="14">
         <v>0.85</v>
       </c>
-      <c r="D43" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A44" s="84" t="s">
+      <c r="D43" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="83" t="s">
         <v>208</v>
       </c>
-      <c r="B44" s="86">
+      <c r="B44" s="85">
         <v>0.08</v>
       </c>
       <c r="C44" s="14">
         <v>0.85</v>
       </c>
-      <c r="D44" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A45" s="84" t="s">
+      <c r="D44" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="83" t="s">
         <v>211</v>
       </c>
-      <c r="B45" s="86">
+      <c r="B45" s="85">
         <v>0.18</v>
       </c>
       <c r="C45" s="14">
         <v>0.85</v>
       </c>
-      <c r="D45" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A46" s="84" t="s">
+      <c r="D45" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="83" t="s">
         <v>212</v>
       </c>
-      <c r="B46" s="86">
+      <c r="B46" s="85">
         <v>0.02</v>
       </c>
       <c r="C46" s="14">
         <v>0.85</v>
       </c>
-      <c r="D46" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A47" s="84" t="s">
+      <c r="D46" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="83" t="s">
         <v>209</v>
       </c>
-      <c r="B47" s="86">
+      <c r="B47" s="85">
         <v>0.45</v>
       </c>
       <c r="C47" s="14">
         <v>0.85</v>
       </c>
-      <c r="D47" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A48" s="84" t="s">
+      <c r="D47" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="B48" s="86">
+      <c r="B48" s="85">
         <v>0.03</v>
       </c>
       <c r="C48" s="14">
         <v>0.85</v>
       </c>
-      <c r="D48" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A49" s="84" t="s">
+      <c r="D48" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="86">
+      <c r="B49" s="85">
         <v>0.11</v>
       </c>
       <c r="C49" s="14">
         <v>0.85</v>
       </c>
-      <c r="D49" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A50" s="84" t="s">
+      <c r="D49" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="83" t="s">
         <v>214</v>
       </c>
-      <c r="B50" s="86">
+      <c r="B50" s="85">
         <v>0.01</v>
       </c>
       <c r="C50" s="14">
         <v>0.85</v>
       </c>
-      <c r="D50" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C51" s="87"/>
+      <c r="D50" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C51" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12619,7 +12571,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -12627,7 +12579,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12665,7 +12617,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -12707,7 +12659,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -12749,7 +12701,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -12791,7 +12743,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -12833,7 +12785,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -12875,7 +12827,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -12917,7 +12869,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -12959,7 +12911,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -13001,7 +12953,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -13043,7 +12995,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -13085,7 +13037,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -13127,7 +13079,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -13169,7 +13121,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -13211,7 +13163,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -13257,11 +13209,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13273,12 +13220,12 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -13301,7 +13248,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -13324,7 +13271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -13347,7 +13294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -13370,7 +13317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -13393,7 +13340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -13416,7 +13363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -13439,7 +13386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -13462,7 +13409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -13485,7 +13432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -13508,7 +13455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -13531,7 +13478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -13554,7 +13501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -13577,7 +13524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -13600,7 +13547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -13623,7 +13570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -13646,7 +13593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -13669,7 +13616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -13692,7 +13639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -13715,7 +13662,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -13738,7 +13685,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -13761,7 +13708,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -13784,7 +13731,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -13807,7 +13754,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -13830,7 +13777,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -13853,7 +13800,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -13876,7 +13823,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -13906,11 +13853,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13922,9 +13864,9 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -13944,7 +13886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -13964,7 +13906,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -13984,7 +13926,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -14004,7 +13946,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>183</v>
       </c>
@@ -14029,7 +13971,7 @@
         <v>0.27300000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>184</v>
       </c>
@@ -14058,11 +14000,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14074,7 +14011,7 @@
       <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -14083,7 +14020,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>116</v>
       </c>
@@ -14100,7 +14037,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>94</v>
       </c>
@@ -14115,7 +14052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -14128,7 +14065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -14143,7 +14080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -14158,7 +14095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -14173,7 +14110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>82</v>
@@ -14188,7 +14125,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" t="s">
         <v>128</v>
@@ -14203,7 +14140,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>129</v>
@@ -14218,7 +14155,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>130</v>
@@ -14233,13 +14170,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
         <v>95</v>
       </c>
@@ -14254,7 +14191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -14266,7 +14203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -14280,7 +14217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -14294,7 +14231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -14308,7 +14245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>82</v>
       </c>
@@ -14322,7 +14259,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>128</v>
       </c>
@@ -14336,7 +14273,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>129</v>
       </c>
@@ -14350,7 +14287,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>130</v>
       </c>
@@ -14364,7 +14301,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>111</v>
       </c>
@@ -14385,11 +14322,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14401,9 +14333,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -14426,7 +14358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -14449,7 +14381,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>24</v>
@@ -14470,7 +14402,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>26</v>
@@ -14491,7 +14423,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
         <v>27</v>
@@ -14512,7 +14444,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -14535,7 +14467,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -14555,7 +14487,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>183</v>
       </c>
@@ -14575,7 +14507,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>184</v>
       </c>
@@ -14595,7 +14527,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>38</v>
       </c>
@@ -14618,7 +14550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
@@ -14638,7 +14570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
@@ -14658,7 +14590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
@@ -14683,11 +14615,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14699,12 +14626,12 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>117</v>
       </c>
@@ -14724,7 +14651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -14745,7 +14672,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>113</v>
       </c>
@@ -14760,7 +14687,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -14777,7 +14704,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>186</v>
       </c>
@@ -14794,7 +14721,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>185</v>
       </c>
@@ -14811,14 +14738,14 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
@@ -14827,7 +14754,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>59</v>
       </c>
@@ -14847,7 +14774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
@@ -14864,7 +14791,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -14881,7 +14808,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
@@ -14898,7 +14825,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
@@ -14915,7 +14842,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
@@ -14932,7 +14859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
@@ -14949,7 +14876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1">
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
@@ -14970,11 +14897,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14989,7 +14911,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -14997,7 +14919,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
@@ -15026,7 +14948,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
@@ -15055,7 +14977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -15078,7 +15000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
@@ -15101,7 +15023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
@@ -15124,7 +15046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>30</v>
       </c>
@@ -15150,7 +15072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -15173,7 +15095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
@@ -15196,7 +15118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
@@ -15219,7 +15141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -15245,7 +15167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -15268,7 +15190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
@@ -15291,7 +15213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
@@ -15314,7 +15236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>33</v>
       </c>
@@ -15340,7 +15262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -15363,7 +15285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -15386,7 +15308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -15409,7 +15331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>37</v>
       </c>
@@ -15435,7 +15357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -15458,7 +15380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
@@ -15481,7 +15403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>27</v>
       </c>
@@ -15504,7 +15426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -15533,7 +15455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -15556,7 +15478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
         <v>183</v>
       </c>
@@ -15579,7 +15501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
         <v>184</v>
       </c>
@@ -15602,7 +15524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -15628,7 +15550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -15651,7 +15573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
         <v>183</v>
       </c>
@@ -15674,7 +15596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
         <v>184</v>
       </c>
@@ -15697,7 +15619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -15723,7 +15645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -15746,7 +15668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
         <v>183</v>
       </c>
@@ -15769,7 +15691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
         <v>184</v>
       </c>
@@ -15792,7 +15714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>33</v>
       </c>
@@ -15818,7 +15740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -15841,7 +15763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
         <v>183</v>
       </c>
@@ -15864,7 +15786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
         <v>184</v>
       </c>
@@ -15887,7 +15809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>37</v>
       </c>
@@ -15913,7 +15835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -15936,7 +15858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
         <v>183</v>
       </c>
@@ -15959,7 +15881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
         <v>184</v>
       </c>
@@ -15982,7 +15904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
         <v>38</v>
       </c>
@@ -16011,7 +15933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
         <v>40</v>
       </c>
@@ -16034,7 +15956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C48" s="4" t="s">
         <v>41</v>
       </c>
@@ -16057,7 +15979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>42</v>
       </c>
@@ -16080,7 +16002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -16106,7 +16028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
         <v>40</v>
       </c>
@@ -16129,7 +16051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C52" s="4" t="s">
         <v>41</v>
       </c>
@@ -16152,7 +16074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
         <v>42</v>
       </c>
@@ -16175,7 +16097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -16201,7 +16123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
         <v>40</v>
       </c>
@@ -16224,7 +16146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C56" s="4" t="s">
         <v>41</v>
       </c>
@@ -16247,7 +16169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>42</v>
       </c>
@@ -16270,7 +16192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -16296,7 +16218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>40</v>
       </c>
@@ -16319,7 +16241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C60" s="4" t="s">
         <v>41</v>
       </c>
@@ -16342,7 +16264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
         <v>42</v>
       </c>
@@ -16365,7 +16287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
         <v>28</v>
       </c>
@@ -16391,7 +16313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C63" s="4" t="s">
         <v>40</v>
       </c>
@@ -16414,7 +16336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C64" s="4" t="s">
         <v>41</v>
       </c>
@@ -16437,7 +16359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C65" s="4" t="s">
         <v>42</v>
       </c>
@@ -16460,7 +16382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
         <v>30</v>
       </c>
@@ -16486,7 +16408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
         <v>40</v>
       </c>
@@ -16509,7 +16431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C68" s="4" t="s">
         <v>41</v>
       </c>
@@ -16532,7 +16454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C69" s="4" t="s">
         <v>42</v>
       </c>
@@ -16555,7 +16477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B70" t="s">
         <v>31</v>
       </c>
@@ -16581,7 +16503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
         <v>40</v>
       </c>
@@ -16604,7 +16526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C72" s="4" t="s">
         <v>41</v>
       </c>
@@ -16627,7 +16549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C73" s="4" t="s">
         <v>42</v>
       </c>
@@ -16650,7 +16572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="10" t="s">
         <v>126</v>
       </c>
@@ -16679,7 +16601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C77" s="4" t="s">
         <v>119</v>
       </c>
@@ -16702,7 +16624,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B78" t="s">
         <v>98</v>
       </c>
@@ -16728,7 +16650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C79" s="4" t="s">
         <v>119</v>
       </c>
@@ -16751,7 +16673,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
         <v>99</v>
       </c>
@@ -16777,7 +16699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C81" s="4" t="s">
         <v>119</v>
       </c>
@@ -16800,7 +16722,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="10" t="s">
         <v>110</v>
       </c>
@@ -16829,7 +16751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C85" s="4" t="s">
         <v>40</v>
       </c>
@@ -16852,7 +16774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C86" s="4" t="s">
         <v>41</v>
       </c>
@@ -16875,7 +16797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C87" s="4" t="s">
         <v>42</v>
       </c>
@@ -16898,17 +16820,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -16923,7 +16840,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -16933,7 +16850,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
@@ -16956,7 +16873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>121</v>
       </c>
@@ -16977,7 +16894,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
@@ -16997,7 +16914,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>120</v>
       </c>
@@ -17020,7 +16937,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
@@ -17040,7 +16957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>48</v>
       </c>
@@ -17060,7 +16977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>142</v>
       </c>
@@ -17080,7 +16997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>127</v>
       </c>
@@ -17100,7 +17017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
@@ -17120,7 +17037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="77" t="s">
         <v>122</v>
       </c>
@@ -17143,7 +17060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="78"/>
       <c r="B13" s="76" t="s">
         <v>57</v>
@@ -17164,8 +17081,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14" customHeight="1"/>
-    <row r="15" spans="1:7">
+    <row r="14" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>187</v>
       </c>
@@ -17188,7 +17105,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
         <v>188</v>
       </c>
@@ -17215,10 +17132,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added IYCF target pop
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="460" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="6" activeTab="18"/>
+    <workbookView xWindow="2600" yWindow="460" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,15 @@
     <sheet name="Odds ratios" sheetId="27" r:id="rId9"/>
     <sheet name="IYCF package odds ratios" sheetId="32" r:id="rId10"/>
     <sheet name="IYCF packages" sheetId="33" r:id="rId11"/>
-    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId12"/>
-    <sheet name="Interventions target population" sheetId="21" r:id="rId13"/>
-    <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId14"/>
-    <sheet name="Interventions anemia" sheetId="30" r:id="rId15"/>
-    <sheet name="Interventions wasting" sheetId="31" r:id="rId16"/>
-    <sheet name="Interventions for children" sheetId="28" r:id="rId17"/>
-    <sheet name="Interventions family planning" sheetId="34" r:id="rId18"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId19"/>
+    <sheet name="IYCF target pop" sheetId="35" r:id="rId12"/>
+    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId13"/>
+    <sheet name="Interventions target population" sheetId="21" r:id="rId14"/>
+    <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId15"/>
+    <sheet name="Interventions anemia" sheetId="30" r:id="rId16"/>
+    <sheet name="Interventions wasting" sheetId="31" r:id="rId17"/>
+    <sheet name="Interventions for children" sheetId="28" r:id="rId18"/>
+    <sheet name="Interventions family planning" sheetId="34" r:id="rId19"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -3625,7 +3626,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="217">
   <si>
     <t>year</t>
   </si>
@@ -7878,16 +7879,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8060,6 +8061,109 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0.3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -8127,7 +8231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
@@ -9302,7 +9406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -9536,7 +9640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -10992,7 +11096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -11083,7 +11187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -11731,7 +11835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -11831,735 +11935,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="14">
-        <v>0.61</v>
-      </c>
-      <c r="C2" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D2" s="14">
-        <v>3.56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="14">
-        <v>0</v>
-      </c>
-      <c r="C3" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="14">
-        <v>0.621</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="14">
-        <v>0.247</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D5" s="14">
-        <v>3.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D6" s="14">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="63">
-        <v>0</v>
-      </c>
-      <c r="C7" s="64">
-        <v>0.85</v>
-      </c>
-      <c r="D7" s="70">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="34">
-        <v>0</v>
-      </c>
-      <c r="C8" s="34">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="19">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="63">
-        <v>0</v>
-      </c>
-      <c r="C9" s="64">
-        <v>0.85</v>
-      </c>
-      <c r="D9" s="70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="34">
-        <v>0</v>
-      </c>
-      <c r="C10" s="34">
-        <v>0.85</v>
-      </c>
-      <c r="D10" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D11" s="14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="65">
-        <v>0</v>
-      </c>
-      <c r="C12" s="66">
-        <v>0.85</v>
-      </c>
-      <c r="D12" s="66">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" s="14">
-        <v>0</v>
-      </c>
-      <c r="C13" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D13" s="14">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="65">
-        <v>0</v>
-      </c>
-      <c r="C14" s="66">
-        <v>0.85</v>
-      </c>
-      <c r="D14" s="66">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" s="14">
-        <v>0</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D15" s="14">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" s="14">
-        <v>0</v>
-      </c>
-      <c r="C16" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D16" s="14">
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="14">
-        <v>0</v>
-      </c>
-      <c r="C17" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="14">
-        <v>0</v>
-      </c>
-      <c r="C18" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D18" s="14">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="14">
-        <v>0</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D19" s="14">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" s="14">
-        <v>0</v>
-      </c>
-      <c r="C20" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D20" s="14">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="14">
-        <v>0</v>
-      </c>
-      <c r="C21" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D21" s="14">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>159</v>
-      </c>
-      <c r="B22" s="14">
-        <v>0</v>
-      </c>
-      <c r="C22" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D22" s="14">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="14">
-        <v>0</v>
-      </c>
-      <c r="C23" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D23" s="14">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B24" s="14">
-        <v>0</v>
-      </c>
-      <c r="C24" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D24" s="14">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25" s="14">
-        <v>0</v>
-      </c>
-      <c r="C25" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D25" s="14">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>166</v>
-      </c>
-      <c r="B26" s="14">
-        <v>0</v>
-      </c>
-      <c r="C26" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D26" s="14">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>167</v>
-      </c>
-      <c r="B27" s="14">
-        <v>0</v>
-      </c>
-      <c r="C27" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D27" s="14">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B28" s="14">
-        <v>0</v>
-      </c>
-      <c r="C28" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D28" s="14">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>169</v>
-      </c>
-      <c r="B29" s="14">
-        <v>0</v>
-      </c>
-      <c r="C29" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D29" s="14">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>170</v>
-      </c>
-      <c r="B30" s="14">
-        <v>0</v>
-      </c>
-      <c r="C30" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D30" s="14">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="14">
-        <v>0</v>
-      </c>
-      <c r="C31" s="14">
-        <v>0.12</v>
-      </c>
-      <c r="D31" s="19">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="14">
-        <v>0</v>
-      </c>
-      <c r="C32" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="D32" s="19">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="14">
-        <v>0</v>
-      </c>
-      <c r="C33" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="D33" s="19">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="14">
-        <v>0</v>
-      </c>
-      <c r="C34" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D34" s="19">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B35" s="19">
-        <v>0</v>
-      </c>
-      <c r="C35" s="14">
-        <v>0.12</v>
-      </c>
-      <c r="D35" s="19">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" s="19">
-        <v>0</v>
-      </c>
-      <c r="C36" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="D36" s="19">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B37" s="19">
-        <v>0</v>
-      </c>
-      <c r="C37" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="D37" s="19">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="C38" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D38" s="19">
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B39" s="14">
-        <v>0</v>
-      </c>
-      <c r="C39" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D39" s="19">
-        <f>180</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B40" s="14">
-        <v>0</v>
-      </c>
-      <c r="C40" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D40" s="19">
-        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
-        <v>10.046400000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="14">
-        <v>0.61</v>
-      </c>
-      <c r="C41" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D41" s="19">
-        <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
-        <v>19.933477200000002</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="83" t="s">
-        <v>206</v>
-      </c>
-      <c r="B42" s="85">
-        <v>0.09</v>
-      </c>
-      <c r="C42" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D42" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="83" t="s">
-        <v>207</v>
-      </c>
-      <c r="B43" s="85">
-        <v>0.02</v>
-      </c>
-      <c r="C43" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D43" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="83" t="s">
-        <v>208</v>
-      </c>
-      <c r="B44" s="85">
-        <v>0.08</v>
-      </c>
-      <c r="C44" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D44" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="83" t="s">
-        <v>211</v>
-      </c>
-      <c r="B45" s="85">
-        <v>0.18</v>
-      </c>
-      <c r="C45" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D45" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="83" t="s">
-        <v>212</v>
-      </c>
-      <c r="B46" s="85">
-        <v>0.02</v>
-      </c>
-      <c r="C46" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D46" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="83" t="s">
-        <v>209</v>
-      </c>
-      <c r="B47" s="85">
-        <v>0.45</v>
-      </c>
-      <c r="C47" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D47" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="83" t="s">
-        <v>210</v>
-      </c>
-      <c r="B48" s="85">
-        <v>0.03</v>
-      </c>
-      <c r="C48" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D48" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="B49" s="85">
-        <v>0.11</v>
-      </c>
-      <c r="C49" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D49" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="83" t="s">
-        <v>214</v>
-      </c>
-      <c r="B50" s="85">
-        <v>0.01</v>
-      </c>
-      <c r="C50" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D50" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C51" s="86"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13204,6 +12579,735 @@
       <c r="L15" s="55">
         <v>196948400</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0.61</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D2" s="14">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.621</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.247</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D6" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="63">
+        <v>0</v>
+      </c>
+      <c r="C7" s="64">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="34">
+        <v>0</v>
+      </c>
+      <c r="C8" s="34">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="19">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="63">
+        <v>0</v>
+      </c>
+      <c r="C9" s="64">
+        <v>0.85</v>
+      </c>
+      <c r="D9" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="34">
+        <v>0</v>
+      </c>
+      <c r="C10" s="34">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D11" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="65">
+        <v>0</v>
+      </c>
+      <c r="C12" s="66">
+        <v>0.85</v>
+      </c>
+      <c r="D12" s="66">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D13" s="14">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="65">
+        <v>0</v>
+      </c>
+      <c r="C14" s="66">
+        <v>0.85</v>
+      </c>
+      <c r="D14" s="66">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="14">
+        <v>0</v>
+      </c>
+      <c r="C18" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="14">
+        <v>0</v>
+      </c>
+      <c r="C21" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="14">
+        <v>0</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D22" s="14">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="14">
+        <v>0</v>
+      </c>
+      <c r="C23" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="14">
+        <v>0</v>
+      </c>
+      <c r="C24" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="14">
+        <v>0</v>
+      </c>
+      <c r="C25" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D25" s="14">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="14">
+        <v>0</v>
+      </c>
+      <c r="C26" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D26" s="14">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="14">
+        <v>0</v>
+      </c>
+      <c r="C27" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D27" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="14">
+        <v>0</v>
+      </c>
+      <c r="C28" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="14">
+        <v>0</v>
+      </c>
+      <c r="C29" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D29" s="14">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="14">
+        <v>0</v>
+      </c>
+      <c r="C30" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D30" s="14">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="14">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="D31" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="14">
+        <v>0</v>
+      </c>
+      <c r="C32" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="D32" s="19">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="14">
+        <v>0</v>
+      </c>
+      <c r="C33" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D33" s="19">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="14">
+        <v>0</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D34" s="19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="19">
+        <v>0</v>
+      </c>
+      <c r="C35" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="D35" s="19">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="19">
+        <v>0</v>
+      </c>
+      <c r="C36" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="D36" s="19">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="19">
+        <v>0</v>
+      </c>
+      <c r="C37" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D37" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C38" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D38" s="19">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="14">
+        <v>0</v>
+      </c>
+      <c r="C39" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D39" s="19">
+        <f>180</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" s="14">
+        <v>0</v>
+      </c>
+      <c r="C40" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D40" s="19">
+        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
+        <v>10.046400000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="14">
+        <v>0.61</v>
+      </c>
+      <c r="C41" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D41" s="19">
+        <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
+        <v>19.933477200000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" s="85">
+        <v>0.09</v>
+      </c>
+      <c r="C42" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D42" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="83" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="85">
+        <v>0.02</v>
+      </c>
+      <c r="C43" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D43" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" s="85">
+        <v>0.08</v>
+      </c>
+      <c r="C44" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D44" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="B45" s="85">
+        <v>0.18</v>
+      </c>
+      <c r="C45" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D45" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="83" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="85">
+        <v>0.02</v>
+      </c>
+      <c r="C46" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D46" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="B47" s="85">
+        <v>0.45</v>
+      </c>
+      <c r="C47" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D47" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="83" t="s">
+        <v>210</v>
+      </c>
+      <c r="B48" s="85">
+        <v>0.03</v>
+      </c>
+      <c r="C48" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D48" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="85">
+        <v>0.11</v>
+      </c>
+      <c r="C49" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D49" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" s="85">
+        <v>0.01</v>
+      </c>
+      <c r="C50" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D50" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C51" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added fractions exposed to delivery modality for IYCF
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="460" windowWidth="20580" windowHeight="13460" tabRatio="500" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,54 +121,6 @@
           </rPr>
           <t xml:space="preserve">
 per 100,000 live births</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction of pregnancies ending in spontaneous abortion</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Number of stillbirths per 1000 TOTAL births</t>
         </r>
       </text>
     </comment>
@@ -192,7 +144,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+Fraction of pregnancies ending in spontaneous abortion</t>
         </r>
       </text>
     </comment>
@@ -216,7 +168,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+Number of stillbirths per 1000 TOTAL births</t>
         </r>
       </text>
     </comment>
@@ -244,7 +196,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0">
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Per 1000 live births</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Per 1000 live births</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="0">
+    <comment ref="A28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0">
+    <comment ref="A34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3626,7 +3626,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="219">
   <si>
     <t>year</t>
   </si>
@@ -4277,6 +4277,12 @@
   </si>
   <si>
     <t>Effectiveness</t>
+  </si>
+  <si>
+    <t>fraction PW attending health facility</t>
+  </si>
+  <si>
+    <t>fraction children attending health facility</t>
   </si>
 </sst>
 </file>
@@ -5068,7 +5074,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5208,6 +5214,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="555">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7064,10 +7071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7119,7 +7126,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="18">
-        <f>(C3+C3*C13/(1000-C13))/(1-C12)</f>
+        <f>(C3+C3*C15/(1000-C15))/(1-C14)</f>
         <v>3677298.8269880489</v>
       </c>
     </row>
@@ -7148,184 +7155,200 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="33"/>
+      <c r="B9" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" s="89">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="10"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="89">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+      <c r="B11" s="33"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="10"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C13" s="19">
         <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C12" s="19">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="19">
-        <v>25.36</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" s="19">
-        <v>25.4</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C15" s="19">
-        <v>34.68</v>
+        <v>25.36</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="19">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="19">
+        <v>34.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C18" s="19">
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="10"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="10" t="s">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="10"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B21" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C21" s="44">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="44">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="44">
-        <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C22" s="44">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="44">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="44">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C25" s="44">
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="33"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="33"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B28" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="52">
+      <c r="C28" s="52">
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C29" s="52">
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="51" t="s">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="52">
+      <c r="C30" s="52">
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="51" t="s">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="52">
+      <c r="C31" s="52">
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="51"/>
-      <c r="C30" s="53"/>
-    </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+      <c r="B32" s="51"/>
+      <c r="C32" s="53"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B34" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C34" s="43">
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="50" t="s">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C35" s="43">
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="50" t="s">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C36" s="43">
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="50" t="s">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C37" s="43">
         <v>1.2542476833820825E-2</v>
       </c>
     </row>
@@ -8063,8 +8086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8092,6 +8115,7 @@
         <v>81</v>
       </c>
       <c r="B2">
+        <f>'Baseline year demographics'!C9</f>
         <v>0.5</v>
       </c>
       <c r="C2">
@@ -8106,6 +8130,7 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <f>'Baseline year demographics'!C10</f>
         <v>0.3</v>
       </c>
       <c r="C3">
@@ -8120,6 +8145,7 @@
         <v>7</v>
       </c>
       <c r="B4">
+        <f>'Baseline year demographics'!C10</f>
         <v>0.3</v>
       </c>
       <c r="C4">
@@ -8134,6 +8160,7 @@
         <v>8</v>
       </c>
       <c r="B5">
+        <f>'Baseline year demographics'!C10</f>
         <v>0.3</v>
       </c>
       <c r="C5">
@@ -8148,6 +8175,7 @@
         <v>9</v>
       </c>
       <c r="B6">
+        <f>'Baseline year demographics'!C10</f>
         <v>0.3</v>
       </c>
       <c r="C6">
@@ -9159,23 +9187,23 @@
         <v>0</v>
       </c>
       <c r="E37" s="35">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="F37" s="35">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="G37" s="35">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="H37" s="35">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="I37" s="35">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
     </row>
@@ -9190,23 +9218,23 @@
         <v>0</v>
       </c>
       <c r="E38" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="F38" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="G38" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="H38" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="I38" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
     </row>
@@ -9221,23 +9249,23 @@
         <v>0</v>
       </c>
       <c r="E39" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="F39" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="G39" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="H39" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="I39" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
     </row>
@@ -9311,23 +9339,23 @@
         <v>0</v>
       </c>
       <c r="E42" s="71">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="F42" s="71">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="G42" s="71">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="H42" s="71">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="I42" s="71">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
     </row>
@@ -9342,23 +9370,23 @@
         <v>0</v>
       </c>
       <c r="E43" s="69">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="F43" s="69">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="G43" s="69">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="H43" s="69">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="I43" s="69">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
     </row>
@@ -9373,23 +9401,23 @@
         <v>0</v>
       </c>
       <c r="E44" s="69">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="F44" s="69">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="G44" s="69">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="H44" s="69">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="I44" s="69">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added IYCF 'Mass media' in different format to ORs sheet for convenience
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15200" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15200" tabRatio="500" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3544,7 +3544,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3626,7 +3626,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="219">
   <si>
     <t>year</t>
   </si>
@@ -4517,7 +4517,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="555">
+  <cellStyleXfs count="565">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4529,6 +4529,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5216,7 +5226,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="555">
+  <cellStyles count="565">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5494,6 +5504,11 @@
     <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5770,6 +5785,11 @@
     <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7073,8 +7093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7361,10 +7381,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7449,38 +7469,44 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="73">
+        <f>D17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E4" s="73">
+        <f t="shared" ref="E4:H4" si="0">E17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F4" s="73">
+        <f t="shared" si="0"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G4" s="73">
+        <f t="shared" si="0"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H4" s="73">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="73"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B5" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D5" s="73">
         <v>2.0299999999999998</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E5" s="73">
         <v>3.07</v>
-      </c>
-      <c r="F4" s="73">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G4" s="73">
-        <v>1.05</v>
-      </c>
-      <c r="H4" s="75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="88"/>
-      <c r="C5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="73">
-        <v>2.17</v>
-      </c>
-      <c r="E5" s="73">
-        <v>2.48</v>
       </c>
       <c r="F5" s="73">
         <v>1.1499999999999999</v>
@@ -7493,23 +7519,21 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="88" t="s">
-        <v>7</v>
-      </c>
+      <c r="B6" s="88"/>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D6" s="73">
-        <v>1</v>
+        <v>2.17</v>
       </c>
       <c r="E6" s="73">
-        <v>1.5</v>
+        <v>2.48</v>
       </c>
       <c r="F6" s="73">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G6" s="73">
-        <v>1.1499999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="H6" s="75">
         <v>1</v>
@@ -7518,27 +7542,32 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B7" s="88"/>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D7" s="73">
-        <v>1</v>
+        <f>D17^(1/5)</f>
+        <v>1.0098057976734853</v>
       </c>
       <c r="E7" s="73">
-        <v>1.5</v>
+        <f t="shared" ref="E7:H7" si="1">E17^(1/5)</f>
+        <v>1.0098057976734853</v>
       </c>
       <c r="F7" s="73">
-        <v>1.25</v>
+        <f t="shared" si="1"/>
+        <v>1.0098057976734853</v>
       </c>
       <c r="G7" s="73">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H7" s="75">
+        <f t="shared" si="1"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H7" s="73">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B8" s="88" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>193</v>
@@ -7547,10 +7576,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="73">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F8" s="73">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="G8" s="73">
         <v>1.1499999999999999</v>
@@ -7568,10 +7597,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="73">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F9" s="73">
-        <v>1.1499999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="G9" s="73">
         <v>1.1000000000000001</v>
@@ -7581,85 +7610,104 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="73">
+        <f>D17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E10" s="73">
+        <f t="shared" ref="E10:H10" si="2">E17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F10" s="73">
+        <f t="shared" si="2"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G10" s="73">
+        <f t="shared" si="2"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H10" s="73">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B11" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="73">
+        <v>1</v>
+      </c>
+      <c r="E11" s="73">
+        <v>1</v>
+      </c>
+      <c r="F11" s="73">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G11" s="73">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H11" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B12" s="88"/>
+      <c r="C12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="73">
+        <v>1</v>
+      </c>
+      <c r="E12" s="73">
+        <v>1</v>
+      </c>
+      <c r="F12" s="73">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G12" s="73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H12" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B13" s="88"/>
+      <c r="C13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="73">
+        <f>D17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E13" s="73">
+        <f t="shared" ref="E13:H13" si="3">E17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F13" s="73">
+        <f t="shared" si="3"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G13" s="73">
+        <f t="shared" si="3"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H13" s="73">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B14" s="88" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="73">
-        <v>1</v>
-      </c>
-      <c r="E10" s="73">
-        <v>1</v>
-      </c>
-      <c r="F10" s="73">
-        <v>1</v>
-      </c>
-      <c r="G10" s="73">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H10" s="75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="88"/>
-      <c r="C11" t="s">
-        <v>194</v>
-      </c>
-      <c r="D11" s="73">
-        <v>1</v>
-      </c>
-      <c r="E11" s="73">
-        <v>1</v>
-      </c>
-      <c r="F11" s="73">
-        <v>1</v>
-      </c>
-      <c r="G11" s="73">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H11" s="75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="79" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" s="81">
-        <v>1.05</v>
-      </c>
-      <c r="E12" s="81">
-        <v>1.05</v>
-      </c>
-      <c r="F12" s="81">
-        <v>1.05</v>
-      </c>
-      <c r="G12" s="81">
-        <v>1.05</v>
-      </c>
-      <c r="H12" s="81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="77" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="88" t="s">
-        <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>193</v>
@@ -7671,12 +7719,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G14" s="73">
-        <v>1.05</v>
-      </c>
-      <c r="H14" s="73">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H14" s="75">
         <v>1</v>
       </c>
     </row>
@@ -7692,150 +7740,147 @@
         <v>1</v>
       </c>
       <c r="F15" s="73">
+        <v>1</v>
+      </c>
+      <c r="G15" s="73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H15" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="88"/>
+      <c r="C16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="73">
+        <f>D17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E16" s="73">
+        <f>E17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F16" s="73">
+        <f t="shared" ref="F16:H16" si="4">F17^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G16" s="73">
+        <f t="shared" si="4"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H16" s="73">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="81">
         <v>1.05</v>
       </c>
-      <c r="G15" s="73">
+      <c r="E17" s="81">
         <v>1.05</v>
       </c>
-      <c r="H15" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="F17" s="81">
+        <v>1.05</v>
+      </c>
+      <c r="G17" s="81">
+        <v>1.05</v>
+      </c>
+      <c r="H17" s="81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="77" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
         <v>193</v>
       </c>
-      <c r="D16" s="73">
-        <v>1</v>
-      </c>
-      <c r="E16" s="73">
-        <v>1</v>
-      </c>
-      <c r="F16" s="73">
+      <c r="D19" s="73">
+        <v>1</v>
+      </c>
+      <c r="E19" s="73">
+        <v>1</v>
+      </c>
+      <c r="F19" s="73">
         <v>1.05</v>
       </c>
-      <c r="G16" s="73">
+      <c r="G19" s="73">
         <v>1.05</v>
       </c>
-      <c r="H16" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="88"/>
-      <c r="C17" t="s">
+      <c r="H19" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="88"/>
+      <c r="C20" t="s">
         <v>194</v>
       </c>
-      <c r="D17" s="73">
-        <v>1</v>
-      </c>
-      <c r="E17" s="73">
-        <v>1</v>
-      </c>
-      <c r="F17" s="73">
+      <c r="D20" s="73">
+        <v>1</v>
+      </c>
+      <c r="E20" s="73">
+        <v>1</v>
+      </c>
+      <c r="F20" s="73">
         <v>1.05</v>
       </c>
-      <c r="G17" s="73">
+      <c r="G20" s="73">
         <v>1.05</v>
       </c>
-      <c r="H17" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D18" s="73">
-        <v>1</v>
-      </c>
-      <c r="E18" s="73">
-        <v>1</v>
-      </c>
-      <c r="F18" s="73">
-        <v>2.5</v>
-      </c>
-      <c r="G18" s="73">
-        <v>2.5</v>
-      </c>
-      <c r="H18" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="88"/>
-      <c r="C19" t="s">
-        <v>194</v>
-      </c>
-      <c r="D19" s="73">
-        <v>1</v>
-      </c>
-      <c r="E19" s="73">
-        <v>1</v>
-      </c>
-      <c r="F19" s="73">
-        <v>2.4</v>
-      </c>
-      <c r="G19" s="73">
-        <v>2.4</v>
-      </c>
-      <c r="H19" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="88" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>193</v>
-      </c>
-      <c r="D20" s="73">
-        <v>1</v>
-      </c>
-      <c r="E20" s="73">
-        <v>1</v>
-      </c>
-      <c r="F20" s="73">
-        <v>2</v>
-      </c>
-      <c r="G20" s="73">
-        <v>2</v>
-      </c>
       <c r="H20" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B21" s="88"/>
       <c r="C21" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D21" s="73">
-        <v>1</v>
+        <f>D34^(1/5)</f>
+        <v>1.0098057976734853</v>
       </c>
       <c r="E21" s="73">
-        <v>1</v>
+        <f t="shared" ref="E21:H21" si="5">E34^(1/5)</f>
+        <v>1.0098057976734853</v>
       </c>
       <c r="F21" s="73">
-        <v>1.9</v>
+        <f t="shared" si="5"/>
+        <v>1.0098057976734853</v>
       </c>
       <c r="G21" s="73">
-        <v>1.9</v>
+        <f t="shared" si="5"/>
+        <v>1.0098057976734853</v>
       </c>
       <c r="H21" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B22" s="88" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>193</v>
@@ -7847,16 +7892,16 @@
         <v>1</v>
       </c>
       <c r="F22" s="73">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="G22" s="73">
-        <v>2</v>
+        <v>1.05</v>
       </c>
       <c r="H22" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B23" s="88"/>
       <c r="C23" t="s">
         <v>194</v>
@@ -7868,50 +7913,286 @@
         <v>1</v>
       </c>
       <c r="F23" s="73">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="G23" s="73">
-        <v>1.9</v>
+        <v>1.05</v>
       </c>
       <c r="H23" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="80" t="s">
-        <v>112</v>
-      </c>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="88"/>
       <c r="C24" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="81">
+      <c r="D24" s="73">
+        <f>D34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E24" s="73">
+        <f t="shared" ref="E24:H24" si="6">E34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F24" s="73">
+        <f t="shared" si="6"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G24" s="73">
+        <f t="shared" si="6"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H24" s="73">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B25" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" s="73">
+        <v>1</v>
+      </c>
+      <c r="E25" s="73">
+        <v>1</v>
+      </c>
+      <c r="F25" s="73">
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="73">
+        <v>2.5</v>
+      </c>
+      <c r="H25" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B26" s="88"/>
+      <c r="C26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="73">
+        <v>1</v>
+      </c>
+      <c r="E26" s="73">
+        <v>1</v>
+      </c>
+      <c r="F26" s="73">
+        <v>2.4</v>
+      </c>
+      <c r="G26" s="73">
+        <v>2.4</v>
+      </c>
+      <c r="H26" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B27" s="88"/>
+      <c r="C27" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" s="73">
+        <f>D34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E27" s="73">
+        <f t="shared" ref="E27:H27" si="7">E34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F27" s="73">
+        <f t="shared" si="7"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G27" s="73">
+        <f t="shared" si="7"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H27" s="73">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B28" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" s="73">
+        <v>1</v>
+      </c>
+      <c r="E28" s="73">
+        <v>1</v>
+      </c>
+      <c r="F28" s="73">
+        <v>2</v>
+      </c>
+      <c r="G28" s="73">
+        <v>2</v>
+      </c>
+      <c r="H28" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B29" s="88"/>
+      <c r="C29" t="s">
+        <v>194</v>
+      </c>
+      <c r="D29" s="73">
+        <v>1</v>
+      </c>
+      <c r="E29" s="73">
+        <v>1</v>
+      </c>
+      <c r="F29" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="G29" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="H29" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B30" s="88"/>
+      <c r="C30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="73">
+        <f>D34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E30" s="73">
+        <f t="shared" ref="E30:H30" si="8">E34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F30" s="73">
+        <f t="shared" si="8"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G30" s="73">
+        <f t="shared" si="8"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H30" s="73">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B31" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" s="73">
+        <v>1</v>
+      </c>
+      <c r="E31" s="73">
+        <v>1</v>
+      </c>
+      <c r="F31" s="73">
+        <v>1</v>
+      </c>
+      <c r="G31" s="73">
+        <v>2</v>
+      </c>
+      <c r="H31" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B32" s="88"/>
+      <c r="C32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="73">
+        <v>1</v>
+      </c>
+      <c r="E32" s="73">
+        <v>1</v>
+      </c>
+      <c r="F32" s="73">
+        <v>1</v>
+      </c>
+      <c r="G32" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="H32" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B33" s="88"/>
+      <c r="C33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="73">
+        <f>D34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="E33" s="73">
+        <f t="shared" ref="E33:H33" si="9">E34^(1/5)</f>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="F33" s="73">
+        <f t="shared" si="9"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="G33" s="73">
+        <f t="shared" si="9"/>
+        <v>1.0098057976734853</v>
+      </c>
+      <c r="H33" s="73">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B34" s="80" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" t="s">
+        <v>204</v>
+      </c>
+      <c r="D34" s="81">
         <v>1.05</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E34" s="81">
         <v>1.05</v>
       </c>
-      <c r="F24" s="81">
+      <c r="F34" s="81">
         <v>1.05</v>
       </c>
-      <c r="G24" s="81">
+      <c r="G34" s="81">
         <v>1.05</v>
       </c>
-      <c r="H24" s="81">
+      <c r="H34" s="81">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7922,8 +8203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7957,6 +8238,9 @@
       <c r="B2" t="s">
         <v>81</v>
       </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
       <c r="E2" s="82"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -8087,7 +8371,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added ORs for CFE covering 'everyone' and PPCF covering those poor
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Nov/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -28,13 +33,13 @@
     <sheet name="Interventions family planning" sheetId="34" r:id="rId19"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -3454,8 +3459,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
+    <author>Sam</author>
     <author xml:space="preserve"> Janka Petravic</author>
-    <author>Sam</author>
   </authors>
   <commentList>
     <comment ref="F5" authorId="0">
@@ -3482,11 +3487,59 @@
         </r>
       </text>
     </comment>
+    <comment ref="B11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This 'dilutes' OR so that we 'cover' everyone with IYCF</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B12" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This assumes we deliver PPCF with education to the poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
@@ -3506,7 +3559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="1">
+    <comment ref="B15" authorId="2">
       <text>
         <r>
           <rPr>
@@ -3530,7 +3583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="2">
+    <comment ref="C17" authorId="1">
       <text>
         <r>
           <rPr>
@@ -3646,7 +3699,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="222">
   <si>
     <t>year</t>
   </si>
@@ -4306,6 +4359,12 @@
   </si>
   <si>
     <t>unmet need for family planning</t>
+  </si>
+  <si>
+    <t>Complementary feeding (adjusted food secure without promotion)</t>
+  </si>
+  <si>
+    <t>Public provision of complementary foods (food insecure)</t>
   </si>
 </sst>
 </file>
@@ -4446,7 +4505,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4501,6 +4560,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -5106,7 +5171,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5248,6 +5313,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="565">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7116,17 +7182,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>114</v>
       </c>
@@ -7137,7 +7203,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -7148,7 +7214,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -7156,7 +7222,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="33" t="s">
         <v>135</v>
       </c>
@@ -7164,7 +7230,7 @@
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -7173,7 +7239,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="33" t="s">
         <v>72</v>
       </c>
@@ -7181,7 +7247,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
@@ -7189,7 +7255,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="33" t="s">
         <v>73</v>
       </c>
@@ -7197,7 +7263,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>217</v>
       </c>
@@ -7205,7 +7271,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>218</v>
       </c>
@@ -7213,7 +7279,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>219</v>
       </c>
@@ -7221,14 +7287,14 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="33"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
         <v>141</v>
       </c>
@@ -7239,7 +7305,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>136</v>
       </c>
@@ -7247,7 +7313,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>137</v>
       </c>
@@ -7255,7 +7321,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>138</v>
       </c>
@@ -7263,7 +7329,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>139</v>
       </c>
@@ -7271,7 +7337,7 @@
         <v>34.68</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>140</v>
       </c>
@@ -7279,11 +7345,11 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
         <v>75</v>
       </c>
@@ -7294,7 +7360,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="33" t="s">
         <v>106</v>
       </c>
@@ -7302,7 +7368,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="33" t="s">
         <v>107</v>
       </c>
@@ -7310,7 +7376,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="33" t="s">
         <v>108</v>
       </c>
@@ -7318,7 +7384,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="33" t="s">
         <v>76</v>
       </c>
@@ -7326,10 +7392,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="33"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>134</v>
       </c>
@@ -7340,7 +7406,7 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="51" t="s">
         <v>128</v>
       </c>
@@ -7348,7 +7414,7 @@
         <v>13550000</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="51" t="s">
         <v>129</v>
       </c>
@@ -7356,7 +7422,7 @@
         <v>12394000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="51" t="s">
         <v>130</v>
       </c>
@@ -7364,11 +7430,11 @@
         <v>9148000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="51"/>
       <c r="C33" s="53"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>125</v>
       </c>
@@ -7379,7 +7445,7 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="50" t="s">
         <v>128</v>
       </c>
@@ -7387,7 +7453,7 @@
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="50" t="s">
         <v>129</v>
       </c>
@@ -7395,7 +7461,7 @@
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="50" t="s">
         <v>130</v>
       </c>
@@ -7407,11 +7473,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7423,14 +7484,14 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>196</v>
       </c>
@@ -7456,7 +7517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
@@ -7482,7 +7543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B3" s="90"/>
       <c r="C3" t="s">
         <v>194</v>
@@ -7504,7 +7565,7 @@
       </c>
       <c r="J3" s="73"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B4" s="90"/>
       <c r="C4" t="s">
         <v>204</v>
@@ -7531,7 +7592,7 @@
       </c>
       <c r="J4" s="73"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B5" s="90" t="s">
         <v>6</v>
       </c>
@@ -7554,7 +7615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B6" s="90"/>
       <c r="C6" t="s">
         <v>194</v>
@@ -7575,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B7" s="90"/>
       <c r="C7" t="s">
         <v>204</v>
@@ -7601,7 +7662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B8" s="90" t="s">
         <v>7</v>
       </c>
@@ -7624,7 +7685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B9" s="90"/>
       <c r="C9" t="s">
         <v>194</v>
@@ -7645,7 +7706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B10" s="90"/>
       <c r="C10" t="s">
         <v>204</v>
@@ -7671,7 +7732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B11" s="90" t="s">
         <v>8</v>
       </c>
@@ -7694,7 +7755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B12" s="90"/>
       <c r="C12" t="s">
         <v>194</v>
@@ -7715,7 +7776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B13" s="90"/>
       <c r="C13" t="s">
         <v>204</v>
@@ -7741,7 +7802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B14" s="90" t="s">
         <v>9</v>
       </c>
@@ -7764,7 +7825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B15" s="90"/>
       <c r="C15" t="s">
         <v>194</v>
@@ -7785,7 +7846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B16" s="90"/>
       <c r="C16" t="s">
         <v>204</v>
@@ -7811,7 +7872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B17" s="87" t="s">
         <v>112</v>
       </c>
@@ -7834,14 +7895,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D18" s="75"/>
       <c r="E18" s="75"/>
       <c r="F18" s="75"/>
       <c r="G18" s="75"/>
       <c r="H18" s="75"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="77" t="s">
         <v>198</v>
       </c>
@@ -7867,7 +7928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B20" s="90"/>
       <c r="C20" t="s">
         <v>194</v>
@@ -7888,7 +7949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B21" s="90"/>
       <c r="C21" t="s">
         <v>204</v>
@@ -7914,7 +7975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B22" s="90" t="s">
         <v>6</v>
       </c>
@@ -7937,7 +7998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B23" s="90"/>
       <c r="C23" t="s">
         <v>194</v>
@@ -7958,7 +8019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B24" s="90"/>
       <c r="C24" t="s">
         <v>204</v>
@@ -7984,7 +8045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B25" s="90" t="s">
         <v>7</v>
       </c>
@@ -8007,7 +8068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B26" s="90"/>
       <c r="C26" t="s">
         <v>194</v>
@@ -8028,7 +8089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B27" s="90"/>
       <c r="C27" t="s">
         <v>204</v>
@@ -8054,7 +8115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B28" s="90" t="s">
         <v>8</v>
       </c>
@@ -8077,7 +8138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B29" s="90"/>
       <c r="C29" t="s">
         <v>194</v>
@@ -8098,7 +8159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B30" s="90"/>
       <c r="C30" t="s">
         <v>204</v>
@@ -8124,7 +8185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B31" s="90" t="s">
         <v>9</v>
       </c>
@@ -8147,7 +8208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B32" s="90"/>
       <c r="C32" t="s">
         <v>194</v>
@@ -8168,7 +8229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B33" s="90"/>
       <c r="C33" t="s">
         <v>204</v>
@@ -8194,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B34" s="79" t="s">
         <v>112</v>
       </c>
@@ -8232,11 +8293,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8248,14 +8304,14 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>200</v>
       </c>
@@ -8272,7 +8328,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>201</v>
       </c>
@@ -8281,25 +8337,25 @@
       </c>
       <c r="E2" s="81"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="81"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="81"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="81"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -8308,7 +8364,7 @@
       </c>
       <c r="E6" s="81"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>112</v>
       </c>
@@ -8318,7 +8374,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>202</v>
       </c>
@@ -8327,38 +8383,38 @@
       </c>
       <c r="E9" s="81"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="81"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="81"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="81"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="81"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="81"/>
       <c r="D14" s="81"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
         <v>203</v>
       </c>
@@ -8367,31 +8423,31 @@
       </c>
       <c r="E16" s="81"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="81"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="81"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="81"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="81"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>112</v>
       </c>
@@ -8401,11 +8457,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8417,9 +8468,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>199</v>
       </c>
@@ -8433,7 +8484,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -8448,7 +8499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -8463,7 +8514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -8478,7 +8529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -8493,7 +8544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -8510,11 +8561,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8529,12 +8575,12 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -8551,7 +8597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
@@ -8568,14 +8614,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -8584,11 +8630,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8600,7 +8641,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="54.83203125" customWidth="1"/>
@@ -8611,7 +8652,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>85</v>
       </c>
@@ -8641,7 +8682,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>80</v>
       </c>
@@ -8670,7 +8711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>176</v>
@@ -8697,7 +8738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>50</v>
       </c>
@@ -8723,7 +8764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="76" t="s">
         <v>57</v>
       </c>
@@ -8749,7 +8790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>161</v>
       </c>
@@ -8777,7 +8818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>84</v>
       </c>
@@ -8806,7 +8847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>172</v>
       </c>
@@ -8834,7 +8875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>83</v>
       </c>
@@ -8863,7 +8904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>173</v>
       </c>
@@ -8892,7 +8933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>179</v>
       </c>
@@ -8918,7 +8959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>189</v>
       </c>
@@ -8944,7 +8985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="4" t="s">
         <v>190</v>
       </c>
@@ -8970,7 +9011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>81</v>
       </c>
@@ -9000,7 +9041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>171</v>
@@ -9027,7 +9068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>174</v>
       </c>
@@ -9054,7 +9095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="4" t="s">
         <v>86</v>
       </c>
@@ -9080,7 +9121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
         <v>175</v>
       </c>
@@ -9107,7 +9148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>151</v>
       </c>
@@ -9134,7 +9175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
         <v>93</v>
       </c>
@@ -9163,7 +9204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>155</v>
       </c>
@@ -9189,7 +9230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>156</v>
       </c>
@@ -9215,7 +9256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>157</v>
       </c>
@@ -9241,7 +9282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>158</v>
       </c>
@@ -9267,7 +9308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>159</v>
       </c>
@@ -9293,7 +9334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>160</v>
       </c>
@@ -9319,7 +9360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" t="s">
         <v>164</v>
@@ -9346,7 +9387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>165</v>
       </c>
@@ -9372,7 +9413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>166</v>
       </c>
@@ -9398,7 +9439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>167</v>
       </c>
@@ -9424,7 +9465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>168</v>
       </c>
@@ -9450,7 +9491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>169</v>
       </c>
@@ -9476,7 +9517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>170</v>
       </c>
@@ -9502,7 +9543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="85" t="s">
         <v>206</v>
       </c>
@@ -9528,7 +9569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="85" t="s">
         <v>207</v>
       </c>
@@ -9554,7 +9595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="85" t="s">
         <v>208</v>
       </c>
@@ -9580,7 +9621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="85" t="s">
         <v>211</v>
       </c>
@@ -9606,7 +9647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="85" t="s">
         <v>212</v>
       </c>
@@ -9632,7 +9673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="85" t="s">
         <v>209</v>
       </c>
@@ -9658,7 +9699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="85" t="s">
         <v>210</v>
       </c>
@@ -9684,7 +9725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="85" t="s">
         <v>213</v>
       </c>
@@ -9710,7 +9751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="85" t="s">
         <v>214</v>
       </c>
@@ -9736,10 +9777,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
         <v>88</v>
       </c>
@@ -9773,7 +9814,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="4" t="s">
         <v>90</v>
       </c>
@@ -9804,7 +9845,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="4" t="s">
         <v>91</v>
       </c>
@@ -9835,7 +9876,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="15.75" customHeight="1">
+    <row r="49" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="4" t="s">
         <v>109</v>
       </c>
@@ -9861,7 +9902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="15.75" customHeight="1">
+    <row r="50" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
@@ -9894,7 +9935,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="15.75" customHeight="1">
+    <row r="51" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="12" t="s">
         <v>180</v>
       </c>
@@ -9925,7 +9966,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="15.75" customHeight="1">
+    <row r="52" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="12" t="s">
         <v>181</v>
       </c>
@@ -9956,7 +9997,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="15.75" customHeight="1">
+    <row r="53" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="12" t="s">
         <v>182</v>
       </c>
@@ -9987,21 +10028,16 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="15.75" customHeight="1">
+    <row r="57" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="2:9" ht="15.75" customHeight="1">
+    <row r="58" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10016,14 +10052,14 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10043,7 +10079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -10063,7 +10099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>54</v>
       </c>
@@ -10080,7 +10116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -10100,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>54</v>
       </c>
@@ -10117,7 +10153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -10137,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>54</v>
       </c>
@@ -10154,7 +10190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -10174,7 +10210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -10193,7 +10229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -10213,7 +10249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>54</v>
       </c>
@@ -10236,11 +10272,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10255,7 +10286,7 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="56.5" customWidth="1"/>
@@ -10264,7 +10295,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14" customHeight="1">
+    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
@@ -10311,7 +10342,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>152</v>
       </c>
@@ -10358,7 +10389,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
         <v>175</v>
       </c>
@@ -10402,7 +10433,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>171</v>
       </c>
@@ -10446,7 +10477,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>174</v>
       </c>
@@ -10490,7 +10521,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>151</v>
       </c>
@@ -10534,7 +10565,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>154</v>
       </c>
@@ -10578,7 +10609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>155</v>
       </c>
@@ -10622,7 +10653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>156</v>
       </c>
@@ -10666,7 +10697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>157</v>
       </c>
@@ -10710,7 +10741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>158</v>
       </c>
@@ -10754,7 +10785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>159</v>
       </c>
@@ -10798,7 +10829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -10842,7 +10873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>164</v>
       </c>
@@ -10886,7 +10917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>165</v>
       </c>
@@ -10930,7 +10961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>166</v>
       </c>
@@ -10974,7 +11005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>167</v>
       </c>
@@ -11018,7 +11049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>168</v>
       </c>
@@ -11062,7 +11093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>169</v>
       </c>
@@ -11106,7 +11137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>170</v>
       </c>
@@ -11150,7 +11181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B21" s="4" t="s">
         <v>84</v>
       </c>
@@ -11194,7 +11225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14" customHeight="1">
+    <row r="22" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="4" t="s">
         <v>172</v>
       </c>
@@ -11238,7 +11269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B23" s="60" t="s">
         <v>83</v>
       </c>
@@ -11282,7 +11313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B24" s="60" t="s">
         <v>173</v>
       </c>
@@ -11326,7 +11357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B25" s="60" t="s">
         <v>87</v>
       </c>
@@ -11370,7 +11401,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>153</v>
       </c>
@@ -11417,7 +11448,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B28" s="4" t="s">
         <v>90</v>
       </c>
@@ -11461,7 +11492,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B29" s="4" t="s">
         <v>91</v>
       </c>
@@ -11505,7 +11536,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B30" s="4" t="s">
         <v>109</v>
       </c>
@@ -11549,7 +11580,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B31" s="61" t="s">
         <v>180</v>
       </c>
@@ -11593,7 +11624,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B32" s="61" t="s">
         <v>181</v>
       </c>
@@ -11637,7 +11668,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="33" spans="2:15">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B33" s="61" t="s">
         <v>182</v>
       </c>
@@ -11681,27 +11712,22 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B43" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11716,13 +11742,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="32.83203125" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
@@ -11745,7 +11771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>191</v>
       </c>
@@ -11768,7 +11794,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>192</v>
       </c>
@@ -11793,11 +11819,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11812,7 +11833,7 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="39.1640625" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
@@ -11823,7 +11844,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -11849,7 +11870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
@@ -11875,7 +11896,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>68</v>
       </c>
@@ -11895,7 +11916,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -11917,7 +11938,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="60" t="s">
         <v>163</v>
@@ -11941,7 +11962,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>161</v>
       </c>
@@ -11967,7 +11988,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>69</v>
       </c>
@@ -11987,7 +12008,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>183</v>
       </c>
@@ -12010,7 +12031,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>69</v>
       </c>
@@ -12030,7 +12051,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>84</v>
       </c>
@@ -12056,7 +12077,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>69</v>
       </c>
@@ -12076,7 +12097,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>183</v>
       </c>
@@ -12099,7 +12120,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>69</v>
       </c>
@@ -12119,7 +12140,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>172</v>
       </c>
@@ -12145,7 +12166,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>69</v>
       </c>
@@ -12165,7 +12186,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>183</v>
       </c>
@@ -12188,7 +12209,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>69</v>
       </c>
@@ -12208,7 +12229,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -12234,7 +12255,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>69</v>
       </c>
@@ -12255,7 +12276,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>183</v>
       </c>
@@ -12279,7 +12300,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>69</v>
       </c>
@@ -12300,7 +12321,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>180</v>
       </c>
@@ -12327,7 +12348,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="12"/>
       <c r="C23" t="s">
         <v>68</v>
@@ -12349,7 +12370,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>181</v>
       </c>
@@ -12375,7 +12396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="12"/>
       <c r="C25" t="s">
         <v>68</v>
@@ -12396,7 +12417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>182</v>
       </c>
@@ -12422,7 +12443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" t="s">
         <v>68</v>
       </c>
@@ -12446,11 +12467,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12465,13 +12481,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>215</v>
       </c>
@@ -12479,7 +12495,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13">
+    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="85" t="s">
         <v>206</v>
       </c>
@@ -12487,7 +12503,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13">
+    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="85" t="s">
         <v>207</v>
       </c>
@@ -12495,7 +12511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13">
+    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="85" t="s">
         <v>208</v>
       </c>
@@ -12503,7 +12519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13">
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="85" t="s">
         <v>211</v>
       </c>
@@ -12511,7 +12527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13">
+    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="85" t="s">
         <v>212</v>
       </c>
@@ -12519,7 +12535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13">
+    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="85" t="s">
         <v>209</v>
       </c>
@@ -12527,7 +12543,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13">
+    <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="85" t="s">
         <v>210</v>
       </c>
@@ -12535,7 +12551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13">
+    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="85" t="s">
         <v>213</v>
       </c>
@@ -12543,7 +12559,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13">
+    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="85" t="s">
         <v>214</v>
       </c>
@@ -12554,11 +12570,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12570,7 +12581,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -12578,7 +12589,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12616,7 +12627,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -12658,7 +12669,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -12700,7 +12711,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -12742,7 +12753,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -12784,7 +12795,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -12826,7 +12837,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -12868,7 +12879,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -12910,7 +12921,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -12952,7 +12963,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -12994,7 +13005,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -13036,7 +13047,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -13078,7 +13089,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -13120,7 +13131,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -13162,7 +13173,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -13208,11 +13219,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13224,7 +13230,7 @@
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -13232,7 +13238,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -13246,7 +13252,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
@@ -13260,7 +13266,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>176</v>
       </c>
@@ -13274,7 +13280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -13288,7 +13294,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>57</v>
       </c>
@@ -13302,7 +13308,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>161</v>
       </c>
@@ -13316,7 +13322,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>84</v>
       </c>
@@ -13330,7 +13336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>172</v>
       </c>
@@ -13344,7 +13350,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
@@ -13358,7 +13364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>173</v>
       </c>
@@ -13372,7 +13378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -13386,7 +13392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -13400,7 +13406,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -13414,7 +13420,7 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>86</v>
       </c>
@@ -13428,7 +13434,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>175</v>
       </c>
@@ -13442,7 +13448,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>151</v>
       </c>
@@ -13456,7 +13462,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -13470,7 +13476,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -13484,7 +13490,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -13498,7 +13504,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -13512,7 +13518,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>158</v>
       </c>
@@ -13526,7 +13532,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -13540,7 +13546,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>160</v>
       </c>
@@ -13554,7 +13560,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -13568,7 +13574,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>165</v>
       </c>
@@ -13582,7 +13588,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -13596,7 +13602,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>167</v>
       </c>
@@ -13610,7 +13616,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -13624,7 +13630,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -13638,7 +13644,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -13652,7 +13658,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>89</v>
       </c>
@@ -13666,7 +13672,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>90</v>
       </c>
@@ -13680,7 +13686,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>91</v>
       </c>
@@ -13694,7 +13700,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>109</v>
       </c>
@@ -13708,7 +13714,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
         <v>180</v>
       </c>
@@ -13722,7 +13728,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
         <v>181</v>
       </c>
@@ -13736,7 +13742,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
         <v>182</v>
       </c>
@@ -13750,7 +13756,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -13764,7 +13770,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>179</v>
       </c>
@@ -13779,7 +13785,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>189</v>
       </c>
@@ -13794,7 +13800,7 @@
         <v>10.046400000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>190</v>
       </c>
@@ -13809,7 +13815,7 @@
         <v>19.933477200000002</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="82" t="s">
         <v>206</v>
       </c>
@@ -13823,7 +13829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="82" t="s">
         <v>207</v>
       </c>
@@ -13837,7 +13843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="82" t="s">
         <v>208</v>
       </c>
@@ -13851,7 +13857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="82" t="s">
         <v>211</v>
       </c>
@@ -13865,7 +13871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="82" t="s">
         <v>212</v>
       </c>
@@ -13879,7 +13885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="82" t="s">
         <v>209</v>
       </c>
@@ -13893,7 +13899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="82" t="s">
         <v>210</v>
       </c>
@@ -13907,7 +13913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="82" t="s">
         <v>213</v>
       </c>
@@ -13921,7 +13927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="82" t="s">
         <v>214</v>
       </c>
@@ -13935,18 +13941,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C51" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13958,12 +13959,12 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -13986,7 +13987,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -14009,7 +14010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -14032,7 +14033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -14055,7 +14056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -14078,7 +14079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -14101,7 +14102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -14124,7 +14125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -14147,7 +14148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -14170,7 +14171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -14193,7 +14194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -14216,7 +14217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -14239,7 +14240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -14262,7 +14263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -14285,7 +14286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -14308,7 +14309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -14331,7 +14332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -14354,7 +14355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -14377,7 +14378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -14400,7 +14401,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -14423,7 +14424,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -14446,7 +14447,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -14469,7 +14470,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -14492,7 +14493,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -14515,7 +14516,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -14538,7 +14539,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -14561,7 +14562,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -14591,11 +14592,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14607,9 +14603,9 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -14629,7 +14625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -14649,7 +14645,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -14669,7 +14665,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -14689,7 +14685,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>183</v>
       </c>
@@ -14714,7 +14710,7 @@
         <v>0.27300000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>184</v>
       </c>
@@ -14743,11 +14739,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14759,7 +14750,7 @@
       <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -14768,7 +14759,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>116</v>
       </c>
@@ -14785,7 +14776,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>94</v>
       </c>
@@ -14800,7 +14791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -14813,7 +14804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -14828,7 +14819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -14843,7 +14834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -14858,7 +14849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>82</v>
@@ -14873,7 +14864,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" t="s">
         <v>128</v>
@@ -14888,7 +14879,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>129</v>
@@ -14903,7 +14894,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>130</v>
@@ -14918,13 +14909,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
         <v>95</v>
       </c>
@@ -14939,7 +14930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -14951,7 +14942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -14965,7 +14956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -14979,7 +14970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -14993,7 +14984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>82</v>
       </c>
@@ -15007,7 +14998,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>128</v>
       </c>
@@ -15021,7 +15012,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>129</v>
       </c>
@@ -15035,7 +15026,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>130</v>
       </c>
@@ -15049,7 +15040,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>111</v>
       </c>
@@ -15070,11 +15061,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -15086,9 +15072,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -15111,7 +15097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -15134,7 +15120,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>24</v>
@@ -15155,7 +15141,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>26</v>
@@ -15176,7 +15162,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
         <v>27</v>
@@ -15197,7 +15183,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -15220,7 +15206,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -15240,7 +15226,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>183</v>
       </c>
@@ -15260,7 +15246,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>184</v>
       </c>
@@ -15280,7 +15266,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>38</v>
       </c>
@@ -15303,7 +15289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
@@ -15323,7 +15309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
@@ -15343,7 +15329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
@@ -15368,11 +15354,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -15384,12 +15365,12 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>117</v>
       </c>
@@ -15409,7 +15390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -15430,7 +15411,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>113</v>
       </c>
@@ -15445,7 +15426,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -15462,7 +15443,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>186</v>
       </c>
@@ -15479,7 +15460,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>185</v>
       </c>
@@ -15496,14 +15477,14 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
@@ -15512,7 +15493,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>59</v>
       </c>
@@ -15532,7 +15513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
@@ -15549,7 +15530,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -15566,7 +15547,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
@@ -15583,7 +15564,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
@@ -15600,7 +15581,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
@@ -15617,7 +15598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
@@ -15634,7 +15615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1">
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
@@ -15655,11 +15636,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -15674,7 +15650,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -15682,7 +15658,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
@@ -15711,7 +15687,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
@@ -15740,7 +15716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -15763,7 +15739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
@@ -15786,7 +15762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
@@ -15809,7 +15785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>30</v>
       </c>
@@ -15835,7 +15811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -15858,7 +15834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
@@ -15881,7 +15857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
@@ -15904,7 +15880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -15930,7 +15906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -15953,7 +15929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
@@ -15976,7 +15952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
@@ -15999,7 +15975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>33</v>
       </c>
@@ -16025,7 +16001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -16048,7 +16024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -16071,7 +16047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -16094,7 +16070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>37</v>
       </c>
@@ -16120,7 +16096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -16143,7 +16119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
@@ -16166,7 +16142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>27</v>
       </c>
@@ -16189,7 +16165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -16218,7 +16194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -16241,7 +16217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
         <v>183</v>
       </c>
@@ -16264,7 +16240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
         <v>184</v>
       </c>
@@ -16287,7 +16263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -16313,7 +16289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -16336,7 +16312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
         <v>183</v>
       </c>
@@ -16359,7 +16335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
         <v>184</v>
       </c>
@@ -16382,7 +16358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -16408,7 +16384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -16431,7 +16407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
         <v>183</v>
       </c>
@@ -16454,7 +16430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
         <v>184</v>
       </c>
@@ -16477,7 +16453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>33</v>
       </c>
@@ -16503,7 +16479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -16526,7 +16502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
         <v>183</v>
       </c>
@@ -16549,7 +16525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
         <v>184</v>
       </c>
@@ -16572,7 +16548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>37</v>
       </c>
@@ -16598,7 +16574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -16621,7 +16597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
         <v>183</v>
       </c>
@@ -16644,7 +16620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
         <v>184</v>
       </c>
@@ -16667,7 +16643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
         <v>38</v>
       </c>
@@ -16696,7 +16672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
         <v>40</v>
       </c>
@@ -16719,7 +16695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C48" s="4" t="s">
         <v>41</v>
       </c>
@@ -16742,7 +16718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>42</v>
       </c>
@@ -16765,7 +16741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -16791,7 +16767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
         <v>40</v>
       </c>
@@ -16814,7 +16790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C52" s="4" t="s">
         <v>41</v>
       </c>
@@ -16837,7 +16813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
         <v>42</v>
       </c>
@@ -16860,7 +16836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -16886,7 +16862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
         <v>40</v>
       </c>
@@ -16909,7 +16885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C56" s="4" t="s">
         <v>41</v>
       </c>
@@ -16932,7 +16908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>42</v>
       </c>
@@ -16955,7 +16931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -16981,7 +16957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>40</v>
       </c>
@@ -17004,7 +16980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C60" s="4" t="s">
         <v>41</v>
       </c>
@@ -17027,7 +17003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
         <v>42</v>
       </c>
@@ -17050,7 +17026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
         <v>28</v>
       </c>
@@ -17076,7 +17052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C63" s="4" t="s">
         <v>40</v>
       </c>
@@ -17099,7 +17075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C64" s="4" t="s">
         <v>41</v>
       </c>
@@ -17122,7 +17098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C65" s="4" t="s">
         <v>42</v>
       </c>
@@ -17145,7 +17121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
         <v>30</v>
       </c>
@@ -17171,7 +17147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
         <v>40</v>
       </c>
@@ -17194,7 +17170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C68" s="4" t="s">
         <v>41</v>
       </c>
@@ -17217,7 +17193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C69" s="4" t="s">
         <v>42</v>
       </c>
@@ -17240,7 +17216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B70" t="s">
         <v>31</v>
       </c>
@@ -17266,7 +17242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
         <v>40</v>
       </c>
@@ -17289,7 +17265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C72" s="4" t="s">
         <v>41</v>
       </c>
@@ -17312,7 +17288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C73" s="4" t="s">
         <v>42</v>
       </c>
@@ -17335,7 +17311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="10" t="s">
         <v>126</v>
       </c>
@@ -17364,7 +17340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C77" s="4" t="s">
         <v>119</v>
       </c>
@@ -17387,7 +17363,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B78" t="s">
         <v>98</v>
       </c>
@@ -17413,7 +17389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C79" s="4" t="s">
         <v>119</v>
       </c>
@@ -17436,7 +17412,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
         <v>99</v>
       </c>
@@ -17462,7 +17438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C81" s="4" t="s">
         <v>119</v>
       </c>
@@ -17485,7 +17461,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="10" t="s">
         <v>110</v>
       </c>
@@ -17514,7 +17490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C85" s="4" t="s">
         <v>40</v>
       </c>
@@ -17537,7 +17513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C86" s="4" t="s">
         <v>41</v>
       </c>
@@ -17560,7 +17536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C87" s="4" t="s">
         <v>42</v>
       </c>
@@ -17583,17 +17559,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -17602,13 +17573,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -17618,7 +17589,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
@@ -17641,7 +17612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>121</v>
       </c>
@@ -17662,7 +17633,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
@@ -17682,7 +17653,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>120</v>
       </c>
@@ -17705,7 +17676,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
@@ -17725,7 +17696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>48</v>
       </c>
@@ -17745,7 +17716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>142</v>
       </c>
@@ -17765,7 +17736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>127</v>
       </c>
@@ -17785,7 +17756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
@@ -17805,77 +17776,98 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14">
-      <c r="A12" s="77" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <f>1 + (E7-1)*(1-'Baseline year demographics'!C7)</f>
+        <v>1.2751999999999999</v>
+      </c>
+      <c r="F11" s="4">
+        <f>1 + (E7-1)*(1-'Baseline year demographics'!C7)</f>
+        <v>1.2751999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="91" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <f>E10/E9</f>
+        <v>1.4937499999999999</v>
+      </c>
+      <c r="F12" s="4">
+        <f>F10/F9</f>
+        <v>1.4937499999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="76" t="s">
+      <c r="B14" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C14" s="6">
         <v>5.16</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D14" s="6">
         <v>5.16</v>
       </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14">
-      <c r="A13" s="78"/>
-      <c r="B13" s="76" t="s">
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="78"/>
+      <c r="B15" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
         <v>1.82</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F15" s="8">
         <v>1.82</v>
       </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14" customHeight="1"/>
-    <row r="15" spans="1:7">
-      <c r="A15" s="10" t="s">
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="60">
-        <v>1.04</v>
-      </c>
-      <c r="D15" s="60">
-        <v>1.04</v>
-      </c>
-      <c r="E15" s="60">
-        <v>1.04</v>
-      </c>
-      <c r="F15" s="60">
-        <v>1.04</v>
-      </c>
-      <c r="G15" s="60">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
@@ -17893,6 +17885,29 @@
         <v>1.04</v>
       </c>
       <c r="G17" s="60">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="60">
+        <v>1.04</v>
+      </c>
+      <c r="D19" s="60">
+        <v>1.04</v>
+      </c>
+      <c r="E19" s="60">
+        <v>1.04</v>
+      </c>
+      <c r="F19" s="60">
+        <v>1.04</v>
+      </c>
+      <c r="G19" s="60">
         <v>1.04</v>
       </c>
     </row>
@@ -17900,10 +17915,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed BFP and CFE from cost coverages tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2404,7 +2404,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2429,7 +2429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="1">
+    <comment ref="D7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2453,7 +2453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="1">
+    <comment ref="D12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2477,7 +2477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="2">
+    <comment ref="A13" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2501,7 +2501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2525,7 +2525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="2">
+    <comment ref="A14" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2549,7 +2549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="2">
+    <comment ref="A21" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2573,7 +2573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="1">
+    <comment ref="D21" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2597,7 +2597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="2">
+    <comment ref="A28" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2621,7 +2621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="1">
+    <comment ref="D28" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2645,7 +2645,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0">
+    <comment ref="C31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2666,6 +2666,78 @@
           </rPr>
           <t xml:space="preserve">
 This is the fraction of the population eating these staples and belongs here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+orton Copenhagen Consensus 2008</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Same effect as iron fortification</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D33" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+orton Copenhagen Consensus 2008</t>
         </r>
       </text>
     </comment>
@@ -2693,27 +2765,27 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="1">
+    <comment ref="C35" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Same effect as iron fortification</t>
+This is the fraction of the population eating these staples and belongs here.</t>
         </r>
       </text>
     </comment>
@@ -2741,7 +2813,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="1">
+    <comment ref="B36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fictional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D36" authorId="3">
       <text>
         <r>
           <rPr>
@@ -2751,7 +2847,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Sam:</t>
         </r>
         <r>
           <rPr>
@@ -2761,31 +2857,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-orton Copenhagen Consensus 2008</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C37" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the fraction of the population eating these staples and belongs here.</t>
+From Nick</t>
         </r>
       </text>
     </comment>
@@ -2809,83 +2881,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-orton Copenhagen Consensus 2008</t>
+Per person per year</t>
         </r>
       </text>
     </comment>
-    <comment ref="B38" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fictional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D38" authorId="3">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-From Nick</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D39" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Per person per year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D40" authorId="1">
+    <comment ref="D38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -3796,7 +3796,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="221">
   <si>
     <t>year</t>
   </si>
@@ -4698,7 +4698,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="565">
+  <cellStyleXfs count="571">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4710,6 +4710,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5412,7 +5418,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="565">
+  <cellStyles count="571">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5695,6 +5701,9 @@
     <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5976,6 +5985,9 @@
     <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -13325,10 +13337,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13355,77 +13367,77 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>176</v>
       </c>
       <c r="B2" s="14">
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="C2" s="14">
         <v>0.85</v>
       </c>
       <c r="D2" s="14">
-        <v>3.56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="B3" s="14">
-        <v>0</v>
+        <v>0.621</v>
       </c>
       <c r="C3" s="14">
         <v>0.85</v>
       </c>
       <c r="D3" s="14">
-        <v>1</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="B4" s="14">
-        <v>0.621</v>
+        <v>0</v>
       </c>
       <c r="C4" s="14">
         <v>0.85</v>
       </c>
       <c r="D4" s="14">
-        <v>0.35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="14">
-        <v>0.247</v>
-      </c>
-      <c r="C5" s="14">
+        <v>84</v>
+      </c>
+      <c r="B5" s="63">
+        <v>0</v>
+      </c>
+      <c r="C5" s="64">
         <v>0.85</v>
       </c>
-      <c r="D5" s="14">
-        <v>3.56</v>
+      <c r="D5" s="70">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="14">
+        <v>172</v>
+      </c>
+      <c r="B6" s="34">
+        <v>0</v>
+      </c>
+      <c r="C6" s="34">
         <v>0.85</v>
       </c>
-      <c r="D6" s="14">
-        <v>48</v>
+      <c r="D6" s="19">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="63">
         <v>0</v>
@@ -13434,12 +13446,12 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="70">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>172</v>
+      <c r="A8" s="33" t="s">
+        <v>173</v>
       </c>
       <c r="B8" s="34">
         <v>0</v>
@@ -13448,40 +13460,40 @@
         <v>0.85</v>
       </c>
       <c r="D8" s="19">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="63">
-        <v>0</v>
-      </c>
-      <c r="C9" s="64">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
         <v>0.85</v>
       </c>
-      <c r="D9" s="70">
-        <v>1</v>
+      <c r="D9" s="14">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="34">
-        <v>0</v>
-      </c>
-      <c r="C10" s="34">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="65">
+        <v>0</v>
+      </c>
+      <c r="C10" s="66">
         <v>0.85</v>
       </c>
-      <c r="D10" s="19">
-        <v>1</v>
+      <c r="D10" s="66">
+        <v>2.99</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="B11" s="14">
         <v>0</v>
@@ -13490,12 +13502,12 @@
         <v>0.85</v>
       </c>
       <c r="D11" s="14">
-        <v>25</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>171</v>
+      <c r="A12" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B12" s="65">
         <v>0</v>
@@ -13504,12 +13516,12 @@
         <v>0.85</v>
       </c>
       <c r="D12" s="66">
-        <v>2.99</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>174</v>
+      <c r="A13" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="B13" s="14">
         <v>0</v>
@@ -13518,26 +13530,26 @@
         <v>0.85</v>
       </c>
       <c r="D13" s="14">
-        <v>2.99</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="65">
-        <v>0</v>
-      </c>
-      <c r="C14" s="66">
+      <c r="A14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="14">
         <v>0.85</v>
       </c>
-      <c r="D14" s="66">
-        <v>1.78</v>
+      <c r="D14" s="14">
+        <v>2.06</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>175</v>
+      <c r="A15" t="s">
+        <v>154</v>
       </c>
       <c r="B15" s="14">
         <v>0</v>
@@ -13546,12 +13558,12 @@
         <v>0.85</v>
       </c>
       <c r="D15" s="14">
-        <v>1.78</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -13560,12 +13572,12 @@
         <v>0.85</v>
       </c>
       <c r="D16" s="14">
-        <v>2.06</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B17" s="14">
         <v>0</v>
@@ -13574,12 +13586,12 @@
         <v>0.85</v>
       </c>
       <c r="D17" s="14">
-        <v>0.55000000000000004</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B18" s="14">
         <v>0</v>
@@ -13588,12 +13600,12 @@
         <v>0.85</v>
       </c>
       <c r="D18" s="14">
-        <v>0.73</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B19" s="14">
         <v>0</v>
@@ -13602,12 +13614,12 @@
         <v>0.85</v>
       </c>
       <c r="D19" s="14">
-        <v>1.78</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B20" s="14">
         <v>0</v>
@@ -13616,12 +13628,12 @@
         <v>0.85</v>
       </c>
       <c r="D20" s="14">
-        <v>0.55000000000000004</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B21" s="14">
         <v>0</v>
@@ -13630,12 +13642,12 @@
         <v>0.85</v>
       </c>
       <c r="D21" s="14">
-        <v>0.73</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B22" s="14">
         <v>0</v>
@@ -13644,12 +13656,12 @@
         <v>0.85</v>
       </c>
       <c r="D22" s="14">
-        <v>1.78</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -13658,12 +13670,12 @@
         <v>0.85</v>
       </c>
       <c r="D23" s="14">
-        <v>0.24</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B24" s="14">
         <v>0</v>
@@ -13672,12 +13684,12 @@
         <v>0.85</v>
       </c>
       <c r="D24" s="14">
-        <v>0.55000000000000004</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B25" s="14">
         <v>0</v>
@@ -13686,12 +13698,12 @@
         <v>0.85</v>
       </c>
       <c r="D25" s="14">
-        <v>0.73</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B26" s="14">
         <v>0</v>
@@ -13700,12 +13712,12 @@
         <v>0.85</v>
       </c>
       <c r="D26" s="14">
-        <v>1.78</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
@@ -13714,12 +13726,12 @@
         <v>0.85</v>
       </c>
       <c r="D27" s="14">
-        <v>0.55000000000000004</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B28" s="14">
         <v>0</v>
@@ -13728,200 +13740,200 @@
         <v>0.85</v>
       </c>
       <c r="D28" s="14">
-        <v>0.73</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>169</v>
+      <c r="A29" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B29" s="14">
         <v>0</v>
       </c>
       <c r="C29" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D29" s="14">
-        <v>1.78</v>
+        <v>0.12</v>
+      </c>
+      <c r="D29" s="19">
+        <v>0.18</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>170</v>
+      <c r="A30" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="B30" s="14">
         <v>0</v>
       </c>
       <c r="C30" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D30" s="14">
-        <v>0.24</v>
+        <v>0.05</v>
+      </c>
+      <c r="D30" s="19">
+        <v>0.13</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B31" s="14">
         <v>0</v>
       </c>
       <c r="C31" s="14">
-        <v>0.12</v>
+        <v>0.8</v>
       </c>
       <c r="D31" s="19">
-        <v>0.18</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B32" s="14">
         <v>0</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D32" s="19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" s="19">
+        <v>0</v>
+      </c>
+      <c r="C33" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="D33" s="19">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="19">
+        <v>0</v>
+      </c>
+      <c r="C34" s="14">
         <v>0.05</v>
       </c>
-      <c r="D32" s="19">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="14">
-        <v>0</v>
-      </c>
-      <c r="C33" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="D33" s="19">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="14">
-        <v>0</v>
-      </c>
-      <c r="C34" s="13">
-        <v>0.85</v>
-      </c>
       <c r="D34" s="19">
-        <v>0.25</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="19">
+        <v>0</v>
+      </c>
+      <c r="C35" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D35" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C36" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D36" s="19">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="14">
+        <v>0</v>
+      </c>
+      <c r="C37" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D37" s="19">
+        <f>180</f>
         <v>180</v>
-      </c>
-      <c r="B35" s="19">
-        <v>0</v>
-      </c>
-      <c r="C35" s="14">
-        <v>0.12</v>
-      </c>
-      <c r="D35" s="19">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" s="19">
-        <v>0</v>
-      </c>
-      <c r="C36" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="D36" s="19">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B37" s="19">
-        <v>0</v>
-      </c>
-      <c r="C37" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="D37" s="19">
-        <v>0.75</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="B38" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="C38" s="14">
+        <v>0</v>
+      </c>
+      <c r="C38" s="13">
         <v>0.85</v>
       </c>
       <c r="D38" s="19">
-        <v>2.61</v>
+        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
+        <v>10.046400000000002</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="B39" s="14">
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C39" s="13">
         <v>0.85</v>
       </c>
       <c r="D39" s="19">
-        <f>180</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B40" s="14">
-        <v>0</v>
-      </c>
-      <c r="C40" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D40" s="19">
-        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
-        <v>10.046400000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="14">
-        <v>0.61</v>
-      </c>
-      <c r="C41" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D41" s="19">
         <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
         <v>19.933477200000002</v>
       </c>
     </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="82" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" s="88">
+        <v>0.09</v>
+      </c>
+      <c r="C40" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D40" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="88">
+        <v>0.02</v>
+      </c>
+      <c r="C41" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D41" s="83">
+        <v>1</v>
+      </c>
+    </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="82" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B42" s="88">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="C42" s="14">
         <v>0.85</v>
@@ -13932,10 +13944,10 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="82" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B43" s="88">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="C43" s="14">
         <v>0.85</v>
@@ -13946,10 +13958,10 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="82" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B44" s="88">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
       <c r="C44" s="14">
         <v>0.85</v>
@@ -13960,10 +13972,10 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="82" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B45" s="88">
-        <v>0.18</v>
+        <v>0.45</v>
       </c>
       <c r="C45" s="14">
         <v>0.85</v>
@@ -13974,10 +13986,10 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="82" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B46" s="88">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C46" s="14">
         <v>0.85</v>
@@ -13988,10 +14000,10 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="82" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B47" s="88">
-        <v>0.45</v>
+        <v>0.11</v>
       </c>
       <c r="C47" s="14">
         <v>0.85</v>
@@ -14002,10 +14014,10 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="82" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B48" s="88">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="C48" s="14">
         <v>0.85</v>
@@ -14014,36 +14026,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="82" t="s">
-        <v>213</v>
-      </c>
-      <c r="B49" s="88">
-        <v>0.11</v>
-      </c>
-      <c r="C49" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D49" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="82" t="s">
-        <v>214</v>
-      </c>
-      <c r="B50" s="88">
-        <v>0.01</v>
-      </c>
-      <c r="C50" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D50" s="83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C51" s="84"/>
+    <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C49" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17676,8 +17660,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updated ORs for CFE and PPCF
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="15" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -4698,7 +4698,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="571">
+  <cellStyleXfs count="577">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4710,6 +4710,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5411,14 +5417,14 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="571">
+  <cellStyles count="577">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5704,6 +5710,9 @@
     <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5988,6 +5997,9 @@
     <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7630,7 +7642,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="92" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -7653,7 +7665,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="91"/>
+      <c r="B3" s="92"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -7675,7 +7687,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="91"/>
+      <c r="B4" s="92"/>
       <c r="C4" t="s">
         <v>204</v>
       </c>
@@ -7702,7 +7714,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="92" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -7725,7 +7737,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="91"/>
+      <c r="B6" s="92"/>
       <c r="C6" t="s">
         <v>194</v>
       </c>
@@ -7746,7 +7758,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="91"/>
+      <c r="B7" s="92"/>
       <c r="C7" t="s">
         <v>204</v>
       </c>
@@ -7772,7 +7784,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="92" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -7795,7 +7807,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="91"/>
+      <c r="B9" s="92"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -7816,7 +7828,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="91"/>
+      <c r="B10" s="92"/>
       <c r="C10" t="s">
         <v>204</v>
       </c>
@@ -7842,7 +7854,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="92" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -7865,7 +7877,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="91"/>
+      <c r="B12" s="92"/>
       <c r="C12" t="s">
         <v>194</v>
       </c>
@@ -7886,7 +7898,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="91"/>
+      <c r="B13" s="92"/>
       <c r="C13" t="s">
         <v>204</v>
       </c>
@@ -7912,7 +7924,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="92" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -7935,7 +7947,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="91"/>
+      <c r="B15" s="92"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -7956,7 +7968,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="91"/>
+      <c r="B16" s="92"/>
       <c r="C16" t="s">
         <v>204</v>
       </c>
@@ -8015,7 +8027,7 @@
       <c r="A19" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="92" t="s">
         <v>81</v>
       </c>
       <c r="C19" t="s">
@@ -8038,7 +8050,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="91"/>
+      <c r="B20" s="92"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
@@ -8059,7 +8071,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="91"/>
+      <c r="B21" s="92"/>
       <c r="C21" t="s">
         <v>204</v>
       </c>
@@ -8085,7 +8097,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="92" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8108,7 +8120,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="91"/>
+      <c r="B23" s="92"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -8129,7 +8141,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="91"/>
+      <c r="B24" s="92"/>
       <c r="C24" t="s">
         <v>204</v>
       </c>
@@ -8155,7 +8167,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="92" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8178,7 +8190,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="91"/>
+      <c r="B26" s="92"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
@@ -8199,7 +8211,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="91"/>
+      <c r="B27" s="92"/>
       <c r="C27" t="s">
         <v>204</v>
       </c>
@@ -8225,7 +8237,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="91" t="s">
+      <c r="B28" s="92" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -8248,7 +8260,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="91"/>
+      <c r="B29" s="92"/>
       <c r="C29" t="s">
         <v>194</v>
       </c>
@@ -8269,7 +8281,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="91"/>
+      <c r="B30" s="92"/>
       <c r="C30" t="s">
         <v>204</v>
       </c>
@@ -8295,7 +8307,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="91" t="s">
+      <c r="B31" s="92" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -8318,7 +8330,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="91"/>
+      <c r="B32" s="92"/>
       <c r="C32" t="s">
         <v>194</v>
       </c>
@@ -8339,7 +8351,7 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="91"/>
+      <c r="B33" s="92"/>
       <c r="C33" t="s">
         <v>204</v>
       </c>
@@ -9049,19 +9061,19 @@
       <c r="C11" s="69">
         <v>0</v>
       </c>
-      <c r="D11" s="92">
+      <c r="D11" s="91">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="E11" s="92">
+      <c r="E11" s="91">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="F11" s="92">
+      <c r="F11" s="91">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="G11" s="92">
+      <c r="G11" s="91">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
@@ -13339,8 +13351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17660,8 +17672,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17883,12 +17895,12 @@
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <f>1 + (E6-1)*(1-'Baseline year demographics'!C7)</f>
-        <v>1.2751999999999999</v>
+        <f>1/(1 + (E6-1)*(1-'Baseline year demographics'!$C$7))</f>
+        <v>0.78419071518193229</v>
       </c>
       <c r="F12" s="4">
-        <f>1 + (E6-1)*(1-'Baseline year demographics'!C7)</f>
-        <v>1.2751999999999999</v>
+        <f>1/(1 + (F6-1)*(1-'Baseline year demographics'!$C$7))</f>
+        <v>0.78419071518193229</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
@@ -17905,12 +17917,12 @@
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f>E9/E8</f>
-        <v>1.4937499999999999</v>
+        <f>1 / (E$9/E$8)</f>
+        <v>0.66945606694560678</v>
       </c>
       <c r="F13" s="4">
-        <f>F9/F8</f>
-        <v>1.4937499999999999</v>
+        <f>1 / (F$9/F$8)</f>
+        <v>0.66945606694560678</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
@@ -17927,12 +17939,12 @@
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f>E9/E8</f>
-        <v>1.4937499999999999</v>
+        <f t="shared" ref="E14:F15" si="0">1 / (E$9/E$8)</f>
+        <v>0.66945606694560678</v>
       </c>
       <c r="F14" s="4">
-        <f>F9/F8</f>
-        <v>1.4937499999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.66945606694560678</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
@@ -17949,12 +17961,12 @@
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <f>E9/E8</f>
-        <v>1.4937499999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.66945606694560678</v>
       </c>
       <c r="F15" s="4">
-        <f>F9/F8</f>
-        <v>1.4937499999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.66945606694560678</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Some example IYCF packages
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="-33000" yWindow="-21140" windowWidth="26660" windowHeight="21140" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3961,7 +3961,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="224">
   <si>
     <t>year</t>
   </si>
@@ -4872,7 +4872,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="583">
+  <cellStyleXfs count="595">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4884,6 +4884,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5604,7 +5616,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="583">
+  <cellStyles count="595">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5896,6 +5908,12 @@
     <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6186,6 +6204,12 @@
     <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7490,7 +7514,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7785,10 +7809,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8536,7 +8560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B33" s="92"/>
       <c r="C33" t="s">
         <v>204</v>
@@ -8562,7 +8586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B34" s="79" t="s">
         <v>112</v>
       </c>
@@ -8584,6 +8608,9 @@
       <c r="H34" s="80">
         <v>1</v>
       </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -8607,8 +8634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8642,31 +8669,43 @@
       <c r="B2" t="s">
         <v>81</v>
       </c>
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
       <c r="E2" s="81"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
       <c r="E3" s="81"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
       <c r="E4" s="81"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>205</v>
+      </c>
       <c r="E5" s="81"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
         <v>205</v>
       </c>
       <c r="E6" s="81"/>
@@ -8677,9 +8716,6 @@
       </c>
       <c r="C7" s="81"/>
       <c r="D7" s="81"/>
-      <c r="E7" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
@@ -8691,15 +8727,15 @@
       <c r="C9" t="s">
         <v>205</v>
       </c>
+      <c r="D9" t="s">
+        <v>205</v>
+      </c>
       <c r="E9" s="81"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>205</v>
-      </c>
       <c r="E10" s="81"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -8766,9 +8802,13 @@
       </c>
       <c r="C21" s="81"/>
       <c r="D21" s="81"/>
+      <c r="E21" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -8975,7 +9015,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9157,7 +9197,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10806,7 +10846,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12352,8 +12392,8 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13750,7 +13790,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15564,7 +15604,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16141,8 +16181,8 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18070,8 +18110,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Script for IYCF optimisation
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4575,9 +4575,6 @@
     <t>Delivery mode</t>
   </si>
   <si>
-    <t>Behaviour</t>
-  </si>
-  <si>
     <t>OR for correct breastfeeding</t>
   </si>
   <si>
@@ -4660,6 +4657,9 @@
   </si>
   <si>
     <t>OR for stunting</t>
+  </si>
+  <si>
+    <t>Odds ratios</t>
   </si>
 </sst>
 </file>
@@ -7634,7 +7634,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="89">
         <v>0.5</v>
@@ -7642,7 +7642,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10" s="89">
         <v>0.3</v>
@@ -7650,7 +7650,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C11" s="89">
         <v>0.1</v>
@@ -7849,8 +7849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7862,10 +7862,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>195</v>
@@ -7888,7 +7888,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="93" t="s">
         <v>81</v>
@@ -7937,7 +7937,7 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B4" s="93"/>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="73">
         <f>D17^(1/2)</f>
@@ -8008,7 +8008,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B7" s="93"/>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" s="73">
         <f>D17^(1/2)</f>
@@ -8078,7 +8078,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B10" s="93"/>
       <c r="C10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="73">
         <v>1</v>
@@ -8147,7 +8147,7 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B13" s="93"/>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="73">
         <v>1</v>
@@ -8215,7 +8215,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B16" s="93"/>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D16" s="73">
         <v>1</v>
@@ -8240,7 +8240,7 @@
         <v>112</v>
       </c>
       <c r="C17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="80">
         <v>1.05</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="77" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B19" s="93" t="s">
         <v>81</v>
@@ -8315,7 +8315,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B21" s="93"/>
       <c r="C21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D21" s="73">
         <f>D34^(1/5)</f>
@@ -8385,7 +8385,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B24" s="93"/>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D24" s="73">
         <f>D34^(1/5)</f>
@@ -8455,7 +8455,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B27" s="93"/>
       <c r="C27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D27" s="73">
         <f>D34^(1/5)</f>
@@ -8525,7 +8525,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B30" s="93"/>
       <c r="C30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D30" s="73">
         <f>D34^(1/5)</f>
@@ -8595,7 +8595,7 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B33" s="93"/>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D33" s="73">
         <f>D34^(1/5)</f>
@@ -8623,7 +8623,7 @@
         <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D34" s="80">
         <v>1.05</v>
@@ -8643,7 +8643,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B36" s="93" t="s">
         <v>81</v>
@@ -8695,7 +8695,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B38" s="93"/>
       <c r="C38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D38" s="73">
         <f>D51^(1/5)</f>
@@ -8765,7 +8765,7 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B41" s="93"/>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="73">
         <f>D51^(1/5)</f>
@@ -8835,7 +8835,7 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B44" s="93"/>
       <c r="C44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D44" s="73">
         <f>D51^(1/5)</f>
@@ -8905,7 +8905,7 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B47" s="93"/>
       <c r="C47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D47" s="73">
         <f>D51^(1/5)</f>
@@ -8975,7 +8975,7 @@
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B50" s="93"/>
       <c r="C50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="73">
         <f>D51^(1/5)</f>
@@ -9002,7 +9002,7 @@
         <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" s="80">
         <v>1</v>
@@ -9063,10 +9063,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>193</v>
@@ -9075,18 +9075,18 @@
         <v>194</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
         <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E2" s="81"/>
     </row>
@@ -9095,7 +9095,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E3" s="81"/>
     </row>
@@ -9104,7 +9104,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E4" s="81"/>
     </row>
@@ -9113,7 +9113,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E5" s="81"/>
     </row>
@@ -9122,7 +9122,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E6" s="81"/>
     </row>
@@ -9135,16 +9135,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" t="s">
         <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="81"/>
     </row>
@@ -9181,7 +9181,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" t="s">
         <v>81</v>
@@ -9219,7 +9219,7 @@
       <c r="C21" s="81"/>
       <c r="D21" s="81"/>
       <c r="E21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -9244,10 +9244,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>193</v>
@@ -9256,12 +9256,12 @@
         <v>194</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
         <v>81</v>
@@ -9339,7 +9339,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" t="s">
         <v>81</v>
@@ -9441,7 +9441,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>193</v>
@@ -9450,7 +9450,7 @@
         <v>194</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -10524,7 +10524,7 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -10550,7 +10550,7 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -10576,7 +10576,7 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
@@ -10602,7 +10602,7 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -10628,7 +10628,7 @@
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="85" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -10654,7 +10654,7 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
@@ -10680,7 +10680,7 @@
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="85" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
@@ -10706,7 +10706,7 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -10732,7 +10732,7 @@
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="85" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -14117,15 +14117,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="86">
         <v>0.9</v>
@@ -14133,7 +14133,7 @@
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="86">
         <v>1</v>
@@ -14141,7 +14141,7 @@
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="86">
         <v>1</v>
@@ -14149,7 +14149,7 @@
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="86">
         <v>1</v>
@@ -14157,7 +14157,7 @@
     </row>
     <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="85" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="86">
         <v>1</v>
@@ -14165,7 +14165,7 @@
     </row>
     <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="86">
         <v>0.93</v>
@@ -14173,7 +14173,7 @@
     </row>
     <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="85" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="86">
         <v>0.5</v>
@@ -14181,7 +14181,7 @@
     </row>
     <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="86">
         <v>0.5</v>
@@ -14189,7 +14189,7 @@
     </row>
     <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="85" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="86">
         <v>0.98</v>
@@ -14768,7 +14768,7 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B40" s="88">
         <v>0.09</v>
@@ -14782,7 +14782,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B41" s="88">
         <v>0.02</v>
@@ -14796,7 +14796,7 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="82" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B42" s="88">
         <v>0.08</v>
@@ -14810,7 +14810,7 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B43" s="88">
         <v>0.18</v>
@@ -14824,7 +14824,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="82" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B44" s="88">
         <v>0.02</v>
@@ -14838,7 +14838,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B45" s="88">
         <v>0.45</v>
@@ -14852,7 +14852,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B46" s="88">
         <v>0.03</v>
@@ -14866,7 +14866,7 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B47" s="88">
         <v>0.11</v>
@@ -14880,7 +14880,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B48" s="88">
         <v>0.01</v>
@@ -18606,7 +18606,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Updated OR for IYCF
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1560" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -5678,9 +5678,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -5691,6 +5688,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="597">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7889,8 +7889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7930,7 +7930,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="108" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -7953,7 +7953,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="98"/>
+      <c r="B3" s="108"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -7975,7 +7975,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="98"/>
+      <c r="B4" s="108"/>
       <c r="C4" t="s">
         <v>204</v>
       </c>
@@ -8002,7 +8002,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8025,7 +8025,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="98"/>
+      <c r="B6" s="108"/>
       <c r="C6" t="s">
         <v>194</v>
       </c>
@@ -8046,7 +8046,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="98"/>
+      <c r="B7" s="108"/>
       <c r="C7" t="s">
         <v>204</v>
       </c>
@@ -8072,7 +8072,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="108" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8095,7 +8095,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="98"/>
+      <c r="B9" s="108"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -8116,7 +8116,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="98"/>
+      <c r="B10" s="108"/>
       <c r="C10" t="s">
         <v>204</v>
       </c>
@@ -8141,7 +8141,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="108" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8164,7 +8164,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="98"/>
+      <c r="B12" s="108"/>
       <c r="C12" t="s">
         <v>194</v>
       </c>
@@ -8185,7 +8185,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="98"/>
+      <c r="B13" s="108"/>
       <c r="C13" t="s">
         <v>204</v>
       </c>
@@ -8209,7 +8209,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8232,7 +8232,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="98"/>
+      <c r="B15" s="108"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -8253,7 +8253,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="98"/>
+      <c r="B16" s="108"/>
       <c r="C16" t="s">
         <v>204</v>
       </c>
@@ -8309,7 +8309,7 @@
       <c r="A19" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="108" t="s">
         <v>81</v>
       </c>
       <c r="C19" t="s">
@@ -8332,7 +8332,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="98"/>
+      <c r="B20" s="108"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
@@ -8353,7 +8353,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="98"/>
+      <c r="B21" s="108"/>
       <c r="C21" t="s">
         <v>204</v>
       </c>
@@ -8379,7 +8379,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8402,7 +8402,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="98"/>
+      <c r="B23" s="108"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -8423,7 +8423,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="98"/>
+      <c r="B24" s="108"/>
       <c r="C24" t="s">
         <v>204</v>
       </c>
@@ -8449,7 +8449,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="108" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8472,7 +8472,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="98"/>
+      <c r="B26" s="108"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
@@ -8493,7 +8493,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="98"/>
+      <c r="B27" s="108"/>
       <c r="C27" t="s">
         <v>204</v>
       </c>
@@ -8519,7 +8519,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="108" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -8542,7 +8542,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="98"/>
+      <c r="B29" s="108"/>
       <c r="C29" t="s">
         <v>194</v>
       </c>
@@ -8563,7 +8563,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="98"/>
+      <c r="B30" s="108"/>
       <c r="C30" t="s">
         <v>204</v>
       </c>
@@ -8589,7 +8589,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -8612,7 +8612,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="98"/>
+      <c r="B32" s="108"/>
       <c r="C32" t="s">
         <v>194</v>
       </c>
@@ -8633,7 +8633,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="98"/>
+      <c r="B33" s="108"/>
       <c r="C33" t="s">
         <v>204</v>
       </c>
@@ -8685,7 +8685,7 @@
       <c r="A36" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="98" t="s">
+      <c r="B36" s="108" t="s">
         <v>81</v>
       </c>
       <c r="C36" t="s">
@@ -8708,7 +8708,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="98"/>
+      <c r="B37" s="108"/>
       <c r="C37" t="s">
         <v>194</v>
       </c>
@@ -8729,7 +8729,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="98"/>
+      <c r="B38" s="108"/>
       <c r="C38" t="s">
         <v>204</v>
       </c>
@@ -8750,7 +8750,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -8773,7 +8773,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="98"/>
+      <c r="B40" s="108"/>
       <c r="C40" t="s">
         <v>194</v>
       </c>
@@ -8794,7 +8794,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="98"/>
+      <c r="B41" s="108"/>
       <c r="C41" t="s">
         <v>204</v>
       </c>
@@ -8815,7 +8815,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="98" t="s">
+      <c r="B42" s="108" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -8838,7 +8838,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="98"/>
+      <c r="B43" s="108"/>
       <c r="C43" t="s">
         <v>194</v>
       </c>
@@ -8859,7 +8859,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="98"/>
+      <c r="B44" s="108"/>
       <c r="C44" t="s">
         <v>204</v>
       </c>
@@ -8880,7 +8880,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="108" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -8896,14 +8896,14 @@
         <v>0.78</v>
       </c>
       <c r="G45" s="73">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H45" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="98"/>
+      <c r="B46" s="108"/>
       <c r="C46" t="s">
         <v>194</v>
       </c>
@@ -8917,14 +8917,14 @@
         <v>0.78</v>
       </c>
       <c r="G46" s="73">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H46" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="98"/>
+      <c r="B47" s="108"/>
       <c r="C47" t="s">
         <v>204</v>
       </c>
@@ -8945,7 +8945,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="98" t="s">
+      <c r="B48" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -8968,7 +8968,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="98"/>
+      <c r="B49" s="108"/>
       <c r="C49" t="s">
         <v>194</v>
       </c>
@@ -8989,7 +8989,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="98"/>
+      <c r="B50" s="108"/>
       <c r="C50" t="s">
         <v>204</v>
       </c>
@@ -9034,6 +9034,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9044,11 +9049,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9059,8 +9059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9088,188 +9088,188 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="102"/>
-      <c r="B3" s="103" t="s">
+      <c r="A3" s="101"/>
+      <c r="B3" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="103"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="102"/>
-      <c r="B4" s="103" t="s">
+      <c r="A4" s="101"/>
+      <c r="B4" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="104"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="103"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103" t="s">
+      <c r="A5" s="101"/>
+      <c r="B5" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="104"/>
+      <c r="E5" s="103"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103" t="s">
+      <c r="A6" s="101"/>
+      <c r="B6" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="103"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="105"/>
-      <c r="B7" s="106" t="s">
+      <c r="A7" s="104"/>
+      <c r="B7" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="108"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="98" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="101"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="100"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="102"/>
-      <c r="B10" s="103" t="s">
+      <c r="A10" s="101"/>
+      <c r="B10" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="104"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="103"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="102"/>
-      <c r="B11" s="103" t="s">
+      <c r="A11" s="101"/>
+      <c r="B11" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="104"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="103"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="102"/>
-      <c r="B12" s="103" t="s">
+      <c r="A12" s="101"/>
+      <c r="B12" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="104"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="103"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="102"/>
-      <c r="B13" s="103" t="s">
+      <c r="A13" s="101"/>
+      <c r="B13" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="E13" s="104"/>
+      <c r="E13" s="103"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106" t="s">
+      <c r="A14" s="104"/>
+      <c r="B14" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="108"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="107"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="100" t="s">
+      <c r="C16" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="E16" s="101"/>
+      <c r="E16" s="100"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="102"/>
-      <c r="B17" s="103" t="s">
+      <c r="A17" s="101"/>
+      <c r="B17" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="103" t="s">
+      <c r="C17" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="E17" s="104"/>
+      <c r="E17" s="103"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="102"/>
-      <c r="B18" s="103" t="s">
+      <c r="A18" s="101"/>
+      <c r="B18" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="104"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="103"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="102"/>
-      <c r="B19" s="103" t="s">
+      <c r="A19" s="101"/>
+      <c r="B19" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="103"/>
-      <c r="D19" s="103"/>
-      <c r="E19" s="104"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="103"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="102"/>
-      <c r="B20" s="103" t="s">
+      <c r="A20" s="101"/>
+      <c r="B20" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="103"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="104"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="103"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="105"/>
-      <c r="B21" s="106" t="s">
+      <c r="A21" s="104"/>
+      <c r="B21" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="108"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="107"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9283,7 +9283,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E8" sqref="E8:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Changed IYCF ORs to stop flow-on effect
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="14" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -7637,8 +7637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7760,13 +7760,13 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="E5" s="62">
-        <v>3.07</v>
+        <v>1</v>
       </c>
       <c r="F5" s="62">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G5" s="62">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H5" s="64">
         <v>1</v>
@@ -7781,13 +7781,13 @@
         <v>2.17</v>
       </c>
       <c r="E6" s="62">
-        <v>2.48</v>
+        <v>1</v>
       </c>
       <c r="F6" s="62">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G6" s="62">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H6" s="64">
         <v>1</v>
@@ -7833,10 +7833,10 @@
         <v>1.5</v>
       </c>
       <c r="F8" s="62">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="G8" s="62">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="H8" s="64">
         <v>1</v>
@@ -7854,10 +7854,10 @@
         <v>1.5</v>
       </c>
       <c r="F9" s="62">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="G9" s="62">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H9" s="64">
         <v>1</v>
@@ -7905,7 +7905,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G11" s="62">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="H11" s="64">
         <v>1</v>
@@ -7926,7 +7926,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G12" s="62">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H12" s="64">
         <v>1</v>
@@ -8511,10 +8511,10 @@
         <v>1</v>
       </c>
       <c r="F39" s="62">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G39" s="62">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H39" s="62">
         <v>1</v>
@@ -8532,10 +8532,10 @@
         <v>1</v>
       </c>
       <c r="F40" s="62">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G40" s="62">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H40" s="62">
         <v>1</v>
@@ -8576,10 +8576,10 @@
         <v>1</v>
       </c>
       <c r="F42" s="62">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G42" s="62">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H42" s="62">
         <v>1</v>
@@ -8597,10 +8597,10 @@
         <v>1</v>
       </c>
       <c r="F43" s="62">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G43" s="62">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H43" s="62">
         <v>1</v>
@@ -11557,7 +11557,7 @@
   </sheetPr>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -13014,7 +13014,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updates for data structures
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -3864,7 +3864,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="238">
   <si>
     <t>year</t>
   </si>
@@ -4901,7 +4901,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="623">
+  <cellStyleXfs count="627">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4913,6 +4913,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5688,7 +5692,7 @@
     <xf numFmtId="165" fontId="13" fillId="2" borderId="3" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="623">
+  <cellStyles count="627">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6000,6 +6004,8 @@
     <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6310,6 +6316,8 @@
     <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -17184,7 +17192,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L1" sqref="L1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18163,21 +18171,25 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83:L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
@@ -18214,8 +18226,20 @@
       <c r="L1" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
@@ -18252,8 +18276,20 @@
       <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -18284,8 +18320,20 @@
       <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
@@ -18316,8 +18364,20 @@
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
@@ -18348,8 +18408,20 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>30</v>
       </c>
@@ -18383,8 +18455,20 @@
       <c r="L6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -18415,8 +18499,20 @@
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
@@ -18447,8 +18543,20 @@
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
@@ -18479,8 +18587,20 @@
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -18514,8 +18634,20 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -18546,8 +18678,20 @@
       <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
@@ -18578,8 +18722,20 @@
       <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
@@ -18610,8 +18766,20 @@
       <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>33</v>
       </c>
@@ -18645,8 +18813,20 @@
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -18677,8 +18857,20 @@
       <c r="L15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -18709,8 +18901,20 @@
       <c r="L16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -18741,8 +18945,20 @@
       <c r="L17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>37</v>
       </c>
@@ -18776,8 +18992,20 @@
       <c r="L18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -18808,8 +19036,20 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
@@ -18840,8 +19080,20 @@
       <c r="L20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>27</v>
       </c>
@@ -18872,8 +19124,20 @@
       <c r="L21">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -18910,8 +19174,20 @@
       <c r="L24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -18942,8 +19218,20 @@
       <c r="L25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
         <v>165</v>
       </c>
@@ -18974,8 +19262,20 @@
       <c r="L26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
         <v>166</v>
       </c>
@@ -19006,8 +19306,20 @@
       <c r="L27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -19041,8 +19353,20 @@
       <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -19073,8 +19397,20 @@
       <c r="L29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
         <v>165</v>
       </c>
@@ -19105,8 +19441,20 @@
       <c r="L30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
         <v>166</v>
       </c>
@@ -19137,8 +19485,20 @@
       <c r="L31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -19172,8 +19532,20 @@
       <c r="L32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -19204,8 +19576,20 @@
       <c r="L33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
         <v>165</v>
       </c>
@@ -19236,8 +19620,20 @@
       <c r="L34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
         <v>166</v>
       </c>
@@ -19268,8 +19664,20 @@
       <c r="L35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>33</v>
       </c>
@@ -19303,8 +19711,20 @@
       <c r="L36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -19335,8 +19755,20 @@
       <c r="L37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
         <v>165</v>
       </c>
@@ -19367,8 +19799,20 @@
       <c r="L38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
         <v>166</v>
       </c>
@@ -19399,8 +19843,20 @@
       <c r="L39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>37</v>
       </c>
@@ -19434,8 +19890,20 @@
       <c r="L40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -19466,8 +19934,20 @@
       <c r="L41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
         <v>165</v>
       </c>
@@ -19498,8 +19978,20 @@
       <c r="L42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
         <v>166</v>
       </c>
@@ -19530,12 +20022,24 @@
       <c r="L43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
         <v>230</v>
       </c>
@@ -19572,8 +20076,20 @@
       <c r="L46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
         <v>235</v>
       </c>
@@ -19604,8 +20120,20 @@
       <c r="L47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B48" t="s">
         <v>30</v>
       </c>
@@ -19639,8 +20167,20 @@
       <c r="L48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>235</v>
       </c>
@@ -19671,8 +20211,20 @@
       <c r="L49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
         <v>32</v>
       </c>
@@ -19706,8 +20258,20 @@
       <c r="L50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
         <v>235</v>
       </c>
@@ -19738,8 +20302,20 @@
       <c r="L51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B52" t="s">
         <v>33</v>
       </c>
@@ -19773,8 +20349,20 @@
       <c r="L52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
         <v>235</v>
       </c>
@@ -19805,8 +20393,20 @@
       <c r="L53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
         <v>37</v>
       </c>
@@ -19840,8 +20440,20 @@
       <c r="L54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
         <v>235</v>
       </c>
@@ -19872,8 +20484,20 @@
       <c r="L55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A56" s="10"/>
       <c r="B56" t="s">
         <v>91</v>
@@ -19908,8 +20532,20 @@
       <c r="L56" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>111</v>
       </c>
@@ -19940,8 +20576,20 @@
       <c r="L57" s="4">
         <v>3.51</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
         <v>92</v>
       </c>
@@ -19975,8 +20623,20 @@
       <c r="L58" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>111</v>
       </c>
@@ -20007,8 +20667,20 @@
       <c r="L59" s="4">
         <v>3.51</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B60" t="s">
         <v>93</v>
       </c>
@@ -20042,8 +20714,20 @@
       <c r="L60" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
         <v>111</v>
       </c>
@@ -20074,12 +20758,24 @@
       <c r="L61" s="4">
         <v>3.51</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
+      <c r="P61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A64" s="10" t="s">
         <v>38</v>
       </c>
@@ -20116,8 +20812,20 @@
       <c r="L64" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M64" s="4">
+        <v>1</v>
+      </c>
+      <c r="N64" s="4">
+        <v>1</v>
+      </c>
+      <c r="O64" s="4">
+        <v>1</v>
+      </c>
+      <c r="P64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C65" s="4" t="s">
         <v>40</v>
       </c>
@@ -20148,8 +20856,20 @@
       <c r="L65" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M65" s="4">
+        <v>1</v>
+      </c>
+      <c r="N65" s="4">
+        <v>1</v>
+      </c>
+      <c r="O65" s="4">
+        <v>1</v>
+      </c>
+      <c r="P65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C66" s="4" t="s">
         <v>41</v>
       </c>
@@ -20180,8 +20900,20 @@
       <c r="L66" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M66" s="4">
+        <v>1</v>
+      </c>
+      <c r="N66" s="4">
+        <v>1</v>
+      </c>
+      <c r="O66" s="4">
+        <v>1</v>
+      </c>
+      <c r="P66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
         <v>42</v>
       </c>
@@ -20212,8 +20944,20 @@
       <c r="L67" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M67" s="4">
+        <v>1</v>
+      </c>
+      <c r="N67" s="4">
+        <v>1</v>
+      </c>
+      <c r="O67" s="4">
+        <v>1</v>
+      </c>
+      <c r="P67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B68" t="s">
         <v>16</v>
       </c>
@@ -20247,8 +20991,20 @@
       <c r="L68" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M68" s="4">
+        <v>1</v>
+      </c>
+      <c r="N68" s="4">
+        <v>1</v>
+      </c>
+      <c r="O68" s="4">
+        <v>1</v>
+      </c>
+      <c r="P68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C69" s="4" t="s">
         <v>40</v>
       </c>
@@ -20279,8 +21035,20 @@
       <c r="L69" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M69" s="4">
+        <v>1</v>
+      </c>
+      <c r="N69" s="4">
+        <v>1</v>
+      </c>
+      <c r="O69" s="4">
+        <v>1</v>
+      </c>
+      <c r="P69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C70" s="4" t="s">
         <v>41</v>
       </c>
@@ -20311,8 +21079,20 @@
       <c r="L70" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M70" s="4">
+        <v>1</v>
+      </c>
+      <c r="N70" s="4">
+        <v>1</v>
+      </c>
+      <c r="O70" s="4">
+        <v>1</v>
+      </c>
+      <c r="P70" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
         <v>42</v>
       </c>
@@ -20343,8 +21123,20 @@
       <c r="L71" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M71" s="4">
+        <v>1</v>
+      </c>
+      <c r="N71" s="4">
+        <v>1</v>
+      </c>
+      <c r="O71" s="4">
+        <v>1</v>
+      </c>
+      <c r="P71" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B72" t="s">
         <v>17</v>
       </c>
@@ -20378,8 +21170,20 @@
       <c r="L72" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M72" s="4">
+        <v>1</v>
+      </c>
+      <c r="N72" s="4">
+        <v>1</v>
+      </c>
+      <c r="O72" s="4">
+        <v>1</v>
+      </c>
+      <c r="P72" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C73" s="4" t="s">
         <v>40</v>
       </c>
@@ -20410,8 +21214,20 @@
       <c r="L73" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M73" s="4">
+        <v>1</v>
+      </c>
+      <c r="N73" s="4">
+        <v>1</v>
+      </c>
+      <c r="O73" s="4">
+        <v>1</v>
+      </c>
+      <c r="P73" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C74" s="4" t="s">
         <v>41</v>
       </c>
@@ -20442,8 +21258,20 @@
       <c r="L74" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M74" s="4">
+        <v>1</v>
+      </c>
+      <c r="N74" s="4">
+        <v>1</v>
+      </c>
+      <c r="O74" s="4">
+        <v>1</v>
+      </c>
+      <c r="P74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C75" s="4" t="s">
         <v>42</v>
       </c>
@@ -20474,8 +21302,20 @@
       <c r="L75" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M75" s="4">
+        <v>1</v>
+      </c>
+      <c r="N75" s="4">
+        <v>1</v>
+      </c>
+      <c r="O75" s="4">
+        <v>1</v>
+      </c>
+      <c r="P75" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B76" t="s">
         <v>22</v>
       </c>
@@ -20509,8 +21349,20 @@
       <c r="L76" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M76" s="4">
+        <v>1</v>
+      </c>
+      <c r="N76" s="4">
+        <v>1</v>
+      </c>
+      <c r="O76" s="4">
+        <v>1</v>
+      </c>
+      <c r="P76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C77" s="4" t="s">
         <v>40</v>
       </c>
@@ -20541,8 +21393,20 @@
       <c r="L77" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M77" s="4">
+        <v>1</v>
+      </c>
+      <c r="N77" s="4">
+        <v>1</v>
+      </c>
+      <c r="O77" s="4">
+        <v>1</v>
+      </c>
+      <c r="P77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C78" s="4" t="s">
         <v>41</v>
       </c>
@@ -20573,8 +21437,20 @@
       <c r="L78" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M78" s="4">
+        <v>1</v>
+      </c>
+      <c r="N78" s="4">
+        <v>1</v>
+      </c>
+      <c r="O78" s="4">
+        <v>1</v>
+      </c>
+      <c r="P78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C79" s="4" t="s">
         <v>42</v>
       </c>
@@ -20605,8 +21481,20 @@
       <c r="L79" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="M79" s="4">
+        <v>1</v>
+      </c>
+      <c r="N79" s="4">
+        <v>1</v>
+      </c>
+      <c r="O79" s="4">
+        <v>1</v>
+      </c>
+      <c r="P79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
         <v>28</v>
       </c>
@@ -20640,8 +21528,20 @@
       <c r="L80" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M80" s="4">
+        <v>1</v>
+      </c>
+      <c r="N80" s="4">
+        <v>1</v>
+      </c>
+      <c r="O80" s="4">
+        <v>1</v>
+      </c>
+      <c r="P80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C81" s="4" t="s">
         <v>40</v>
       </c>
@@ -20672,8 +21572,20 @@
       <c r="L81" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M81" s="4">
+        <v>1</v>
+      </c>
+      <c r="N81" s="4">
+        <v>1</v>
+      </c>
+      <c r="O81" s="4">
+        <v>1</v>
+      </c>
+      <c r="P81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C82" s="4" t="s">
         <v>41</v>
       </c>
@@ -20704,8 +21616,20 @@
       <c r="L82" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M82" s="4">
+        <v>1</v>
+      </c>
+      <c r="N82" s="4">
+        <v>1</v>
+      </c>
+      <c r="O82" s="4">
+        <v>1</v>
+      </c>
+      <c r="P82" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C83" s="4" t="s">
         <v>42</v>
       </c>
@@ -20736,8 +21660,20 @@
       <c r="L83" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M83" s="4">
+        <v>1</v>
+      </c>
+      <c r="N83" s="4">
+        <v>1</v>
+      </c>
+      <c r="O83" s="4">
+        <v>1</v>
+      </c>
+      <c r="P83" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B84" t="s">
         <v>30</v>
       </c>
@@ -20771,8 +21707,20 @@
       <c r="L84" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M84" s="4">
+        <v>1</v>
+      </c>
+      <c r="N84" s="4">
+        <v>1</v>
+      </c>
+      <c r="O84" s="4">
+        <v>1</v>
+      </c>
+      <c r="P84" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C85" s="4" t="s">
         <v>40</v>
       </c>
@@ -20803,8 +21751,20 @@
       <c r="L85" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M85" s="4">
+        <v>1</v>
+      </c>
+      <c r="N85" s="4">
+        <v>1</v>
+      </c>
+      <c r="O85" s="4">
+        <v>1</v>
+      </c>
+      <c r="P85" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C86" s="4" t="s">
         <v>41</v>
       </c>
@@ -20835,8 +21795,20 @@
       <c r="L86" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M86" s="4">
+        <v>1</v>
+      </c>
+      <c r="N86" s="4">
+        <v>1</v>
+      </c>
+      <c r="O86" s="4">
+        <v>1</v>
+      </c>
+      <c r="P86" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C87" s="4" t="s">
         <v>42</v>
       </c>
@@ -20867,8 +21839,20 @@
       <c r="L87" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M87" s="4">
+        <v>1</v>
+      </c>
+      <c r="N87" s="4">
+        <v>1</v>
+      </c>
+      <c r="O87" s="4">
+        <v>1</v>
+      </c>
+      <c r="P87" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B88" t="s">
         <v>31</v>
       </c>
@@ -20902,8 +21886,20 @@
       <c r="L88" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M88" s="4">
+        <v>1</v>
+      </c>
+      <c r="N88" s="4">
+        <v>1</v>
+      </c>
+      <c r="O88" s="4">
+        <v>1</v>
+      </c>
+      <c r="P88" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C89" s="4" t="s">
         <v>40</v>
       </c>
@@ -20934,8 +21930,20 @@
       <c r="L89" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M89" s="4">
+        <v>1</v>
+      </c>
+      <c r="N89" s="4">
+        <v>1</v>
+      </c>
+      <c r="O89" s="4">
+        <v>1</v>
+      </c>
+      <c r="P89" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C90" s="4" t="s">
         <v>41</v>
       </c>
@@ -20966,8 +21974,20 @@
       <c r="L90" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M90" s="4">
+        <v>1</v>
+      </c>
+      <c r="N90" s="4">
+        <v>1</v>
+      </c>
+      <c r="O90" s="4">
+        <v>1</v>
+      </c>
+      <c r="P90" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C91" s="4" t="s">
         <v>42</v>
       </c>
@@ -20998,8 +22018,20 @@
       <c r="L91" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M91" s="4">
+        <v>1</v>
+      </c>
+      <c r="N91" s="4">
+        <v>1</v>
+      </c>
+      <c r="O91" s="4">
+        <v>1</v>
+      </c>
+      <c r="P91" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A94" s="10" t="s">
         <v>104</v>
       </c>
@@ -21036,8 +22068,20 @@
       <c r="L94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M94">
+        <v>1</v>
+      </c>
+      <c r="N94">
+        <v>1</v>
+      </c>
+      <c r="O94">
+        <v>1</v>
+      </c>
+      <c r="P94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C95" s="4" t="s">
         <v>40</v>
       </c>
@@ -21068,8 +22112,20 @@
       <c r="L95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M95">
+        <v>1</v>
+      </c>
+      <c r="N95">
+        <v>1</v>
+      </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
+      <c r="P95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C96" s="4" t="s">
         <v>41</v>
       </c>
@@ -21100,8 +22156,20 @@
       <c r="L96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M96">
+        <v>1</v>
+      </c>
+      <c r="N96">
+        <v>1</v>
+      </c>
+      <c r="O96">
+        <v>1</v>
+      </c>
+      <c r="P96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C97" s="4" t="s">
         <v>42</v>
       </c>
@@ -21132,8 +22200,20 @@
       <c r="L97">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M97">
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
+      <c r="O97">
+        <v>1</v>
+      </c>
+      <c r="P97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A100" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added birth info to spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -3108,6 +3108,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+made these values up
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -3995,7 +4020,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="249">
   <si>
     <t>year</t>
   </si>
@@ -4726,9 +4751,6 @@
     <t>Birth age order</t>
   </si>
   <si>
-    <t>RR birth</t>
-  </si>
-  <si>
     <t>Fraction</t>
   </si>
   <si>
@@ -4738,10 +4760,13 @@
     <t>Index</t>
   </si>
   <si>
-    <t>birth age intervention</t>
-  </si>
-  <si>
     <t>Birth age intervention</t>
+  </si>
+  <si>
+    <t>RR age order</t>
+  </si>
+  <si>
+    <t>RR interval</t>
   </si>
 </sst>
 </file>
@@ -5086,7 +5111,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="641">
+  <cellStyleXfs count="643">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5728,8 +5753,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5940,8 +5967,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="641">
+  <cellStyles count="643">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6262,6 +6292,7 @@
     <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6581,6 +6612,7 @@
     <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -11214,7 +11246,7 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
       <c r="B37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -11514,7 +11546,7 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
@@ -14830,7 +14862,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -14865,7 +14897,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="102" t="s">
         <v>52</v>
@@ -15026,7 +15058,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -15602,10 +15634,18 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A41" s="93"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="95"/>
-      <c r="D41" s="96"/>
+      <c r="A41" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="B41" s="128">
+        <v>0.1</v>
+      </c>
+      <c r="C41" s="129">
+        <v>0.85</v>
+      </c>
+      <c r="D41" s="130">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
       <c r="A42" s="93"/>
@@ -17095,7 +17135,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -17106,13 +17146,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -17243,8 +17283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -17515,14 +17555,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>243</v>
-      </c>
       <c r="B20" s="10" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>247</v>
+      </c>
       <c r="B21" s="112" t="s">
         <v>232</v>
       </c>
@@ -17702,6 +17742,9 @@
       <c r="G31" s="116"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A32" s="10" t="s">
+        <v>248</v>
+      </c>
       <c r="B32" s="111" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
demo script for birth age intervervention
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -14862,7 +14862,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -14903,13 +14903,13 @@
         <v>52</v>
       </c>
       <c r="C2" s="125">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D2" s="125">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="E2" s="125">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F2" s="9"/>
     </row>

</xml_diff>

<commit_message>
added wash interventions to spreadsheet and code, added demo script
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-73700" yWindow="-3280" windowWidth="25600" windowHeight="14660" tabRatio="500" firstSheet="19" activeTab="20"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="24780" windowHeight="14520" tabRatio="500" firstSheet="19" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3133,6 +3133,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="D42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ruth made up wash unit costs
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -4020,7 +4045,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="254">
   <si>
     <t>year</t>
   </si>
@@ -4767,6 +4792,21 @@
   </si>
   <si>
     <t>RR interval</t>
+  </si>
+  <si>
+    <t>WASH: Improved water source</t>
+  </si>
+  <si>
+    <t>WASH: Piped water</t>
+  </si>
+  <si>
+    <t>WASH: Improved sanitation</t>
+  </si>
+  <si>
+    <t>WASH: Hygenic disposal</t>
+  </si>
+  <si>
+    <t>WASH: Handwashing</t>
   </si>
 </sst>
 </file>
@@ -4981,7 +5021,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -5015,19 +5055,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -5111,7 +5138,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="643">
+  <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5755,8 +5782,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5885,13 +5932,11 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5901,25 +5946,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -5967,11 +6008,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="643">
+  <cellStyles count="663">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6293,6 +6335,16 @@
     <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6613,6 +6665,16 @@
     <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7916,7 +7978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -8001,7 +8063,7 @@
       <c r="B9" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C9" s="87">
+      <c r="C9" s="85">
         <v>0.5</v>
       </c>
     </row>
@@ -8009,7 +8071,7 @@
       <c r="B10" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="87">
+      <c r="C10" s="85">
         <v>0.3</v>
       </c>
     </row>
@@ -8017,7 +8079,7 @@
       <c r="B11" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="87">
+      <c r="C11" s="85">
         <v>0.1</v>
       </c>
     </row>
@@ -8435,7 +8497,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>57</v>
       </c>
       <c r="C12" s="4">
@@ -8457,7 +8519,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="88" t="s">
+      <c r="B13" s="86" t="s">
         <v>161</v>
       </c>
       <c r="C13" s="4">
@@ -8479,7 +8541,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="B14" s="88" t="s">
+      <c r="B14" s="86" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="4">
@@ -8501,7 +8563,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="86" t="s">
         <v>172</v>
       </c>
       <c r="C15" s="4">
@@ -8670,7 +8732,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="124" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -8693,7 +8755,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="108"/>
+      <c r="B3" s="124"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -8715,7 +8777,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="108"/>
+      <c r="B4" s="124"/>
       <c r="C4" t="s">
         <v>204</v>
       </c>
@@ -8742,7 +8804,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="124" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8765,7 +8827,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="108"/>
+      <c r="B6" s="124"/>
       <c r="C6" t="s">
         <v>194</v>
       </c>
@@ -8786,7 +8848,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="108"/>
+      <c r="B7" s="124"/>
       <c r="C7" t="s">
         <v>204</v>
       </c>
@@ -8812,7 +8874,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="124" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8835,7 +8897,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="108"/>
+      <c r="B9" s="124"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -8856,7 +8918,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="108"/>
+      <c r="B10" s="124"/>
       <c r="C10" t="s">
         <v>204</v>
       </c>
@@ -8881,7 +8943,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="124" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8904,7 +8966,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="108"/>
+      <c r="B12" s="124"/>
       <c r="C12" t="s">
         <v>194</v>
       </c>
@@ -8925,7 +8987,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="108"/>
+      <c r="B13" s="124"/>
       <c r="C13" t="s">
         <v>204</v>
       </c>
@@ -8949,7 +9011,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="124" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8972,7 +9034,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="108"/>
+      <c r="B15" s="124"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -8993,7 +9055,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="108"/>
+      <c r="B16" s="124"/>
       <c r="C16" t="s">
         <v>204</v>
       </c>
@@ -9016,7 +9078,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="84" t="s">
         <v>112</v>
       </c>
       <c r="C17" t="s">
@@ -9049,7 +9111,7 @@
       <c r="A19" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="124" t="s">
         <v>81</v>
       </c>
       <c r="C19" t="s">
@@ -9072,7 +9134,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="108"/>
+      <c r="B20" s="124"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
@@ -9093,7 +9155,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="108"/>
+      <c r="B21" s="124"/>
       <c r="C21" t="s">
         <v>204</v>
       </c>
@@ -9119,7 +9181,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="124" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -9142,7 +9204,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="108"/>
+      <c r="B23" s="124"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -9163,7 +9225,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="108"/>
+      <c r="B24" s="124"/>
       <c r="C24" t="s">
         <v>204</v>
       </c>
@@ -9189,7 +9251,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="124" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -9212,7 +9274,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="108"/>
+      <c r="B26" s="124"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
@@ -9233,7 +9295,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="108"/>
+      <c r="B27" s="124"/>
       <c r="C27" t="s">
         <v>204</v>
       </c>
@@ -9259,7 +9321,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="108" t="s">
+      <c r="B28" s="124" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -9282,7 +9344,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="108"/>
+      <c r="B29" s="124"/>
       <c r="C29" t="s">
         <v>194</v>
       </c>
@@ -9303,7 +9365,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="108"/>
+      <c r="B30" s="124"/>
       <c r="C30" t="s">
         <v>204</v>
       </c>
@@ -9329,7 +9391,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="108" t="s">
+      <c r="B31" s="124" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9352,7 +9414,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="108"/>
+      <c r="B32" s="124"/>
       <c r="C32" t="s">
         <v>194</v>
       </c>
@@ -9373,7 +9435,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="108"/>
+      <c r="B33" s="124"/>
       <c r="C33" t="s">
         <v>204</v>
       </c>
@@ -9425,7 +9487,7 @@
       <c r="A36" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="108" t="s">
+      <c r="B36" s="124" t="s">
         <v>81</v>
       </c>
       <c r="C36" t="s">
@@ -9448,7 +9510,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="108"/>
+      <c r="B37" s="124"/>
       <c r="C37" t="s">
         <v>194</v>
       </c>
@@ -9469,7 +9531,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="108"/>
+      <c r="B38" s="124"/>
       <c r="C38" t="s">
         <v>204</v>
       </c>
@@ -9490,7 +9552,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="108" t="s">
+      <c r="B39" s="124" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9513,7 +9575,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="B40" s="108"/>
+      <c r="B40" s="124"/>
       <c r="C40" t="s">
         <v>194</v>
       </c>
@@ -9534,7 +9596,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="108"/>
+      <c r="B41" s="124"/>
       <c r="C41" t="s">
         <v>204</v>
       </c>
@@ -9555,7 +9617,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="108" t="s">
+      <c r="B42" s="124" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9578,7 +9640,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="B43" s="108"/>
+      <c r="B43" s="124"/>
       <c r="C43" t="s">
         <v>194</v>
       </c>
@@ -9599,7 +9661,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="B44" s="108"/>
+      <c r="B44" s="124"/>
       <c r="C44" t="s">
         <v>204</v>
       </c>
@@ -9620,7 +9682,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="B45" s="108" t="s">
+      <c r="B45" s="124" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9643,7 +9705,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="B46" s="108"/>
+      <c r="B46" s="124"/>
       <c r="C46" t="s">
         <v>194</v>
       </c>
@@ -9664,7 +9726,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="B47" s="108"/>
+      <c r="B47" s="124"/>
       <c r="C47" t="s">
         <v>204</v>
       </c>
@@ -9685,7 +9747,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="108" t="s">
+      <c r="B48" s="124" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9708,7 +9770,7 @@
       </c>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="108"/>
+      <c r="B49" s="124"/>
       <c r="C49" t="s">
         <v>194</v>
       </c>
@@ -9729,7 +9791,7 @@
       </c>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="108"/>
+      <c r="B50" s="124"/>
       <c r="C50" t="s">
         <v>204</v>
       </c>
@@ -9750,30 +9812,35 @@
       </c>
     </row>
     <row r="51" spans="2:8">
-      <c r="B51" s="90" t="s">
+      <c r="B51" s="88" t="s">
         <v>112</v>
       </c>
       <c r="C51" t="s">
         <v>204</v>
       </c>
-      <c r="D51" s="97">
-        <v>1</v>
-      </c>
-      <c r="E51" s="97">
-        <v>1</v>
-      </c>
-      <c r="F51" s="97">
+      <c r="D51" s="94">
+        <v>1</v>
+      </c>
+      <c r="E51" s="94">
+        <v>1</v>
+      </c>
+      <c r="F51" s="94">
         <v>0.95</v>
       </c>
-      <c r="G51" s="97">
+      <c r="G51" s="94">
         <v>0.95</v>
       </c>
-      <c r="H51" s="97">
+      <c r="H51" s="94">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9784,11 +9851,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9833,188 +9895,188 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="100"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102" t="s">
+      <c r="A3" s="98"/>
+      <c r="B3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="100"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="101"/>
-      <c r="B4" s="102" t="s">
+      <c r="A4" s="98"/>
+      <c r="B4" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="103"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="100"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="101"/>
-      <c r="B5" s="102" t="s">
+      <c r="A5" s="98"/>
+      <c r="B5" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="102" t="s">
+      <c r="C5" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="102" t="s">
+      <c r="D5" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="103"/>
+      <c r="E5" s="100"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="101"/>
-      <c r="B6" s="102" t="s">
+      <c r="A6" s="98"/>
+      <c r="B6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="103"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="100"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="104"/>
-      <c r="B7" s="105" t="s">
+      <c r="A7" s="101"/>
+      <c r="B7" s="102" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="107"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="104"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="100"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="101"/>
-      <c r="B10" s="102" t="s">
+      <c r="A10" s="98"/>
+      <c r="B10" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="103"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="100"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="101"/>
-      <c r="B11" s="102" t="s">
+      <c r="A11" s="98"/>
+      <c r="B11" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="101"/>
-      <c r="B12" s="102" t="s">
+      <c r="A12" s="98"/>
+      <c r="B12" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="102"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="103"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="100"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="101"/>
-      <c r="B13" s="102" t="s">
+      <c r="A13" s="98"/>
+      <c r="B13" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="102" t="s">
+      <c r="D13" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="E13" s="103"/>
+      <c r="E13" s="100"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="104"/>
-      <c r="B14" s="105" t="s">
+      <c r="A14" s="101"/>
+      <c r="B14" s="102" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="107"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="104"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="C16" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="D16" s="99" t="s">
+      <c r="D16" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="E16" s="100"/>
+      <c r="E16" s="97"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="101"/>
-      <c r="B17" s="102" t="s">
+      <c r="A17" s="98"/>
+      <c r="B17" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="102" t="s">
+      <c r="C17" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="E17" s="103"/>
+      <c r="E17" s="100"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="101"/>
-      <c r="B18" s="102" t="s">
+      <c r="A18" s="98"/>
+      <c r="B18" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="103"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="100"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="101"/>
-      <c r="B19" s="102" t="s">
+      <c r="A19" s="98"/>
+      <c r="B19" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="102"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="103"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="100"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="101"/>
-      <c r="B20" s="102" t="s">
+      <c r="A20" s="98"/>
+      <c r="B20" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="102"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="103"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="100"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="104"/>
-      <c r="B21" s="105" t="s">
+      <c r="A21" s="101"/>
+      <c r="B21" s="102" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="106"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="107"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="104"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10308,8 +10370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -10611,19 +10673,19 @@
       <c r="C11" s="69">
         <v>0</v>
       </c>
-      <c r="D11" s="89">
+      <c r="D11" s="87">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="E11" s="89">
+      <c r="E11" s="87">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="F11" s="89">
+      <c r="F11" s="87">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="G11" s="89">
+      <c r="G11" s="87">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
@@ -11219,7 +11281,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B36" s="83" t="s">
+      <c r="B36" s="82" t="s">
         <v>225</v>
       </c>
       <c r="C36" s="3">
@@ -11520,12 +11582,134 @@
       <c r="A46" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B49" s="4"/>
-    </row>
-    <row r="50" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B50" s="4"/>
+      <c r="B46" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B47" t="s">
+        <v>250</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3">
+        <v>1</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B48" t="s">
+        <v>251</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3">
+        <v>1</v>
+      </c>
+      <c r="H48" s="3">
+        <v>1</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B49" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <v>1</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B50" t="s">
+        <v>253</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3">
+        <v>1</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11546,8 +11730,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection sqref="A1:F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -13340,10 +13524,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -13974,6 +14158,341 @@
       </c>
       <c r="H27" s="12">
         <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="12">
+        <v>1</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12">
+        <v>1</v>
+      </c>
+      <c r="G28" s="12">
+        <v>1</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>250</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1</v>
+      </c>
+      <c r="G31" s="12">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>252</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="H42" s="12">
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -14678,13 +15197,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="13">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="82" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="84">
+      <c r="B2" s="83">
         <v>0.9</v>
       </c>
-      <c r="C2" s="91">
+      <c r="C2" s="89">
         <v>0.09</v>
       </c>
       <c r="D2">
@@ -14696,13 +15215,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="13">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="82" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="84">
-        <v>1</v>
-      </c>
-      <c r="C3" s="91">
+      <c r="B3" s="83">
+        <v>1</v>
+      </c>
+      <c r="C3" s="89">
         <v>0.02</v>
       </c>
       <c r="D3">
@@ -14714,13 +15233,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="13">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="84">
-        <v>1</v>
-      </c>
-      <c r="C4" s="91">
+      <c r="B4" s="83">
+        <v>1</v>
+      </c>
+      <c r="C4" s="89">
         <v>0.08</v>
       </c>
       <c r="D4">
@@ -14732,13 +15251,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="13">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="84">
-        <v>1</v>
-      </c>
-      <c r="C5" s="91">
+      <c r="B5" s="83">
+        <v>1</v>
+      </c>
+      <c r="C5" s="89">
         <v>0.18</v>
       </c>
       <c r="D5">
@@ -14750,13 +15269,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="13">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="B6" s="84">
-        <v>1</v>
-      </c>
-      <c r="C6" s="91">
+      <c r="B6" s="83">
+        <v>1</v>
+      </c>
+      <c r="C6" s="89">
         <v>0.02</v>
       </c>
       <c r="D6">
@@ -14768,13 +15287,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="13">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="84">
+      <c r="B7" s="83">
         <v>0.93</v>
       </c>
-      <c r="C7" s="91">
+      <c r="C7" s="89">
         <v>0.45</v>
       </c>
       <c r="D7">
@@ -14786,13 +15305,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="13">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B8" s="84">
+      <c r="B8" s="83">
         <v>0.5</v>
       </c>
-      <c r="C8" s="91">
+      <c r="C8" s="89">
         <v>0.03</v>
       </c>
       <c r="D8">
@@ -14804,13 +15323,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="13">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="82" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="84">
+      <c r="B9" s="83">
         <v>0.5</v>
       </c>
-      <c r="C9" s="91">
+      <c r="C9" s="89">
         <v>0.11</v>
       </c>
       <c r="D9">
@@ -14822,13 +15341,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="13">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="B10" s="84">
+      <c r="B10" s="83">
         <v>0.98</v>
       </c>
-      <c r="C10" s="91">
+      <c r="C10" s="89">
         <v>0.01</v>
       </c>
       <c r="D10">
@@ -14861,7 +15380,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -14881,16 +15400,16 @@
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="124" t="s">
+      <c r="D1" s="120" t="s">
         <v>233</v>
       </c>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="120" t="s">
         <v>234</v>
       </c>
       <c r="F1" s="1"/>
@@ -14899,33 +15418,33 @@
       <c r="A2" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="125">
+      <c r="C2" s="121">
         <v>0.8</v>
       </c>
-      <c r="D2" s="125">
+      <c r="D2" s="121">
         <v>0.8</v>
       </c>
-      <c r="E2" s="125">
+      <c r="E2" s="121">
         <v>0.8</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="125">
+      <c r="C3" s="121">
         <f>'Distributions births'!C2</f>
         <v>0.15</v>
       </c>
-      <c r="D3" s="125">
+      <c r="D3" s="121">
         <f>'Distributions births'!C3</f>
         <v>0.03</v>
       </c>
-      <c r="E3" s="125">
+      <c r="E3" s="121">
         <f>'Distributions births'!C4</f>
         <v>0</v>
       </c>
@@ -14956,73 +15475,73 @@
     <row r="14" spans="1:13">
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="127"/>
+      <c r="J14" s="122"/>
+      <c r="K14" s="106"/>
+      <c r="L14" s="123"/>
       <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13">
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="127"/>
+      <c r="K15" s="106"/>
+      <c r="L15" s="123"/>
       <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13">
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="110"/>
-      <c r="L16" s="127"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="123"/>
       <c r="M16" s="11"/>
     </row>
     <row r="17" spans="8:13">
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="110"/>
-      <c r="L17" s="127"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="123"/>
       <c r="M17" s="11"/>
     </row>
     <row r="18" spans="8:13">
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="127"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="123"/>
       <c r="M18" s="11"/>
     </row>
     <row r="19" spans="8:13">
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="110"/>
-      <c r="L19" s="127"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="123"/>
       <c r="M19" s="11"/>
     </row>
     <row r="20" spans="8:13">
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="127"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="123"/>
       <c r="M20" s="11"/>
     </row>
     <row r="21" spans="8:13">
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="110"/>
-      <c r="L21" s="127"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="123"/>
       <c r="M21" s="11"/>
     </row>
     <row r="22" spans="8:13">
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="127"/>
+      <c r="K22" s="106"/>
+      <c r="L22" s="123"/>
       <c r="M22" s="11"/>
     </row>
     <row r="23" spans="8:13">
@@ -15057,8 +15576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -15622,75 +16141,113 @@
       <c r="A40" s="81" t="s">
         <v>225</v>
       </c>
-      <c r="B40" s="86">
+      <c r="B40" s="125">
         <v>0.5</v>
       </c>
-      <c r="C40" s="92">
+      <c r="C40" s="14">
         <v>0.85</v>
       </c>
-      <c r="D40" s="82">
+      <c r="D40" s="19">
         <f>SUM('Interventions family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="90" t="s">
         <v>246</v>
       </c>
-      <c r="B41" s="128">
+      <c r="B41" s="125">
         <v>0.1</v>
       </c>
-      <c r="C41" s="129">
+      <c r="C41" s="14">
         <v>0.85</v>
       </c>
-      <c r="D41" s="130">
+      <c r="D41" s="19">
         <v>0.8</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A42" s="93"/>
-      <c r="B42" s="94"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="96"/>
+      <c r="A42" t="s">
+        <v>249</v>
+      </c>
+      <c r="B42" s="125">
+        <v>0.84</v>
+      </c>
+      <c r="C42" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D42" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A43" s="93"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="95"/>
-      <c r="D43" s="96"/>
+      <c r="A43" t="s">
+        <v>250</v>
+      </c>
+      <c r="B43" s="125">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C43" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D43" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A44" s="93"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="95"/>
-      <c r="D44" s="96"/>
+      <c r="A44" t="s">
+        <v>251</v>
+      </c>
+      <c r="B44" s="125">
+        <v>0.69</v>
+      </c>
+      <c r="C44" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D44" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A45" s="93"/>
-      <c r="B45" s="94"/>
-      <c r="C45" s="95"/>
-      <c r="D45" s="96"/>
+      <c r="A45" t="s">
+        <v>252</v>
+      </c>
+      <c r="B45" s="125">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="C45" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D45" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A46" s="93"/>
-      <c r="B46" s="94"/>
-      <c r="C46" s="95"/>
-      <c r="D46" s="96"/>
+      <c r="A46" t="s">
+        <v>253</v>
+      </c>
+      <c r="B46" s="125">
+        <v>0.4</v>
+      </c>
+      <c r="C46" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="D46" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A47" s="93"/>
-      <c r="B47" s="94"/>
-      <c r="C47" s="95"/>
-      <c r="D47" s="96"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="93"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A48" s="93"/>
-      <c r="B48" s="94"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="96"/>
+      <c r="B48" s="91"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="93"/>
     </row>
     <row r="49" spans="3:3" ht="15.75" customHeight="1">
-      <c r="C49" s="95"/>
+      <c r="C49" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17156,115 +17713,115 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="115" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="116" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="109">
+      <c r="C2" s="105">
         <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="116" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="109">
+      <c r="C3" s="105">
         <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="116" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="109">
+      <c r="C4" s="105">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="117" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="109">
+      <c r="C5" s="105">
         <v>0.19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="117" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="105">
         <v>0.39</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="117" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="109">
+      <c r="C7" s="105">
         <v>0.19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="109">
+      <c r="C8" s="105">
         <v>1E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="118" t="s">
         <v>239</v>
       </c>
-      <c r="C9" s="109">
+      <c r="C9" s="105">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="118" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="109">
+      <c r="C10" s="105">
         <v>0.04</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="C11" s="109"/>
+      <c r="C11" s="105"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="119" t="s">
+      <c r="A12" s="115" t="s">
         <v>241</v>
       </c>
-      <c r="B12" s="110" t="s">
+      <c r="B12" s="106" t="s">
         <v>228</v>
       </c>
-      <c r="C12" s="109">
+      <c r="C12" s="105">
         <v>0.34</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="106" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="109">
+      <c r="C13" s="105">
         <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="106" t="s">
         <v>230</v>
       </c>
-      <c r="C14" s="109">
+      <c r="C14" s="105">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="B15" s="110" t="s">
+      <c r="B15" s="106" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="109">
+      <c r="C15" s="105">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -17563,268 +18120,268 @@
       <c r="A21" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="108" t="s">
         <v>232</v>
       </c>
-      <c r="C21" s="115">
-        <v>1</v>
-      </c>
-      <c r="D21" s="115">
+      <c r="C21" s="111">
+        <v>1</v>
+      </c>
+      <c r="D21" s="111">
         <v>1.52</v>
       </c>
-      <c r="E21" s="115">
+      <c r="E21" s="111">
         <v>1.75</v>
       </c>
-      <c r="F21" s="115">
+      <c r="F21" s="111">
         <v>3.14</v>
       </c>
-      <c r="G21" s="116"/>
+      <c r="G21" s="112"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B22" s="112" t="s">
+      <c r="B22" s="108" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="115">
-        <v>1</v>
-      </c>
-      <c r="D22" s="115">
+      <c r="C22" s="111">
+        <v>1</v>
+      </c>
+      <c r="D22" s="111">
         <v>1.2</v>
       </c>
-      <c r="E22" s="115">
+      <c r="E22" s="111">
         <v>1.4</v>
       </c>
-      <c r="F22" s="115">
+      <c r="F22" s="111">
         <v>1.6</v>
       </c>
-      <c r="G22" s="116"/>
+      <c r="G22" s="112"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B23" s="112" t="s">
+      <c r="B23" s="108" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="115">
-        <v>1</v>
-      </c>
-      <c r="D23" s="115">
+      <c r="C23" s="111">
+        <v>1</v>
+      </c>
+      <c r="D23" s="111">
         <v>1.2</v>
       </c>
-      <c r="E23" s="115">
+      <c r="E23" s="111">
         <v>1.4</v>
       </c>
-      <c r="F23" s="115">
+      <c r="F23" s="111">
         <v>1.6</v>
       </c>
-      <c r="G23" s="116"/>
+      <c r="G23" s="112"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B24" s="113" t="s">
+      <c r="B24" s="109" t="s">
         <v>235</v>
       </c>
-      <c r="C24" s="115">
-        <v>1</v>
-      </c>
-      <c r="D24" s="115">
+      <c r="C24" s="111">
+        <v>1</v>
+      </c>
+      <c r="D24" s="111">
         <v>1.52</v>
       </c>
-      <c r="E24" s="115">
+      <c r="E24" s="111">
         <v>1.75</v>
       </c>
-      <c r="F24" s="115">
+      <c r="F24" s="111">
         <v>1.73</v>
       </c>
-      <c r="G24" s="116"/>
+      <c r="G24" s="112"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B25" s="113" t="s">
+      <c r="B25" s="109" t="s">
         <v>236</v>
       </c>
-      <c r="C25" s="115">
-        <v>1</v>
-      </c>
-      <c r="D25" s="115">
-        <v>1</v>
-      </c>
-      <c r="E25" s="115">
-        <v>1</v>
-      </c>
-      <c r="F25" s="115">
-        <v>1</v>
-      </c>
-      <c r="G25" s="116"/>
+      <c r="C25" s="111">
+        <v>1</v>
+      </c>
+      <c r="D25" s="111">
+        <v>1</v>
+      </c>
+      <c r="E25" s="111">
+        <v>1</v>
+      </c>
+      <c r="F25" s="111">
+        <v>1</v>
+      </c>
+      <c r="G25" s="112"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B26" s="113" t="s">
+      <c r="B26" s="109" t="s">
         <v>237</v>
       </c>
-      <c r="C26" s="115">
-        <v>1</v>
-      </c>
-      <c r="D26" s="115">
-        <v>1</v>
-      </c>
-      <c r="E26" s="115">
-        <v>1</v>
-      </c>
-      <c r="F26" s="115">
-        <v>1</v>
-      </c>
-      <c r="G26" s="116"/>
+      <c r="C26" s="111">
+        <v>1</v>
+      </c>
+      <c r="D26" s="111">
+        <v>1</v>
+      </c>
+      <c r="E26" s="111">
+        <v>1</v>
+      </c>
+      <c r="F26" s="111">
+        <v>1</v>
+      </c>
+      <c r="G26" s="112"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B27" s="114" t="s">
+      <c r="B27" s="110" t="s">
         <v>238</v>
       </c>
-      <c r="C27" s="115">
-        <v>1</v>
-      </c>
-      <c r="D27" s="115">
+      <c r="C27" s="111">
+        <v>1</v>
+      </c>
+      <c r="D27" s="111">
         <v>1.52</v>
       </c>
-      <c r="E27" s="115">
+      <c r="E27" s="111">
         <v>1.75</v>
       </c>
-      <c r="F27" s="115">
+      <c r="F27" s="111">
         <v>1.52</v>
       </c>
-      <c r="G27" s="116"/>
+      <c r="G27" s="112"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B28" s="114" t="s">
+      <c r="B28" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="C28" s="115">
-        <v>1</v>
-      </c>
-      <c r="D28" s="115">
-        <v>1</v>
-      </c>
-      <c r="E28" s="115">
+      <c r="C28" s="111">
+        <v>1</v>
+      </c>
+      <c r="D28" s="111">
+        <v>1</v>
+      </c>
+      <c r="E28" s="111">
         <v>1.33</v>
       </c>
-      <c r="F28" s="115">
-        <v>1</v>
-      </c>
-      <c r="G28" s="116"/>
+      <c r="F28" s="111">
+        <v>1</v>
+      </c>
+      <c r="G28" s="112"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B29" s="114" t="s">
+      <c r="B29" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="C29" s="115">
-        <v>1</v>
-      </c>
-      <c r="D29" s="115">
-        <v>1</v>
-      </c>
-      <c r="E29" s="115">
+      <c r="C29" s="111">
+        <v>1</v>
+      </c>
+      <c r="D29" s="111">
+        <v>1</v>
+      </c>
+      <c r="E29" s="111">
         <v>1.33</v>
       </c>
-      <c r="F29" s="115">
-        <v>1</v>
-      </c>
-      <c r="G29" s="116"/>
+      <c r="F29" s="111">
+        <v>1</v>
+      </c>
+      <c r="G29" s="112"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112"/>
+      <c r="G30" s="112"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="B31" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C31" s="117"/>
-      <c r="D31" s="117"/>
-      <c r="E31" s="117"/>
-      <c r="F31" s="117"/>
-      <c r="G31" s="116"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="112"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B32" s="111" t="s">
+      <c r="B32" s="107" t="s">
         <v>228</v>
       </c>
-      <c r="C32" s="115">
-        <v>1</v>
-      </c>
-      <c r="D32" s="118">
-        <v>1</v>
-      </c>
-      <c r="E32" s="118">
-        <v>1</v>
-      </c>
-      <c r="F32" s="118">
-        <v>1</v>
-      </c>
-      <c r="G32" s="116"/>
+      <c r="C32" s="111">
+        <v>1</v>
+      </c>
+      <c r="D32" s="114">
+        <v>1</v>
+      </c>
+      <c r="E32" s="114">
+        <v>1</v>
+      </c>
+      <c r="F32" s="114">
+        <v>1</v>
+      </c>
+      <c r="G32" s="112"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B33" s="111" t="s">
+      <c r="B33" s="107" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="115">
-        <v>1</v>
-      </c>
-      <c r="D33" s="118">
+      <c r="C33" s="111">
+        <v>1</v>
+      </c>
+      <c r="D33" s="114">
         <v>1.41</v>
       </c>
-      <c r="E33" s="118">
+      <c r="E33" s="114">
         <v>1.49</v>
       </c>
-      <c r="F33" s="118">
+      <c r="F33" s="114">
         <v>3.03</v>
       </c>
-      <c r="G33" s="116"/>
+      <c r="G33" s="112"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="107" t="s">
         <v>230</v>
       </c>
-      <c r="C34" s="115">
-        <v>1</v>
-      </c>
-      <c r="D34" s="118">
+      <c r="C34" s="111">
+        <v>1</v>
+      </c>
+      <c r="D34" s="114">
         <v>1.18</v>
       </c>
-      <c r="E34" s="118">
+      <c r="E34" s="114">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F34" s="118">
+      <c r="F34" s="114">
         <v>1.77</v>
       </c>
-      <c r="G34" s="116"/>
+      <c r="G34" s="112"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B35" s="111" t="s">
+      <c r="B35" s="107" t="s">
         <v>231</v>
       </c>
-      <c r="C35" s="115">
-        <v>1</v>
-      </c>
-      <c r="D35" s="118">
-        <v>1</v>
-      </c>
-      <c r="E35" s="118">
-        <v>1</v>
-      </c>
-      <c r="F35" s="118">
-        <v>1</v>
-      </c>
-      <c r="G35" s="116"/>
+      <c r="C35" s="111">
+        <v>1</v>
+      </c>
+      <c r="D35" s="114">
+        <v>1</v>
+      </c>
+      <c r="E35" s="114">
+        <v>1</v>
+      </c>
+      <c r="F35" s="114">
+        <v>1</v>
+      </c>
+      <c r="G35" s="112"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" customHeight="1">
-      <c r="C36" s="116"/>
-      <c r="D36" s="116"/>
-      <c r="E36" s="116"/>
-      <c r="F36" s="116"/>
-      <c r="G36" s="116"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="116"/>
-      <c r="J36" s="116"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="112"/>
+      <c r="G36" s="112"/>
+      <c r="H36" s="112"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="112"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17845,7 +18402,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Small changes to data
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -421,26 +421,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-If user wants this, it must be checked for </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>all populations</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> b/c they are all targetted at once.</t>
+We currently do not have 'appropriate complementary feeding' data to use, so this does nothing.</t>
         </r>
       </text>
     </comment>
@@ -454,7 +435,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -474,12 +455,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1.5*unit cost of BFP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0">
-      <text>
+If user wants this, it must be checked for </t>
+        </r>
         <r>
           <rPr>
             <b/>
@@ -488,7 +465,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Sam:</t>
+          <t>all populations</t>
         </r>
         <r>
           <rPr>
@@ -497,32 +474,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-0.5* unit cost of BFP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Totally fictional</t>
+          <t xml:space="preserve"> b/c they are all targetted at once.</t>
         </r>
       </text>
     </comment>
@@ -533,35 +485,34 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author xml:space="preserve"> Janka Petravic</author>
-    <author>Microsoft Office User</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Poor pregnant women - all target population</t>
+1.5*unit cost of BFP</t>
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="1">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -571,7 +522,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Sam:</t>
         </r>
         <r>
           <rPr>
@@ -581,11 +532,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+0.5* unit cost of BFP</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="1">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -595,7 +546,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Sam:</t>
         </r>
         <r>
           <rPr>
@@ -605,55 +556,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% at risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% at risk from malaria</t>
+Totally fictional</t>
         </r>
       </text>
     </comment>
@@ -666,10 +569,9 @@
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
     <author>Microsoft Office User</author>
-    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -689,11 +591,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+Poor pregnant women - all target population</t>
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="1">
+    <comment ref="C9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -703,9 +605,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -715,11 +615,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="1">
+    <comment ref="D9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -729,9 +629,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -741,11 +639,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="1">
+    <comment ref="C11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -755,9 +653,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -767,11 +663,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="1">
+    <comment ref="D11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -781,9 +677,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -793,464 +687,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Source: WHO guidelines on sprinkles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Effect on iron-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Only in malaria risk</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-made this number up
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Same effect as iron fortification</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -1261,11 +698,36 @@
 <file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author xml:space="preserve"> Janka Petravic</author>
     <author>Microsoft Office User</author>
-    <author>Sam</author>
+    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="F21" authorId="0">
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1275,7 +737,9 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -1285,11 +749,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-WHO statement</t>
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="1">
+    <comment ref="M2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1299,7 +763,9 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -1309,11 +775,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="1">
+    <comment ref="N2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1323,7 +789,9 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -1333,7 +801,490 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Source: WHO guidelines on sprinkles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Effect on iron-deficiency anemia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Only in malaria risk</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E30" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+made this number up
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Same effect as iron fortification</t>
         </r>
       </text>
     </comment>
@@ -1344,30 +1295,79 @@
 <file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Ruth</author>
+    <author>Microsoft Office User</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="F21" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Ruth made these numbers up</t>
+WHO statement</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
         </r>
       </text>
     </comment>
@@ -1376,6 +1376,40 @@
 </file>
 
 <file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ruth made these numbers up</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
@@ -2422,7 +2456,7 @@
 </comments>
 </file>
 
-<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
@@ -2553,7 +2587,7 @@
 </comments>
 </file>
 
-<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
@@ -3159,7 +3193,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3179,7 +3213,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-From Jakub's book, annual incidence of severe acute wasting is annual prevalence * 1.6  (p. 147). Assuming the same to be true for moderate wasting.</t>
+We don't model deaths through severe diarrhoea specifically, only deaths through diarrhoea</t>
         </r>
       </text>
     </comment>
@@ -3191,10 +3225,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
-    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3214,271 +3247,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Using prevalence of iron-deficient anaemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fictional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-WHO database from 2001; hemoglobin &lt;110 g/L, includes mild (all-cause anemia). Consistent with Khan 2016 70.8% anemia in 6-23 months and Stevens overall ~51%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-WHO database from 2001</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Khan 2016</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST &lt; 110 g/L, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST - &lt;120 g/L, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fictional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Stevens: 42% of global childhood anemia is ID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L6" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Stevens</t>
+From Jakub's book, annual incidence of severe acute wasting is annual prevalence * 1.6  (p. 147). Assuming the same to be true for moderate wasting.</t>
         </r>
       </text>
     </comment>
@@ -3489,19 +3258,295 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author>Sam</author>
+    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E16" authorId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Using prevalence of iron-deficient anaemia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Arial"/>
-          </rPr>
-          <t>Nick:
-Any breastfeeding. Other categories don't matter for this age upwards as relative risks are the same.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO database from 2001; hemoglobin &lt;110 g/L, includes mild (all-cause anemia). Consistent with Khan 2016 70.8% anemia in 6-23 months and Stevens overall ~51%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO database from 2001</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Khan 2016</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST &lt; 110 g/L, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST - &lt;120 g/L, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Stevens: 42% of global childhood anemia is ID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Stevens</t>
         </r>
       </text>
     </comment>
@@ -3512,54 +3557,19 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author xml:space="preserve"> Janka Petravic</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="E16" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Term AGA should be given by a formula in the spreadsheet. The result should be greyed to indicate that it is calculated.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Kozuki 2012, for hematocrit &lt;90g/L</t>
+          </rPr>
+          <t>Nick:
+Any breastfeeding. Other categories don't matter for this age upwards as relative risks are the same.</t>
         </r>
       </text>
     </comment>
@@ -3570,30 +3580,54 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Sam</author>
+    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="A46" authorId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Not modelling death through anaemia</t>
+Term AGA should be given by a formula in the spreadsheet. The result should be greyed to indicate that it is calculated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kozuki 2012, for hematocrit &lt;90g/L</t>
         </r>
       </text>
     </comment>
@@ -3605,11 +3639,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
-    <author>Janka Petravic</author>
-    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0">
+    <comment ref="A46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3629,199 +3661,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-May not need these beyond calculation below</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F12" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST: 1.11</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This calculation 'dilutes' OR so that we cover 'everyone' with IYCF, not just frac poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This assumes we deliver PPCF with education to the poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This assumes we deliver PPCF with education to the poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This assumes we deliver PPCF with education to the poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This should be changed later I guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This should be changed later I guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fictional</t>
+Not modelling death through anaemia</t>
         </r>
       </text>
     </comment>
@@ -3833,9 +3673,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
+    <author>Janka Petravic</author>
+    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3855,7 +3697,199 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-We currently do not have 'appropriate complementary feeding' data to use, so this does nothing.</t>
+May not need these beyond calculation below</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST: 1.11</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This calculation 'dilutes' OR so that we cover 'everyone' with IYCF, not just frac poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This assumes we deliver PPCF with education to the poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This assumes we deliver PPCF with education to the poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This assumes we deliver PPCF with education to the poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This should be changed later I guess</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This should be changed later I guess</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional</t>
         </r>
       </text>
     </comment>
@@ -3864,7 +3898,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="235">
   <si>
     <t>year</t>
   </si>
@@ -4472,18 +4506,6 @@
     <t>under 5 mortality</t>
   </si>
   <si>
-    <t>Fraction MAM to SAM</t>
-  </si>
-  <si>
-    <t>Fraction SAM to MAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction severe diarrhoea </t>
-  </si>
-  <si>
-    <t>OR stunting condition</t>
-  </si>
-  <si>
     <t>OR stunting progression</t>
   </si>
   <si>
@@ -4569,6 +4591,18 @@
   </si>
   <si>
     <t>OR anaemia by condition</t>
+  </si>
+  <si>
+    <t>OR stunting by condition</t>
+  </si>
+  <si>
+    <t>fraction MAM to SAM</t>
+  </si>
+  <si>
+    <t>fraction SAM to MAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fraction severe diarrhoea </t>
   </si>
 </sst>
 </file>
@@ -7612,8 +7646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7719,7 +7753,7 @@
     </row>
     <row r="12" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c r="C12" s="47">
         <v>0.9</v>
@@ -7727,7 +7761,7 @@
     </row>
     <row r="13" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="C13" s="47">
         <v>0.4</v>
@@ -7735,7 +7769,7 @@
     </row>
     <row r="14" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="C14" s="69">
         <v>0.2</v>
@@ -7896,7 +7930,7 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B37" s="92" t="s">
         <v>118</v>
@@ -7950,7 +7984,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B43" s="92" t="s">
         <v>122</v>
@@ -9206,7 +9240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -9640,10 +9674,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10002,7 +10036,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>79</v>
@@ -11061,7 +11095,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>82</v>
@@ -11533,7 +11567,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>106</v>
@@ -11599,7 +11633,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="47" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>106</v>
@@ -15021,13 +15055,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>27</v>
@@ -15036,10 +15070,10 @@
         <v>36</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -15296,10 +15330,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -15524,7 +15558,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>149</v>
@@ -16145,11 +16179,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16191,7 +16225,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B2" s="90">
         <v>7.0000000000000001E-3</v>
@@ -16447,13 +16481,14 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B10" s="90">
         <v>0</v>
       </c>
       <c r="C10" s="90">
-        <v>0.14810000000000001</v>
+        <f>14.81% * 0.2</f>
+        <v>2.9620000000000004E-2</v>
       </c>
       <c r="D10" s="90">
         <v>0.14810000000000001</v>
@@ -16479,22 +16514,22 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>28</v>
+        <v>228</v>
       </c>
       <c r="B11" s="90">
         <v>0</v>
       </c>
       <c r="C11" s="90">
-        <v>0.2883</v>
+        <v>0</v>
       </c>
       <c r="D11" s="90">
-        <v>0.2883</v>
+        <v>0</v>
       </c>
       <c r="E11" s="90">
-        <v>0.2883</v>
+        <v>0</v>
       </c>
       <c r="F11" s="90">
-        <v>0.2883</v>
+        <v>0</v>
       </c>
       <c r="G11" s="31">
         <v>0</v>
@@ -16511,22 +16546,22 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="90">
         <v>0</v>
       </c>
       <c r="C12" s="90">
-        <v>4.1000000000000002E-2</v>
+        <v>0.2883</v>
       </c>
       <c r="D12" s="90">
-        <v>4.1000000000000002E-2</v>
+        <v>0.2883</v>
       </c>
       <c r="E12" s="90">
-        <v>4.1000000000000002E-2</v>
+        <v>0.2883</v>
       </c>
       <c r="F12" s="90">
-        <v>4.1000000000000002E-2</v>
+        <v>0.2883</v>
       </c>
       <c r="G12" s="31">
         <v>0</v>
@@ -16543,22 +16578,22 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="13">
+        <v>29</v>
+      </c>
+      <c r="B13" s="90">
         <v>0</v>
       </c>
       <c r="C13" s="90">
-        <v>5.0099999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="D13" s="90">
-        <v>5.0099999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="E13" s="90">
-        <v>5.0099999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="F13" s="90">
-        <v>5.0099999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G13" s="31">
         <v>0</v>
@@ -16575,22 +16610,22 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="13">
         <v>0</v>
       </c>
       <c r="C14" s="90">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0099999999999999E-2</v>
       </c>
       <c r="D14" s="90">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0099999999999999E-2</v>
       </c>
       <c r="E14" s="90">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0099999999999999E-2</v>
       </c>
       <c r="F14" s="90">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0099999999999999E-2</v>
       </c>
       <c r="G14" s="31">
         <v>0</v>
@@ -16607,22 +16642,22 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13">
         <v>0</v>
       </c>
       <c r="C15" s="90">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D15" s="90">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E15" s="90">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F15" s="90">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="G15" s="31">
         <v>0</v>
@@ -16639,22 +16674,22 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
       </c>
       <c r="C16" s="90">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D16" s="90">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E16" s="90">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F16" s="90">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G16" s="31">
         <v>0</v>
@@ -16671,22 +16706,22 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
       </c>
       <c r="C17" s="90">
-        <v>0.14510000000000001</v>
+        <v>0</v>
       </c>
       <c r="D17" s="90">
-        <v>0.14510000000000001</v>
+        <v>0</v>
       </c>
       <c r="E17" s="90">
-        <v>0.14510000000000001</v>
+        <v>0</v>
       </c>
       <c r="F17" s="90">
-        <v>0.14510000000000001</v>
+        <v>0</v>
       </c>
       <c r="G17" s="31">
         <v>0</v>
@@ -16703,22 +16738,22 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="13">
         <v>0</v>
       </c>
       <c r="C18" s="90">
-        <v>0.31130000000000002</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="D18" s="90">
-        <v>0.31130000000000002</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="E18" s="90">
-        <v>0.31130000000000002</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="F18" s="90">
-        <v>0.31130000000000002</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="G18" s="31">
         <v>0</v>
@@ -16735,39 +16770,39 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="31">
-        <v>0</v>
-      </c>
-      <c r="C19" s="31">
-        <v>0</v>
-      </c>
-      <c r="D19" s="31">
-        <v>0</v>
-      </c>
-      <c r="E19" s="31">
-        <v>0</v>
-      </c>
-      <c r="F19" s="31">
-        <v>0</v>
-      </c>
-      <c r="G19" s="91">
-        <v>2.5899999999999999E-2</v>
-      </c>
-      <c r="H19" s="91">
-        <v>2.5899999999999999E-2</v>
-      </c>
-      <c r="I19" s="91">
-        <v>2.5899999999999999E-2</v>
-      </c>
-      <c r="J19" s="91">
-        <v>2.5899999999999999E-2</v>
+        <v>35</v>
+      </c>
+      <c r="B19" s="13">
+        <v>0</v>
+      </c>
+      <c r="C19" s="90">
+        <v>0.31130000000000002</v>
+      </c>
+      <c r="D19" s="90">
+        <v>0.31130000000000002</v>
+      </c>
+      <c r="E19" s="90">
+        <v>0.31130000000000002</v>
+      </c>
+      <c r="F19" s="90">
+        <v>0.31130000000000002</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0</v>
+      </c>
+      <c r="H19" s="31">
+        <v>0</v>
+      </c>
+      <c r="I19" s="31">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="31">
         <v>0</v>
@@ -16785,21 +16820,21 @@
         <v>0</v>
       </c>
       <c r="G20" s="91">
-        <v>7.1000000000000004E-3</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="H20" s="91">
-        <v>7.1000000000000004E-3</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="I20" s="91">
-        <v>7.1000000000000004E-3</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="J20" s="91">
-        <v>7.1000000000000004E-3</v>
+        <v>2.5899999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="31">
         <v>0</v>
@@ -16817,21 +16852,21 @@
         <v>0</v>
       </c>
       <c r="G21" s="91">
-        <v>0.25590000000000002</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="H21" s="91">
-        <v>0.25590000000000002</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="I21" s="91">
-        <v>0.25590000000000002</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="J21" s="91">
-        <v>0.25590000000000002</v>
+        <v>7.1000000000000004E-3</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="31">
         <v>0</v>
@@ -16849,21 +16884,21 @@
         <v>0</v>
       </c>
       <c r="G22" s="91">
-        <v>0.1464</v>
+        <v>0.25590000000000002</v>
       </c>
       <c r="H22" s="91">
-        <v>0.1464</v>
+        <v>0.25590000000000002</v>
       </c>
       <c r="I22" s="91">
-        <v>0.1464</v>
+        <v>0.25590000000000002</v>
       </c>
       <c r="J22" s="91">
-        <v>0.1464</v>
+        <v>0.25590000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="31">
         <v>0</v>
@@ -16881,21 +16916,21 @@
         <v>0</v>
       </c>
       <c r="G23" s="91">
-        <v>1.7600000000000001E-2</v>
+        <v>0.1464</v>
       </c>
       <c r="H23" s="91">
-        <v>1.7600000000000001E-2</v>
+        <v>0.1464</v>
       </c>
       <c r="I23" s="91">
-        <v>1.7600000000000001E-2</v>
+        <v>0.1464</v>
       </c>
       <c r="J23" s="91">
-        <v>1.7600000000000001E-2</v>
+        <v>0.1464</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" s="31">
         <v>0</v>
@@ -16913,21 +16948,21 @@
         <v>0</v>
       </c>
       <c r="G24" s="91">
-        <v>1.8100000000000002E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="H24" s="91">
-        <v>1.8100000000000002E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="I24" s="91">
-        <v>1.8100000000000002E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="J24" s="91">
-        <v>1.8100000000000002E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="31">
         <v>0</v>
@@ -16945,21 +16980,21 @@
         <v>0</v>
       </c>
       <c r="G25" s="91">
-        <v>1.14E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="H25" s="91">
-        <v>1.14E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="I25" s="91">
-        <v>1.14E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="J25" s="91">
-        <v>1.14E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="31">
         <v>0</v>
@@ -16977,47 +17012,79 @@
         <v>0</v>
       </c>
       <c r="G26" s="91">
-        <v>0.15129999999999999</v>
+        <v>1.14E-2</v>
       </c>
       <c r="H26" s="91">
-        <v>0.15129999999999999</v>
+        <v>1.14E-2</v>
       </c>
       <c r="I26" s="91">
-        <v>0.15129999999999999</v>
+        <v>1.14E-2</v>
       </c>
       <c r="J26" s="91">
-        <v>0.15129999999999999</v>
+        <v>1.14E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="31">
+        <v>0</v>
+      </c>
+      <c r="C27" s="31">
+        <v>0</v>
+      </c>
+      <c r="D27" s="31">
+        <v>0</v>
+      </c>
+      <c r="E27" s="31">
+        <v>0</v>
+      </c>
+      <c r="F27" s="31">
+        <v>0</v>
+      </c>
+      <c r="G27" s="91">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="H27" s="91">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="I27" s="91">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="J27" s="91">
+        <v>0.15129999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="31">
-        <v>0</v>
-      </c>
-      <c r="C27" s="31">
-        <v>0</v>
-      </c>
-      <c r="D27" s="31">
-        <v>0</v>
-      </c>
-      <c r="E27" s="31">
-        <v>0</v>
-      </c>
-      <c r="F27" s="31">
-        <v>0</v>
-      </c>
-      <c r="G27" s="91">
+      <c r="B28" s="31">
+        <v>0</v>
+      </c>
+      <c r="C28" s="31">
+        <v>0</v>
+      </c>
+      <c r="D28" s="31">
+        <v>0</v>
+      </c>
+      <c r="E28" s="31">
+        <v>0</v>
+      </c>
+      <c r="F28" s="31">
+        <v>0</v>
+      </c>
+      <c r="G28" s="91">
         <v>0.36630000000000001</v>
       </c>
-      <c r="H27" s="91">
+      <c r="H28" s="91">
         <v>0.36630000000000001</v>
       </c>
-      <c r="I27" s="91">
+      <c r="I28" s="91">
         <v>0.36630000000000001</v>
       </c>
-      <c r="J27" s="91">
+      <c r="J28" s="91">
         <v>0.36630000000000001</v>
       </c>
     </row>
@@ -17028,6 +17095,7 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17063,7 +17131,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B2" s="15">
         <v>2.4300000000000002</v>
@@ -17083,7 +17151,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B3" s="31">
         <v>5.1999999999999998E-2</v>
@@ -17200,7 +17268,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>12</v>
@@ -17247,10 +17315,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
         <v>218</v>
-      </c>
-      <c r="B2" t="s">
-        <v>222</v>
       </c>
       <c r="C2" s="102">
         <f>1-C3</f>
@@ -17307,7 +17375,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C3" s="102">
         <f>C6</f>
@@ -17381,10 +17449,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C5" s="37">
         <v>0.1</v>
@@ -17428,10 +17496,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C6" s="37">
         <v>0.05</v>
@@ -17475,10 +17543,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C7" s="94">
         <v>0.01</v>
@@ -17929,10 +17997,10 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="11">
@@ -17947,7 +18015,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -18012,10 +18080,10 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -18163,7 +18231,7 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
@@ -18234,7 +18302,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -19132,7 +19200,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>14</v>
@@ -20031,13 +20099,13 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B46" t="s">
+        <v>225</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="B46" t="s">
-        <v>229</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -20081,7 +20149,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -20128,7 +20196,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -20172,7 +20240,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -20219,7 +20287,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -20263,7 +20331,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D51" s="4">
         <v>1</v>
@@ -20310,7 +20378,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D52" s="4">
         <v>1</v>
@@ -20354,7 +20422,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
@@ -20401,7 +20469,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
@@ -20445,7 +20513,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
@@ -20493,7 +20561,7 @@
         <v>87</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D56" s="4">
         <v>1</v>
@@ -20537,7 +20605,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D57" s="4">
         <v>1</v>
@@ -20584,7 +20652,7 @@
         <v>88</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
@@ -20628,7 +20696,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D59" s="4">
         <v>1</v>
@@ -20675,7 +20743,7 @@
         <v>89</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D60" s="4">
         <v>1</v>
@@ -20719,7 +20787,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D61" s="4">
         <v>1</v>
@@ -20770,7 +20838,7 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>37</v>
@@ -21486,7 +21554,7 @@
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>37</v>
@@ -22023,10 +22091,10 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A94" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>37</v>
@@ -22220,8 +22288,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22259,7 +22327,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -22283,10 +22351,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C4">
         <v>1.04</v>
@@ -22576,7 +22644,7 @@
         <v>157</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C21" s="47">
         <v>1.04</v>
@@ -22599,7 +22667,7 @@
         <v>158</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C23" s="47">
         <v>1.04</v>
@@ -22619,10 +22687,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B25" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C25" s="47">
         <v>1</v>

</xml_diff>

<commit_message>
Updates to relevant program areas
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -595,54 +595,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% at risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% at risk from malaria</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C11" authorId="1">
       <text>
         <r>
@@ -668,6 +620,54 @@
       </text>
     </comment>
     <comment ref="D11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -3898,7 +3898,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="238">
   <si>
     <t>year</t>
   </si>
@@ -4545,9 +4545,6 @@
     <t>Anaemia</t>
   </si>
   <si>
-    <t>Dependency</t>
-  </si>
-  <si>
     <t>Family planning</t>
   </si>
   <si>
@@ -4603,6 +4600,18 @@
   </si>
   <si>
     <t xml:space="preserve">fraction severe diarrhoea </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>Birth outcomes</t>
+  </si>
+  <si>
+    <t>Mortality</t>
   </si>
 </sst>
 </file>
@@ -7753,7 +7762,7 @@
     </row>
     <row r="12" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C12" s="47">
         <v>0.9</v>
@@ -7761,7 +7770,7 @@
     </row>
     <row r="13" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C13" s="47">
         <v>0.4</v>
@@ -7769,7 +7778,7 @@
     </row>
     <row r="14" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C14" s="69">
         <v>0.2</v>
@@ -7930,7 +7939,7 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B37" s="92" t="s">
         <v>118</v>
@@ -7984,7 +7993,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B43" s="92" t="s">
         <v>122</v>
@@ -9215,6 +9224,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9225,11 +9239,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9240,7 +9249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+    <sheetView zoomScale="133" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -9738,10 +9747,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9884,21 +9893,21 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="36">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="D8" s="36">
-        <v>0.35</v>
-      </c>
-      <c r="E8" s="36">
-        <v>0</v>
-      </c>
-      <c r="F8" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
         <v>0</v>
       </c>
     </row>
@@ -9906,24 +9915,22 @@
       <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="C9">
-        <f>'Baseline year demographics'!$C$8</f>
-        <v>0.1</v>
-      </c>
-      <c r="D9">
-        <f>'Baseline year demographics'!$C$8</f>
-        <v>0.1</v>
-      </c>
-      <c r="E9" s="36">
-        <v>0</v>
-      </c>
-      <c r="F9" s="36">
-        <v>0</v>
+      <c r="C9" s="36">
+        <v>1</v>
+      </c>
+      <c r="D9" s="36">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
-        <v>80</v>
+      <c r="A10" t="s">
+        <v>126</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -9957,6 +9964,45 @@
         <v>0</v>
       </c>
       <c r="F11" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0.35</v>
+      </c>
+      <c r="D12" s="36">
+        <v>0.35</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0</v>
+      </c>
+      <c r="F12" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <f>'Baseline year demographics'!$C$8</f>
+        <v>0.1</v>
+      </c>
+      <c r="D13">
+        <f>'Baseline year demographics'!$C$8</f>
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="36">
+        <v>0</v>
+      </c>
+      <c r="F13" s="36">
         <v>0</v>
       </c>
     </row>
@@ -9975,7 +10021,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11522,7 +11568,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11567,7 +11613,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>106</v>
@@ -11633,7 +11679,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>106</v>
@@ -12373,8 +12419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15036,10 +15082,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15049,11 +15095,14 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>213</v>
       </c>
@@ -15073,15 +15122,27 @@
         <v>216</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>151</v>
       </c>
@@ -15089,153 +15150,255 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="H22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C23" t="s">
+        <v>175</v>
+      </c>
+      <c r="H23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C29" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="H29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C30" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C31" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>134</v>
       </c>
@@ -15246,29 +15409,35 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B33" t="s">
         <v>175</v>
       </c>
+      <c r="C33" t="s">
+        <v>175</v>
+      </c>
       <c r="D33" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B34" t="s">
         <v>175</v>
       </c>
+      <c r="C34" t="s">
+        <v>175</v>
+      </c>
       <c r="D34" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>76</v>
       </c>
@@ -15276,7 +15445,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>145</v>
       </c>
@@ -15284,7 +15453,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>159</v>
       </c>
@@ -15292,7 +15461,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>160</v>
       </c>
@@ -15300,14 +15469,20 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>148</v>
+      </c>
+      <c r="J40" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -15320,7 +15495,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15333,7 +15508,7 @@
         <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -15542,7 +15717,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15558,7 +15733,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>149</v>
@@ -16183,7 +16358,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16225,7 +16400,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="90">
         <v>7.0000000000000001E-3</v>
@@ -16481,7 +16656,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="90">
         <v>0</v>
@@ -16514,7 +16689,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" s="90">
         <v>0</v>
@@ -17131,7 +17306,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="15">
         <v>2.4300000000000002</v>
@@ -17151,7 +17326,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3" s="31">
         <v>5.1999999999999998E-2</v>
@@ -17318,111 +17493,111 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C2" s="102">
-        <f>1-C3</f>
+        <f t="shared" ref="C2:O2" si="0">1-C3</f>
         <v>0.95</v>
       </c>
       <c r="D2" s="102">
-        <f>1-D3</f>
+        <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
       <c r="E2" s="102">
-        <f>1-E3</f>
+        <f t="shared" si="0"/>
         <v>0.68920000000000003</v>
       </c>
       <c r="F2" s="102">
-        <f>1-F3</f>
+        <f t="shared" si="0"/>
         <v>0.76900000000000002</v>
       </c>
       <c r="G2" s="102">
-        <f>1-G3</f>
+        <f t="shared" si="0"/>
         <v>0.82065999999999995</v>
       </c>
       <c r="H2" s="102">
-        <f>1-H3</f>
+        <f t="shared" si="0"/>
         <v>0.76419999999999999</v>
       </c>
       <c r="I2" s="102">
-        <f>1-I3</f>
+        <f t="shared" si="0"/>
         <v>0.76419999999999999</v>
       </c>
       <c r="J2" s="102">
-        <f>1-J3</f>
+        <f t="shared" si="0"/>
         <v>0.76419999999999999</v>
       </c>
       <c r="K2" s="102">
-        <f>1-K3</f>
+        <f t="shared" si="0"/>
         <v>0.76419999999999999</v>
       </c>
       <c r="L2" s="102">
-        <f>1-L3</f>
+        <f t="shared" si="0"/>
         <v>0.7762</v>
       </c>
       <c r="M2" s="102">
-        <f>1-M3</f>
+        <f t="shared" si="0"/>
         <v>0.7762</v>
       </c>
       <c r="N2" s="102">
-        <f>1-N3</f>
+        <f t="shared" si="0"/>
         <v>0.7762</v>
       </c>
       <c r="O2" s="102">
-        <f>1-O3</f>
+        <f t="shared" si="0"/>
         <v>0.7762</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C3" s="102">
         <f>C6</f>
         <v>0.05</v>
       </c>
       <c r="D3" s="102">
-        <f t="shared" ref="D3:N3" si="0">D6</f>
+        <f t="shared" ref="D3:N3" si="1">D6</f>
         <v>0.05</v>
       </c>
       <c r="E3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.31079999999999997</v>
       </c>
       <c r="F3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23100000000000001</v>
       </c>
       <c r="G3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17934</v>
       </c>
       <c r="H3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23580000000000001</v>
       </c>
       <c r="I3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23580000000000001</v>
       </c>
       <c r="J3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23580000000000001</v>
       </c>
       <c r="K3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23580000000000001</v>
       </c>
       <c r="L3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2238</v>
       </c>
       <c r="M3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2238</v>
       </c>
       <c r="N3" s="102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2238</v>
       </c>
       <c r="O3" s="102">
@@ -17452,7 +17627,7 @@
         <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C5" s="37">
         <v>0.1</v>
@@ -17499,7 +17674,7 @@
         <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" s="37">
         <v>0.05</v>
@@ -17546,7 +17721,7 @@
         <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7" s="94">
         <v>0.01</v>
@@ -17927,7 +18102,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18000,7 +18175,7 @@
         <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="11">
@@ -18015,7 +18190,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -18083,7 +18258,7 @@
         <v>205</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -18302,7 +18477,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -19200,7 +19375,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>14</v>
@@ -20102,10 +20277,10 @@
         <v>214</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -20149,7 +20324,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -20196,7 +20371,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -20240,7 +20415,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -20287,7 +20462,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -20331,7 +20506,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" s="4">
         <v>1</v>
@@ -20378,7 +20553,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D52" s="4">
         <v>1</v>
@@ -20422,7 +20597,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
@@ -20469,7 +20644,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
@@ -20513,7 +20688,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
@@ -20561,7 +20736,7 @@
         <v>87</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D56" s="4">
         <v>1</v>
@@ -20605,7 +20780,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D57" s="4">
         <v>1</v>
@@ -20652,7 +20827,7 @@
         <v>88</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
@@ -20696,7 +20871,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D59" s="4">
         <v>1</v>
@@ -20743,7 +20918,7 @@
         <v>89</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D60" s="4">
         <v>1</v>
@@ -20787,7 +20962,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D61" s="4">
         <v>1</v>
@@ -20838,7 +21013,7 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>37</v>
@@ -21554,7 +21729,7 @@
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>37</v>
@@ -22091,10 +22266,10 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A94" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B94" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>227</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>37</v>
@@ -22289,7 +22464,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22351,10 +22526,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4">
         <v>1.04</v>
@@ -22644,7 +22819,7 @@
         <v>157</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C21" s="47">
         <v>1.04</v>
@@ -22667,7 +22842,7 @@
         <v>158</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C23" s="47">
         <v>1.04</v>
@@ -22687,10 +22862,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C25" s="47">
         <v>1</v>

</xml_diff>

<commit_message>
Adjustments to dependencies sheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="15" activeTab="19"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="15" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2459,11 +2459,12 @@
 <file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Sam</author>
     <author>Microsoft Office User</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2473,6 +2474,54 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+When one intervention cannot exceed 1-cov of another</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+When one program cannot exceed cov of another</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
           <t>Microsoft Office User:</t>
         </r>
         <r>
@@ -2487,7 +2536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="1">
+    <comment ref="A12" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2511,7 +2560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="1">
+    <comment ref="A13" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2535,7 +2584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="1">
+    <comment ref="A22" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2559,7 +2608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="1">
+    <comment ref="A24" authorId="2">
       <text>
         <r>
           <rPr>
@@ -3898,7 +3947,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="239">
   <si>
     <t>year</t>
   </si>
@@ -4605,13 +4654,16 @@
     <t>None</t>
   </si>
   <si>
-    <t>Dependencies</t>
-  </si>
-  <si>
     <t>Birth outcomes</t>
   </si>
   <si>
     <t>Mortality</t>
+  </si>
+  <si>
+    <t>Exclusive dependencie</t>
+  </si>
+  <si>
+    <t>Threshold dependency</t>
   </si>
 </sst>
 </file>
@@ -15084,7 +15136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -15122,10 +15174,10 @@
         <v>216</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>215</v>
@@ -15492,96 +15544,101 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="65" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
added misc interventions into spreadsheet and added a tab for interventions PW
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="24780" windowHeight="14520" tabRatio="500" firstSheet="19" activeTab="21"/>
+    <workbookView xWindow="-69360" yWindow="-3800" windowWidth="28040" windowHeight="17620" tabRatio="500" firstSheet="18" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,11 @@
     <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId16"/>
     <sheet name="Interventions anemia" sheetId="30" r:id="rId17"/>
     <sheet name="Interventions wasting" sheetId="31" r:id="rId18"/>
-    <sheet name="Interventions for children" sheetId="28" r:id="rId19"/>
-    <sheet name="Interventions family planning" sheetId="34" r:id="rId20"/>
-    <sheet name="Interventions birth age" sheetId="37" r:id="rId21"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId22"/>
+    <sheet name="Interventions for PW" sheetId="38" r:id="rId19"/>
+    <sheet name="Interventions for children" sheetId="28" r:id="rId20"/>
+    <sheet name="Interventions family planning" sheetId="34" r:id="rId21"/>
+    <sheet name="Interventions birth age" sheetId="37" r:id="rId22"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId23"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -2502,30 +2503,79 @@
 <file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Ruth</author>
+    <author>Microsoft Office User</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="F21" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Ruth made these numbers up</t>
+WHO statement</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
         </r>
       </text>
     </comment>
@@ -2537,10 +2587,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
-    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2560,33 +2609,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-made numbers up for effectiveness</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-assume target pop is WRA &lt;18 years, then this is just  birth age distribution for
- this age
-</t>
+Ruth made these numbers up</t>
         </r>
       </text>
     </comment>
@@ -2595,6 +2618,67 @@
 </file>
 
 <file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+    <author xml:space="preserve"> Janka Petravic</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+made numbers up for effectiveness</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+assume target pop is WRA &lt;18 years, then this is just  birth age distribution for
+ this age
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -4045,7 +4129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="260">
   <si>
     <t>year</t>
   </si>
@@ -4807,6 +4891,24 @@
   </si>
   <si>
     <t>WASH: Handwashing</t>
+  </si>
+  <si>
+    <t>Oral rehydration salts</t>
+  </si>
+  <si>
+    <t>Zinc for treatment</t>
+  </si>
+  <si>
+    <t>Calcium Supplementation</t>
+  </si>
+  <si>
+    <t>Calcium supplementation</t>
+  </si>
+  <si>
+    <t>Mg for pre-eclampsia</t>
+  </si>
+  <si>
+    <t>Mg for eclampsia</t>
   </si>
 </sst>
 </file>
@@ -5138,7 +5240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="663">
+  <cellStyleXfs count="695">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5802,8 +5904,40 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6008,12 +6142,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="663">
+  <cellStyles count="695">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6345,6 +6484,22 @@
     <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6675,6 +6830,22 @@
     <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -8732,7 +8903,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="125" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -8755,7 +8926,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="124"/>
+      <c r="B3" s="125"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -8777,7 +8948,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="124"/>
+      <c r="B4" s="125"/>
       <c r="C4" t="s">
         <v>204</v>
       </c>
@@ -8804,7 +8975,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="125" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8827,7 +8998,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="124"/>
+      <c r="B6" s="125"/>
       <c r="C6" t="s">
         <v>194</v>
       </c>
@@ -8848,7 +9019,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="124"/>
+      <c r="B7" s="125"/>
       <c r="C7" t="s">
         <v>204</v>
       </c>
@@ -8874,7 +9045,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="125" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8897,7 +9068,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="124"/>
+      <c r="B9" s="125"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -8918,7 +9089,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="124"/>
+      <c r="B10" s="125"/>
       <c r="C10" t="s">
         <v>204</v>
       </c>
@@ -8943,7 +9114,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="125" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8966,7 +9137,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="124"/>
+      <c r="B12" s="125"/>
       <c r="C12" t="s">
         <v>194</v>
       </c>
@@ -8987,7 +9158,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="124"/>
+      <c r="B13" s="125"/>
       <c r="C13" t="s">
         <v>204</v>
       </c>
@@ -9011,7 +9182,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="125" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -9034,7 +9205,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="124"/>
+      <c r="B15" s="125"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -9055,7 +9226,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="124"/>
+      <c r="B16" s="125"/>
       <c r="C16" t="s">
         <v>204</v>
       </c>
@@ -9111,7 +9282,7 @@
       <c r="A19" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="124" t="s">
+      <c r="B19" s="125" t="s">
         <v>81</v>
       </c>
       <c r="C19" t="s">
@@ -9134,7 +9305,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="124"/>
+      <c r="B20" s="125"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
@@ -9155,7 +9326,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="124"/>
+      <c r="B21" s="125"/>
       <c r="C21" t="s">
         <v>204</v>
       </c>
@@ -9181,7 +9352,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="124" t="s">
+      <c r="B22" s="125" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -9204,7 +9375,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="124"/>
+      <c r="B23" s="125"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -9225,7 +9396,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="124"/>
+      <c r="B24" s="125"/>
       <c r="C24" t="s">
         <v>204</v>
       </c>
@@ -9251,7 +9422,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="124" t="s">
+      <c r="B25" s="125" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -9274,7 +9445,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="124"/>
+      <c r="B26" s="125"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
@@ -9295,7 +9466,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="124"/>
+      <c r="B27" s="125"/>
       <c r="C27" t="s">
         <v>204</v>
       </c>
@@ -9321,7 +9492,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="124" t="s">
+      <c r="B28" s="125" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -9344,7 +9515,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="124"/>
+      <c r="B29" s="125"/>
       <c r="C29" t="s">
         <v>194</v>
       </c>
@@ -9365,7 +9536,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="124"/>
+      <c r="B30" s="125"/>
       <c r="C30" t="s">
         <v>204</v>
       </c>
@@ -9391,7 +9562,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="125" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9414,7 +9585,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="124"/>
+      <c r="B32" s="125"/>
       <c r="C32" t="s">
         <v>194</v>
       </c>
@@ -9435,7 +9606,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="124"/>
+      <c r="B33" s="125"/>
       <c r="C33" t="s">
         <v>204</v>
       </c>
@@ -9487,7 +9658,7 @@
       <c r="A36" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="125" t="s">
         <v>81</v>
       </c>
       <c r="C36" t="s">
@@ -9510,7 +9681,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="124"/>
+      <c r="B37" s="125"/>
       <c r="C37" t="s">
         <v>194</v>
       </c>
@@ -9531,7 +9702,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="124"/>
+      <c r="B38" s="125"/>
       <c r="C38" t="s">
         <v>204</v>
       </c>
@@ -9552,7 +9723,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="124" t="s">
+      <c r="B39" s="125" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9575,7 +9746,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="B40" s="124"/>
+      <c r="B40" s="125"/>
       <c r="C40" t="s">
         <v>194</v>
       </c>
@@ -9596,7 +9767,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="124"/>
+      <c r="B41" s="125"/>
       <c r="C41" t="s">
         <v>204</v>
       </c>
@@ -9617,7 +9788,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="124" t="s">
+      <c r="B42" s="125" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9640,7 +9811,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="B43" s="124"/>
+      <c r="B43" s="125"/>
       <c r="C43" t="s">
         <v>194</v>
       </c>
@@ -9661,7 +9832,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="B44" s="124"/>
+      <c r="B44" s="125"/>
       <c r="C44" t="s">
         <v>204</v>
       </c>
@@ -9682,7 +9853,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="B45" s="124" t="s">
+      <c r="B45" s="125" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9705,7 +9876,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="B46" s="124"/>
+      <c r="B46" s="125"/>
       <c r="C46" t="s">
         <v>194</v>
       </c>
@@ -9726,7 +9897,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="B47" s="124"/>
+      <c r="B47" s="125"/>
       <c r="C47" t="s">
         <v>204</v>
       </c>
@@ -9747,7 +9918,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="124" t="s">
+      <c r="B48" s="125" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9770,7 +9941,7 @@
       </c>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="124"/>
+      <c r="B49" s="125"/>
       <c r="C49" t="s">
         <v>194</v>
       </c>
@@ -9791,7 +9962,7 @@
       </c>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="124"/>
+      <c r="B50" s="125"/>
       <c r="C50" t="s">
         <v>204</v>
       </c>
@@ -9836,11 +10007,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9851,6 +10017,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10368,10 +10539,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -11709,6 +11880,162 @@
       </c>
       <c r="I50" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B52" t="s">
+        <v>254</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B53" t="s">
+        <v>255</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B54" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B55" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B56" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>1</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11728,10 +12055,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -11948,6 +12275,43 @@
       </c>
       <c r="F11" s="46">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="46">
+        <v>0.12</v>
+      </c>
+      <c r="D12" s="46">
+        <v>0</v>
+      </c>
+      <c r="E12" s="46">
+        <v>0.12</v>
+      </c>
+      <c r="F12" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="46">
+        <v>1</v>
+      </c>
+      <c r="F13" s="46">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -13524,10 +13888,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -13535,7 +13899,7 @@
     <col min="1" max="1" width="39.1640625" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
@@ -13552,948 +13916,575 @@
         <v>51</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>257</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G2" s="31">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H2" s="31">
-        <v>0.33500000000000002</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
         <v>68</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.3</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.62</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="11"/>
-      <c r="B5" s="60" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="61">
-        <v>0</v>
-      </c>
-      <c r="E5" s="61">
-        <v>0</v>
-      </c>
-      <c r="F5" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G5" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H5" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.59</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>184</v>
+        <v>259</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="61">
-        <v>0</v>
-      </c>
-      <c r="E6" s="61">
-        <v>0</v>
-      </c>
-      <c r="F6" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G6" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H6" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="C7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="61">
-        <v>0</v>
-      </c>
-      <c r="E7" s="61">
-        <v>0</v>
-      </c>
-      <c r="F7" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="G7" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H7" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A7" s="11"/>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="B8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="61">
-        <v>0</v>
-      </c>
-      <c r="E8" s="61">
-        <v>0</v>
-      </c>
-      <c r="F8" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G8" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H8" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="C9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="61">
-        <v>0</v>
-      </c>
-      <c r="E9" s="61">
-        <v>0</v>
-      </c>
-      <c r="F9" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="G9" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H9" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D10" s="61">
-        <v>0</v>
-      </c>
-      <c r="E10" s="61">
-        <v>0</v>
-      </c>
-      <c r="F10" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G10" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H10" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="61">
-        <v>0</v>
-      </c>
-      <c r="E11" s="61">
-        <v>0</v>
-      </c>
-      <c r="F11" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="G11" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H11" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>183</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" s="61">
-        <v>0</v>
-      </c>
-      <c r="E12" s="61">
-        <v>0</v>
-      </c>
-      <c r="F12" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G12" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H12" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="61">
-        <v>0</v>
-      </c>
-      <c r="E13" s="61">
-        <v>0</v>
-      </c>
-      <c r="F13" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="G13" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H13" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="61">
-        <v>0</v>
-      </c>
-      <c r="E14" s="61">
-        <v>0</v>
-      </c>
-      <c r="F14" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G14" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H14" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="C15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="61">
-        <v>0</v>
-      </c>
-      <c r="E15" s="61">
-        <v>0</v>
-      </c>
-      <c r="F15" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="G15" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H15" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" t="s">
-        <v>183</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="61">
-        <v>0</v>
-      </c>
-      <c r="E16" s="61">
-        <v>0</v>
-      </c>
-      <c r="F16" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G16" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H16" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="C17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="61">
-        <v>0</v>
-      </c>
-      <c r="E17" s="61">
-        <v>0</v>
-      </c>
-      <c r="F17" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="G17" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H17" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>179</v>
-      </c>
-      <c r="B18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="61">
-        <v>0</v>
-      </c>
-      <c r="E18" s="61">
-        <v>0</v>
-      </c>
-      <c r="F18" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G18" s="62">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H18" s="62">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="C19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="61">
-        <v>0</v>
-      </c>
-      <c r="E19" s="61">
-        <v>0</v>
-      </c>
-      <c r="F19" s="61">
-        <v>0.7</v>
-      </c>
-      <c r="G19" s="61">
-        <v>0.62</v>
-      </c>
-      <c r="H19" s="61">
-        <v>0.62</v>
-      </c>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="B20" t="s">
-        <v>183</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="67">
-        <v>0</v>
-      </c>
-      <c r="E20" s="67">
-        <v>0</v>
-      </c>
-      <c r="F20" s="67">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G20" s="68">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H20" s="68">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="C21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="67">
-        <v>0</v>
-      </c>
-      <c r="E21" s="67">
-        <v>0</v>
-      </c>
-      <c r="F21" s="67">
-        <v>0.84</v>
-      </c>
-      <c r="G21" s="67">
-        <v>0.62</v>
-      </c>
-      <c r="H21" s="67">
-        <v>0.62</v>
-      </c>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="E22" s="12">
-        <v>0</v>
-      </c>
-      <c r="F22" s="12">
-        <v>0</v>
-      </c>
-      <c r="G22" s="12">
-        <v>0</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0</v>
-      </c>
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="12"/>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="E23" s="12">
-        <v>0</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0</v>
-      </c>
-      <c r="G23" s="12">
-        <v>0</v>
-      </c>
-      <c r="H23" s="12">
-        <v>0</v>
-      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0</v>
-      </c>
-      <c r="G24" s="12">
-        <v>0</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0</v>
-      </c>
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="12"/>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="E25" s="12">
-        <v>0</v>
-      </c>
-      <c r="F25" s="12">
-        <v>0</v>
-      </c>
-      <c r="G25" s="12">
-        <v>0</v>
-      </c>
-      <c r="H25" s="12">
-        <v>0</v>
-      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
-      <c r="F26" s="12">
-        <v>0</v>
-      </c>
-      <c r="G26" s="12">
-        <v>0</v>
-      </c>
-      <c r="H26" s="12">
-        <v>0</v>
-      </c>
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="C27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="E27" s="12">
-        <v>0</v>
-      </c>
-      <c r="F27" s="12">
-        <v>0</v>
-      </c>
-      <c r="G27" s="12">
-        <v>0</v>
-      </c>
-      <c r="H27" s="12">
-        <v>0</v>
-      </c>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>249</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="12">
-        <v>1</v>
-      </c>
-      <c r="E28" s="12">
-        <v>1</v>
-      </c>
-      <c r="F28" s="12">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12">
-        <v>1</v>
-      </c>
-      <c r="H28" s="12">
-        <v>1</v>
-      </c>
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="E29" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="F29" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="G29" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="H29" s="12">
-        <v>0.17</v>
-      </c>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="E30" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="F30" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="G30" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="H30" s="12">
-        <v>0.17</v>
-      </c>
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>250</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="12">
-        <v>1</v>
-      </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="12">
-        <v>1</v>
-      </c>
-      <c r="G31" s="12">
-        <v>1</v>
-      </c>
-      <c r="H31" s="12">
-        <v>1</v>
-      </c>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="C32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="E32" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="F32" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="G32" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="H32" s="12">
-        <v>0.69</v>
-      </c>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="E33" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="F33" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="H33" s="12">
-        <v>0.69</v>
-      </c>
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>251</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
+      <c r="A34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="E35" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="F35" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="G35" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="H35" s="12">
-        <v>0.36</v>
-      </c>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="E36" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="F36" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="G36" s="12">
-        <v>0.36</v>
-      </c>
-      <c r="H36" s="12">
-        <v>0.36</v>
-      </c>
+      <c r="A36" s="11"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>252</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="E38" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F38" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="G38" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="H38" s="12">
-        <v>0.2</v>
-      </c>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="E39" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F39" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="G39" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="H39" s="12">
-        <v>0.2</v>
-      </c>
+      <c r="A39" s="11"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" t="s">
-        <v>253</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
+      <c r="A40" s="11"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="C41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="E41" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="F41" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="G41" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="H41" s="12">
-        <v>0.48</v>
-      </c>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="E42" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="F42" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="G42" s="12">
-        <v>0.48</v>
-      </c>
-      <c r="H42" s="12">
-        <v>0.48</v>
-      </c>
+      <c r="A42" s="11"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="11"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="11"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="11"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15166,6 +15157,1218 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G2" s="31">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H2" s="31">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="11"/>
+      <c r="B5" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="61">
+        <v>0</v>
+      </c>
+      <c r="E5" s="61">
+        <v>0</v>
+      </c>
+      <c r="F5" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G5" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H5" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="61">
+        <v>0</v>
+      </c>
+      <c r="E6" s="61">
+        <v>0</v>
+      </c>
+      <c r="F6" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G6" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H6" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="C7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="61">
+        <v>0</v>
+      </c>
+      <c r="E7" s="61">
+        <v>0</v>
+      </c>
+      <c r="F7" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="G7" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H7" s="61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="61">
+        <v>0</v>
+      </c>
+      <c r="E8" s="61">
+        <v>0</v>
+      </c>
+      <c r="F8" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G8" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H8" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="C9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="61">
+        <v>0</v>
+      </c>
+      <c r="E9" s="61">
+        <v>0</v>
+      </c>
+      <c r="F9" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="G9" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H9" s="61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="61">
+        <v>0</v>
+      </c>
+      <c r="E10" s="61">
+        <v>0</v>
+      </c>
+      <c r="F10" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G10" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H10" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="C11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="61">
+        <v>0</v>
+      </c>
+      <c r="E11" s="61">
+        <v>0</v>
+      </c>
+      <c r="F11" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="G11" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H11" s="61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="61">
+        <v>0</v>
+      </c>
+      <c r="E12" s="61">
+        <v>0</v>
+      </c>
+      <c r="F12" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G12" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H12" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="C13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="61">
+        <v>0</v>
+      </c>
+      <c r="E13" s="61">
+        <v>0</v>
+      </c>
+      <c r="F13" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="G13" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H13" s="61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="61">
+        <v>0</v>
+      </c>
+      <c r="E14" s="61">
+        <v>0</v>
+      </c>
+      <c r="F14" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G14" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H14" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="61">
+        <v>0</v>
+      </c>
+      <c r="E15" s="61">
+        <v>0</v>
+      </c>
+      <c r="F15" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="G15" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H15" s="61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
+      <c r="E16" s="61">
+        <v>0</v>
+      </c>
+      <c r="F16" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G16" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H16" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="C17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="61">
+        <v>0</v>
+      </c>
+      <c r="E17" s="61">
+        <v>0</v>
+      </c>
+      <c r="F17" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="G17" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H17" s="61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="61">
+        <v>0</v>
+      </c>
+      <c r="E18" s="61">
+        <v>0</v>
+      </c>
+      <c r="F18" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G18" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H18" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="61">
+        <v>0</v>
+      </c>
+      <c r="E19" s="61">
+        <v>0</v>
+      </c>
+      <c r="F19" s="61">
+        <v>0.7</v>
+      </c>
+      <c r="G19" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H19" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="67">
+        <v>0</v>
+      </c>
+      <c r="E20" s="67">
+        <v>0</v>
+      </c>
+      <c r="F20" s="67">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G20" s="68">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H20" s="68">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="C21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="67">
+        <v>0</v>
+      </c>
+      <c r="E21" s="67">
+        <v>0</v>
+      </c>
+      <c r="F21" s="67">
+        <v>0.84</v>
+      </c>
+      <c r="G21" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="H21" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="12"/>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0</v>
+      </c>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="12"/>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="12">
+        <v>1</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12">
+        <v>1</v>
+      </c>
+      <c r="G28" s="12">
+        <v>1</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>250</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1</v>
+      </c>
+      <c r="G31" s="12">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>252</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="H42" s="12">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="12">
+        <v>1</v>
+      </c>
+      <c r="G43" s="12">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E44" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H44" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="C45" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="E45" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="F45" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="G45" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="H45" s="12">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1</v>
+      </c>
+      <c r="E46" s="12">
+        <v>1</v>
+      </c>
+      <c r="F46" s="12">
+        <v>1</v>
+      </c>
+      <c r="G46" s="12">
+        <v>1</v>
+      </c>
+      <c r="H46" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="E47" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="F47" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="G47" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="H47" s="12">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="C48" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="F48" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="G48" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="H48" s="12">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>254</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="E49" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="H49" s="12">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="12">
+        <v>0.93</v>
+      </c>
+      <c r="E50" s="12">
+        <v>0.93</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0.93</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0.93</v>
+      </c>
+      <c r="H50" s="12">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>255</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="12">
+        <v>1</v>
+      </c>
+      <c r="E51" s="12">
+        <v>1</v>
+      </c>
+      <c r="F51" s="12">
+        <v>1</v>
+      </c>
+      <c r="G51" s="12">
+        <v>1</v>
+      </c>
+      <c r="H51" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="E52" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="F52" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="H52" s="12">
+        <v>0.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15373,7 +16576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -15572,12 +16775,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -16141,7 +17344,7 @@
       <c r="A40" s="81" t="s">
         <v>225</v>
       </c>
-      <c r="B40" s="125">
+      <c r="B40" s="124">
         <v>0.5</v>
       </c>
       <c r="C40" s="14">
@@ -16156,7 +17359,7 @@
       <c r="A41" s="90" t="s">
         <v>246</v>
       </c>
-      <c r="B41" s="125">
+      <c r="B41" s="124">
         <v>0.1</v>
       </c>
       <c r="C41" s="14">
@@ -16170,7 +17373,7 @@
       <c r="A42" t="s">
         <v>249</v>
       </c>
-      <c r="B42" s="125">
+      <c r="B42" s="124">
         <v>0.84</v>
       </c>
       <c r="C42" s="13">
@@ -16184,7 +17387,7 @@
       <c r="A43" t="s">
         <v>250</v>
       </c>
-      <c r="B43" s="125">
+      <c r="B43" s="124">
         <v>0.14000000000000001</v>
       </c>
       <c r="C43" s="13">
@@ -16198,7 +17401,7 @@
       <c r="A44" t="s">
         <v>251</v>
       </c>
-      <c r="B44" s="125">
+      <c r="B44" s="124">
         <v>0.69</v>
       </c>
       <c r="C44" s="13">
@@ -16212,7 +17415,7 @@
       <c r="A45" t="s">
         <v>252</v>
       </c>
-      <c r="B45" s="125">
+      <c r="B45" s="124">
         <v>0.38700000000000001</v>
       </c>
       <c r="C45" s="13">
@@ -16226,7 +17429,7 @@
       <c r="A46" t="s">
         <v>253</v>
       </c>
-      <c r="B46" s="125">
+      <c r="B46" s="124">
         <v>0.4</v>
       </c>
       <c r="C46" s="13">
@@ -16237,17 +17440,88 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B47" s="91"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="93"/>
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="91">
+        <v>0</v>
+      </c>
+      <c r="C47" s="92">
+        <v>0.85</v>
+      </c>
+      <c r="D47" s="93">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B48" s="91"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="93"/>
-    </row>
-    <row r="49" spans="3:3" ht="15.75" customHeight="1">
-      <c r="C49" s="92"/>
+      <c r="A48" t="s">
+        <v>254</v>
+      </c>
+      <c r="B48" s="91">
+        <v>0</v>
+      </c>
+      <c r="C48" s="92">
+        <v>0.85</v>
+      </c>
+      <c r="D48" s="93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A49" t="s">
+        <v>255</v>
+      </c>
+      <c r="B49" s="126">
+        <v>0</v>
+      </c>
+      <c r="C49" s="92">
+        <v>0.85</v>
+      </c>
+      <c r="D49" s="127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A50" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B50" s="126">
+        <v>0</v>
+      </c>
+      <c r="C50" s="92">
+        <v>0.85</v>
+      </c>
+      <c r="D50" s="127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A51" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B51" s="126">
+        <v>0</v>
+      </c>
+      <c r="C51" s="92">
+        <v>0.85</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A52" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" s="126">
+        <v>0</v>
+      </c>
+      <c r="C52" s="92">
+        <v>0.85</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -18402,7 +19676,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Swapped key order of risk distributions, now have program risk areas
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4660,10 +4660,10 @@
     <t>Mortality</t>
   </si>
   <si>
-    <t>Exclusive dependencie</t>
-  </si>
-  <si>
     <t>Threshold dependency</t>
+  </si>
+  <si>
+    <t>Exclusion dependency</t>
   </si>
 </sst>
 </file>
@@ -15547,7 +15547,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15562,10 +15562,10 @@
         <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
removed zinc error in csv and wrote script to get all interventions outcomes
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-69360" yWindow="-3800" windowWidth="28040" windowHeight="17620" tabRatio="500" firstSheet="18" activeTab="18"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="22380" windowHeight="14260" tabRatio="500" firstSheet="21" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2687,7 +2687,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2712,7 +2712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="1">
+    <comment ref="D6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2736,7 +2736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="1">
+    <comment ref="D11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2757,6 +2757,54 @@
           </rPr>
           <t xml:space="preserve">
 o data in the book, made up as = to IFAS for non-pregnant in hospital</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fictional</t>
         </r>
       </text>
     </comment>
@@ -2780,11 +2828,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+Also brestfeeding women up to 6 months?</t>
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="A20" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2794,7 +2842,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Ruth:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -2804,11 +2852,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-fictional</t>
+There is no unit cost for this to impact the budget.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="2">
+    <comment ref="D20" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Government subsidy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2828,11 +2900,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
+There is no unit cost for this to impact the budget.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="2">
+    <comment ref="D27" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Government subsidy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2842,7 +2938,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Ruth:</t>
         </r>
         <r>
           <rPr>
@@ -2852,11 +2948,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-There is no unit cost for this to impact the budget.</t>
+This is the fraction of the population eating these staples and belongs here.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="1">
+    <comment ref="D31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2876,35 +2972,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Government subsidy</t>
+orton Copenhagen Consensus 2008</t>
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-There is no unit cost for this to impact the budget.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="1">
+    <comment ref="A32" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2924,31 +2996,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Government subsidy</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C31" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the fraction of the population eating these staples and belongs here.</t>
+Same effect as iron fortification</t>
         </r>
       </text>
     </comment>
@@ -2976,7 +3024,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="1">
+    <comment ref="D33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2996,31 +3044,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Same effect as iron fortification</t>
+orton Copenhagen Consensus 2008</t>
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="1">
+    <comment ref="C34" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-orton Copenhagen Consensus 2008</t>
+This is the fraction of the population eating these staples and belongs here.</t>
         </r>
       </text>
     </comment>
@@ -3048,7 +3096,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="0">
+    <comment ref="B35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3068,11 +3116,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This is the fraction of the population eating these staples and belongs here.</t>
+fictional</t>
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="1">
+    <comment ref="D35" authorId="3">
       <text>
         <r>
           <rPr>
@@ -3082,7 +3130,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Sam:</t>
         </r>
         <r>
           <rPr>
@@ -3092,35 +3140,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-orton Copenhagen Consensus 2008</t>
+From Nick</t>
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fictional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D36" authorId="3">
+    <comment ref="D36" authorId="1">
       <text>
         <r>
           <rPr>
@@ -3130,7 +3154,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -3140,7 +3164,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-From Nick</t>
+Per person per year</t>
         </r>
       </text>
     </comment>
@@ -3164,35 +3188,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per person per year</t>
+Made up, a bit less per treatment than PPCF per year</t>
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Made up, a bit less per treatment than PPCF per year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B41" authorId="0">
+    <comment ref="B40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3217,7 +3217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="0">
+    <comment ref="D41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -4129,7 +4129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="260">
   <si>
     <t>year</t>
   </si>
@@ -5937,7 +5937,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6081,9 +6081,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -6143,13 +6140,15 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="695">
@@ -8150,7 +8149,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -8456,7 +8455,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -8649,7 +8648,7 @@
         <v>120</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -8903,7 +8902,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="127" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -8926,7 +8925,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="125"/>
+      <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -8948,7 +8947,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="125"/>
+      <c r="B4" s="127"/>
       <c r="C4" t="s">
         <v>204</v>
       </c>
@@ -8975,7 +8974,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="127" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8998,7 +8997,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" t="s">
         <v>194</v>
       </c>
@@ -9019,7 +9018,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" t="s">
         <v>204</v>
       </c>
@@ -9045,7 +9044,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="127" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -9068,7 +9067,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -9089,7 +9088,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="125"/>
+      <c r="B10" s="127"/>
       <c r="C10" t="s">
         <v>204</v>
       </c>
@@ -9114,7 +9113,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -9137,7 +9136,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="125"/>
+      <c r="B12" s="127"/>
       <c r="C12" t="s">
         <v>194</v>
       </c>
@@ -9158,7 +9157,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="125"/>
+      <c r="B13" s="127"/>
       <c r="C13" t="s">
         <v>204</v>
       </c>
@@ -9182,7 +9181,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="125" t="s">
+      <c r="B14" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -9205,7 +9204,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="125"/>
+      <c r="B15" s="127"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -9226,7 +9225,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="125"/>
+      <c r="B16" s="127"/>
       <c r="C16" t="s">
         <v>204</v>
       </c>
@@ -9282,7 +9281,7 @@
       <c r="A19" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="127" t="s">
         <v>81</v>
       </c>
       <c r="C19" t="s">
@@ -9305,7 +9304,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="125"/>
+      <c r="B20" s="127"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
@@ -9326,7 +9325,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="125"/>
+      <c r="B21" s="127"/>
       <c r="C21" t="s">
         <v>204</v>
       </c>
@@ -9352,7 +9351,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="125" t="s">
+      <c r="B22" s="127" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -9375,7 +9374,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="125"/>
+      <c r="B23" s="127"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -9396,7 +9395,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="125"/>
+      <c r="B24" s="127"/>
       <c r="C24" t="s">
         <v>204</v>
       </c>
@@ -9422,7 +9421,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="125" t="s">
+      <c r="B25" s="127" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -9445,7 +9444,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="125"/>
+      <c r="B26" s="127"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
@@ -9466,7 +9465,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="125"/>
+      <c r="B27" s="127"/>
       <c r="C27" t="s">
         <v>204</v>
       </c>
@@ -9492,7 +9491,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -9515,7 +9514,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="125"/>
+      <c r="B29" s="127"/>
       <c r="C29" t="s">
         <v>194</v>
       </c>
@@ -9536,7 +9535,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="125"/>
+      <c r="B30" s="127"/>
       <c r="C30" t="s">
         <v>204</v>
       </c>
@@ -9562,7 +9561,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="125" t="s">
+      <c r="B31" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9585,7 +9584,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="125"/>
+      <c r="B32" s="127"/>
       <c r="C32" t="s">
         <v>194</v>
       </c>
@@ -9606,7 +9605,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="125"/>
+      <c r="B33" s="127"/>
       <c r="C33" t="s">
         <v>204</v>
       </c>
@@ -9658,7 +9657,7 @@
       <c r="A36" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="125" t="s">
+      <c r="B36" s="127" t="s">
         <v>81</v>
       </c>
       <c r="C36" t="s">
@@ -9681,7 +9680,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="125"/>
+      <c r="B37" s="127"/>
       <c r="C37" t="s">
         <v>194</v>
       </c>
@@ -9702,7 +9701,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="125"/>
+      <c r="B38" s="127"/>
       <c r="C38" t="s">
         <v>204</v>
       </c>
@@ -9723,7 +9722,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="125" t="s">
+      <c r="B39" s="127" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9746,7 +9745,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="B40" s="125"/>
+      <c r="B40" s="127"/>
       <c r="C40" t="s">
         <v>194</v>
       </c>
@@ -9767,7 +9766,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="125"/>
+      <c r="B41" s="127"/>
       <c r="C41" t="s">
         <v>204</v>
       </c>
@@ -9788,7 +9787,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="125" t="s">
+      <c r="B42" s="127" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9811,7 +9810,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="B43" s="125"/>
+      <c r="B43" s="127"/>
       <c r="C43" t="s">
         <v>194</v>
       </c>
@@ -9832,7 +9831,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="B44" s="125"/>
+      <c r="B44" s="127"/>
       <c r="C44" t="s">
         <v>204</v>
       </c>
@@ -9853,7 +9852,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="B45" s="125" t="s">
+      <c r="B45" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9876,7 +9875,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="B46" s="125"/>
+      <c r="B46" s="127"/>
       <c r="C46" t="s">
         <v>194</v>
       </c>
@@ -9897,7 +9896,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="B47" s="125"/>
+      <c r="B47" s="127"/>
       <c r="C47" t="s">
         <v>204</v>
       </c>
@@ -9918,7 +9917,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="125" t="s">
+      <c r="B48" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9941,7 +9940,7 @@
       </c>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="125"/>
+      <c r="B49" s="127"/>
       <c r="C49" t="s">
         <v>194</v>
       </c>
@@ -9962,7 +9961,7 @@
       </c>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="125"/>
+      <c r="B50" s="127"/>
       <c r="C50" t="s">
         <v>204</v>
       </c>
@@ -9989,24 +9988,29 @@
       <c r="C51" t="s">
         <v>204</v>
       </c>
-      <c r="D51" s="94">
-        <v>1</v>
-      </c>
-      <c r="E51" s="94">
-        <v>1</v>
-      </c>
-      <c r="F51" s="94">
+      <c r="D51" s="91">
+        <v>1</v>
+      </c>
+      <c r="E51" s="91">
+        <v>1</v>
+      </c>
+      <c r="F51" s="91">
         <v>0.95</v>
       </c>
-      <c r="G51" s="94">
+      <c r="G51" s="91">
         <v>0.95</v>
       </c>
-      <c r="H51" s="94">
+      <c r="H51" s="91">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -10017,11 +10021,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10066,188 +10065,188 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="92" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="98"/>
-      <c r="B3" s="99" t="s">
+      <c r="A3" s="95"/>
+      <c r="B3" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="97"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="98"/>
-      <c r="B4" s="99" t="s">
+      <c r="A4" s="95"/>
+      <c r="B4" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="97"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99" t="s">
+      <c r="A5" s="95"/>
+      <c r="B5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="99" t="s">
+      <c r="C5" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="99" t="s">
+      <c r="D5" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="100"/>
+      <c r="E5" s="97"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="98"/>
-      <c r="B6" s="99" t="s">
+      <c r="A6" s="95"/>
+      <c r="B6" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="100"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="101"/>
-      <c r="B7" s="102" t="s">
+      <c r="A7" s="98"/>
+      <c r="B7" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="92" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="94"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99" t="s">
+      <c r="A10" s="95"/>
+      <c r="B10" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="100"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="97"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="98"/>
-      <c r="B11" s="99" t="s">
+      <c r="A11" s="95"/>
+      <c r="B11" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="100"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="97"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="98"/>
-      <c r="B12" s="99" t="s">
+      <c r="A12" s="95"/>
+      <c r="B12" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="100"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="97"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="98"/>
-      <c r="B13" s="99" t="s">
+      <c r="A13" s="95"/>
+      <c r="B13" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="E13" s="100"/>
+      <c r="E13" s="97"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="101"/>
-      <c r="B14" s="102" t="s">
+      <c r="A14" s="98"/>
+      <c r="B14" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="101"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="96" t="s">
+      <c r="C16" s="93" t="s">
         <v>205</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="93" t="s">
         <v>205</v>
       </c>
-      <c r="E16" s="97"/>
+      <c r="E16" s="94"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="98"/>
-      <c r="B17" s="99" t="s">
+      <c r="A17" s="95"/>
+      <c r="B17" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="E17" s="100"/>
+      <c r="E17" s="97"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="98"/>
-      <c r="B18" s="99" t="s">
+      <c r="A18" s="95"/>
+      <c r="B18" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="100"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="97"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="98"/>
-      <c r="B19" s="99" t="s">
+      <c r="A19" s="95"/>
+      <c r="B19" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="100"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="97"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="98"/>
-      <c r="B20" s="99" t="s">
+      <c r="A20" s="95"/>
+      <c r="B20" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="97"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="101"/>
-      <c r="B21" s="102" t="s">
+      <c r="A21" s="98"/>
+      <c r="B21" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="103"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="104"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10541,8 +10540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -13890,7 +13889,7 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
@@ -13938,8 +13937,8 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
@@ -13981,8 +13980,8 @@
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
@@ -13999,8 +13998,8 @@
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="11"/>
@@ -14022,8 +14021,8 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="128"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="11"/>
@@ -14042,8 +14041,8 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
+      <c r="G10" s="124"/>
+      <c r="H10" s="124"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="11"/>
@@ -14062,8 +14061,8 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="124"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="11"/>
@@ -14082,8 +14081,8 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11"/>
@@ -14102,8 +14101,8 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="128"/>
-      <c r="H16" s="128"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="11"/>
@@ -14122,8 +14121,8 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="11"/>
@@ -14143,8 +14142,8 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="124"/>
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9">
@@ -15159,8 +15158,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -16130,7 +16129,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>28</v>
@@ -16196,7 +16195,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>30</v>
@@ -16603,16 +16602,16 @@
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="117" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="120" t="s">
+      <c r="D1" s="117" t="s">
         <v>233</v>
       </c>
-      <c r="E1" s="120" t="s">
+      <c r="E1" s="117" t="s">
         <v>234</v>
       </c>
       <c r="F1" s="1"/>
@@ -16621,33 +16620,33 @@
       <c r="A2" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="121">
+      <c r="C2" s="118">
         <v>0.8</v>
       </c>
-      <c r="D2" s="121">
+      <c r="D2" s="118">
         <v>0.8</v>
       </c>
-      <c r="E2" s="121">
+      <c r="E2" s="118">
         <v>0.8</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="121">
+      <c r="C3" s="118">
         <f>'Distributions births'!C2</f>
         <v>0.15</v>
       </c>
-      <c r="D3" s="121">
+      <c r="D3" s="118">
         <f>'Distributions births'!C3</f>
         <v>0.03</v>
       </c>
-      <c r="E3" s="121">
+      <c r="E3" s="118">
         <f>'Distributions births'!C4</f>
         <v>0</v>
       </c>
@@ -16678,73 +16677,73 @@
     <row r="14" spans="1:13">
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="122"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="123"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="120"/>
       <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13">
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="123"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="120"/>
       <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13">
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="123"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="120"/>
       <c r="M16" s="11"/>
     </row>
     <row r="17" spans="8:13">
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="123"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="120"/>
       <c r="M17" s="11"/>
     </row>
     <row r="18" spans="8:13">
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="123"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="120"/>
       <c r="M18" s="11"/>
     </row>
     <row r="19" spans="8:13">
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="123"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="120"/>
       <c r="M19" s="11"/>
     </row>
     <row r="20" spans="8:13">
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="123"/>
+      <c r="K20" s="103"/>
+      <c r="L20" s="120"/>
       <c r="M20" s="11"/>
     </row>
     <row r="21" spans="8:13">
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="123"/>
+      <c r="K21" s="103"/>
+      <c r="L21" s="120"/>
       <c r="M21" s="11"/>
     </row>
     <row r="22" spans="8:13">
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="123"/>
+      <c r="K22" s="103"/>
+      <c r="L22" s="120"/>
       <c r="M22" s="11"/>
     </row>
     <row r="23" spans="8:13">
@@ -16777,10 +16776,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -16807,161 +16806,161 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="B2" s="14">
-        <v>0</v>
+        <v>0.621</v>
       </c>
       <c r="C2" s="14">
         <v>0.85</v>
       </c>
       <c r="D2" s="14">
-        <v>1</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="B3" s="14">
-        <v>0.621</v>
+        <v>0</v>
       </c>
       <c r="C3" s="14">
         <v>0.85</v>
       </c>
       <c r="D3" s="14">
-        <v>0.35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="14">
-        <v>0</v>
-      </c>
-      <c r="C4" s="14">
+        <v>84</v>
+      </c>
+      <c r="B4" s="63">
+        <v>0</v>
+      </c>
+      <c r="C4" s="64">
         <v>0.85</v>
       </c>
-      <c r="D4" s="14">
-        <v>48</v>
+      <c r="D4" s="70">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="63">
-        <v>0</v>
-      </c>
-      <c r="C5" s="64">
+        <v>172</v>
+      </c>
+      <c r="B5" s="34">
+        <v>0</v>
+      </c>
+      <c r="C5" s="34">
         <v>0.85</v>
       </c>
-      <c r="D5" s="70">
-        <v>50</v>
+      <c r="D5" s="19">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B6" s="34">
-        <v>0</v>
-      </c>
-      <c r="C6" s="34">
+        <v>83</v>
+      </c>
+      <c r="B6" s="63">
+        <v>0</v>
+      </c>
+      <c r="C6" s="64">
         <v>0.85</v>
       </c>
-      <c r="D6" s="19">
-        <v>51</v>
+      <c r="D6" s="70">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="63">
-        <v>0</v>
-      </c>
-      <c r="C7" s="64">
+      <c r="A7" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="34">
+        <v>0</v>
+      </c>
+      <c r="C7" s="34">
         <v>0.85</v>
       </c>
-      <c r="D7" s="70">
+      <c r="D7" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="34">
-        <v>0</v>
-      </c>
-      <c r="C8" s="34">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14">
         <v>0.85</v>
       </c>
-      <c r="D8" s="19">
-        <v>1</v>
+      <c r="D8" s="14">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="14">
-        <v>0</v>
-      </c>
-      <c r="C9" s="14">
+        <v>171</v>
+      </c>
+      <c r="B9" s="65">
+        <v>0</v>
+      </c>
+      <c r="C9" s="66">
         <v>0.85</v>
       </c>
-      <c r="D9" s="14">
-        <v>25</v>
+      <c r="D9" s="66">
+        <v>2.99</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B10" s="65">
-        <v>0</v>
-      </c>
-      <c r="C10" s="66">
+        <v>174</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
         <v>0.85</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="14">
         <v>2.99</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="A11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="65">
+        <v>0</v>
+      </c>
+      <c r="C11" s="66">
         <v>0.85</v>
       </c>
-      <c r="D11" s="14">
-        <v>2.99</v>
+      <c r="D11" s="66">
+        <v>1.78</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="65">
-        <v>0</v>
-      </c>
-      <c r="C12" s="66">
+        <v>175</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0</v>
+      </c>
+      <c r="C12" s="14">
         <v>0.85</v>
       </c>
-      <c r="D12" s="66">
+      <c r="D12" s="14">
         <v>1.78</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>175</v>
+      <c r="A13" t="s">
+        <v>151</v>
       </c>
       <c r="B13" s="14">
         <v>0</v>
@@ -16970,12 +16969,12 @@
         <v>0.85</v>
       </c>
       <c r="D13" s="14">
-        <v>1.78</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B14" s="14">
         <v>0</v>
@@ -16984,12 +16983,12 @@
         <v>0.85</v>
       </c>
       <c r="D14" s="14">
-        <v>2.06</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B15" s="14">
         <v>0</v>
@@ -16998,12 +16997,12 @@
         <v>0.85</v>
       </c>
       <c r="D15" s="14">
-        <v>0.55000000000000004</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -17012,12 +17011,12 @@
         <v>0.85</v>
       </c>
       <c r="D16" s="14">
-        <v>0.73</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B17" s="14">
         <v>0</v>
@@ -17026,12 +17025,12 @@
         <v>0.85</v>
       </c>
       <c r="D17" s="14">
-        <v>1.78</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B18" s="14">
         <v>0</v>
@@ -17040,12 +17039,12 @@
         <v>0.85</v>
       </c>
       <c r="D18" s="14">
-        <v>0.55000000000000004</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B19" s="14">
         <v>0</v>
@@ -17054,12 +17053,12 @@
         <v>0.85</v>
       </c>
       <c r="D19" s="14">
-        <v>0.73</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B20" s="14">
         <v>0</v>
@@ -17068,12 +17067,12 @@
         <v>0.85</v>
       </c>
       <c r="D20" s="14">
-        <v>1.78</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B21" s="14">
         <v>0</v>
@@ -17082,12 +17081,12 @@
         <v>0.85</v>
       </c>
       <c r="D21" s="14">
-        <v>0.24</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B22" s="14">
         <v>0</v>
@@ -17096,12 +17095,12 @@
         <v>0.85</v>
       </c>
       <c r="D22" s="14">
-        <v>0.55000000000000004</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -17110,12 +17109,12 @@
         <v>0.85</v>
       </c>
       <c r="D23" s="14">
-        <v>0.73</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B24" s="14">
         <v>0</v>
@@ -17124,12 +17123,12 @@
         <v>0.85</v>
       </c>
       <c r="D24" s="14">
-        <v>1.78</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B25" s="14">
         <v>0</v>
@@ -17138,12 +17137,12 @@
         <v>0.85</v>
       </c>
       <c r="D25" s="14">
-        <v>0.55000000000000004</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B26" s="14">
         <v>0</v>
@@ -17152,12 +17151,12 @@
         <v>0.85</v>
       </c>
       <c r="D26" s="14">
-        <v>0.73</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
@@ -17166,138 +17165,139 @@
         <v>0.85</v>
       </c>
       <c r="D27" s="14">
-        <v>1.78</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A28" t="s">
-        <v>170</v>
+      <c r="A28" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B28" s="14">
         <v>0</v>
       </c>
       <c r="C28" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="D28" s="14">
-        <v>0.24</v>
+        <v>0.12</v>
+      </c>
+      <c r="D28" s="19">
+        <v>0.18</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" s="14">
         <v>0</v>
       </c>
       <c r="C29" s="14">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
       <c r="D29" s="19">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B30" s="14">
         <v>0</v>
       </c>
       <c r="C30" s="14">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="D30" s="19">
-        <v>0.13</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B31" s="14">
         <v>0</v>
       </c>
-      <c r="C31" s="14">
-        <v>0.8</v>
+      <c r="C31" s="13">
+        <v>0.85</v>
       </c>
       <c r="D31" s="19">
-        <v>0.74</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" s="14">
-        <v>0</v>
-      </c>
-      <c r="C32" s="13">
-        <v>0.85</v>
+      <c r="A32" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="19">
+        <v>0</v>
+      </c>
+      <c r="C32" s="14">
+        <v>0.12</v>
       </c>
       <c r="D32" s="19">
-        <v>0.25</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B33" s="19">
         <v>0</v>
       </c>
       <c r="C33" s="14">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
       <c r="D33" s="19">
-        <v>0.19</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B34" s="19">
         <v>0</v>
       </c>
       <c r="C34" s="14">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="D34" s="19">
-        <v>0.14000000000000001</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A35" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="19">
-        <v>0</v>
+      <c r="A35" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="14">
+        <v>0.2</v>
       </c>
       <c r="C35" s="14">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D35" s="19">
-        <v>0.75</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
       <c r="B36" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="C36" s="14">
+        <v>0</v>
+      </c>
+      <c r="C36" s="13">
         <v>0.85</v>
       </c>
       <c r="D36" s="19">
-        <v>2.61</v>
+        <f>180</f>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B37" s="14">
         <v>0</v>
@@ -17306,75 +17306,74 @@
         <v>0.85</v>
       </c>
       <c r="D37" s="19">
-        <f>180</f>
-        <v>180</v>
+        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
+        <v>10.046400000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B38" s="14">
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C38" s="13">
         <v>0.85</v>
       </c>
       <c r="D38" s="19">
-        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
-        <v>10.046400000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A39" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" s="14">
-        <v>0.61</v>
-      </c>
-      <c r="C39" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="D39" s="19">
         <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
         <v>19.933477200000002</v>
       </c>
     </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A39" s="81" t="s">
+        <v>225</v>
+      </c>
+      <c r="B39" s="121">
+        <v>0.5</v>
+      </c>
+      <c r="C39" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D39" s="19">
+        <f>SUM('Interventions family planning'!E2:E10)</f>
+        <v>0.82100000000000006</v>
+      </c>
+    </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A40" s="81" t="s">
-        <v>225</v>
-      </c>
-      <c r="B40" s="124">
-        <v>0.5</v>
+      <c r="A40" s="90" t="s">
+        <v>246</v>
+      </c>
+      <c r="B40" s="121">
+        <v>0.1</v>
       </c>
       <c r="C40" s="14">
         <v>0.85</v>
       </c>
       <c r="D40" s="19">
-        <f>SUM('Interventions family planning'!E2:E10)</f>
-        <v>0.82100000000000006</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A41" s="90" t="s">
-        <v>246</v>
-      </c>
-      <c r="B41" s="124">
-        <v>0.1</v>
-      </c>
-      <c r="C41" s="14">
+      <c r="A41" t="s">
+        <v>249</v>
+      </c>
+      <c r="B41" s="121">
+        <v>0.84</v>
+      </c>
+      <c r="C41" s="13">
         <v>0.85</v>
       </c>
       <c r="D41" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>249</v>
-      </c>
-      <c r="B42" s="124">
-        <v>0.84</v>
+        <v>250</v>
+      </c>
+      <c r="B42" s="121">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C42" s="13">
         <v>0.85</v>
@@ -17385,10 +17384,10 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>250</v>
-      </c>
-      <c r="B43" s="124">
-        <v>0.14000000000000001</v>
+        <v>251</v>
+      </c>
+      <c r="B43" s="121">
+        <v>0.69</v>
       </c>
       <c r="C43" s="13">
         <v>0.85</v>
@@ -17399,10 +17398,10 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
       <c r="A44" t="s">
-        <v>251</v>
-      </c>
-      <c r="B44" s="124">
-        <v>0.69</v>
+        <v>252</v>
+      </c>
+      <c r="B44" s="121">
+        <v>0.38700000000000001</v>
       </c>
       <c r="C44" s="13">
         <v>0.85</v>
@@ -17413,10 +17412,10 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>252</v>
-      </c>
-      <c r="B45" s="124">
-        <v>0.38700000000000001</v>
+        <v>253</v>
+      </c>
+      <c r="B45" s="121">
+        <v>0.4</v>
       </c>
       <c r="C45" s="13">
         <v>0.85</v>
@@ -17427,99 +17426,85 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>253</v>
-      </c>
-      <c r="B46" s="124">
-        <v>0.4</v>
-      </c>
-      <c r="C46" s="13">
+        <v>176</v>
+      </c>
+      <c r="B46" s="122">
+        <v>0</v>
+      </c>
+      <c r="C46" s="125">
         <v>0.85</v>
       </c>
-      <c r="D46" s="19">
+      <c r="D46" s="123">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1">
       <c r="A47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="91">
-        <v>0</v>
-      </c>
-      <c r="C47" s="92">
+        <v>254</v>
+      </c>
+      <c r="B47" s="122">
+        <v>0</v>
+      </c>
+      <c r="C47" s="125">
         <v>0.85</v>
       </c>
-      <c r="D47" s="93">
+      <c r="D47" s="123">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1">
       <c r="A48" t="s">
-        <v>254</v>
-      </c>
-      <c r="B48" s="91">
-        <v>0</v>
-      </c>
-      <c r="C48" s="92">
+        <v>255</v>
+      </c>
+      <c r="B48" s="122">
+        <v>0</v>
+      </c>
+      <c r="C48" s="125">
         <v>0.85</v>
       </c>
-      <c r="D48" s="93">
+      <c r="D48" s="123">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A49" t="s">
-        <v>255</v>
-      </c>
-      <c r="B49" s="126">
-        <v>0</v>
-      </c>
-      <c r="C49" s="92">
+      <c r="A49" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="122">
+        <v>0</v>
+      </c>
+      <c r="C49" s="125">
         <v>0.85</v>
       </c>
-      <c r="D49" s="127">
+      <c r="D49" s="123">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B50" s="126">
-        <v>0</v>
-      </c>
-      <c r="C50" s="92">
+        <v>258</v>
+      </c>
+      <c r="B50" s="122">
+        <v>0</v>
+      </c>
+      <c r="C50" s="125">
         <v>0.85</v>
       </c>
-      <c r="D50" s="127">
+      <c r="D50" s="126">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="B51" s="126">
-        <v>0</v>
-      </c>
-      <c r="C51" s="92">
+        <v>259</v>
+      </c>
+      <c r="B51" s="122">
+        <v>0</v>
+      </c>
+      <c r="C51" s="125">
         <v>0.85</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A52" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="B52" s="126">
-        <v>0</v>
-      </c>
-      <c r="C52" s="92">
-        <v>0.85</v>
-      </c>
-      <c r="D52">
+      <c r="D51" s="126">
         <v>1</v>
       </c>
     </row>
@@ -18987,115 +18972,115 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="112" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="105">
+      <c r="C2" s="102">
         <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="113" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="105">
+      <c r="C3" s="102">
         <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="105">
+      <c r="C4" s="102">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="114" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="105">
+      <c r="C5" s="102">
         <v>0.19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="114" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="105">
+      <c r="C6" s="102">
         <v>0.39</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="114" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="105">
+      <c r="C7" s="102">
         <v>0.19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="115" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="105">
+      <c r="C8" s="102">
         <v>1E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="C9" s="105">
+      <c r="C9" s="102">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="115" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="105">
+      <c r="C10" s="102">
         <v>0.04</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="C11" s="105"/>
+      <c r="C11" s="102"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="115" t="s">
+      <c r="A12" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="C12" s="105">
+      <c r="C12" s="102">
         <v>0.34</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="103" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="105">
+      <c r="C13" s="102">
         <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="103" t="s">
         <v>230</v>
       </c>
-      <c r="C14" s="105">
+      <c r="C14" s="102">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="105">
+      <c r="C15" s="102">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -19394,268 +19379,268 @@
       <c r="A21" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="105" t="s">
         <v>232</v>
       </c>
-      <c r="C21" s="111">
-        <v>1</v>
-      </c>
-      <c r="D21" s="111">
+      <c r="C21" s="108">
+        <v>1</v>
+      </c>
+      <c r="D21" s="108">
         <v>1.52</v>
       </c>
-      <c r="E21" s="111">
+      <c r="E21" s="108">
         <v>1.75</v>
       </c>
-      <c r="F21" s="111">
+      <c r="F21" s="108">
         <v>3.14</v>
       </c>
-      <c r="G21" s="112"/>
+      <c r="G21" s="109"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="111">
-        <v>1</v>
-      </c>
-      <c r="D22" s="111">
+      <c r="C22" s="108">
+        <v>1</v>
+      </c>
+      <c r="D22" s="108">
         <v>1.2</v>
       </c>
-      <c r="E22" s="111">
+      <c r="E22" s="108">
         <v>1.4</v>
       </c>
-      <c r="F22" s="111">
+      <c r="F22" s="108">
         <v>1.6</v>
       </c>
-      <c r="G22" s="112"/>
+      <c r="G22" s="109"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="111">
-        <v>1</v>
-      </c>
-      <c r="D23" s="111">
+      <c r="C23" s="108">
+        <v>1</v>
+      </c>
+      <c r="D23" s="108">
         <v>1.2</v>
       </c>
-      <c r="E23" s="111">
+      <c r="E23" s="108">
         <v>1.4</v>
       </c>
-      <c r="F23" s="111">
+      <c r="F23" s="108">
         <v>1.6</v>
       </c>
-      <c r="G23" s="112"/>
+      <c r="G23" s="109"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="C24" s="111">
-        <v>1</v>
-      </c>
-      <c r="D24" s="111">
+      <c r="C24" s="108">
+        <v>1</v>
+      </c>
+      <c r="D24" s="108">
         <v>1.52</v>
       </c>
-      <c r="E24" s="111">
+      <c r="E24" s="108">
         <v>1.75</v>
       </c>
-      <c r="F24" s="111">
+      <c r="F24" s="108">
         <v>1.73</v>
       </c>
-      <c r="G24" s="112"/>
+      <c r="G24" s="109"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="106" t="s">
         <v>236</v>
       </c>
-      <c r="C25" s="111">
-        <v>1</v>
-      </c>
-      <c r="D25" s="111">
-        <v>1</v>
-      </c>
-      <c r="E25" s="111">
-        <v>1</v>
-      </c>
-      <c r="F25" s="111">
-        <v>1</v>
-      </c>
-      <c r="G25" s="112"/>
+      <c r="C25" s="108">
+        <v>1</v>
+      </c>
+      <c r="D25" s="108">
+        <v>1</v>
+      </c>
+      <c r="E25" s="108">
+        <v>1</v>
+      </c>
+      <c r="F25" s="108">
+        <v>1</v>
+      </c>
+      <c r="G25" s="109"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B26" s="109" t="s">
+      <c r="B26" s="106" t="s">
         <v>237</v>
       </c>
-      <c r="C26" s="111">
-        <v>1</v>
-      </c>
-      <c r="D26" s="111">
-        <v>1</v>
-      </c>
-      <c r="E26" s="111">
-        <v>1</v>
-      </c>
-      <c r="F26" s="111">
-        <v>1</v>
-      </c>
-      <c r="G26" s="112"/>
+      <c r="C26" s="108">
+        <v>1</v>
+      </c>
+      <c r="D26" s="108">
+        <v>1</v>
+      </c>
+      <c r="E26" s="108">
+        <v>1</v>
+      </c>
+      <c r="F26" s="108">
+        <v>1</v>
+      </c>
+      <c r="G26" s="109"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="107" t="s">
         <v>238</v>
       </c>
-      <c r="C27" s="111">
-        <v>1</v>
-      </c>
-      <c r="D27" s="111">
+      <c r="C27" s="108">
+        <v>1</v>
+      </c>
+      <c r="D27" s="108">
         <v>1.52</v>
       </c>
-      <c r="E27" s="111">
+      <c r="E27" s="108">
         <v>1.75</v>
       </c>
-      <c r="F27" s="111">
+      <c r="F27" s="108">
         <v>1.52</v>
       </c>
-      <c r="G27" s="112"/>
+      <c r="G27" s="109"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="107" t="s">
         <v>239</v>
       </c>
-      <c r="C28" s="111">
-        <v>1</v>
-      </c>
-      <c r="D28" s="111">
-        <v>1</v>
-      </c>
-      <c r="E28" s="111">
+      <c r="C28" s="108">
+        <v>1</v>
+      </c>
+      <c r="D28" s="108">
+        <v>1</v>
+      </c>
+      <c r="E28" s="108">
         <v>1.33</v>
       </c>
-      <c r="F28" s="111">
-        <v>1</v>
-      </c>
-      <c r="G28" s="112"/>
+      <c r="F28" s="108">
+        <v>1</v>
+      </c>
+      <c r="G28" s="109"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B29" s="110" t="s">
+      <c r="B29" s="107" t="s">
         <v>240</v>
       </c>
-      <c r="C29" s="111">
-        <v>1</v>
-      </c>
-      <c r="D29" s="111">
-        <v>1</v>
-      </c>
-      <c r="E29" s="111">
+      <c r="C29" s="108">
+        <v>1</v>
+      </c>
+      <c r="D29" s="108">
+        <v>1</v>
+      </c>
+      <c r="E29" s="108">
         <v>1.33</v>
       </c>
-      <c r="F29" s="111">
-        <v>1</v>
-      </c>
-      <c r="G29" s="112"/>
+      <c r="F29" s="108">
+        <v>1</v>
+      </c>
+      <c r="G29" s="109"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C30" s="112"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="112"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="109"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="B31" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
-      <c r="G31" s="112"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="110"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="109"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B32" s="107" t="s">
+      <c r="B32" s="104" t="s">
         <v>228</v>
       </c>
-      <c r="C32" s="111">
-        <v>1</v>
-      </c>
-      <c r="D32" s="114">
-        <v>1</v>
-      </c>
-      <c r="E32" s="114">
-        <v>1</v>
-      </c>
-      <c r="F32" s="114">
-        <v>1</v>
-      </c>
-      <c r="G32" s="112"/>
+      <c r="C32" s="108">
+        <v>1</v>
+      </c>
+      <c r="D32" s="111">
+        <v>1</v>
+      </c>
+      <c r="E32" s="111">
+        <v>1</v>
+      </c>
+      <c r="F32" s="111">
+        <v>1</v>
+      </c>
+      <c r="G32" s="109"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B33" s="107" t="s">
+      <c r="B33" s="104" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="111">
-        <v>1</v>
-      </c>
-      <c r="D33" s="114">
+      <c r="C33" s="108">
+        <v>1</v>
+      </c>
+      <c r="D33" s="111">
         <v>1.41</v>
       </c>
-      <c r="E33" s="114">
+      <c r="E33" s="111">
         <v>1.49</v>
       </c>
-      <c r="F33" s="114">
+      <c r="F33" s="111">
         <v>3.03</v>
       </c>
-      <c r="G33" s="112"/>
+      <c r="G33" s="109"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B34" s="107" t="s">
+      <c r="B34" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="C34" s="111">
-        <v>1</v>
-      </c>
-      <c r="D34" s="114">
+      <c r="C34" s="108">
+        <v>1</v>
+      </c>
+      <c r="D34" s="111">
         <v>1.18</v>
       </c>
-      <c r="E34" s="114">
+      <c r="E34" s="111">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F34" s="114">
+      <c r="F34" s="111">
         <v>1.77</v>
       </c>
-      <c r="G34" s="112"/>
+      <c r="G34" s="109"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B35" s="107" t="s">
+      <c r="B35" s="104" t="s">
         <v>231</v>
       </c>
-      <c r="C35" s="111">
-        <v>1</v>
-      </c>
-      <c r="D35" s="114">
-        <v>1</v>
-      </c>
-      <c r="E35" s="114">
-        <v>1</v>
-      </c>
-      <c r="F35" s="114">
-        <v>1</v>
-      </c>
-      <c r="G35" s="112"/>
+      <c r="C35" s="108">
+        <v>1</v>
+      </c>
+      <c r="D35" s="111">
+        <v>1</v>
+      </c>
+      <c r="E35" s="111">
+        <v>1</v>
+      </c>
+      <c r="F35" s="111">
+        <v>1</v>
+      </c>
+      <c r="G35" s="109"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" customHeight="1">
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="112"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="112"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="109"/>
+      <c r="F36" s="109"/>
+      <c r="G36" s="109"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="109"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Reading program dependencies, small fixes
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37020" yWindow="-20620" windowWidth="29760" windowHeight="19040" tabRatio="500" firstSheet="14" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId17"/>
     <sheet name="Interventions family planning" sheetId="34" r:id="rId18"/>
     <sheet name="Interventions target population" sheetId="21" r:id="rId19"/>
-    <sheet name="Program areas" sheetId="36" r:id="rId20"/>
-    <sheet name="Program dependencies" sheetId="40" r:id="rId21"/>
+    <sheet name="Program dependencies" sheetId="40" r:id="rId20"/>
+    <sheet name="Program areas" sheetId="36" r:id="rId21"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId22"/>
+    <sheet name="Population risk areas" sheetId="41" r:id="rId23"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -3947,7 +3948,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="242">
   <si>
     <t>year</t>
   </si>
@@ -4648,9 +4649,6 @@
     <t>fraction SAM to MAM</t>
   </si>
   <si>
-    <t xml:space="preserve">fraction severe diarrhoea </t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -4664,6 +4662,18 @@
   </si>
   <si>
     <t>Exclusion dependency</t>
+  </si>
+  <si>
+    <t>fraction severe diarrhoea</t>
+  </si>
+  <si>
+    <t>Wasting prevention</t>
+  </si>
+  <si>
+    <t>Wasting treatment</t>
+  </si>
+  <si>
+    <t>Public provision of complementary foods with iron, Public provision of complementary foods with iron (malaria area)</t>
   </si>
 </sst>
 </file>
@@ -5778,10 +5788,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="3" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="631">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7717,7 +7727,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7744,7 +7754,7 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="108">
+      <c r="C2" s="107">
         <v>2016</v>
       </c>
     </row>
@@ -7847,7 +7857,7 @@
     </row>
     <row r="15" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C15" s="69">
         <v>0.2</v>
@@ -8189,7 +8199,7 @@
       <c r="A2" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>75</v>
       </c>
       <c r="C2" t="s">
@@ -8212,7 +8222,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="107"/>
+      <c r="B3" s="108"/>
       <c r="C3" t="s">
         <v>164</v>
       </c>
@@ -8234,7 +8244,7 @@
       <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="107"/>
+      <c r="B4" s="108"/>
       <c r="C4" t="s">
         <v>174</v>
       </c>
@@ -8261,7 +8271,7 @@
       <c r="J4" s="57"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8284,7 +8294,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="107"/>
+      <c r="B6" s="108"/>
       <c r="C6" t="s">
         <v>164</v>
       </c>
@@ -8305,7 +8315,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="107"/>
+      <c r="B7" s="108"/>
       <c r="C7" t="s">
         <v>174</v>
       </c>
@@ -8331,7 +8341,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="108" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8354,7 +8364,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="107"/>
+      <c r="B9" s="108"/>
       <c r="C9" t="s">
         <v>164</v>
       </c>
@@ -8375,7 +8385,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="107"/>
+      <c r="B10" s="108"/>
       <c r="C10" t="s">
         <v>174</v>
       </c>
@@ -8400,7 +8410,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="108" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8423,7 +8433,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="107"/>
+      <c r="B12" s="108"/>
       <c r="C12" t="s">
         <v>164</v>
       </c>
@@ -8444,7 +8454,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="107"/>
+      <c r="B13" s="108"/>
       <c r="C13" t="s">
         <v>174</v>
       </c>
@@ -8468,7 +8478,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8491,7 +8501,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="107"/>
+      <c r="B15" s="108"/>
       <c r="C15" t="s">
         <v>164</v>
       </c>
@@ -8512,7 +8522,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="107"/>
+      <c r="B16" s="108"/>
       <c r="C16" t="s">
         <v>174</v>
       </c>
@@ -8568,7 +8578,7 @@
       <c r="A19" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="108" t="s">
         <v>75</v>
       </c>
       <c r="C19" t="s">
@@ -8591,7 +8601,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="107"/>
+      <c r="B20" s="108"/>
       <c r="C20" t="s">
         <v>164</v>
       </c>
@@ -8612,7 +8622,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="107"/>
+      <c r="B21" s="108"/>
       <c r="C21" t="s">
         <v>174</v>
       </c>
@@ -8638,7 +8648,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8661,7 +8671,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="107"/>
+      <c r="B23" s="108"/>
       <c r="C23" t="s">
         <v>164</v>
       </c>
@@ -8682,7 +8692,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="107"/>
+      <c r="B24" s="108"/>
       <c r="C24" t="s">
         <v>174</v>
       </c>
@@ -8708,7 +8718,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="108" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8731,7 +8741,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="107"/>
+      <c r="B26" s="108"/>
       <c r="C26" t="s">
         <v>164</v>
       </c>
@@ -8752,7 +8762,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="107"/>
+      <c r="B27" s="108"/>
       <c r="C27" t="s">
         <v>174</v>
       </c>
@@ -8778,7 +8788,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="108" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -8801,7 +8811,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="107"/>
+      <c r="B29" s="108"/>
       <c r="C29" t="s">
         <v>164</v>
       </c>
@@ -8822,7 +8832,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="107"/>
+      <c r="B30" s="108"/>
       <c r="C30" t="s">
         <v>174</v>
       </c>
@@ -8848,7 +8858,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="107" t="s">
+      <c r="B31" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -8871,7 +8881,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="107"/>
+      <c r="B32" s="108"/>
       <c r="C32" t="s">
         <v>164</v>
       </c>
@@ -8892,7 +8902,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="107"/>
+      <c r="B33" s="108"/>
       <c r="C33" t="s">
         <v>174</v>
       </c>
@@ -8944,7 +8954,7 @@
       <c r="A36" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B36" s="107" t="s">
+      <c r="B36" s="108" t="s">
         <v>75</v>
       </c>
       <c r="C36" t="s">
@@ -8967,7 +8977,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="107"/>
+      <c r="B37" s="108"/>
       <c r="C37" t="s">
         <v>164</v>
       </c>
@@ -8988,7 +8998,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="107"/>
+      <c r="B38" s="108"/>
       <c r="C38" t="s">
         <v>174</v>
       </c>
@@ -9009,7 +9019,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9032,7 +9042,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="107"/>
+      <c r="B40" s="108"/>
       <c r="C40" t="s">
         <v>164</v>
       </c>
@@ -9053,7 +9063,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="107"/>
+      <c r="B41" s="108"/>
       <c r="C41" t="s">
         <v>174</v>
       </c>
@@ -9074,7 +9084,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="107" t="s">
+      <c r="B42" s="108" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9097,7 +9107,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="107"/>
+      <c r="B43" s="108"/>
       <c r="C43" t="s">
         <v>164</v>
       </c>
@@ -9118,7 +9128,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="107"/>
+      <c r="B44" s="108"/>
       <c r="C44" t="s">
         <v>174</v>
       </c>
@@ -9139,7 +9149,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="108" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9162,7 +9172,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="107"/>
+      <c r="B46" s="108"/>
       <c r="C46" t="s">
         <v>164</v>
       </c>
@@ -9183,7 +9193,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="107"/>
+      <c r="B47" s="108"/>
       <c r="C47" t="s">
         <v>174</v>
       </c>
@@ -9204,7 +9214,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="107" t="s">
+      <c r="B48" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9227,7 +9237,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="107"/>
+      <c r="B49" s="108"/>
       <c r="C49" t="s">
         <v>164</v>
       </c>
@@ -9248,7 +9258,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="107"/>
+      <c r="B50" s="108"/>
       <c r="C50" t="s">
         <v>174</v>
       </c>
@@ -9293,11 +9303,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9308,6 +9313,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9319,7 +9329,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9380,12 +9390,8 @@
       <c r="B5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="84" t="s">
-        <v>175</v>
-      </c>
-      <c r="D5" s="84" t="s">
-        <v>175</v>
-      </c>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
       <c r="E5" s="85"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -9449,12 +9455,8 @@
       <c r="B13" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="84" t="s">
-        <v>175</v>
-      </c>
-      <c r="D13" s="84" t="s">
-        <v>175</v>
-      </c>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -9473,12 +9475,8 @@
       <c r="B16" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="81" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="81" t="s">
-        <v>175</v>
-      </c>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="82"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -9486,12 +9484,8 @@
       <c r="B17" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>175</v>
-      </c>
-      <c r="D17" s="84" t="s">
-        <v>175</v>
-      </c>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="85"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -11637,7 +11631,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12488,8 +12482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13172,16 +13166,16 @@
         <v>0</v>
       </c>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K16" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L16" s="3">
         <v>0</v>
@@ -13216,20 +13210,16 @@
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f>1*'Baseline year demographics'!D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="3">
-        <f>1*'Baseline year demographics'!E9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="3">
-        <f>1*'Baseline year demographics'!F9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="3">
-        <f>1*'Baseline year demographics'!G9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
@@ -13264,16 +13254,16 @@
         <v>0</v>
       </c>
       <c r="H18" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J18" s="32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K18" s="32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L18" s="3">
         <v>0</v>
@@ -13308,20 +13298,16 @@
         <v>0</v>
       </c>
       <c r="H19" s="32">
-        <f>1*'Baseline year demographics'!D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="32">
-        <f>1*'Baseline year demographics'!E9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="32">
-        <f>1*'Baseline year demographics'!F9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="32">
-        <f>1*'Baseline year demographics'!G9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="3">
         <v>0</v>
@@ -14236,28 +14222,28 @@
         <v>1</v>
       </c>
       <c r="H41" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J41" s="32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K41" s="32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L41" s="32">
         <v>1</v>
       </c>
       <c r="M41" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N41" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O41" s="32">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15150,421 +15136,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="I4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>126</v>
-      </c>
-      <c r="H22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" t="s">
-        <v>175</v>
-      </c>
-      <c r="H23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" t="s">
-        <v>175</v>
-      </c>
-      <c r="H24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" t="s">
-        <v>175</v>
-      </c>
-      <c r="H31" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
-        <v>175</v>
-      </c>
-      <c r="C33" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" t="s">
-        <v>175</v>
-      </c>
-      <c r="C34" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A36" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D38" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J40" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A40"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15579,10 +15155,10 @@
         <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -15660,84 +15236,87 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>134</v>
+      </c>
+      <c r="B32" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
@@ -15778,6 +15357,21 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -15787,12 +15381,426 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="J4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>175</v>
+      </c>
+      <c r="I23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" t="s">
+        <v>175</v>
+      </c>
+      <c r="I24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K40" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16425,6 +16433,18 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -18481,8 +18501,8 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
spreadshhet changes and script modification for mega table
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="0" windowWidth="22380" windowHeight="14260" tabRatio="500" firstSheet="21" activeTab="22"/>
+    <workbookView xWindow="-70680" yWindow="-4680" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="20" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -4129,7 +4129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="259">
   <si>
     <t>year</t>
   </si>
@@ -4296,9 +4296,6 @@
     <t>affected fraction</t>
   </si>
   <si>
-    <t>Prophylactic zinc supplementation</t>
-  </si>
-  <si>
     <t>Breastfeeding promotion</t>
   </si>
   <si>
@@ -4896,9 +4893,6 @@
     <t>Oral rehydration salts</t>
   </si>
   <si>
-    <t>Zinc for treatment</t>
-  </si>
-  <si>
     <t>Calcium Supplementation</t>
   </si>
   <si>
@@ -4909,6 +4903,9 @@
   </si>
   <si>
     <t>Mg for eclampsia</t>
+  </si>
+  <si>
+    <t>Zinc for treatment + ORS</t>
   </si>
 </sst>
 </file>
@@ -5240,7 +5237,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="695">
+  <cellStyleXfs count="725">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5252,6 +5249,36 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6151,7 +6178,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="695">
+  <cellStyles count="725">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6499,6 +6526,21 @@
     <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6845,6 +6887,21 @@
     <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -8160,18 +8217,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -8190,7 +8247,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" s="54">
         <v>171684000</v>
@@ -8207,7 +8264,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="19">
         <v>0.35199999999999998</v>
@@ -8215,7 +8272,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="17">
         <v>0.36</v>
@@ -8223,7 +8280,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="B8" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="19">
         <v>0.1</v>
@@ -8231,7 +8288,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="B9" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="85">
         <v>0.5</v>
@@ -8239,7 +8296,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10" s="85">
         <v>0.3</v>
@@ -8247,7 +8304,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C11" s="85">
         <v>0.1</v>
@@ -8262,10 +8319,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="19">
         <v>176</v>
@@ -8273,7 +8330,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" s="19">
         <v>0.13</v>
@@ -8281,7 +8338,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="19">
         <v>25.36</v>
@@ -8289,7 +8346,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="B17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C17" s="19">
         <v>25.4</v>
@@ -8297,7 +8354,7 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="B18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="19">
         <v>34.68</v>
@@ -8305,7 +8362,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="B19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="19">
         <v>39.32</v>
@@ -8317,10 +8374,10 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="44">
         <v>0.3</v>
@@ -8328,7 +8385,7 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="B23" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="44">
         <v>0.8</v>
@@ -8336,7 +8393,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="B24" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="44">
         <v>0.12</v>
@@ -8344,7 +8401,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="B25" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="44">
         <v>0.05</v>
@@ -8352,7 +8409,7 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="B26" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="44">
         <v>0.05</v>
@@ -8363,10 +8420,10 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="52">
         <v>8634000</v>
@@ -8374,7 +8431,7 @@
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1">
       <c r="B30" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="52">
         <v>13550000</v>
@@ -8382,7 +8439,7 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="B31" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" s="52">
         <v>12394000</v>
@@ -8390,7 +8447,7 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="B32" s="51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="52">
         <v>9148000</v>
@@ -8402,10 +8459,10 @@
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="43">
         <v>0.29978973218277538</v>
@@ -8413,7 +8470,7 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
       <c r="B36" s="50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="43">
         <v>0.52556568434139284</v>
@@ -8421,7 +8478,7 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
       <c r="B37" s="50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="43">
         <v>0.16210210664201097</v>
@@ -8429,7 +8486,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
       <c r="B38" s="50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" s="43">
         <v>1.2542476833820825E-2</v>
@@ -8473,7 +8530,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>6</v>
@@ -8493,10 +8550,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="4">
@@ -8534,7 +8591,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>47</v>
@@ -8577,7 +8634,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -8597,7 +8654,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -8645,10 +8702,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -8668,7 +8725,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="86" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -8690,7 +8747,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -8712,7 +8769,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="B14" s="86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -8734,7 +8791,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="B15" s="86" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -8756,10 +8813,10 @@
     </row>
     <row r="17" spans="1:7" ht="14">
       <c r="A17" s="77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" s="76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6">
         <v>5.16</v>
@@ -8780,7 +8837,7 @@
     <row r="18" spans="1:7" ht="14">
       <c r="A18" s="78"/>
       <c r="B18" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -8801,7 +8858,7 @@
     <row r="19" spans="1:7" ht="14" customHeight="1"/>
     <row r="20" spans="1:7">
       <c r="A20" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>28</v>
@@ -8824,7 +8881,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>28</v>
@@ -8874,13 +8931,13 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>6</v>
@@ -8900,13 +8957,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="127" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="73">
         <v>1.85</v>
@@ -8927,7 +8984,7 @@
     <row r="3" spans="1:10">
       <c r="B3" s="127"/>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="73">
         <v>1.9</v>
@@ -8949,7 +9006,7 @@
     <row r="4" spans="1:10">
       <c r="B4" s="127"/>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="73">
         <f>D17^(1/2)</f>
@@ -8978,7 +9035,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D5" s="73">
         <v>2.0299999999999998</v>
@@ -8999,7 +9056,7 @@
     <row r="6" spans="1:10">
       <c r="B6" s="127"/>
       <c r="C6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D6" s="73">
         <v>2.17</v>
@@ -9020,7 +9077,7 @@
     <row r="7" spans="1:10">
       <c r="B7" s="127"/>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" s="73">
         <f>D17^(1/2)</f>
@@ -9048,7 +9105,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="73">
         <v>1</v>
@@ -9069,7 +9126,7 @@
     <row r="9" spans="1:10">
       <c r="B9" s="127"/>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" s="73">
         <v>1</v>
@@ -9090,7 +9147,7 @@
     <row r="10" spans="1:10">
       <c r="B10" s="127"/>
       <c r="C10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="73">
         <v>1</v>
@@ -9117,7 +9174,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="73">
         <v>1</v>
@@ -9138,7 +9195,7 @@
     <row r="12" spans="1:10">
       <c r="B12" s="127"/>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D12" s="73">
         <v>1</v>
@@ -9159,7 +9216,7 @@
     <row r="13" spans="1:10">
       <c r="B13" s="127"/>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="73">
         <v>1</v>
@@ -9185,7 +9242,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" s="73">
         <v>1</v>
@@ -9206,7 +9263,7 @@
     <row r="15" spans="1:10">
       <c r="B15" s="127"/>
       <c r="C15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="73">
         <v>1</v>
@@ -9227,7 +9284,7 @@
     <row r="16" spans="1:10">
       <c r="B16" s="127"/>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D16" s="73">
         <v>1</v>
@@ -9249,10 +9306,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="80">
         <v>1.05</v>
@@ -9279,13 +9336,13 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="77" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B19" s="127" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="73">
         <v>1</v>
@@ -9306,7 +9363,7 @@
     <row r="20" spans="1:8">
       <c r="B20" s="127"/>
       <c r="C20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D20" s="73">
         <v>1</v>
@@ -9327,7 +9384,7 @@
     <row r="21" spans="1:8">
       <c r="B21" s="127"/>
       <c r="C21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D21" s="73">
         <f>D34^(1/5)</f>
@@ -9355,7 +9412,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="73">
         <v>1</v>
@@ -9376,7 +9433,7 @@
     <row r="23" spans="1:8">
       <c r="B23" s="127"/>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="73">
         <v>1</v>
@@ -9397,7 +9454,7 @@
     <row r="24" spans="1:8">
       <c r="B24" s="127"/>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D24" s="73">
         <f>D34^(1/5)</f>
@@ -9425,7 +9482,7 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" s="73">
         <v>1</v>
@@ -9446,7 +9503,7 @@
     <row r="26" spans="1:8">
       <c r="B26" s="127"/>
       <c r="C26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D26" s="73">
         <v>1</v>
@@ -9467,7 +9524,7 @@
     <row r="27" spans="1:8">
       <c r="B27" s="127"/>
       <c r="C27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D27" s="73">
         <f>D34^(1/5)</f>
@@ -9495,7 +9552,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D28" s="73">
         <v>1</v>
@@ -9516,7 +9573,7 @@
     <row r="29" spans="1:8">
       <c r="B29" s="127"/>
       <c r="C29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D29" s="73">
         <v>1</v>
@@ -9537,7 +9594,7 @@
     <row r="30" spans="1:8">
       <c r="B30" s="127"/>
       <c r="C30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D30" s="73">
         <f>D34^(1/5)</f>
@@ -9565,7 +9622,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D31" s="73">
         <v>1</v>
@@ -9586,7 +9643,7 @@
     <row r="32" spans="1:8">
       <c r="B32" s="127"/>
       <c r="C32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D32" s="73">
         <v>1</v>
@@ -9607,7 +9664,7 @@
     <row r="33" spans="1:8">
       <c r="B33" s="127"/>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D33" s="73">
         <f>D34^(1/5)</f>
@@ -9632,10 +9689,10 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" s="79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D34" s="80">
         <v>1.05</v>
@@ -9655,13 +9712,13 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B36" s="127" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D36" s="73">
         <v>1</v>
@@ -9682,7 +9739,7 @@
     <row r="37" spans="1:8">
       <c r="B37" s="127"/>
       <c r="C37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D37" s="73">
         <v>1</v>
@@ -9703,7 +9760,7 @@
     <row r="38" spans="1:8">
       <c r="B38" s="127"/>
       <c r="C38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D38" s="73">
         <v>1</v>
@@ -9726,7 +9783,7 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D39" s="73">
         <v>1</v>
@@ -9747,7 +9804,7 @@
     <row r="40" spans="1:8">
       <c r="B40" s="127"/>
       <c r="C40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D40" s="73">
         <v>1</v>
@@ -9768,7 +9825,7 @@
     <row r="41" spans="1:8">
       <c r="B41" s="127"/>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="73">
         <v>1</v>
@@ -9791,7 +9848,7 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D42" s="73">
         <v>1</v>
@@ -9812,7 +9869,7 @@
     <row r="43" spans="1:8">
       <c r="B43" s="127"/>
       <c r="C43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D43" s="73">
         <v>1</v>
@@ -9833,7 +9890,7 @@
     <row r="44" spans="1:8">
       <c r="B44" s="127"/>
       <c r="C44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D44" s="73">
         <v>1</v>
@@ -9856,7 +9913,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D45" s="73">
         <v>1</v>
@@ -9877,7 +9934,7 @@
     <row r="46" spans="1:8">
       <c r="B46" s="127"/>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D46" s="73">
         <v>1</v>
@@ -9898,7 +9955,7 @@
     <row r="47" spans="1:8">
       <c r="B47" s="127"/>
       <c r="C47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D47" s="73">
         <v>1</v>
@@ -9921,7 +9978,7 @@
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D48" s="73">
         <v>1</v>
@@ -9942,7 +9999,7 @@
     <row r="49" spans="2:8">
       <c r="B49" s="127"/>
       <c r="C49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D49" s="73">
         <v>1</v>
@@ -9963,7 +10020,7 @@
     <row r="50" spans="2:8">
       <c r="B50" s="127"/>
       <c r="C50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="73">
         <v>1</v>
@@ -9983,10 +10040,10 @@
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" s="91">
         <v>1</v>
@@ -10049,27 +10106,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="93"/>
       <c r="D2" s="93"/>
@@ -10099,10 +10156,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E5" s="97"/>
     </row>
@@ -10118,7 +10175,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="98"/>
       <c r="B7" s="99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="100"/>
       <c r="D7" s="100"/>
@@ -10126,10 +10183,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="92" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" s="93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
@@ -10168,17 +10225,17 @@
         <v>9</v>
       </c>
       <c r="C13" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D13" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="97"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="98"/>
       <c r="B14" s="99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="100"/>
       <c r="D14" s="100"/>
@@ -10186,16 +10243,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" s="93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16" s="93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E16" s="94"/>
     </row>
@@ -10205,10 +10262,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D17" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E17" s="97"/>
     </row>
@@ -10242,7 +10299,7 @@
     <row r="21" spans="1:5">
       <c r="A21" s="98"/>
       <c r="B21" s="99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
@@ -10275,27 +10332,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <f>'Baseline year demographics'!C9</f>
@@ -10370,10 +10427,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <f>1.5*0.61</f>
@@ -10538,10 +10595,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -10557,7 +10614,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>46</v>
@@ -10578,19 +10635,19 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -10617,7 +10674,7 @@
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -10669,7 +10726,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -10695,7 +10752,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -10723,7 +10780,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -10752,7 +10809,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -10780,7 +10837,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="B9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -10809,7 +10866,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -10838,7 +10895,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" s="69">
         <v>0</v>
@@ -10868,7 +10925,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" s="69">
         <v>0</v>
@@ -10894,7 +10951,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="B13" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" s="69">
         <v>0</v>
@@ -10920,10 +10977,10 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -10951,7 +11008,7 @@
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -10977,7 +11034,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="B17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -11004,7 +11061,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="B18" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -11030,7 +11087,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="B19" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -11057,7 +11114,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -11084,10 +11141,10 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -11113,7 +11170,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -11139,7 +11196,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -11165,7 +11222,7 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -11191,7 +11248,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="B26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -11217,7 +11274,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -11243,7 +11300,7 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="B28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -11270,7 +11327,7 @@
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -11296,7 +11353,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="B30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -11322,7 +11379,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="B31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -11348,7 +11405,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="B32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -11374,7 +11431,7 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1">
       <c r="B33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
@@ -11400,7 +11457,7 @@
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
       <c r="B34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -11426,7 +11483,7 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1">
       <c r="B35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
@@ -11452,7 +11509,7 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
       <c r="B36" s="82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -11478,7 +11535,7 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
       <c r="B37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -11505,7 +11562,7 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1">
       <c r="B38" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
@@ -11536,7 +11593,7 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
       <c r="B39" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -11567,7 +11624,7 @@
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -11598,7 +11655,7 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1">
       <c r="B41" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
@@ -11624,7 +11681,7 @@
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1">
       <c r="B42" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="35">
         <f>'Baseline year demographics'!$C$8</f>
@@ -11657,7 +11714,7 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1">
       <c r="B43" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -11688,7 +11745,7 @@
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1">
       <c r="B44" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -11719,7 +11776,7 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1">
       <c r="B45" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
@@ -11750,10 +11807,10 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
@@ -11779,7 +11836,7 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1">
       <c r="B47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
@@ -11805,7 +11862,7 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1">
       <c r="B48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -11831,7 +11888,7 @@
     </row>
     <row r="49" spans="2:9" ht="15.75" customHeight="1">
       <c r="B49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C49" s="3">
         <v>1</v>
@@ -11857,7 +11914,7 @@
     </row>
     <row r="50" spans="2:9" ht="15.75" customHeight="1">
       <c r="B50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -11883,7 +11940,7 @@
     </row>
     <row r="51" spans="2:9" ht="15.75" customHeight="1">
       <c r="B51" t="s">
-        <v>55</v>
+        <v>253</v>
       </c>
       <c r="C51" s="3">
         <v>1</v>
@@ -11909,7 +11966,7 @@
     </row>
     <row r="52" spans="2:9" ht="15.75" customHeight="1">
       <c r="B52" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
@@ -11934,26 +11991,26 @@
       </c>
     </row>
     <row r="53" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>255</v>
       </c>
       <c r="C53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="3">
         <v>0</v>
@@ -11961,7 +12018,7 @@
     </row>
     <row r="54" spans="2:9" ht="15.75" customHeight="1">
       <c r="B54" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C54" s="3">
         <v>0</v>
@@ -11987,7 +12044,7 @@
     </row>
     <row r="55" spans="2:9" ht="15.75" customHeight="1">
       <c r="B55" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C55" s="3">
         <v>0</v>
@@ -12008,32 +12065,6 @@
         <v>1</v>
       </c>
       <c r="I55" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B56" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C56" s="3">
-        <v>0</v>
-      </c>
-      <c r="D56" s="3">
-        <v>0</v>
-      </c>
-      <c r="E56" s="3">
-        <v>0</v>
-      </c>
-      <c r="F56" s="3">
-        <v>0</v>
-      </c>
-      <c r="G56" s="3">
-        <v>0</v>
-      </c>
-      <c r="H56" s="3">
-        <v>1</v>
-      </c>
-      <c r="I56" s="3">
         <v>0</v>
       </c>
     </row>
@@ -12089,7 +12120,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
@@ -12126,7 +12157,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
@@ -12163,7 +12194,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -12200,7 +12231,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
@@ -12239,7 +12270,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
@@ -12278,7 +12309,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B12" t="s">
         <v>52</v>
@@ -12368,36 +12399,36 @@
         <v>10</v>
       </c>
       <c r="H1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>149</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="60">
         <v>1</v>
@@ -12441,7 +12472,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" s="61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C3" s="60">
         <v>1</v>
@@ -12485,7 +12516,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="B4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -12529,7 +12560,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="B5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -12573,7 +12604,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -12617,7 +12648,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="B7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -12661,7 +12692,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -12705,7 +12736,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -12749,7 +12780,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -12793,7 +12824,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="B11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -12837,7 +12868,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="B12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -12881,7 +12912,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="B13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -12925,7 +12956,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="B14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -12969,7 +13000,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="B15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -13013,7 +13044,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="B16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -13057,7 +13088,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="B17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -13101,7 +13132,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="B18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -13145,7 +13176,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="B19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -13189,7 +13220,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="B20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -13233,7 +13264,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="B21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -13277,7 +13308,7 @@
     </row>
     <row r="22" spans="1:15" ht="14" customHeight="1">
       <c r="B22" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -13321,7 +13352,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="B23" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -13365,7 +13396,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="B24" s="60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -13409,7 +13440,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="B25" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25">
         <v>0.83</v>
@@ -13453,10 +13484,10 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -13500,7 +13531,7 @@
     </row>
     <row r="28" spans="1:15">
       <c r="B28" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -13544,7 +13575,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="B29" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -13588,7 +13619,7 @@
     </row>
     <row r="30" spans="1:15">
       <c r="B30" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -13632,7 +13663,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="B31" s="61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -13676,7 +13707,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="B32" s="61" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -13720,7 +13751,7 @@
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="61" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -13808,7 +13839,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>6</v>
@@ -13828,10 +13859,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="60">
         <v>1</v>
@@ -13851,10 +13882,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="60">
         <v>1</v>
@@ -13890,7 +13921,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -13915,7 +13946,7 @@
         <v>51</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="74"/>
       <c r="F1" s="74"/>
@@ -13924,13 +13955,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -13942,7 +13973,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="4">
         <v>0.2</v>
@@ -13954,13 +13985,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -13973,7 +14004,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="11"/>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="12">
         <v>0.59</v>
@@ -13985,13 +14016,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="12">
         <v>1</v>
@@ -14004,7 +14035,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="11"/>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="12">
         <v>0.6</v>
@@ -14521,34 +14552,34 @@
         <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>53</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -15158,8 +15189,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -15207,7 +15238,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -15227,7 +15258,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -15249,7 +15280,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -15270,10 +15301,10 @@
     <row r="5" spans="1:8">
       <c r="A5" s="11"/>
       <c r="B5" s="60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="61">
         <v>0</v>
@@ -15293,13 +15324,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="61">
         <v>0</v>
@@ -15319,7 +15350,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="61">
         <v>0</v>
@@ -15339,10 +15370,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="B8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="61">
         <v>0</v>
@@ -15362,7 +15393,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="61">
         <v>0</v>
@@ -15382,13 +15413,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="61">
         <v>0</v>
@@ -15408,7 +15439,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="C11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="61">
         <v>0</v>
@@ -15428,10 +15459,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="61">
         <v>0</v>
@@ -15451,7 +15482,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="C13" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="61">
         <v>0</v>
@@ -15471,13 +15502,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="61">
         <v>0</v>
@@ -15497,7 +15528,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="C15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="61">
         <v>0</v>
@@ -15517,10 +15548,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="61">
         <v>0</v>
@@ -15540,7 +15571,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="C17" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="61">
         <v>0</v>
@@ -15560,13 +15591,13 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18" s="61">
         <v>0</v>
@@ -15586,7 +15617,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="C19" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="61">
         <v>0</v>
@@ -15607,10 +15638,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="B20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" s="67">
         <v>0</v>
@@ -15631,7 +15662,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="C21" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="67">
         <v>0</v>
@@ -15652,13 +15683,13 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="12">
         <v>0.7</v>
@@ -15680,7 +15711,7 @@
     <row r="23" spans="1:9">
       <c r="A23" s="12"/>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="12">
         <v>0.46</v>
@@ -15701,13 +15732,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="12">
         <v>0.7</v>
@@ -15728,7 +15759,7 @@
     <row r="25" spans="1:9">
       <c r="A25" s="12"/>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="12">
         <v>0.46</v>
@@ -15748,13 +15779,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D26" s="12">
         <v>0.7</v>
@@ -15774,7 +15805,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="C27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="12">
         <v>0.46</v>
@@ -15794,13 +15825,13 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D28" s="12">
         <v>1</v>
@@ -15820,7 +15851,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="C29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="12">
         <v>0.17</v>
@@ -15841,7 +15872,7 @@
     <row r="30" spans="1:9">
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="12">
         <v>0.17</v>
@@ -15861,13 +15892,13 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="12">
         <v>1</v>
@@ -15887,7 +15918,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="C32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="12">
         <v>0.69</v>
@@ -15908,7 +15939,7 @@
     <row r="33" spans="1:8">
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="12">
         <v>0.69</v>
@@ -15928,13 +15959,13 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -15954,7 +15985,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="C35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="12">
         <v>0.36</v>
@@ -15975,7 +16006,7 @@
     <row r="36" spans="1:8">
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" s="12">
         <v>0.36</v>
@@ -15995,13 +16026,13 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -16021,7 +16052,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="C38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" s="12">
         <v>0.2</v>
@@ -16042,7 +16073,7 @@
     <row r="39" spans="1:8">
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D39" s="12">
         <v>0.2</v>
@@ -16062,13 +16093,13 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -16088,7 +16119,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="12">
         <v>0.48</v>
@@ -16109,7 +16140,7 @@
     <row r="42" spans="1:8">
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="12">
         <v>0.48</v>
@@ -16129,13 +16160,13 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D43" s="12">
         <v>1</v>
@@ -16155,7 +16186,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="C44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="12">
         <v>0.5</v>
@@ -16175,7 +16206,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="C45" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" s="12">
         <v>0.65</v>
@@ -16195,13 +16226,13 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46" s="12">
         <v>1</v>
@@ -16221,7 +16252,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="C47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D47" s="12">
         <v>0.49</v>
@@ -16241,7 +16272,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="C48" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="12">
         <v>0.52</v>
@@ -16261,13 +16292,13 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D49" s="12">
         <v>0.88</v>
@@ -16287,7 +16318,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="C50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D50" s="12">
         <v>0.93</v>
@@ -16307,13 +16338,13 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D51" s="12">
         <v>1</v>
@@ -16333,22 +16364,22 @@
     </row>
     <row r="52" spans="1:8">
       <c r="C52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D52" s="12">
-        <v>0.23</v>
+        <v>0.86</v>
       </c>
       <c r="E52" s="12">
-        <v>0.23</v>
+        <v>0.86</v>
       </c>
       <c r="F52" s="12">
-        <v>0.23</v>
+        <v>0.86</v>
       </c>
       <c r="G52" s="12">
-        <v>0.23</v>
+        <v>0.86</v>
       </c>
       <c r="H52" s="12">
-        <v>0.23</v>
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -16383,24 +16414,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>216</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13">
       <c r="A2" s="82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="83">
         <v>0.9</v>
@@ -16418,7 +16449,7 @@
     </row>
     <row r="3" spans="1:5" ht="13">
       <c r="A3" s="82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="83">
         <v>1</v>
@@ -16436,7 +16467,7 @@
     </row>
     <row r="4" spans="1:5" ht="13">
       <c r="A4" s="82" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="83">
         <v>1</v>
@@ -16454,7 +16485,7 @@
     </row>
     <row r="5" spans="1:5" ht="13">
       <c r="A5" s="82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="83">
         <v>1</v>
@@ -16472,7 +16503,7 @@
     </row>
     <row r="6" spans="1:5" ht="13">
       <c r="A6" s="82" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="83">
         <v>1</v>
@@ -16490,7 +16521,7 @@
     </row>
     <row r="7" spans="1:5" ht="13">
       <c r="A7" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="83">
         <v>0.93</v>
@@ -16508,7 +16539,7 @@
     </row>
     <row r="8" spans="1:5" ht="13">
       <c r="A8" s="82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="83">
         <v>0.5</v>
@@ -16526,7 +16557,7 @@
     </row>
     <row r="9" spans="1:5" ht="13">
       <c r="A9" s="82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="83">
         <v>0.5</v>
@@ -16544,7 +16575,7 @@
     </row>
     <row r="10" spans="1:5" ht="13">
       <c r="A10" s="82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="83">
         <v>0.98</v>
@@ -16606,19 +16637,19 @@
         <v>51</v>
       </c>
       <c r="C1" s="117" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="117" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="E1" s="117" t="s">
         <v>233</v>
-      </c>
-      <c r="E1" s="117" t="s">
-        <v>234</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" s="96" t="s">
         <v>52</v>
@@ -16779,7 +16810,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -16795,13 +16826,13 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -16820,7 +16851,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="14">
         <v>0</v>
@@ -16834,7 +16865,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="63">
         <v>0</v>
@@ -16848,7 +16879,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="34">
         <v>0</v>
@@ -16862,7 +16893,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="63">
         <v>0</v>
@@ -16876,7 +16907,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="34">
         <v>0</v>
@@ -16890,7 +16921,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -16904,7 +16935,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="65">
         <v>0</v>
@@ -16918,7 +16949,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -16932,7 +16963,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="65">
         <v>0</v>
@@ -16946,7 +16977,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12" s="14">
         <v>0</v>
@@ -16960,7 +16991,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" s="14">
         <v>0</v>
@@ -16974,7 +17005,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="14">
         <v>0</v>
@@ -16988,7 +17019,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="14">
         <v>0</v>
@@ -17002,7 +17033,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -17016,7 +17047,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="14">
         <v>0</v>
@@ -17030,7 +17061,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" s="14">
         <v>0</v>
@@ -17044,7 +17075,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="14">
         <v>0</v>
@@ -17058,7 +17089,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B20" s="14">
         <v>0</v>
@@ -17072,7 +17103,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="14">
         <v>0</v>
@@ -17086,7 +17117,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B22" s="14">
         <v>0</v>
@@ -17100,7 +17131,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -17114,7 +17145,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" s="14">
         <v>0</v>
@@ -17128,7 +17159,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" s="14">
         <v>0</v>
@@ -17142,7 +17173,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="14">
         <v>0</v>
@@ -17156,7 +17187,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
@@ -17170,7 +17201,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="14">
         <v>0</v>
@@ -17184,7 +17215,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="14">
         <v>0</v>
@@ -17198,7 +17229,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="14">
         <v>0</v>
@@ -17212,7 +17243,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="14">
         <v>0</v>
@@ -17226,7 +17257,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="19">
         <v>0</v>
@@ -17240,7 +17271,7 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B33" s="19">
         <v>0</v>
@@ -17254,7 +17285,7 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B34" s="19">
         <v>0</v>
@@ -17268,7 +17299,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="14">
         <v>0.2</v>
@@ -17282,7 +17313,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B36" s="14">
         <v>0</v>
@@ -17297,7 +17328,7 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B37" s="14">
         <v>0</v>
@@ -17312,7 +17343,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B38" s="14">
         <v>0.61</v>
@@ -17327,7 +17358,7 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1">
       <c r="A39" s="81" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B39" s="121">
         <v>0.5</v>
@@ -17342,10 +17373,10 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
       <c r="A40" s="90" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B40" s="121">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="14">
         <v>0.85</v>
@@ -17356,7 +17387,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B41" s="121">
         <v>0.84</v>
@@ -17370,7 +17401,7 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B42" s="121">
         <v>0.14000000000000001</v>
@@ -17384,7 +17415,7 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B43" s="121">
         <v>0.69</v>
@@ -17398,7 +17429,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
       <c r="A44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B44" s="121">
         <v>0.38700000000000001</v>
@@ -17412,7 +17443,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B45" s="121">
         <v>0.4</v>
@@ -17426,7 +17457,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B46" s="122">
         <v>0</v>
@@ -17440,7 +17471,7 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1">
       <c r="A47" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B47" s="122">
         <v>0</v>
@@ -17454,7 +17485,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1">
       <c r="A48" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B48" s="122">
         <v>0</v>
@@ -17463,12 +17494,12 @@
         <v>0.85</v>
       </c>
       <c r="D48" s="123">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B49" s="122">
         <v>0</v>
@@ -17482,7 +17513,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B50" s="122">
         <v>0</v>
@@ -17496,7 +17527,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B51" s="122">
         <v>0</v>
@@ -17553,7 +17584,7 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -17949,7 +17980,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="19">
         <v>0</v>
@@ -17972,7 +18003,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="19">
         <v>0</v>
@@ -17995,7 +18026,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="19">
         <v>0</v>
@@ -18018,7 +18049,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="19">
         <v>0</v>
@@ -18041,7 +18072,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -18064,7 +18095,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -18087,7 +18118,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -18110,7 +18141,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="19">
         <v>0</v>
@@ -18133,7 +18164,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -18221,7 +18252,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="34">
         <v>5.1999999999999998E-2</v>
@@ -18261,7 +18292,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" s="60">
         <f>Distributions!C10/100 * 2.6</f>
@@ -18286,7 +18317,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="60">
         <f>Distributions!C11/100 * 2.6</f>
@@ -18340,24 +18371,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -18431,7 +18462,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="10"/>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="19">
         <v>0</v>
@@ -18446,7 +18477,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="10"/>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="19">
         <v>0</v>
@@ -18461,7 +18492,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="10"/>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="19">
         <v>0</v>
@@ -18476,7 +18507,7 @@
     <row r="10" spans="1:5">
       <c r="A10" s="10"/>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="19">
         <v>0</v>
@@ -18496,7 +18527,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -18565,7 +18596,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="19">
         <v>0</v>
@@ -18579,7 +18610,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="19">
         <v>0</v>
@@ -18593,7 +18624,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" s="19">
         <v>0</v>
@@ -18607,7 +18638,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C21" s="19">
         <v>0</v>
@@ -18621,10 +18652,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" t="s">
         <v>111</v>
-      </c>
-      <c r="B24" t="s">
-        <v>112</v>
       </c>
       <c r="C24" s="40">
         <v>0.01</v>
@@ -18812,7 +18843,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="17">
         <v>15</v>
@@ -18832,7 +18863,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" s="17">
         <v>4.9000000000000004</v>
@@ -18962,21 +18993,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="112" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B2" s="113" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C2" s="102">
         <v>0.15</v>
@@ -18984,7 +19015,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="113" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3" s="102">
         <v>0.03</v>
@@ -18992,7 +19023,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="113" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" s="102">
         <v>0</v>
@@ -19000,7 +19031,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="114" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C5" s="102">
         <v>0.19</v>
@@ -19008,7 +19039,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="B6" s="114" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="102">
         <v>0.39</v>
@@ -19016,7 +19047,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="114" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C7" s="102">
         <v>0.19</v>
@@ -19024,7 +19055,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="115" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" s="102">
         <v>1E-3</v>
@@ -19032,7 +19063,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="115" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C9" s="102">
         <v>7.0000000000000001E-3</v>
@@ -19040,7 +19071,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="115" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" s="102">
         <v>0.04</v>
@@ -19051,10 +19082,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="112" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B12" s="103" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12" s="102">
         <v>0.34</v>
@@ -19062,7 +19093,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" s="103" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C13" s="102">
         <v>0.05</v>
@@ -19070,7 +19101,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" s="103" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C14" s="102">
         <v>7.0000000000000007E-2</v>
@@ -19078,7 +19109,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" s="102">
         <v>0.55000000000000004</v>
@@ -19110,10 +19141,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>44</v>
@@ -19133,7 +19164,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="20">
         <f>1-D2-E2-F2</f>
@@ -19151,7 +19182,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="45"/>
       <c r="D3" s="11">
@@ -19166,7 +19197,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -19183,7 +19214,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="72">
         <v>1</v>
@@ -19200,7 +19231,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="B6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" s="72">
         <v>1</v>
@@ -19233,7 +19264,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
@@ -19372,15 +19403,15 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B21" s="105" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C21" s="108">
         <v>1</v>
@@ -19398,7 +19429,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="B22" s="105" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C22" s="108">
         <v>1</v>
@@ -19416,7 +19447,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="105" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C23" s="108">
         <v>1</v>
@@ -19434,7 +19465,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="106" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C24" s="108">
         <v>1</v>
@@ -19452,7 +19483,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="106" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C25" s="108">
         <v>1</v>
@@ -19470,7 +19501,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="B26" s="106" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C26" s="108">
         <v>1</v>
@@ -19488,7 +19519,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="B27" s="107" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C27" s="108">
         <v>1</v>
@@ -19506,7 +19537,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="B28" s="107" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C28" s="108">
         <v>1</v>
@@ -19524,7 +19555,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="B29" s="107" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" s="108">
         <v>1</v>
@@ -19549,7 +19580,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="B31" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C31" s="110"/>
       <c r="D31" s="110"/>
@@ -19559,10 +19590,10 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B32" s="104" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C32" s="108">
         <v>1</v>
@@ -19580,7 +19611,7 @@
     </row>
     <row r="33" spans="2:10" ht="15.75" customHeight="1">
       <c r="B33" s="104" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C33" s="108">
         <v>1</v>
@@ -19598,7 +19629,7 @@
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1">
       <c r="B34" s="104" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C34" s="108">
         <v>1</v>
@@ -19616,7 +19647,7 @@
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1">
       <c r="B35" s="104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C35" s="108">
         <v>1</v>
@@ -19661,7 +19692,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -19675,7 +19706,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -19699,7 +19730,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -20234,7 +20265,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="C26" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -20257,7 +20288,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="C27" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -20329,7 +20360,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="C30" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
@@ -20352,7 +20383,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="C31" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
@@ -20424,7 +20455,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="C34" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -20447,7 +20478,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="C35" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
@@ -20519,7 +20550,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="C38" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
@@ -20542,7 +20573,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="C39" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -20614,7 +20645,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="C42" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -20637,7 +20668,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="C43" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -21328,13 +21359,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D76" s="4">
         <v>1</v>
@@ -21357,7 +21388,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D77" s="4">
         <v>1</v>
@@ -21380,10 +21411,10 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D78" s="4">
         <v>1</v>
@@ -21406,7 +21437,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -21429,10 +21460,10 @@
     </row>
     <row r="80" spans="1:9">
       <c r="B80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -21455,7 +21486,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -21478,10 +21509,10 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
new estimated unit costs for WASH
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-70680" yWindow="-4680" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="20" activeTab="22"/>
+    <workbookView xWindow="-67480" yWindow="-4300" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="20" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -10063,11 +10063,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -10078,6 +10073,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -16809,8 +16809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -17396,7 +17396,7 @@
         <v>0.85</v>
       </c>
       <c r="D41" s="19">
-        <v>1</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
@@ -17410,7 +17410,7 @@
         <v>0.85</v>
       </c>
       <c r="D42" s="19">
-        <v>1</v>
+        <v>231.85</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
@@ -17424,7 +17424,7 @@
         <v>0.85</v>
       </c>
       <c r="D43" s="19">
-        <v>1</v>
+        <v>50.26</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
@@ -17438,7 +17438,7 @@
         <v>0.85</v>
       </c>
       <c r="D44" s="19">
-        <v>1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
added fraction zinc deficient in target pop for zinc supplementation
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-67480" yWindow="-4300" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="20" activeTab="22"/>
+    <workbookView xWindow="-67480" yWindow="-4300" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -428,13 +428,13 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
     <author>Janka Petravic</author>
-    <author>Ruth</author>
     <author>Sam</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -444,6 +444,30 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction zinc deficient 0.3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t>Janka Petravic:</t>
         </r>
         <r>
@@ -458,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="1">
+    <comment ref="E7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -483,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="1">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="1">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -532,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="1">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -580,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0">
+    <comment ref="H15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -700,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I23" authorId="0">
+    <comment ref="I23" authorId="1">
       <text>
         <r>
           <rPr>
@@ -748,7 +772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I30" authorId="0">
+    <comment ref="I30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -772,7 +796,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="1">
+    <comment ref="I37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -10597,8 +10621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -10683,13 +10707,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F3" s="3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G3" s="3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H3" s="3">
         <v>0</v>
@@ -16809,7 +16833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed affected frraction in spreadsheet for PPCF + iron effect on wasting, and added reduction in stunting update in params.py
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-67480" yWindow="-4300" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="14" activeTab="16"/>
+    <workbookView xWindow="-67480" yWindow="-4300" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -9702,6 +9702,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9712,11 +9717,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11909,7 +11909,7 @@
   </sheetPr>
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -14603,8 +14603,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -14842,13 +14842,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="61">
-        <v>0.33500000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="G10" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="H10" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -14885,13 +14885,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="61">
-        <v>0.33500000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="G12" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="H12" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -14931,13 +14931,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="61">
-        <v>0.33500000000000002</v>
+        <v>0.04</v>
       </c>
       <c r="G14" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.04</v>
       </c>
       <c r="H14" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -14974,13 +14974,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="61">
-        <v>0.33500000000000002</v>
+        <v>0.04</v>
       </c>
       <c r="G16" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.04</v>
       </c>
       <c r="H16" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" spans="1:9">

</xml_diff>

<commit_message>
Changed project to Constants
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="-32240" yWindow="-18520" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3948,7 +3948,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="241">
   <si>
     <t>year</t>
   </si>
@@ -4596,9 +4596,6 @@
   </si>
   <si>
     <t>Family planning</t>
-  </si>
-  <si>
-    <t>Diarrheoa</t>
   </si>
   <si>
     <t>not anaemic</t>
@@ -7841,7 +7838,7 @@
     </row>
     <row r="13" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="47">
         <v>0.9</v>
@@ -7849,7 +7846,7 @@
     </row>
     <row r="14" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C14" s="47">
         <v>0.4</v>
@@ -7857,7 +7854,7 @@
     </row>
     <row r="15" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C15" s="69">
         <v>0.2</v>
@@ -8018,7 +8015,7 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B38" s="92" t="s">
         <v>118</v>
@@ -8072,7 +8069,7 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B44" s="92" t="s">
         <v>122</v>
@@ -9303,6 +9300,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9313,11 +9315,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11676,7 +11673,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>106</v>
@@ -11742,7 +11739,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>106</v>
@@ -12482,7 +12479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+    <sheetView topLeftCell="B12" workbookViewId="0">
       <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
@@ -15155,10 +15152,10 @@
         <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -15316,7 +15313,7 @@
         <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
@@ -15386,7 +15383,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15415,28 +15412,28 @@
         <v>214</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>239</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>240</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>215</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -15799,7 +15796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -15816,7 +15813,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>149</v>
@@ -16495,7 +16492,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="90">
         <v>7.0000000000000001E-3</v>
@@ -16751,7 +16748,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B10" s="90">
         <v>0</v>
@@ -16784,7 +16781,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11" s="90">
         <v>0</v>
@@ -17373,8 +17370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17401,7 +17398,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="15">
         <v>2.4300000000000002</v>
@@ -17421,7 +17418,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="31">
         <v>5.1999999999999998E-2</v>
@@ -17588,7 +17585,7 @@
         <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="102">
         <f t="shared" ref="C2:O2" si="0">1-C3</f>
@@ -17645,7 +17642,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" s="102">
         <f>C6</f>
@@ -17722,7 +17719,7 @@
         <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="37">
         <v>0.1</v>
@@ -17769,7 +17766,7 @@
         <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" s="37">
         <v>0.05</v>
@@ -17816,7 +17813,7 @@
         <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="94">
         <v>0.01</v>
@@ -18270,7 +18267,7 @@
         <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="11">
@@ -18285,7 +18282,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -18353,7 +18350,7 @@
         <v>205</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -18572,7 +18569,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -19470,7 +19467,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>14</v>
@@ -20372,10 +20369,10 @@
         <v>214</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -20419,7 +20416,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -20466,7 +20463,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -20510,7 +20507,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -20557,7 +20554,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -20601,7 +20598,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D51" s="4">
         <v>1</v>
@@ -20648,7 +20645,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D52" s="4">
         <v>1</v>
@@ -20692,7 +20689,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
@@ -20739,7 +20736,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
@@ -20783,7 +20780,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
@@ -20831,7 +20828,7 @@
         <v>87</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D56" s="4">
         <v>1</v>
@@ -20875,7 +20872,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D57" s="4">
         <v>1</v>
@@ -20922,7 +20919,7 @@
         <v>88</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
@@ -20966,7 +20963,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D59" s="4">
         <v>1</v>
@@ -21013,7 +21010,7 @@
         <v>89</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D60" s="4">
         <v>1</v>
@@ -21057,7 +21054,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D61" s="4">
         <v>1</v>
@@ -21108,7 +21105,7 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>37</v>
@@ -21824,7 +21821,7 @@
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>37</v>
@@ -22361,10 +22358,10 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A94" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B94" s="11" t="s">
         <v>225</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>226</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>37</v>
@@ -22621,10 +22618,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C4">
         <v>1.04</v>
@@ -22914,7 +22911,7 @@
         <v>157</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C21" s="47">
         <v>1.04</v>
@@ -22937,7 +22934,7 @@
         <v>158</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C23" s="47">
         <v>1.04</v>
@@ -22957,10 +22954,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C25" s="47">
         <v>1</v>

</xml_diff>

<commit_message>
Sorting to implement program dependencies
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32240" yWindow="-18520" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="12" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3948,7 +3948,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="241">
   <si>
     <t>year</t>
   </si>
@@ -4994,7 +4994,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="631">
+  <cellStyleXfs count="639">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5006,6 +5006,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5790,7 +5798,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="631">
+  <cellStyles count="639">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6106,6 +6114,10 @@
     <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6420,6 +6432,10 @@
     <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7723,7 +7739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -12479,8 +12495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14466,7 +14482,10 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="10"/>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="10" t="s">
         <v>81</v>
       </c>
     </row>
@@ -15136,8 +15155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15197,6 +15216,9 @@
       <c r="A9" t="s">
         <v>140</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -15207,6 +15229,9 @@
       <c r="A11" t="s">
         <v>141</v>
       </c>
+      <c r="C11" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -15217,6 +15242,9 @@
       <c r="A13" t="s">
         <v>142</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -15227,88 +15255,121 @@
       <c r="A15" t="s">
         <v>139</v>
       </c>
+      <c r="C15" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C17" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B26" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B27" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B28" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>134</v>
       </c>
@@ -15316,57 +15377,75 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="C34" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="30" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B39" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B40" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>173</v>
       </c>
@@ -17370,7 +17449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to the coverage adjustments for programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4994,7 +4994,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="639">
+  <cellStyleXfs count="645">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5006,6 +5006,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5798,7 +5804,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="639">
+  <cellStyles count="645">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6118,6 +6124,9 @@
     <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6436,6 +6445,9 @@
     <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -15156,14 +15168,14 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
A bunch of functions to move children through time
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="12" activeTab="19"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="12" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -12507,8 +12507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15167,8 +15167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
updates to spreadsheet for mega table run, added custom fixed costs to optimisation.py and added optimisation script for all version 2 interventions
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-67480" yWindow="-4300" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="-70560" yWindow="-4260" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -10236,8 +10236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B38" sqref="A38:XFD40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -10436,8 +10436,7 @@
         <v>0.32400000000000001</v>
       </c>
       <c r="G7" s="30">
-        <f>'Baseline year demographics'!$C$7*(1-'Baseline year demographics'!C8)</f>
-        <v>0.32400000000000001</v>
+        <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -14603,8 +14602,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updates to IYCF for mega run optimisations, target pop for wash, ORS, zinc no longer inc <1 months
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-70560" yWindow="-4260" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="-69340" yWindow="-4680" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="20" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3769,7 +3769,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="256">
   <si>
     <t>year</t>
   </si>
@@ -4868,7 +4868,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="729">
+  <cellStyleXfs count="731">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5598,8 +5598,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5809,11 +5811,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="729">
+  <cellStyles count="731">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6178,6 +6181,7 @@
     <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6541,6 +6545,7 @@
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -8558,7 +8563,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -8598,7 +8603,7 @@
       <c r="A2" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="128" t="s">
         <v>80</v>
       </c>
       <c r="C2" t="s">
@@ -8621,7 +8626,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="127"/>
+      <c r="B3" s="128"/>
       <c r="C3" t="s">
         <v>190</v>
       </c>
@@ -8643,7 +8648,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="127"/>
+      <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>200</v>
       </c>
@@ -8670,7 +8675,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="128" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8680,20 +8685,20 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="E5" s="73">
-        <v>3.07</v>
+        <v>1</v>
       </c>
       <c r="F5" s="73">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G5" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H5" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="127"/>
+      <c r="B6" s="128"/>
       <c r="C6" t="s">
         <v>190</v>
       </c>
@@ -8701,20 +8706,20 @@
         <v>2.17</v>
       </c>
       <c r="E6" s="73">
-        <v>2.48</v>
+        <v>1</v>
       </c>
       <c r="F6" s="73">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G6" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H6" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="127"/>
+      <c r="B7" s="128"/>
       <c r="C7" t="s">
         <v>200</v>
       </c>
@@ -8723,24 +8728,21 @@
         <v>1.0246950765959599</v>
       </c>
       <c r="E7" s="73">
-        <f>E17^(1/3)</f>
-        <v>1.0163963568148535</v>
+        <v>1</v>
       </c>
       <c r="F7" s="73">
-        <f>F17^(1/4)</f>
-        <v>1.0122722344290394</v>
+        <v>1</v>
       </c>
       <c r="G7" s="73">
-        <f t="shared" ref="G7:H7" si="1">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H7" s="73">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H7" si="1">H17^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="127" t="s">
+      <c r="B8" s="128" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8753,17 +8755,17 @@
         <v>1.5</v>
       </c>
       <c r="F8" s="73">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="G8" s="73">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="H8" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="127"/>
+      <c r="B9" s="128"/>
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -8774,17 +8776,17 @@
         <v>1.5</v>
       </c>
       <c r="F9" s="73">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="G9" s="73">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H9" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="127"/>
+      <c r="B10" s="128"/>
       <c r="C10" t="s">
         <v>200</v>
       </c>
@@ -8796,20 +8798,18 @@
         <v>1.0163963568148535</v>
       </c>
       <c r="F10" s="73">
-        <f>F17^(1/4)</f>
-        <v>1.0122722344290394</v>
+        <v>1</v>
       </c>
       <c r="G10" s="73">
-        <f t="shared" ref="G10:H10" si="2">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H10" s="73">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H10" si="2">H17^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="127" t="s">
+      <c r="B11" s="128" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8825,14 +8825,14 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G11" s="73">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="H11" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="127"/>
+      <c r="B12" s="128"/>
       <c r="C12" t="s">
         <v>190</v>
       </c>
@@ -8846,14 +8846,14 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G12" s="73">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H12" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="127"/>
+      <c r="B13" s="128"/>
       <c r="C13" t="s">
         <v>200</v>
       </c>
@@ -8868,16 +8868,15 @@
         <v>1.0122722344290394</v>
       </c>
       <c r="G13" s="73">
-        <f t="shared" ref="G13:H13" si="3">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H13" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="H13" si="3">H17^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="127" t="s">
+      <c r="B14" s="128" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8900,7 +8899,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="127"/>
+      <c r="B15" s="128"/>
       <c r="C15" t="s">
         <v>190</v>
       </c>
@@ -8921,7 +8920,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="127"/>
+      <c r="B16" s="128"/>
       <c r="C16" t="s">
         <v>200</v>
       </c>
@@ -8977,7 +8976,7 @@
       <c r="A19" s="77" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="127" t="s">
+      <c r="B19" s="128" t="s">
         <v>80</v>
       </c>
       <c r="C19" t="s">
@@ -8990,17 +8989,17 @@
         <v>1</v>
       </c>
       <c r="F19" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G19" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H19" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="127"/>
+      <c r="B20" s="128"/>
       <c r="C20" t="s">
         <v>190</v>
       </c>
@@ -9011,17 +9010,17 @@
         <v>1</v>
       </c>
       <c r="F20" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G20" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H20" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="127"/>
+      <c r="B21" s="128"/>
       <c r="C21" t="s">
         <v>200</v>
       </c>
@@ -9030,24 +9029,21 @@
         <v>1.0098057976734853</v>
       </c>
       <c r="E21" s="73">
-        <f t="shared" ref="E21:H21" si="5">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F21" s="73">
-        <f t="shared" si="5"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G21" s="73">
-        <f t="shared" si="5"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H21" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H21" si="5">H34^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="127" t="s">
+      <c r="B22" s="128" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -9060,17 +9056,17 @@
         <v>1</v>
       </c>
       <c r="F22" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G22" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H22" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="127"/>
+      <c r="B23" s="128"/>
       <c r="C23" t="s">
         <v>190</v>
       </c>
@@ -9081,43 +9077,39 @@
         <v>1</v>
       </c>
       <c r="F23" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G23" s="73">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H23" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="127"/>
+      <c r="B24" s="128"/>
       <c r="C24" t="s">
         <v>200</v>
       </c>
       <c r="D24" s="73">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E24" s="73">
-        <f t="shared" ref="E24:H24" si="6">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F24" s="73">
-        <f t="shared" si="6"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G24" s="73">
-        <f t="shared" si="6"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H24" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H24" si="6">H34^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="127" t="s">
+      <c r="B25" s="128" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -9130,17 +9122,17 @@
         <v>1</v>
       </c>
       <c r="F25" s="73">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="73">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H25" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="127"/>
+      <c r="B26" s="128"/>
       <c r="C26" t="s">
         <v>190</v>
       </c>
@@ -9151,43 +9143,39 @@
         <v>1</v>
       </c>
       <c r="F26" s="73">
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="G26" s="73">
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="H26" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="127"/>
+      <c r="B27" s="128"/>
       <c r="C27" t="s">
         <v>200</v>
       </c>
       <c r="D27" s="73">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E27" s="73">
-        <f t="shared" ref="E27:H27" si="7">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F27" s="73">
-        <f t="shared" si="7"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G27" s="73">
-        <f t="shared" si="7"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H27" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="H27" si="7">H34^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="127" t="s">
+      <c r="B28" s="128" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -9203,14 +9191,14 @@
         <v>2</v>
       </c>
       <c r="G28" s="73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="127"/>
+      <c r="B29" s="128"/>
       <c r="C29" t="s">
         <v>190</v>
       </c>
@@ -9224,40 +9212,36 @@
         <v>1.9</v>
       </c>
       <c r="G29" s="73">
-        <v>1.9</v>
+        <v>1</v>
       </c>
       <c r="H29" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="127"/>
+      <c r="B30" s="128"/>
       <c r="C30" t="s">
         <v>200</v>
       </c>
       <c r="D30" s="73">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E30" s="73">
-        <f t="shared" ref="E30:H30" si="8">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F30" s="73">
-        <f t="shared" si="8"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G30" s="73">
-        <f t="shared" si="8"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H30" s="73">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="H30" si="8">H34^(1/5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="127" t="s">
+      <c r="B31" s="128" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9280,7 +9264,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="127"/>
+      <c r="B32" s="128"/>
       <c r="C32" t="s">
         <v>190</v>
       </c>
@@ -9301,28 +9285,23 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="127"/>
+      <c r="B33" s="128"/>
       <c r="C33" t="s">
         <v>200</v>
       </c>
       <c r="D33" s="73">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E33" s="73">
-        <f t="shared" ref="E33:H33" si="9">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F33" s="73">
-        <f t="shared" si="9"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G33" s="73">
-        <f t="shared" si="9"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H33" s="73">
-        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -9353,7 +9332,7 @@
       <c r="A36" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="B36" s="127" t="s">
+      <c r="B36" s="128" t="s">
         <v>80</v>
       </c>
       <c r="C36" t="s">
@@ -9366,17 +9345,17 @@
         <v>1</v>
       </c>
       <c r="F36" s="73">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G36" s="73">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H36" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="127"/>
+      <c r="B37" s="128"/>
       <c r="C37" t="s">
         <v>190</v>
       </c>
@@ -9387,17 +9366,17 @@
         <v>1</v>
       </c>
       <c r="F37" s="73">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G37" s="73">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H37" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="127"/>
+      <c r="B38" s="128"/>
       <c r="C38" t="s">
         <v>200</v>
       </c>
@@ -9408,17 +9387,17 @@
         <v>1</v>
       </c>
       <c r="F38" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G38" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H38" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="127" t="s">
+      <c r="B39" s="128" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9431,17 +9410,17 @@
         <v>1</v>
       </c>
       <c r="F39" s="73">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G39" s="73">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H39" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="B40" s="127"/>
+      <c r="B40" s="128"/>
       <c r="C40" t="s">
         <v>190</v>
       </c>
@@ -9452,17 +9431,17 @@
         <v>1</v>
       </c>
       <c r="F40" s="73">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G40" s="73">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H40" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="127"/>
+      <c r="B41" s="128"/>
       <c r="C41" t="s">
         <v>200</v>
       </c>
@@ -9473,17 +9452,17 @@
         <v>1</v>
       </c>
       <c r="F41" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G41" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H41" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="127" t="s">
+      <c r="B42" s="128" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9496,17 +9475,17 @@
         <v>1</v>
       </c>
       <c r="F42" s="73">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G42" s="73">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H42" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="B43" s="127"/>
+      <c r="B43" s="128"/>
       <c r="C43" t="s">
         <v>190</v>
       </c>
@@ -9517,17 +9496,17 @@
         <v>1</v>
       </c>
       <c r="F43" s="73">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G43" s="73">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H43" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="B44" s="127"/>
+      <c r="B44" s="128"/>
       <c r="C44" t="s">
         <v>200</v>
       </c>
@@ -9538,17 +9517,17 @@
         <v>1</v>
       </c>
       <c r="F44" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G44" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H44" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="B45" s="127" t="s">
+      <c r="B45" s="128" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9571,7 +9550,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="B46" s="127"/>
+      <c r="B46" s="128"/>
       <c r="C46" t="s">
         <v>190</v>
       </c>
@@ -9592,7 +9571,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="B47" s="127"/>
+      <c r="B47" s="128"/>
       <c r="C47" t="s">
         <v>200</v>
       </c>
@@ -9603,17 +9582,17 @@
         <v>1</v>
       </c>
       <c r="F47" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G47" s="73">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H47" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="127" t="s">
+      <c r="B48" s="128" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9636,7 +9615,7 @@
       </c>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="127"/>
+      <c r="B49" s="128"/>
       <c r="C49" t="s">
         <v>190</v>
       </c>
@@ -9657,7 +9636,7 @@
       </c>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="127"/>
+      <c r="B50" s="128"/>
       <c r="C50" t="s">
         <v>200</v>
       </c>
@@ -9733,7 +9712,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -9777,7 +9756,9 @@
         <v>6</v>
       </c>
       <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
+      <c r="D3" s="96" t="s">
+        <v>201</v>
+      </c>
       <c r="E3" s="97"/>
     </row>
     <row r="4" spans="1:5">
@@ -9786,7 +9767,9 @@
         <v>7</v>
       </c>
       <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
+      <c r="D4" s="96" t="s">
+        <v>201</v>
+      </c>
       <c r="E4" s="97"/>
     </row>
     <row r="5" spans="1:5">
@@ -9794,9 +9777,7 @@
       <c r="B5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="96" t="s">
-        <v>201</v>
-      </c>
+      <c r="C5" s="96"/>
       <c r="D5" s="96" t="s">
         <v>201</v>
       </c>
@@ -9808,7 +9789,9 @@
         <v>9</v>
       </c>
       <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
+      <c r="D6" s="127" t="s">
+        <v>201</v>
+      </c>
       <c r="E6" s="97"/>
     </row>
     <row r="7" spans="1:5">
@@ -9863,12 +9846,8 @@
       <c r="B13" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="D13" s="96" t="s">
-        <v>201</v>
-      </c>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="97"/>
     </row>
     <row r="14" spans="1:5">
@@ -9887,12 +9866,8 @@
       <c r="B16" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="93" t="s">
-        <v>201</v>
-      </c>
-      <c r="D16" s="93" t="s">
-        <v>201</v>
-      </c>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="94"/>
     </row>
     <row r="17" spans="1:5">
@@ -9900,12 +9875,8 @@
       <c r="B17" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="D17" s="96" t="s">
-        <v>201</v>
-      </c>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="97"/>
     </row>
     <row r="18" spans="1:5">
@@ -10236,8 +10207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -14602,8 +14573,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -14752,13 +14723,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G6" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.36</v>
+      </c>
+      <c r="G6" s="61">
+        <v>0.36</v>
       </c>
       <c r="H6" s="62">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -14778,7 +14749,7 @@
         <v>0.62</v>
       </c>
       <c r="H7" s="61">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -14795,13 +14766,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="61">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G8" s="62">
-        <v>0.33500000000000002</v>
+        <v>0.36</v>
+      </c>
+      <c r="G8" s="61">
+        <v>0.36</v>
       </c>
       <c r="H8" s="62">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -14821,7 +14792,7 @@
         <v>0.62</v>
       </c>
       <c r="H9" s="61">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -14847,7 +14818,7 @@
         <v>0.32</v>
       </c>
       <c r="H10" s="62">
-        <v>0.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -14867,7 +14838,7 @@
         <v>0.62</v>
       </c>
       <c r="H11" s="61">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -14890,7 +14861,7 @@
         <v>0.32</v>
       </c>
       <c r="H12" s="62">
-        <v>0.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -14910,7 +14881,7 @@
         <v>0.62</v>
       </c>
       <c r="H13" s="61">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -14936,7 +14907,7 @@
         <v>0.04</v>
       </c>
       <c r="H14" s="62">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -14956,7 +14927,7 @@
         <v>0.62</v>
       </c>
       <c r="H15" s="61">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -14979,7 +14950,7 @@
         <v>0.04</v>
       </c>
       <c r="H16" s="62">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -14999,7 +14970,7 @@
         <v>0.62</v>
       </c>
       <c r="H17" s="61">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -15314,7 +15285,7 @@
         <v>120</v>
       </c>
       <c r="D31" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" s="12">
         <v>1</v>
@@ -15334,7 +15305,7 @@
         <v>67</v>
       </c>
       <c r="D32" s="12">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="E32" s="12">
         <v>0.69</v>
@@ -15355,7 +15326,7 @@
         <v>68</v>
       </c>
       <c r="D33" s="12">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="E33" s="12">
         <v>0.69</v>
@@ -15381,7 +15352,7 @@
         <v>120</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -15401,7 +15372,7 @@
         <v>67</v>
       </c>
       <c r="D35" s="12">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="E35" s="12">
         <v>0.36</v>
@@ -15422,7 +15393,7 @@
         <v>68</v>
       </c>
       <c r="D36" s="12">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="E36" s="12">
         <v>0.36</v>
@@ -15448,7 +15419,7 @@
         <v>120</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -15468,7 +15439,7 @@
         <v>67</v>
       </c>
       <c r="D38" s="12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E38" s="12">
         <v>0.2</v>
@@ -15489,7 +15460,7 @@
         <v>68</v>
       </c>
       <c r="D39" s="12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E39" s="12">
         <v>0.2</v>
@@ -15515,7 +15486,7 @@
         <v>120</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -15535,7 +15506,7 @@
         <v>67</v>
       </c>
       <c r="D41" s="12">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="E41" s="12">
         <v>0.48</v>
@@ -15556,7 +15527,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="12">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="E42" s="12">
         <v>0.48</v>
@@ -15582,7 +15553,7 @@
         <v>120</v>
       </c>
       <c r="D43" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="12">
         <v>1</v>
@@ -15602,7 +15573,7 @@
         <v>67</v>
       </c>
       <c r="D44" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E44" s="12">
         <v>0.5</v>
@@ -15622,7 +15593,7 @@
         <v>68</v>
       </c>
       <c r="D45" s="12">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="E45" s="12">
         <v>0.65</v>
@@ -15714,7 +15685,7 @@
         <v>120</v>
       </c>
       <c r="D49" s="12">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="E49" s="12">
         <v>0.88</v>
@@ -15734,7 +15705,7 @@
         <v>67</v>
       </c>
       <c r="D50" s="12">
-        <v>0.93</v>
+        <v>0</v>
       </c>
       <c r="E50" s="12">
         <v>0.93</v>
@@ -15760,7 +15731,7 @@
         <v>120</v>
       </c>
       <c r="D51" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" s="12">
         <v>1</v>
@@ -15780,7 +15751,7 @@
         <v>67</v>
       </c>
       <c r="D52" s="12">
-        <v>0.86</v>
+        <v>0</v>
       </c>
       <c r="E52" s="12">
         <v>0.86</v>
@@ -16222,7 +16193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -19063,7 +19034,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A75" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed neonatal diarrhea in interventions for children tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-69340" yWindow="-4680" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="20" activeTab="19"/>
+    <workbookView xWindow="-69340" yWindow="-4680" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3769,7 +3769,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="256">
   <si>
     <t>year</t>
   </si>
@@ -4677,7 +4677,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4747,6 +4747,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4868,7 +4880,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="731">
+  <cellStyleXfs count="749">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5600,8 +5612,26 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5815,8 +5845,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="731">
+  <cellStyles count="749">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6182,6 +6216,15 @@
     <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6546,6 +6589,15 @@
     <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -14571,10 +14623,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -15208,17 +15260,17 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" t="s">
+      <c r="A28" s="129" t="s">
         <v>245</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="130" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D28" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="12">
         <v>1</v>
@@ -15234,11 +15286,13 @@
       </c>
     </row>
     <row r="29" spans="1:9">
+      <c r="A29" s="129"/>
+      <c r="B29" s="129"/>
       <c r="C29" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="12">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="E29" s="12">
         <v>0.17</v>
@@ -15254,12 +15308,13 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="4"/>
+      <c r="A30" s="129"/>
+      <c r="B30" s="130"/>
       <c r="C30" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="12">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="E30" s="12">
         <v>0.17</v>
@@ -15275,10 +15330,10 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" t="s">
+      <c r="A31" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="130" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -15301,6 +15356,8 @@
       </c>
     </row>
     <row r="32" spans="1:9">
+      <c r="A32" s="129"/>
+      <c r="B32" s="129"/>
       <c r="C32" t="s">
         <v>67</v>
       </c>
@@ -15321,7 +15378,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="4"/>
+      <c r="A33" s="129"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="4" t="s">
         <v>68</v>
       </c>
@@ -15342,10 +15400,10 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" t="s">
+      <c r="A34" s="129" t="s">
         <v>247</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="130" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -15368,6 +15426,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
+      <c r="A35" s="129"/>
+      <c r="B35" s="129"/>
       <c r="C35" t="s">
         <v>67</v>
       </c>
@@ -15388,7 +15448,8 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="B36" s="4"/>
+      <c r="A36" s="129"/>
+      <c r="B36" s="130"/>
       <c r="C36" s="4" t="s">
         <v>68</v>
       </c>
@@ -15409,10 +15470,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" t="s">
+      <c r="A37" s="129" t="s">
         <v>248</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="130" t="s">
         <v>28</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -15435,6 +15496,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
+      <c r="A38" s="129"/>
+      <c r="B38" s="129"/>
       <c r="C38" t="s">
         <v>67</v>
       </c>
@@ -15455,7 +15518,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="4"/>
+      <c r="A39" s="129"/>
+      <c r="B39" s="130"/>
       <c r="C39" s="4" t="s">
         <v>68</v>
       </c>
@@ -15476,10 +15540,10 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" t="s">
+      <c r="A40" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="130" t="s">
         <v>28</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -15502,6 +15566,8 @@
       </c>
     </row>
     <row r="41" spans="1:8">
+      <c r="A41" s="129"/>
+      <c r="B41" s="129"/>
       <c r="C41" t="s">
         <v>67</v>
       </c>
@@ -15522,7 +15588,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="4"/>
+      <c r="A42" s="129"/>
+      <c r="B42" s="130"/>
       <c r="C42" s="4" t="s">
         <v>68</v>
       </c>
@@ -15543,77 +15610,81 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>28</v>
+      <c r="A43" s="131" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" s="131" t="s">
+        <v>11</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D43" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8">
+      <c r="A44" s="131"/>
+      <c r="B44" s="131"/>
       <c r="C44" t="s">
         <v>67</v>
       </c>
       <c r="D44" s="12">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="E44" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F44" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G44" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H44" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
+      <c r="A45" s="131"/>
+      <c r="B45" s="132"/>
       <c r="C45" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="12">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="E45" s="12">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="F45" s="12">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="G45" s="12">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="H45" s="12">
-        <v>0.65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>172</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>30</v>
+      <c r="A46" s="131" t="s">
+        <v>246</v>
+      </c>
+      <c r="B46" s="131" t="s">
+        <v>11</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>120</v>
@@ -15622,149 +15693,751 @@
         <v>1</v>
       </c>
       <c r="E46" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8">
+      <c r="A47" s="131"/>
+      <c r="B47" s="131"/>
       <c r="C47" t="s">
         <v>67</v>
       </c>
       <c r="D47" s="12">
-        <v>0.49</v>
+        <v>0.69</v>
       </c>
       <c r="E47" s="12">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="F47" s="12">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="G47" s="12">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="H47" s="12">
-        <v>0.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8">
+      <c r="A48" s="131"/>
+      <c r="B48" s="132"/>
       <c r="C48" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D48" s="12">
-        <v>0.52</v>
+        <v>0.69</v>
       </c>
       <c r="E48" s="12">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="F48" s="12">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="G48" s="12">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="H48" s="12">
-        <v>0.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" t="s">
-        <v>250</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>28</v>
+      <c r="A49" s="131" t="s">
+        <v>247</v>
+      </c>
+      <c r="B49" s="131" t="s">
+        <v>11</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="12">
-        <v>0</v>
-      </c>
-      <c r="E49" s="12">
-        <v>0.88</v>
-      </c>
-      <c r="F49" s="12">
-        <v>0.88</v>
-      </c>
-      <c r="G49" s="12">
-        <v>0.88</v>
-      </c>
-      <c r="H49" s="12">
-        <v>0.88</v>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8">
+      <c r="A50" s="131"/>
+      <c r="B50" s="131"/>
       <c r="C50" t="s">
         <v>67</v>
       </c>
       <c r="D50" s="12">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="E50" s="12">
+        <v>0</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0</v>
+      </c>
+      <c r="H50" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="131"/>
+      <c r="B51" s="132"/>
+      <c r="C51" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="E51" s="12">
+        <v>0</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0</v>
+      </c>
+      <c r="H51" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="131" t="s">
+        <v>248</v>
+      </c>
+      <c r="B52" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="131"/>
+      <c r="B53" s="131"/>
+      <c r="C53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E53" s="12">
+        <v>0</v>
+      </c>
+      <c r="F53" s="12">
+        <v>0</v>
+      </c>
+      <c r="G53" s="12">
+        <v>0</v>
+      </c>
+      <c r="H53" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="131"/>
+      <c r="B54" s="132"/>
+      <c r="C54" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0</v>
+      </c>
+      <c r="H54" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="131" t="s">
+        <v>249</v>
+      </c>
+      <c r="B55" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="131"/>
+      <c r="B56" s="131"/>
+      <c r="C56" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="E56" s="12">
+        <v>0</v>
+      </c>
+      <c r="F56" s="12">
+        <v>0</v>
+      </c>
+      <c r="G56" s="12">
+        <v>0</v>
+      </c>
+      <c r="H56" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="131"/>
+      <c r="B57" s="132"/>
+      <c r="C57" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="E57" s="12">
+        <v>0</v>
+      </c>
+      <c r="F57" s="12">
+        <v>0</v>
+      </c>
+      <c r="G57" s="12">
+        <v>0</v>
+      </c>
+      <c r="H57" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="129" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="130" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0</v>
+      </c>
+      <c r="E58" s="12">
+        <v>1</v>
+      </c>
+      <c r="F58" s="12">
+        <v>1</v>
+      </c>
+      <c r="G58" s="12">
+        <v>1</v>
+      </c>
+      <c r="H58" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="129"/>
+      <c r="B59" s="129"/>
+      <c r="C59" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="12">
+        <v>0</v>
+      </c>
+      <c r="E59" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F59" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G59" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H59" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="129"/>
+      <c r="B60" s="129"/>
+      <c r="C60" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" s="12">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="F60" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="G60" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="H60" s="12">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="129" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" s="130" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="12">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12">
+        <v>1</v>
+      </c>
+      <c r="F61" s="12">
+        <v>1</v>
+      </c>
+      <c r="G61" s="12">
+        <v>1</v>
+      </c>
+      <c r="H61" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="129"/>
+      <c r="B62" s="129"/>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" s="12">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="F62" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="G62" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="H62" s="12">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="129"/>
+      <c r="B63" s="129"/>
+      <c r="C63" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="12">
+        <v>0</v>
+      </c>
+      <c r="E63" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="F63" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="G63" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="H63" s="12">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="129" t="s">
+        <v>250</v>
+      </c>
+      <c r="B64" s="130" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="12">
+        <v>0</v>
+      </c>
+      <c r="E64" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="F64" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="G64" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="H64" s="12">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="129"/>
+      <c r="B65" s="129"/>
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="12">
+        <v>0</v>
+      </c>
+      <c r="E65" s="12">
         <v>0.93</v>
       </c>
-      <c r="F50" s="12">
+      <c r="F65" s="12">
         <v>0.93</v>
       </c>
-      <c r="G50" s="12">
+      <c r="G65" s="12">
         <v>0.93</v>
       </c>
-      <c r="H50" s="12">
+      <c r="H65" s="12">
         <v>0.93</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
+    <row r="66" spans="1:8">
+      <c r="A66" s="129" t="s">
         <v>255</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B66" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="12">
-        <v>0</v>
-      </c>
-      <c r="E51" s="12">
-        <v>1</v>
-      </c>
-      <c r="F51" s="12">
-        <v>1</v>
-      </c>
-      <c r="G51" s="12">
-        <v>1</v>
-      </c>
-      <c r="H51" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="C52" t="s">
+      <c r="D66" s="12">
+        <v>0</v>
+      </c>
+      <c r="E66" s="12">
+        <v>1</v>
+      </c>
+      <c r="F66" s="12">
+        <v>1</v>
+      </c>
+      <c r="G66" s="12">
+        <v>1</v>
+      </c>
+      <c r="H66" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="129"/>
+      <c r="B67" s="129"/>
+      <c r="C67" t="s">
         <v>67</v>
       </c>
-      <c r="D52" s="12">
-        <v>0</v>
-      </c>
-      <c r="E52" s="12">
+      <c r="D67" s="12">
+        <v>0</v>
+      </c>
+      <c r="E67" s="12">
         <v>0.86</v>
       </c>
-      <c r="F52" s="12">
+      <c r="F67" s="12">
         <v>0.86</v>
       </c>
-      <c r="G52" s="12">
+      <c r="G67" s="12">
         <v>0.86</v>
       </c>
-      <c r="H52" s="12">
+      <c r="H67" s="12">
         <v>0.86</v>
       </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="131" t="s">
+        <v>172</v>
+      </c>
+      <c r="B68" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D68" s="12">
+        <v>1</v>
+      </c>
+      <c r="E68" s="12">
+        <v>0</v>
+      </c>
+      <c r="F68" s="12">
+        <v>0</v>
+      </c>
+      <c r="G68" s="12">
+        <v>0</v>
+      </c>
+      <c r="H68" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="131"/>
+      <c r="B69" s="131"/>
+      <c r="C69" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E69" s="12">
+        <v>0</v>
+      </c>
+      <c r="F69" s="12">
+        <v>0</v>
+      </c>
+      <c r="G69" s="12">
+        <v>0</v>
+      </c>
+      <c r="H69" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="131"/>
+      <c r="B70" s="131"/>
+      <c r="C70" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="E70" s="12">
+        <v>0</v>
+      </c>
+      <c r="F70" s="12">
+        <v>0</v>
+      </c>
+      <c r="G70" s="12">
+        <v>0</v>
+      </c>
+      <c r="H70" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="131" t="s">
+        <v>172</v>
+      </c>
+      <c r="B71" s="132" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D71" s="12">
+        <v>1</v>
+      </c>
+      <c r="E71" s="12">
+        <v>0</v>
+      </c>
+      <c r="F71" s="12">
+        <v>0</v>
+      </c>
+      <c r="G71" s="12">
+        <v>0</v>
+      </c>
+      <c r="H71" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="131"/>
+      <c r="B72" s="131"/>
+      <c r="C72" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="E72" s="12">
+        <v>0</v>
+      </c>
+      <c r="F72" s="12">
+        <v>0</v>
+      </c>
+      <c r="G72" s="12">
+        <v>0</v>
+      </c>
+      <c r="H72" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="131"/>
+      <c r="B73" s="131"/>
+      <c r="C73" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="E73" s="12">
+        <v>0</v>
+      </c>
+      <c r="F73" s="12">
+        <v>0</v>
+      </c>
+      <c r="G73" s="12">
+        <v>0</v>
+      </c>
+      <c r="H73" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="131" t="s">
+        <v>250</v>
+      </c>
+      <c r="B74" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="E74" s="12">
+        <v>0</v>
+      </c>
+      <c r="F74" s="12">
+        <v>0</v>
+      </c>
+      <c r="G74" s="12">
+        <v>0</v>
+      </c>
+      <c r="H74" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="131"/>
+      <c r="B75" s="131"/>
+      <c r="C75" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D75" s="12">
+        <v>0.93</v>
+      </c>
+      <c r="E75" s="12">
+        <v>0</v>
+      </c>
+      <c r="F75" s="12">
+        <v>0</v>
+      </c>
+      <c r="G75" s="12">
+        <v>0</v>
+      </c>
+      <c r="H75" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="131" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D76" s="12">
+        <v>1</v>
+      </c>
+      <c r="E76" s="12">
+        <v>0</v>
+      </c>
+      <c r="F76" s="12">
+        <v>0</v>
+      </c>
+      <c r="G76" s="12">
+        <v>0</v>
+      </c>
+      <c r="H76" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="131"/>
+      <c r="B77" s="131"/>
+      <c r="C77" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="E77" s="12">
+        <v>0</v>
+      </c>
+      <c r="F77" s="12">
+        <v>0</v>
+      </c>
+      <c r="G77" s="12">
+        <v>0</v>
+      </c>
+      <c r="H77" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16897,8 +17570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Calculating birth and pregnancy information
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -18,23 +18,24 @@
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId4"/>
     <sheet name="Prevalence of anaemia" sheetId="29" r:id="rId5"/>
     <sheet name="Distributions" sheetId="5" r:id="rId6"/>
-    <sheet name="Birth outcomes &amp; risks" sheetId="6" r:id="rId7"/>
-    <sheet name="Relative risks" sheetId="26" r:id="rId8"/>
-    <sheet name="Odds ratios" sheetId="27" r:id="rId9"/>
-    <sheet name="IYCF package odds ratios" sheetId="32" r:id="rId10"/>
-    <sheet name="IYCF packages" sheetId="33" r:id="rId11"/>
-    <sheet name="IYCF cost &amp; coverage" sheetId="35" r:id="rId12"/>
-    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId13"/>
-    <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId14"/>
-    <sheet name="Interventions anemia" sheetId="30" r:id="rId15"/>
-    <sheet name="Interventions wasting" sheetId="31" r:id="rId16"/>
-    <sheet name="Interventions for children" sheetId="28" r:id="rId17"/>
-    <sheet name="Interventions family planning" sheetId="34" r:id="rId18"/>
-    <sheet name="Interventions target population" sheetId="21" r:id="rId19"/>
-    <sheet name="Program dependencies" sheetId="40" r:id="rId20"/>
-    <sheet name="Program areas" sheetId="36" r:id="rId21"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId22"/>
-    <sheet name="Population risk areas" sheetId="41" r:id="rId23"/>
+    <sheet name="Distribution births" sheetId="42" r:id="rId7"/>
+    <sheet name="Birth outcomes &amp; risks" sheetId="6" r:id="rId8"/>
+    <sheet name="Relative risks" sheetId="26" r:id="rId9"/>
+    <sheet name="Odds ratios" sheetId="27" r:id="rId10"/>
+    <sheet name="IYCF package odds ratios" sheetId="32" r:id="rId11"/>
+    <sheet name="IYCF packages" sheetId="33" r:id="rId12"/>
+    <sheet name="IYCF cost &amp; coverage" sheetId="35" r:id="rId13"/>
+    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId14"/>
+    <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId15"/>
+    <sheet name="Interventions anemia" sheetId="30" r:id="rId16"/>
+    <sheet name="Interventions wasting" sheetId="31" r:id="rId17"/>
+    <sheet name="Interventions for children" sheetId="28" r:id="rId18"/>
+    <sheet name="Interventions family planning" sheetId="34" r:id="rId19"/>
+    <sheet name="Interventions target population" sheetId="21" r:id="rId20"/>
+    <sheet name="Program dependencies" sheetId="40" r:id="rId21"/>
+    <sheet name="Program areas" sheetId="36" r:id="rId22"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId23"/>
+    <sheet name="Population risk areas" sheetId="41" r:id="rId24"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -3948,7 +3949,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="259">
   <si>
     <t>year</t>
   </si>
@@ -4671,6 +4672,60 @@
   </si>
   <si>
     <t>WRA 40-49 years</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>Birth age order</t>
+  </si>
+  <si>
+    <t>Less than 18 years first birth</t>
+  </si>
+  <si>
+    <t>Less than 18 years second and third births</t>
+  </si>
+  <si>
+    <t>Less than 18 years greater than third birth</t>
+  </si>
+  <si>
+    <t>18 - 34 years old first birth</t>
+  </si>
+  <si>
+    <t>18 - 34 years old second and third births</t>
+  </si>
+  <si>
+    <t>18 - 34 years old greater than third birth</t>
+  </si>
+  <si>
+    <t>35-49 years old first birth</t>
+  </si>
+  <si>
+    <t>35-49 years old second and third births</t>
+  </si>
+  <si>
+    <t>35-49 years old greater than third birth</t>
+  </si>
+  <si>
+    <t>Birth intervals</t>
+  </si>
+  <si>
+    <t>First birth</t>
+  </si>
+  <si>
+    <t>less than 18 months</t>
+  </si>
+  <si>
+    <t>18-23 months</t>
+  </si>
+  <si>
+    <t>24 months or greater</t>
   </si>
 </sst>
 </file>
@@ -4802,7 +4857,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4860,6 +4915,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5647,7 +5714,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5808,6 +5875,25 @@
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="651">
@@ -8193,6 +8279,440 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="4">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4">
+        <v>361.6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>174.7</v>
+      </c>
+      <c r="G2" s="4">
+        <v>174.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4">
+        <v>1.04</v>
+      </c>
+      <c r="D4">
+        <v>1.04</v>
+      </c>
+      <c r="E4">
+        <v>1.04</v>
+      </c>
+      <c r="F4">
+        <v>1.04</v>
+      </c>
+      <c r="G4">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <f>1/(1 + (E7-1)*(1-'Baseline year demographics'!$C$8))</f>
+        <v>0.78419071518193229</v>
+      </c>
+      <c r="F13" s="4">
+        <f>1/(1 + (F7-1)*(1-'Baseline year demographics'!$C$8))</f>
+        <v>0.78419071518193229</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <f>1 / (E$10/E$9)</f>
+        <v>0.66945606694560678</v>
+      </c>
+      <c r="F14" s="4">
+        <f>1 / (F$10/F$9)</f>
+        <v>0.66945606694560678</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" ref="E15:F16" si="0">1 / (E$10/E$9)</f>
+        <v>0.66945606694560678</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>0.66945606694560678</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.66945606694560678</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.66945606694560678</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="6">
+        <v>5.16</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5.16</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="62"/>
+      <c r="B19" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.82</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1.82</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="D21" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="E21" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="F21" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="G21" s="47">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="D23" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="E23" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="F23" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="G23" s="47">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="47">
+        <v>1</v>
+      </c>
+      <c r="D25" s="47">
+        <v>1</v>
+      </c>
+      <c r="E25" s="47">
+        <v>1</v>
+      </c>
+      <c r="F25" s="47">
+        <v>1</v>
+      </c>
+      <c r="G25" s="47">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9340,6 +9860,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9350,18 +9875,13 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -9568,7 +10088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -9765,7 +10285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
@@ -9842,7 +10362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -10113,7 +10633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -11569,7 +12089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -11660,7 +12180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -12308,7 +12828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -12515,7 +13035,656 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="21">
+        <v>3095470</v>
+      </c>
+      <c r="C2" s="22">
+        <v>15402200</v>
+      </c>
+      <c r="D2" s="22">
+        <v>8785700</v>
+      </c>
+      <c r="E2" s="22">
+        <v>13889200</v>
+      </c>
+      <c r="F2" s="22">
+        <v>12671800</v>
+      </c>
+      <c r="G2" s="22">
+        <v>9362400</v>
+      </c>
+      <c r="H2" s="23">
+        <f>D2+E2+F2+G2</f>
+        <v>44709100</v>
+      </c>
+      <c r="I2" s="24">
+        <f t="shared" ref="I2:I15" si="0">(B2 + 25.36*B2/(1000-25.36))/(1-0.13)</f>
+        <v>3650590.4685349194</v>
+      </c>
+      <c r="J2" s="25">
+        <f t="shared" ref="J2:J15" si="1">D2/H2</f>
+        <v>0.19650809343064388</v>
+      </c>
+      <c r="K2" s="23">
+        <f>H2-I2</f>
+        <v>41058509.531465083</v>
+      </c>
+      <c r="L2" s="42">
+        <v>173766200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="21">
+        <v>3071259</v>
+      </c>
+      <c r="C3" s="22">
+        <v>15629400.000000002</v>
+      </c>
+      <c r="D3" s="22">
+        <v>8937400.0000000019</v>
+      </c>
+      <c r="E3" s="22">
+        <v>14228400.000000002</v>
+      </c>
+      <c r="F3" s="22">
+        <v>12949600</v>
+      </c>
+      <c r="G3" s="22">
+        <v>9576800</v>
+      </c>
+      <c r="H3" s="23">
+        <f t="shared" ref="H3:H15" si="2">D3+E3+F3+G3</f>
+        <v>45692200</v>
+      </c>
+      <c r="I3" s="24">
+        <f t="shared" si="0"/>
+        <v>3622037.632993402</v>
+      </c>
+      <c r="J3" s="25">
+        <f t="shared" si="1"/>
+        <v>0.19560012431005733</v>
+      </c>
+      <c r="K3" s="23">
+        <f t="shared" ref="K3:K15" si="3">H3-I3</f>
+        <v>42070162.3670066</v>
+      </c>
+      <c r="L3" s="42">
+        <v>175848400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="21">
+        <v>3045241</v>
+      </c>
+      <c r="C4" s="22">
+        <v>15856600.000000002</v>
+      </c>
+      <c r="D4" s="22">
+        <v>9089100.0000000019</v>
+      </c>
+      <c r="E4" s="22">
+        <v>14567600.000000002</v>
+      </c>
+      <c r="F4" s="22">
+        <v>13227400</v>
+      </c>
+      <c r="G4" s="22">
+        <v>9791200.0000000019</v>
+      </c>
+      <c r="H4" s="23">
+        <f t="shared" si="2"/>
+        <v>46675300</v>
+      </c>
+      <c r="I4" s="24">
+        <f t="shared" si="0"/>
+        <v>3591353.7424015561</v>
+      </c>
+      <c r="J4" s="25">
+        <f t="shared" si="1"/>
+        <v>0.19473040344679096</v>
+      </c>
+      <c r="K4" s="23">
+        <f t="shared" si="3"/>
+        <v>43083946.257598445</v>
+      </c>
+      <c r="L4" s="42">
+        <v>177930600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="21">
+        <v>3017266</v>
+      </c>
+      <c r="C5" s="22">
+        <v>16083800.000000004</v>
+      </c>
+      <c r="D5" s="22">
+        <v>9240800.0000000037</v>
+      </c>
+      <c r="E5" s="22">
+        <v>14906800.000000004</v>
+      </c>
+      <c r="F5" s="22">
+        <v>13505200</v>
+      </c>
+      <c r="G5" s="22">
+        <v>10005600.000000004</v>
+      </c>
+      <c r="H5" s="23">
+        <f t="shared" si="2"/>
+        <v>47658400.000000015</v>
+      </c>
+      <c r="I5" s="24">
+        <f t="shared" si="0"/>
+        <v>3558361.8967828737</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" si="1"/>
+        <v>0.19389656387960991</v>
+      </c>
+      <c r="K5" s="23">
+        <f t="shared" si="3"/>
+        <v>44100038.10321714</v>
+      </c>
+      <c r="L5" s="42">
+        <v>180012800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="21">
+        <v>2990677</v>
+      </c>
+      <c r="C6" s="22">
+        <v>16311000.000000004</v>
+      </c>
+      <c r="D6" s="22">
+        <v>9392500.0000000037</v>
+      </c>
+      <c r="E6" s="22">
+        <v>15246000.000000004</v>
+      </c>
+      <c r="F6" s="22">
+        <v>13783000</v>
+      </c>
+      <c r="G6" s="22">
+        <v>10220000.000000004</v>
+      </c>
+      <c r="H6" s="23">
+        <f t="shared" si="2"/>
+        <v>48641500.000000015</v>
+      </c>
+      <c r="I6" s="24">
+        <f t="shared" si="0"/>
+        <v>3527004.6069471212</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" si="1"/>
+        <v>0.1930964300031866</v>
+      </c>
+      <c r="K6" s="23">
+        <f t="shared" si="3"/>
+        <v>45114495.393052891</v>
+      </c>
+      <c r="L6" s="42">
+        <v>182095000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B7" s="21">
+        <v>2962144</v>
+      </c>
+      <c r="C7" s="22">
+        <v>16190600.000000004</v>
+      </c>
+      <c r="D7" s="22">
+        <v>9004300.0000000037</v>
+      </c>
+      <c r="E7" s="22">
+        <v>15785700.000000004</v>
+      </c>
+      <c r="F7" s="22">
+        <v>13711700</v>
+      </c>
+      <c r="G7" s="22">
+        <v>10609600.000000004</v>
+      </c>
+      <c r="H7" s="23">
+        <f t="shared" si="2"/>
+        <v>49111300.000000015</v>
+      </c>
+      <c r="I7" s="24">
+        <f t="shared" si="0"/>
+        <v>3493354.6934158299</v>
+      </c>
+      <c r="J7" s="25">
+        <f t="shared" si="1"/>
+        <v>0.1833447699409301</v>
+      </c>
+      <c r="K7" s="23">
+        <f t="shared" si="3"/>
+        <v>45617945.306584187</v>
+      </c>
+      <c r="L7" s="42">
+        <v>183822800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B8" s="21">
+        <v>2931643</v>
+      </c>
+      <c r="C8" s="22">
+        <v>16070200.000000004</v>
+      </c>
+      <c r="D8" s="22">
+        <v>8616100.0000000019</v>
+      </c>
+      <c r="E8" s="22">
+        <v>16325400.000000004</v>
+      </c>
+      <c r="F8" s="22">
+        <v>13640400</v>
+      </c>
+      <c r="G8" s="22">
+        <v>10999200.000000002</v>
+      </c>
+      <c r="H8" s="23">
+        <f t="shared" si="2"/>
+        <v>49581100.000000007</v>
+      </c>
+      <c r="I8" s="24">
+        <f t="shared" si="0"/>
+        <v>3457383.8521927581</v>
+      </c>
+      <c r="J8" s="25">
+        <f t="shared" si="1"/>
+        <v>0.17377791134121673</v>
+      </c>
+      <c r="K8" s="23">
+        <f t="shared" si="3"/>
+        <v>46123716.147807248</v>
+      </c>
+      <c r="L8" s="42">
+        <v>185550600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B9" s="21">
+        <v>2899255</v>
+      </c>
+      <c r="C9" s="22">
+        <v>15949800.000000006</v>
+      </c>
+      <c r="D9" s="22">
+        <v>8227900.0000000019</v>
+      </c>
+      <c r="E9" s="22">
+        <v>16865100.000000004</v>
+      </c>
+      <c r="F9" s="22">
+        <v>13569100</v>
+      </c>
+      <c r="G9" s="22">
+        <v>11388800</v>
+      </c>
+      <c r="H9" s="23">
+        <f t="shared" si="2"/>
+        <v>50050900.000000007</v>
+      </c>
+      <c r="I9" s="24">
+        <f t="shared" si="0"/>
+        <v>3419187.609265219</v>
+      </c>
+      <c r="J9" s="25">
+        <f t="shared" si="1"/>
+        <v>0.16439065031797631</v>
+      </c>
+      <c r="K9" s="23">
+        <f t="shared" si="3"/>
+        <v>46631712.390734792</v>
+      </c>
+      <c r="L9" s="42">
+        <v>187278400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="21">
+        <v>2865008</v>
+      </c>
+      <c r="C10" s="22">
+        <v>15829400.000000006</v>
+      </c>
+      <c r="D10" s="22">
+        <v>7839700.0000000019</v>
+      </c>
+      <c r="E10" s="22">
+        <v>17404800.000000004</v>
+      </c>
+      <c r="F10" s="22">
+        <v>13497800</v>
+      </c>
+      <c r="G10" s="22">
+        <v>11778400</v>
+      </c>
+      <c r="H10" s="23">
+        <f t="shared" si="2"/>
+        <v>50520700.000000007</v>
+      </c>
+      <c r="I10" s="24">
+        <f t="shared" si="0"/>
+        <v>3378798.9859621613</v>
+      </c>
+      <c r="J10" s="25">
+        <f t="shared" si="1"/>
+        <v>0.15517797655218554</v>
+      </c>
+      <c r="K10" s="23">
+        <f t="shared" si="3"/>
+        <v>47141901.014037848</v>
+      </c>
+      <c r="L10" s="42">
+        <v>189006200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>2026</v>
+      </c>
+      <c r="B11" s="21">
+        <v>2836142</v>
+      </c>
+      <c r="C11" s="22">
+        <v>15709000.000000006</v>
+      </c>
+      <c r="D11" s="22">
+        <v>7451500.0000000019</v>
+      </c>
+      <c r="E11" s="22">
+        <v>17944500</v>
+      </c>
+      <c r="F11" s="22">
+        <v>13426500</v>
+      </c>
+      <c r="G11" s="22">
+        <v>12168000</v>
+      </c>
+      <c r="H11" s="23">
+        <f t="shared" si="2"/>
+        <v>50990500</v>
+      </c>
+      <c r="I11" s="24">
+        <f t="shared" si="0"/>
+        <v>3344756.3544830228</v>
+      </c>
+      <c r="J11" s="25">
+        <f t="shared" si="1"/>
+        <v>0.1461350643747365</v>
+      </c>
+      <c r="K11" s="23">
+        <f t="shared" si="3"/>
+        <v>47645743.645516977</v>
+      </c>
+      <c r="L11" s="42">
+        <v>190734000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>2027</v>
+      </c>
+      <c r="B12" s="21">
+        <v>2805541</v>
+      </c>
+      <c r="C12" s="22">
+        <v>15358200.000000006</v>
+      </c>
+      <c r="D12" s="22">
+        <v>7411700.0000000019</v>
+      </c>
+      <c r="E12" s="22">
+        <v>17710400</v>
+      </c>
+      <c r="F12" s="22">
+        <v>13766300</v>
+      </c>
+      <c r="G12" s="22">
+        <v>12445000</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="2"/>
+        <v>51333400</v>
+      </c>
+      <c r="I12" s="24">
+        <f t="shared" si="0"/>
+        <v>3308667.5799422786</v>
+      </c>
+      <c r="J12" s="25">
+        <f t="shared" si="1"/>
+        <v>0.14438357872262508</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="3"/>
+        <v>48024732.420057721</v>
+      </c>
+      <c r="L12" s="42">
+        <v>192287600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>2028</v>
+      </c>
+      <c r="B13" s="21">
+        <v>2773236</v>
+      </c>
+      <c r="C13" s="22">
+        <v>15007400.000000007</v>
+      </c>
+      <c r="D13" s="22">
+        <v>7371900.0000000019</v>
+      </c>
+      <c r="E13" s="22">
+        <v>17476300</v>
+      </c>
+      <c r="F13" s="22">
+        <v>14106100</v>
+      </c>
+      <c r="G13" s="22">
+        <v>12722000</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="2"/>
+        <v>51676300</v>
+      </c>
+      <c r="I13" s="24">
+        <f t="shared" si="0"/>
+        <v>3270569.2216684073</v>
+      </c>
+      <c r="J13" s="25">
+        <f t="shared" si="1"/>
+        <v>0.14265533716616713</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="3"/>
+        <v>48405730.778331593</v>
+      </c>
+      <c r="L13" s="42">
+        <v>193841200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>2029</v>
+      </c>
+      <c r="B14" s="21">
+        <v>2739273</v>
+      </c>
+      <c r="C14" s="22">
+        <v>14656600.000000007</v>
+      </c>
+      <c r="D14" s="22">
+        <v>7332100.0000000009</v>
+      </c>
+      <c r="E14" s="22">
+        <v>17242200</v>
+      </c>
+      <c r="F14" s="22">
+        <v>14445900</v>
+      </c>
+      <c r="G14" s="22">
+        <v>12999000</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="2"/>
+        <v>52019200</v>
+      </c>
+      <c r="I14" s="24">
+        <f t="shared" si="0"/>
+        <v>3230515.5289875376</v>
+      </c>
+      <c r="J14" s="25">
+        <f t="shared" si="1"/>
+        <v>0.14094988004429135</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="3"/>
+        <v>48788684.471012466</v>
+      </c>
+      <c r="L14" s="42">
+        <v>195394800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>2030</v>
+      </c>
+      <c r="B15" s="21">
+        <v>2703670</v>
+      </c>
+      <c r="C15" s="22">
+        <v>14305800.000000007</v>
+      </c>
+      <c r="D15" s="22">
+        <v>7292300.0000000009</v>
+      </c>
+      <c r="E15" s="22">
+        <v>17008100</v>
+      </c>
+      <c r="F15" s="22">
+        <v>14785700</v>
+      </c>
+      <c r="G15" s="22">
+        <v>13276000</v>
+      </c>
+      <c r="H15" s="23">
+        <f t="shared" si="2"/>
+        <v>52362100</v>
+      </c>
+      <c r="I15" s="24">
+        <f t="shared" si="0"/>
+        <v>3188527.7298968509</v>
+      </c>
+      <c r="J15" s="25">
+        <f t="shared" si="1"/>
+        <v>0.139266759736527</v>
+      </c>
+      <c r="K15" s="23">
+        <f t="shared" si="3"/>
+        <v>49173572.270103149</v>
+      </c>
+      <c r="L15" s="42">
+        <v>196948400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
@@ -14526,656 +15695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="17.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
-        <v>2017</v>
-      </c>
-      <c r="B2" s="21">
-        <v>3095470</v>
-      </c>
-      <c r="C2" s="22">
-        <v>15402200</v>
-      </c>
-      <c r="D2" s="22">
-        <v>8785700</v>
-      </c>
-      <c r="E2" s="22">
-        <v>13889200</v>
-      </c>
-      <c r="F2" s="22">
-        <v>12671800</v>
-      </c>
-      <c r="G2" s="22">
-        <v>9362400</v>
-      </c>
-      <c r="H2" s="23">
-        <f>D2+E2+F2+G2</f>
-        <v>44709100</v>
-      </c>
-      <c r="I2" s="24">
-        <f t="shared" ref="I2:I15" si="0">(B2 + 25.36*B2/(1000-25.36))/(1-0.13)</f>
-        <v>3650590.4685349194</v>
-      </c>
-      <c r="J2" s="25">
-        <f t="shared" ref="J2:J15" si="1">D2/H2</f>
-        <v>0.19650809343064388</v>
-      </c>
-      <c r="K2" s="23">
-        <f>H2-I2</f>
-        <v>41058509.531465083</v>
-      </c>
-      <c r="L2" s="42">
-        <v>173766200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>2018</v>
-      </c>
-      <c r="B3" s="21">
-        <v>3071259</v>
-      </c>
-      <c r="C3" s="22">
-        <v>15629400.000000002</v>
-      </c>
-      <c r="D3" s="22">
-        <v>8937400.0000000019</v>
-      </c>
-      <c r="E3" s="22">
-        <v>14228400.000000002</v>
-      </c>
-      <c r="F3" s="22">
-        <v>12949600</v>
-      </c>
-      <c r="G3" s="22">
-        <v>9576800</v>
-      </c>
-      <c r="H3" s="23">
-        <f t="shared" ref="H3:H15" si="2">D3+E3+F3+G3</f>
-        <v>45692200</v>
-      </c>
-      <c r="I3" s="24">
-        <f t="shared" si="0"/>
-        <v>3622037.632993402</v>
-      </c>
-      <c r="J3" s="25">
-        <f t="shared" si="1"/>
-        <v>0.19560012431005733</v>
-      </c>
-      <c r="K3" s="23">
-        <f t="shared" ref="K3:K15" si="3">H3-I3</f>
-        <v>42070162.3670066</v>
-      </c>
-      <c r="L3" s="42">
-        <v>175848400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="B4" s="21">
-        <v>3045241</v>
-      </c>
-      <c r="C4" s="22">
-        <v>15856600.000000002</v>
-      </c>
-      <c r="D4" s="22">
-        <v>9089100.0000000019</v>
-      </c>
-      <c r="E4" s="22">
-        <v>14567600.000000002</v>
-      </c>
-      <c r="F4" s="22">
-        <v>13227400</v>
-      </c>
-      <c r="G4" s="22">
-        <v>9791200.0000000019</v>
-      </c>
-      <c r="H4" s="23">
-        <f t="shared" si="2"/>
-        <v>46675300</v>
-      </c>
-      <c r="I4" s="24">
-        <f t="shared" si="0"/>
-        <v>3591353.7424015561</v>
-      </c>
-      <c r="J4" s="25">
-        <f t="shared" si="1"/>
-        <v>0.19473040344679096</v>
-      </c>
-      <c r="K4" s="23">
-        <f t="shared" si="3"/>
-        <v>43083946.257598445</v>
-      </c>
-      <c r="L4" s="42">
-        <v>177930600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>2020</v>
-      </c>
-      <c r="B5" s="21">
-        <v>3017266</v>
-      </c>
-      <c r="C5" s="22">
-        <v>16083800.000000004</v>
-      </c>
-      <c r="D5" s="22">
-        <v>9240800.0000000037</v>
-      </c>
-      <c r="E5" s="22">
-        <v>14906800.000000004</v>
-      </c>
-      <c r="F5" s="22">
-        <v>13505200</v>
-      </c>
-      <c r="G5" s="22">
-        <v>10005600.000000004</v>
-      </c>
-      <c r="H5" s="23">
-        <f t="shared" si="2"/>
-        <v>47658400.000000015</v>
-      </c>
-      <c r="I5" s="24">
-        <f t="shared" si="0"/>
-        <v>3558361.8967828737</v>
-      </c>
-      <c r="J5" s="25">
-        <f t="shared" si="1"/>
-        <v>0.19389656387960991</v>
-      </c>
-      <c r="K5" s="23">
-        <f t="shared" si="3"/>
-        <v>44100038.10321714</v>
-      </c>
-      <c r="L5" s="42">
-        <v>180012800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B6" s="21">
-        <v>2990677</v>
-      </c>
-      <c r="C6" s="22">
-        <v>16311000.000000004</v>
-      </c>
-      <c r="D6" s="22">
-        <v>9392500.0000000037</v>
-      </c>
-      <c r="E6" s="22">
-        <v>15246000.000000004</v>
-      </c>
-      <c r="F6" s="22">
-        <v>13783000</v>
-      </c>
-      <c r="G6" s="22">
-        <v>10220000.000000004</v>
-      </c>
-      <c r="H6" s="23">
-        <f t="shared" si="2"/>
-        <v>48641500.000000015</v>
-      </c>
-      <c r="I6" s="24">
-        <f t="shared" si="0"/>
-        <v>3527004.6069471212</v>
-      </c>
-      <c r="J6" s="25">
-        <f t="shared" si="1"/>
-        <v>0.1930964300031866</v>
-      </c>
-      <c r="K6" s="23">
-        <f t="shared" si="3"/>
-        <v>45114495.393052891</v>
-      </c>
-      <c r="L6" s="42">
-        <v>182095000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B7" s="21">
-        <v>2962144</v>
-      </c>
-      <c r="C7" s="22">
-        <v>16190600.000000004</v>
-      </c>
-      <c r="D7" s="22">
-        <v>9004300.0000000037</v>
-      </c>
-      <c r="E7" s="22">
-        <v>15785700.000000004</v>
-      </c>
-      <c r="F7" s="22">
-        <v>13711700</v>
-      </c>
-      <c r="G7" s="22">
-        <v>10609600.000000004</v>
-      </c>
-      <c r="H7" s="23">
-        <f t="shared" si="2"/>
-        <v>49111300.000000015</v>
-      </c>
-      <c r="I7" s="24">
-        <f t="shared" si="0"/>
-        <v>3493354.6934158299</v>
-      </c>
-      <c r="J7" s="25">
-        <f t="shared" si="1"/>
-        <v>0.1833447699409301</v>
-      </c>
-      <c r="K7" s="23">
-        <f t="shared" si="3"/>
-        <v>45617945.306584187</v>
-      </c>
-      <c r="L7" s="42">
-        <v>183822800</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
-        <v>2023</v>
-      </c>
-      <c r="B8" s="21">
-        <v>2931643</v>
-      </c>
-      <c r="C8" s="22">
-        <v>16070200.000000004</v>
-      </c>
-      <c r="D8" s="22">
-        <v>8616100.0000000019</v>
-      </c>
-      <c r="E8" s="22">
-        <v>16325400.000000004</v>
-      </c>
-      <c r="F8" s="22">
-        <v>13640400</v>
-      </c>
-      <c r="G8" s="22">
-        <v>10999200.000000002</v>
-      </c>
-      <c r="H8" s="23">
-        <f t="shared" si="2"/>
-        <v>49581100.000000007</v>
-      </c>
-      <c r="I8" s="24">
-        <f t="shared" si="0"/>
-        <v>3457383.8521927581</v>
-      </c>
-      <c r="J8" s="25">
-        <f t="shared" si="1"/>
-        <v>0.17377791134121673</v>
-      </c>
-      <c r="K8" s="23">
-        <f t="shared" si="3"/>
-        <v>46123716.147807248</v>
-      </c>
-      <c r="L8" s="42">
-        <v>185550600</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
-        <v>2024</v>
-      </c>
-      <c r="B9" s="21">
-        <v>2899255</v>
-      </c>
-      <c r="C9" s="22">
-        <v>15949800.000000006</v>
-      </c>
-      <c r="D9" s="22">
-        <v>8227900.0000000019</v>
-      </c>
-      <c r="E9" s="22">
-        <v>16865100.000000004</v>
-      </c>
-      <c r="F9" s="22">
-        <v>13569100</v>
-      </c>
-      <c r="G9" s="22">
-        <v>11388800</v>
-      </c>
-      <c r="H9" s="23">
-        <f t="shared" si="2"/>
-        <v>50050900.000000007</v>
-      </c>
-      <c r="I9" s="24">
-        <f t="shared" si="0"/>
-        <v>3419187.609265219</v>
-      </c>
-      <c r="J9" s="25">
-        <f t="shared" si="1"/>
-        <v>0.16439065031797631</v>
-      </c>
-      <c r="K9" s="23">
-        <f t="shared" si="3"/>
-        <v>46631712.390734792</v>
-      </c>
-      <c r="L9" s="42">
-        <v>187278400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
-        <v>2025</v>
-      </c>
-      <c r="B10" s="21">
-        <v>2865008</v>
-      </c>
-      <c r="C10" s="22">
-        <v>15829400.000000006</v>
-      </c>
-      <c r="D10" s="22">
-        <v>7839700.0000000019</v>
-      </c>
-      <c r="E10" s="22">
-        <v>17404800.000000004</v>
-      </c>
-      <c r="F10" s="22">
-        <v>13497800</v>
-      </c>
-      <c r="G10" s="22">
-        <v>11778400</v>
-      </c>
-      <c r="H10" s="23">
-        <f t="shared" si="2"/>
-        <v>50520700.000000007</v>
-      </c>
-      <c r="I10" s="24">
-        <f t="shared" si="0"/>
-        <v>3378798.9859621613</v>
-      </c>
-      <c r="J10" s="25">
-        <f t="shared" si="1"/>
-        <v>0.15517797655218554</v>
-      </c>
-      <c r="K10" s="23">
-        <f t="shared" si="3"/>
-        <v>47141901.014037848</v>
-      </c>
-      <c r="L10" s="42">
-        <v>189006200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
-        <v>2026</v>
-      </c>
-      <c r="B11" s="21">
-        <v>2836142</v>
-      </c>
-      <c r="C11" s="22">
-        <v>15709000.000000006</v>
-      </c>
-      <c r="D11" s="22">
-        <v>7451500.0000000019</v>
-      </c>
-      <c r="E11" s="22">
-        <v>17944500</v>
-      </c>
-      <c r="F11" s="22">
-        <v>13426500</v>
-      </c>
-      <c r="G11" s="22">
-        <v>12168000</v>
-      </c>
-      <c r="H11" s="23">
-        <f t="shared" si="2"/>
-        <v>50990500</v>
-      </c>
-      <c r="I11" s="24">
-        <f t="shared" si="0"/>
-        <v>3344756.3544830228</v>
-      </c>
-      <c r="J11" s="25">
-        <f t="shared" si="1"/>
-        <v>0.1461350643747365</v>
-      </c>
-      <c r="K11" s="23">
-        <f t="shared" si="3"/>
-        <v>47645743.645516977</v>
-      </c>
-      <c r="L11" s="42">
-        <v>190734000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
-        <v>2027</v>
-      </c>
-      <c r="B12" s="21">
-        <v>2805541</v>
-      </c>
-      <c r="C12" s="22">
-        <v>15358200.000000006</v>
-      </c>
-      <c r="D12" s="22">
-        <v>7411700.0000000019</v>
-      </c>
-      <c r="E12" s="22">
-        <v>17710400</v>
-      </c>
-      <c r="F12" s="22">
-        <v>13766300</v>
-      </c>
-      <c r="G12" s="22">
-        <v>12445000</v>
-      </c>
-      <c r="H12" s="23">
-        <f t="shared" si="2"/>
-        <v>51333400</v>
-      </c>
-      <c r="I12" s="24">
-        <f t="shared" si="0"/>
-        <v>3308667.5799422786</v>
-      </c>
-      <c r="J12" s="25">
-        <f t="shared" si="1"/>
-        <v>0.14438357872262508</v>
-      </c>
-      <c r="K12" s="23">
-        <f t="shared" si="3"/>
-        <v>48024732.420057721</v>
-      </c>
-      <c r="L12" s="42">
-        <v>192287600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
-        <v>2028</v>
-      </c>
-      <c r="B13" s="21">
-        <v>2773236</v>
-      </c>
-      <c r="C13" s="22">
-        <v>15007400.000000007</v>
-      </c>
-      <c r="D13" s="22">
-        <v>7371900.0000000019</v>
-      </c>
-      <c r="E13" s="22">
-        <v>17476300</v>
-      </c>
-      <c r="F13" s="22">
-        <v>14106100</v>
-      </c>
-      <c r="G13" s="22">
-        <v>12722000</v>
-      </c>
-      <c r="H13" s="23">
-        <f t="shared" si="2"/>
-        <v>51676300</v>
-      </c>
-      <c r="I13" s="24">
-        <f t="shared" si="0"/>
-        <v>3270569.2216684073</v>
-      </c>
-      <c r="J13" s="25">
-        <f t="shared" si="1"/>
-        <v>0.14265533716616713</v>
-      </c>
-      <c r="K13" s="23">
-        <f t="shared" si="3"/>
-        <v>48405730.778331593</v>
-      </c>
-      <c r="L13" s="42">
-        <v>193841200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
-        <v>2029</v>
-      </c>
-      <c r="B14" s="21">
-        <v>2739273</v>
-      </c>
-      <c r="C14" s="22">
-        <v>14656600.000000007</v>
-      </c>
-      <c r="D14" s="22">
-        <v>7332100.0000000009</v>
-      </c>
-      <c r="E14" s="22">
-        <v>17242200</v>
-      </c>
-      <c r="F14" s="22">
-        <v>14445900</v>
-      </c>
-      <c r="G14" s="22">
-        <v>12999000</v>
-      </c>
-      <c r="H14" s="23">
-        <f t="shared" si="2"/>
-        <v>52019200</v>
-      </c>
-      <c r="I14" s="24">
-        <f t="shared" si="0"/>
-        <v>3230515.5289875376</v>
-      </c>
-      <c r="J14" s="25">
-        <f t="shared" si="1"/>
-        <v>0.14094988004429135</v>
-      </c>
-      <c r="K14" s="23">
-        <f t="shared" si="3"/>
-        <v>48788684.471012466</v>
-      </c>
-      <c r="L14" s="42">
-        <v>195394800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="3">
-        <v>2030</v>
-      </c>
-      <c r="B15" s="21">
-        <v>2703670</v>
-      </c>
-      <c r="C15" s="22">
-        <v>14305800.000000007</v>
-      </c>
-      <c r="D15" s="22">
-        <v>7292300.0000000009</v>
-      </c>
-      <c r="E15" s="22">
-        <v>17008100</v>
-      </c>
-      <c r="F15" s="22">
-        <v>14785700</v>
-      </c>
-      <c r="G15" s="22">
-        <v>13276000</v>
-      </c>
-      <c r="H15" s="23">
-        <f t="shared" si="2"/>
-        <v>52362100</v>
-      </c>
-      <c r="I15" s="24">
-        <f t="shared" si="0"/>
-        <v>3188527.7298968509</v>
-      </c>
-      <c r="J15" s="25">
-        <f t="shared" si="1"/>
-        <v>0.139266759736527</v>
-      </c>
-      <c r="K15" s="23">
-        <f t="shared" si="3"/>
-        <v>49173572.270103149</v>
-      </c>
-      <c r="L15" s="42">
-        <v>196948400</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
@@ -15481,7 +16001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
@@ -15895,7 +16415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
@@ -16536,7 +17056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -18293,6 +18813,150 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+      <c r="A2" s="109" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="115" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="111">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+      <c r="B3" s="110" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="111">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+      <c r="B4" s="110" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+      <c r="B5" s="112" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="111">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+      <c r="B6" s="112" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="111">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+      <c r="B7" s="112" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="111">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="B8" s="113" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="111">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+      <c r="B9" s="113" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" s="111">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+      <c r="B10" s="113" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="111">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C11" s="111"/>
+    </row>
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A12" s="109" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="114" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" s="111">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="B13" s="114" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="111">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="B14" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="B15" s="114" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="111">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -18594,7 +19258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -22649,438 +23313,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:G25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="64.5" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="4">
-        <v>45</v>
-      </c>
-      <c r="E2" s="4">
-        <v>361.6</v>
-      </c>
-      <c r="F2" s="4">
-        <v>174.7</v>
-      </c>
-      <c r="G2" s="4">
-        <v>174.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C4">
-        <v>1.04</v>
-      </c>
-      <c r="D4">
-        <v>1.04</v>
-      </c>
-      <c r="E4">
-        <v>1.04</v>
-      </c>
-      <c r="F4">
-        <v>1.04</v>
-      </c>
-      <c r="G4">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.43</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.43</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2.39</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2.39</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <f>1/(1 + (E7-1)*(1-'Baseline year demographics'!$C$8))</f>
-        <v>0.78419071518193229</v>
-      </c>
-      <c r="F13" s="4">
-        <f>1/(1 + (F7-1)*(1-'Baseline year demographics'!$C$8))</f>
-        <v>0.78419071518193229</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <f>1 / (E$10/E$9)</f>
-        <v>0.66945606694560678</v>
-      </c>
-      <c r="F14" s="4">
-        <f>1 / (F$10/F$9)</f>
-        <v>0.66945606694560678</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" ref="E15:F16" si="0">1 / (E$10/E$9)</f>
-        <v>0.66945606694560678</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0.66945606694560678</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>0.66945606694560678</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0.66945606694560678</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="6">
-        <v>5.16</v>
-      </c>
-      <c r="D18" s="6">
-        <v>5.16</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="8">
-        <v>1</v>
-      </c>
-      <c r="G18" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1.82</v>
-      </c>
-      <c r="F19" s="8">
-        <v>1.82</v>
-      </c>
-      <c r="G19" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C21" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="D21" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="E21" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="F21" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="G21" s="47">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="D23" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="E23" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="F23" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="G23" s="47">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B25" t="s">
-        <v>222</v>
-      </c>
-      <c r="C25" s="47">
-        <v>1</v>
-      </c>
-      <c r="D25" s="47">
-        <v>1</v>
-      </c>
-      <c r="E25" s="47">
-        <v>1</v>
-      </c>
-      <c r="F25" s="47">
-        <v>1</v>
-      </c>
-      <c r="G25" s="47">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added RR for birth intervals etc
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-37340" yWindow="-20080" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3949,7 +3949,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="261">
   <si>
     <t>year</t>
   </si>
@@ -4726,6 +4726,12 @@
   </si>
   <si>
     <t>24 months or greater</t>
+  </si>
+  <si>
+    <t>RR age order</t>
+  </si>
+  <si>
+    <t>RR interval</t>
   </si>
 </sst>
 </file>
@@ -5061,7 +5067,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="651">
+  <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5713,8 +5719,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5895,8 +5913,30 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="651">
+  <cellStyles count="663">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6222,6 +6262,12 @@
     <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6546,6 +6592,12 @@
     <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7849,7 +7901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -18817,7 +18869,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18953,15 +19005,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19200,7 +19253,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
@@ -19217,7 +19270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5" t="s">
         <v>43</v>
       </c>
@@ -19234,7 +19287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
         <v>24</v>
       </c>
@@ -19250,6 +19303,272 @@
       <c r="F19" s="5">
         <v>1</v>
       </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23" s="116" t="s">
+        <v>245</v>
+      </c>
+      <c r="C23" s="117">
+        <v>1</v>
+      </c>
+      <c r="D23" s="117">
+        <v>1.52</v>
+      </c>
+      <c r="E23" s="117">
+        <v>1.75</v>
+      </c>
+      <c r="F23" s="117">
+        <v>3.14</v>
+      </c>
+      <c r="G23" s="118"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="116" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24" s="117">
+        <v>1</v>
+      </c>
+      <c r="D24" s="117">
+        <v>1.2</v>
+      </c>
+      <c r="E24" s="117">
+        <v>1.4</v>
+      </c>
+      <c r="F24" s="117">
+        <v>1.6</v>
+      </c>
+      <c r="G24" s="118"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="116" t="s">
+        <v>247</v>
+      </c>
+      <c r="C25" s="117">
+        <v>1</v>
+      </c>
+      <c r="D25" s="117">
+        <v>1.2</v>
+      </c>
+      <c r="E25" s="117">
+        <v>1.4</v>
+      </c>
+      <c r="F25" s="117">
+        <v>1.6</v>
+      </c>
+      <c r="G25" s="118"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="119" t="s">
+        <v>248</v>
+      </c>
+      <c r="C26" s="117">
+        <v>1</v>
+      </c>
+      <c r="D26" s="117">
+        <v>1.52</v>
+      </c>
+      <c r="E26" s="117">
+        <v>1.75</v>
+      </c>
+      <c r="F26" s="117">
+        <v>1.73</v>
+      </c>
+      <c r="G26" s="118"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="119" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27" s="117">
+        <v>1</v>
+      </c>
+      <c r="D27" s="117">
+        <v>1</v>
+      </c>
+      <c r="E27" s="117">
+        <v>1</v>
+      </c>
+      <c r="F27" s="117">
+        <v>1</v>
+      </c>
+      <c r="G27" s="118"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="119" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" s="117">
+        <v>1</v>
+      </c>
+      <c r="D28" s="117">
+        <v>1</v>
+      </c>
+      <c r="E28" s="117">
+        <v>1</v>
+      </c>
+      <c r="F28" s="117">
+        <v>1</v>
+      </c>
+      <c r="G28" s="118"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="120" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="117">
+        <v>1</v>
+      </c>
+      <c r="D29" s="117">
+        <v>1.52</v>
+      </c>
+      <c r="E29" s="117">
+        <v>1.75</v>
+      </c>
+      <c r="F29" s="117">
+        <v>1.52</v>
+      </c>
+      <c r="G29" s="118"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="120" t="s">
+        <v>252</v>
+      </c>
+      <c r="C30" s="117">
+        <v>1</v>
+      </c>
+      <c r="D30" s="117">
+        <v>1</v>
+      </c>
+      <c r="E30" s="117">
+        <v>1.33</v>
+      </c>
+      <c r="F30" s="117">
+        <v>1</v>
+      </c>
+      <c r="G30" s="118"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="120" t="s">
+        <v>253</v>
+      </c>
+      <c r="C31" s="117">
+        <v>1</v>
+      </c>
+      <c r="D31" s="117">
+        <v>1</v>
+      </c>
+      <c r="E31" s="117">
+        <v>1.33</v>
+      </c>
+      <c r="F31" s="117">
+        <v>1</v>
+      </c>
+      <c r="G31" s="118"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="122"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="117"/>
+      <c r="G32" s="118"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="10"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="118"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B35" s="122" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" s="117">
+        <v>1</v>
+      </c>
+      <c r="D35" s="123">
+        <v>1</v>
+      </c>
+      <c r="E35" s="123">
+        <v>1</v>
+      </c>
+      <c r="F35" s="123">
+        <v>1</v>
+      </c>
+      <c r="G35" s="118"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="122" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="117">
+        <v>1</v>
+      </c>
+      <c r="D36" s="123">
+        <v>1.41</v>
+      </c>
+      <c r="E36" s="123">
+        <v>1.49</v>
+      </c>
+      <c r="F36" s="123">
+        <v>3.03</v>
+      </c>
+      <c r="G36" s="118"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="122" t="s">
+        <v>257</v>
+      </c>
+      <c r="C37" s="117">
+        <v>1</v>
+      </c>
+      <c r="D37" s="123">
+        <v>1.18</v>
+      </c>
+      <c r="E37" s="123">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F37" s="123">
+        <v>1.77</v>
+      </c>
+      <c r="G37" s="118"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="122" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" s="117">
+        <v>1</v>
+      </c>
+      <c r="D38" s="123">
+        <v>1</v>
+      </c>
+      <c r="E38" s="123">
+        <v>1</v>
+      </c>
+      <c r="F38" s="123">
+        <v>1</v>
+      </c>
+      <c r="G38" s="118"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Creating new age group for newborns, some fixes
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37340" yWindow="-20080" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="-37340" yWindow="-20080" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3949,7 +3949,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="257">
   <si>
     <t>year</t>
   </si>
@@ -4660,18 +4660,6 @@
   </si>
   <si>
     <t>Public provision of complementary foods with iron, Public provision of complementary foods with iron (malaria area)</t>
-  </si>
-  <si>
-    <t>WRA 15-19 years</t>
-  </si>
-  <si>
-    <t>WRA 20-29 years</t>
-  </si>
-  <si>
-    <t>WRA 30-39 years</t>
-  </si>
-  <si>
-    <t>WRA 40-49 years</t>
   </si>
   <si>
     <t>Index</t>
@@ -13091,8 +13079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13114,16 +13102,16 @@
         <v>61</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>237</v>
+        <v>115</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>238</v>
+        <v>116</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>239</v>
+        <v>117</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>240</v>
+        <v>118</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>62</v>
@@ -18868,7 +18856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -18881,21 +18869,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="109" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B2" s="115" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C2" s="111">
         <v>0.15</v>
@@ -18903,7 +18891,7 @@
     </row>
     <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B3" s="110" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C3" s="111">
         <v>0.03</v>
@@ -18911,7 +18899,7 @@
     </row>
     <row r="4" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B4" s="110" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C4" s="111">
         <v>0</v>
@@ -18919,7 +18907,7 @@
     </row>
     <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.15">
       <c r="B5" s="112" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C5" s="111">
         <v>0.19</v>
@@ -18927,7 +18915,7 @@
     </row>
     <row r="6" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B6" s="112" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C6" s="111">
         <v>0.39</v>
@@ -18935,7 +18923,7 @@
     </row>
     <row r="7" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B7" s="112" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C7" s="111">
         <v>0.19</v>
@@ -18943,7 +18931,7 @@
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B8" s="113" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C8" s="111">
         <v>1E-3</v>
@@ -18951,7 +18939,7 @@
     </row>
     <row r="9" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B9" s="113" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C9" s="111">
         <v>7.0000000000000001E-3</v>
@@ -18959,7 +18947,7 @@
     </row>
     <row r="10" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B10" s="113" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C10" s="111">
         <v>0.04</v>
@@ -18970,10 +18958,10 @@
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="109" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B12" s="114" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C12" s="111">
         <v>0.34</v>
@@ -18981,7 +18969,7 @@
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B13" s="114" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C13" s="111">
         <v>0.05</v>
@@ -18989,7 +18977,7 @@
     </row>
     <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B14" s="114" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C14" s="111">
         <v>7.0000000000000007E-2</v>
@@ -18997,7 +18985,7 @@
     </row>
     <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B15" s="114" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C15" s="111">
         <v>0.55000000000000004</v>
@@ -19013,8 +19001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19309,10 +19297,10 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B23" s="116" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C23" s="117">
         <v>1</v>
@@ -19330,7 +19318,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="116" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C24" s="117">
         <v>1</v>
@@ -19348,7 +19336,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="116" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C25" s="117">
         <v>1</v>
@@ -19366,7 +19354,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="119" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C26" s="117">
         <v>1</v>
@@ -19384,7 +19372,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="119" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C27" s="117">
         <v>1</v>
@@ -19402,7 +19390,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="119" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C28" s="117">
         <v>1</v>
@@ -19420,7 +19408,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="120" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C29" s="117">
         <v>1</v>
@@ -19438,7 +19426,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="120" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C30" s="117">
         <v>1</v>
@@ -19456,7 +19444,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="120" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C31" s="117">
         <v>1</v>
@@ -19497,10 +19485,10 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B35" s="122" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C35" s="117">
         <v>1</v>
@@ -19518,7 +19506,7 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="122" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C36" s="117">
         <v>1</v>
@@ -19536,7 +19524,7 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="122" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C37" s="117">
         <v>1</v>
@@ -19554,7 +19542,7 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="122" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C38" s="117">
         <v>1</v>
@@ -19584,8 +19572,8 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
fixed fortification target population issues
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-69340" yWindow="-4680" windowWidth="27680" windowHeight="18100" tabRatio="500" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="840" yWindow="0" windowWidth="23320" windowHeight="13560" tabRatio="500" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1009,7 +1009,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating wheat</t>
+Fraction eating wheat
+amongst those not subsistence farming
+</t>
         </r>
       </text>
     </comment>
@@ -2215,7 +2217,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+LiST
+RUTH: removed LiST value and replaced with target population
+</t>
         </r>
       </text>
     </comment>
@@ -4880,7 +4884,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="749">
+  <cellStyleXfs count="767">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4892,6 +4896,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5842,15 +5864,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="749">
+  <cellStyles count="767">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6225,6 +6247,15 @@
     <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6598,6 +6629,15 @@
     <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7901,8 +7941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -8614,7 +8654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -8655,7 +8695,7 @@
       <c r="A2" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="132" t="s">
         <v>80</v>
       </c>
       <c r="C2" t="s">
@@ -8678,7 +8718,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="128"/>
+      <c r="B3" s="132"/>
       <c r="C3" t="s">
         <v>190</v>
       </c>
@@ -8700,7 +8740,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="128"/>
+      <c r="B4" s="132"/>
       <c r="C4" t="s">
         <v>200</v>
       </c>
@@ -8727,7 +8767,7 @@
       <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="132" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8750,7 +8790,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="128"/>
+      <c r="B6" s="132"/>
       <c r="C6" t="s">
         <v>190</v>
       </c>
@@ -8771,7 +8811,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="128"/>
+      <c r="B7" s="132"/>
       <c r="C7" t="s">
         <v>200</v>
       </c>
@@ -8794,7 +8834,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="132" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8817,7 +8857,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="128"/>
+      <c r="B9" s="132"/>
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -8838,7 +8878,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="128"/>
+      <c r="B10" s="132"/>
       <c r="C10" t="s">
         <v>200</v>
       </c>
@@ -8861,7 +8901,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="132" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8884,7 +8924,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="128"/>
+      <c r="B12" s="132"/>
       <c r="C12" t="s">
         <v>190</v>
       </c>
@@ -8905,7 +8945,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="128"/>
+      <c r="B13" s="132"/>
       <c r="C13" t="s">
         <v>200</v>
       </c>
@@ -8928,7 +8968,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="128" t="s">
+      <c r="B14" s="132" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8951,7 +8991,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="128"/>
+      <c r="B15" s="132"/>
       <c r="C15" t="s">
         <v>190</v>
       </c>
@@ -8972,7 +9012,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="128"/>
+      <c r="B16" s="132"/>
       <c r="C16" t="s">
         <v>200</v>
       </c>
@@ -9028,7 +9068,7 @@
       <c r="A19" s="77" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="132" t="s">
         <v>80</v>
       </c>
       <c r="C19" t="s">
@@ -9051,7 +9091,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="128"/>
+      <c r="B20" s="132"/>
       <c r="C20" t="s">
         <v>190</v>
       </c>
@@ -9072,7 +9112,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="128"/>
+      <c r="B21" s="132"/>
       <c r="C21" t="s">
         <v>200</v>
       </c>
@@ -9095,7 +9135,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="132" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -9118,7 +9158,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="128"/>
+      <c r="B23" s="132"/>
       <c r="C23" t="s">
         <v>190</v>
       </c>
@@ -9139,7 +9179,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="128"/>
+      <c r="B24" s="132"/>
       <c r="C24" t="s">
         <v>200</v>
       </c>
@@ -9161,7 +9201,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="128" t="s">
+      <c r="B25" s="132" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -9184,7 +9224,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="128"/>
+      <c r="B26" s="132"/>
       <c r="C26" t="s">
         <v>190</v>
       </c>
@@ -9205,7 +9245,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="128"/>
+      <c r="B27" s="132"/>
       <c r="C27" t="s">
         <v>200</v>
       </c>
@@ -9227,7 +9267,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="128" t="s">
+      <c r="B28" s="132" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -9250,7 +9290,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="128"/>
+      <c r="B29" s="132"/>
       <c r="C29" t="s">
         <v>190</v>
       </c>
@@ -9271,7 +9311,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="128"/>
+      <c r="B30" s="132"/>
       <c r="C30" t="s">
         <v>200</v>
       </c>
@@ -9293,7 +9333,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="128" t="s">
+      <c r="B31" s="132" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9316,7 +9356,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="128"/>
+      <c r="B32" s="132"/>
       <c r="C32" t="s">
         <v>190</v>
       </c>
@@ -9337,7 +9377,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="128"/>
+      <c r="B33" s="132"/>
       <c r="C33" t="s">
         <v>200</v>
       </c>
@@ -9384,7 +9424,7 @@
       <c r="A36" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="B36" s="128" t="s">
+      <c r="B36" s="132" t="s">
         <v>80</v>
       </c>
       <c r="C36" t="s">
@@ -9407,7 +9447,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="128"/>
+      <c r="B37" s="132"/>
       <c r="C37" t="s">
         <v>190</v>
       </c>
@@ -9428,7 +9468,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="128"/>
+      <c r="B38" s="132"/>
       <c r="C38" t="s">
         <v>200</v>
       </c>
@@ -9449,7 +9489,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="128" t="s">
+      <c r="B39" s="132" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9472,7 +9512,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="B40" s="128"/>
+      <c r="B40" s="132"/>
       <c r="C40" t="s">
         <v>190</v>
       </c>
@@ -9493,7 +9533,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="128"/>
+      <c r="B41" s="132"/>
       <c r="C41" t="s">
         <v>200</v>
       </c>
@@ -9514,7 +9554,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="B42" s="128" t="s">
+      <c r="B42" s="132" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9537,7 +9577,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="B43" s="128"/>
+      <c r="B43" s="132"/>
       <c r="C43" t="s">
         <v>190</v>
       </c>
@@ -9558,7 +9598,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="B44" s="128"/>
+      <c r="B44" s="132"/>
       <c r="C44" t="s">
         <v>200</v>
       </c>
@@ -9579,7 +9619,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="B45" s="128" t="s">
+      <c r="B45" s="132" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9602,7 +9642,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="B46" s="128"/>
+      <c r="B46" s="132"/>
       <c r="C46" t="s">
         <v>190</v>
       </c>
@@ -9623,7 +9663,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="B47" s="128"/>
+      <c r="B47" s="132"/>
       <c r="C47" t="s">
         <v>200</v>
       </c>
@@ -9644,7 +9684,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="128" t="s">
+      <c r="B48" s="132" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9667,7 +9707,7 @@
       </c>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="128"/>
+      <c r="B49" s="132"/>
       <c r="C49" t="s">
         <v>190</v>
       </c>
@@ -9688,7 +9728,7 @@
       </c>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="128"/>
+      <c r="B50" s="132"/>
       <c r="C50" t="s">
         <v>200</v>
       </c>
@@ -9733,11 +9773,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9748,6 +9783,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10259,8 +10299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -11291,24 +11331,24 @@
         <v>0</v>
       </c>
       <c r="E40" s="71">
-        <f>'Baseline year demographics'!$C$24</f>
-        <v>0.12</v>
+        <f>'Baseline year demographics'!$C$24*(1-'Baseline year demographics'!C22)</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="F40" s="71">
-        <f>'Baseline year demographics'!$C$24</f>
-        <v>0.12</v>
+        <f>'Baseline year demographics'!$C$24*(1-'Baseline year demographics'!C22)</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="G40" s="71">
-        <f>'Baseline year demographics'!$C$24</f>
-        <v>0.12</v>
+        <f>'Baseline year demographics'!$C$24*(1-'Baseline year demographics'!C22)</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="H40" s="71">
-        <f>'Baseline year demographics'!$C$24</f>
-        <v>0.12</v>
+        <f>'Baseline year demographics'!$C$24*(1-'Baseline year demographics'!C22)</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="I40" s="71">
-        <f>'Baseline year demographics'!$C$24</f>
-        <v>0.12</v>
+        <f>'Baseline year demographics'!$C$24*(1-'Baseline year demographics'!C22)</f>
+        <v>8.3999999999999991E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1">
@@ -11322,24 +11362,24 @@
         <v>0</v>
       </c>
       <c r="E41" s="69">
-        <f>'Baseline year demographics'!$C$25</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$25*(1-'Baseline year demographics'!C22)</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="F41" s="69">
-        <f>'Baseline year demographics'!$C$25</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$25*(1-'Baseline year demographics'!C22)</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="G41" s="69">
-        <f>'Baseline year demographics'!$C$25</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$25*(1-'Baseline year demographics'!C22)</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="H41" s="69">
-        <f>'Baseline year demographics'!$C$25</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$25*(1-'Baseline year demographics'!C22)</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="I41" s="69">
-        <f>'Baseline year demographics'!$C$25</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$25*(1-'Baseline year demographics'!C22)</f>
+        <v>3.4999999999999996E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1">
@@ -11353,24 +11393,24 @@
         <v>0</v>
       </c>
       <c r="E42" s="69">
-        <f>'Baseline year demographics'!$C$23</f>
-        <v>0.8</v>
+        <f>'Baseline year demographics'!$C$23*(1-'Baseline year demographics'!C22)</f>
+        <v>0.55999999999999994</v>
       </c>
       <c r="F42" s="69">
-        <f>'Baseline year demographics'!$C$23</f>
-        <v>0.8</v>
+        <f>'Baseline year demographics'!$C$23*(1-'Baseline year demographics'!C22)</f>
+        <v>0.55999999999999994</v>
       </c>
       <c r="G42" s="69">
-        <f>'Baseline year demographics'!$C$23</f>
-        <v>0.8</v>
+        <f>'Baseline year demographics'!$C$23*(1-'Baseline year demographics'!C22)</f>
+        <v>0.55999999999999994</v>
       </c>
       <c r="H42" s="69">
-        <f>'Baseline year demographics'!$C$23</f>
-        <v>0.8</v>
+        <f>'Baseline year demographics'!$C$23*(1-'Baseline year demographics'!C22)</f>
+        <v>0.55999999999999994</v>
       </c>
       <c r="I42" s="69">
-        <f>'Baseline year demographics'!$C$23</f>
-        <v>0.8</v>
+        <f>'Baseline year demographics'!$C$23*(1-'Baseline year demographics'!C22)</f>
+        <v>0.55999999999999994</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1">
@@ -11931,7 +11971,7 @@
   </sheetPr>
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -14625,8 +14665,8 @@
   </sheetPr>
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -15128,7 +15168,8 @@
         <v>120</v>
       </c>
       <c r="D22" s="12">
-        <v>0.7</v>
+        <f>'Interventions target population'!E40</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="E22" s="12">
         <v>0</v>
@@ -15177,7 +15218,8 @@
         <v>120</v>
       </c>
       <c r="D24" s="12">
-        <v>0.7</v>
+        <f>'Interventions target population'!E41</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="E24" s="12">
         <v>0</v>
@@ -15224,7 +15266,8 @@
         <v>120</v>
       </c>
       <c r="D26" s="12">
-        <v>0.7</v>
+        <f>'Interventions target population'!E42</f>
+        <v>0.55999999999999994</v>
       </c>
       <c r="E26" s="12">
         <v>0</v>
@@ -15260,10 +15303,10 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="129" t="s">
+      <c r="A28" s="128" t="s">
         <v>245</v>
       </c>
-      <c r="B28" s="130" t="s">
+      <c r="B28" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -15286,8 +15329,8 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="129"/>
-      <c r="B29" s="129"/>
+      <c r="A29" s="128"/>
+      <c r="B29" s="128"/>
       <c r="C29" t="s">
         <v>67</v>
       </c>
@@ -15308,8 +15351,8 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="129"/>
-      <c r="B30" s="130"/>
+      <c r="A30" s="128"/>
+      <c r="B30" s="129"/>
       <c r="C30" s="4" t="s">
         <v>68</v>
       </c>
@@ -15330,10 +15373,10 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="129" t="s">
+      <c r="A31" s="128" t="s">
         <v>246</v>
       </c>
-      <c r="B31" s="130" t="s">
+      <c r="B31" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -15356,8 +15399,8 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="129"/>
-      <c r="B32" s="129"/>
+      <c r="A32" s="128"/>
+      <c r="B32" s="128"/>
       <c r="C32" t="s">
         <v>67</v>
       </c>
@@ -15378,8 +15421,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="129"/>
-      <c r="B33" s="130"/>
+      <c r="A33" s="128"/>
+      <c r="B33" s="129"/>
       <c r="C33" s="4" t="s">
         <v>68</v>
       </c>
@@ -15400,10 +15443,10 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="129" t="s">
+      <c r="A34" s="128" t="s">
         <v>247</v>
       </c>
-      <c r="B34" s="130" t="s">
+      <c r="B34" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -15426,8 +15469,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="129"/>
-      <c r="B35" s="129"/>
+      <c r="A35" s="128"/>
+      <c r="B35" s="128"/>
       <c r="C35" t="s">
         <v>67</v>
       </c>
@@ -15448,8 +15491,8 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="129"/>
-      <c r="B36" s="130"/>
+      <c r="A36" s="128"/>
+      <c r="B36" s="129"/>
       <c r="C36" s="4" t="s">
         <v>68</v>
       </c>
@@ -15470,10 +15513,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="129" t="s">
+      <c r="A37" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="B37" s="130" t="s">
+      <c r="B37" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -15496,8 +15539,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="129"/>
-      <c r="B38" s="129"/>
+      <c r="A38" s="128"/>
+      <c r="B38" s="128"/>
       <c r="C38" t="s">
         <v>67</v>
       </c>
@@ -15518,8 +15561,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="129"/>
-      <c r="B39" s="130"/>
+      <c r="A39" s="128"/>
+      <c r="B39" s="129"/>
       <c r="C39" s="4" t="s">
         <v>68</v>
       </c>
@@ -15540,10 +15583,10 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="129" t="s">
+      <c r="A40" s="128" t="s">
         <v>249</v>
       </c>
-      <c r="B40" s="130" t="s">
+      <c r="B40" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -15566,8 +15609,8 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="129"/>
-      <c r="B41" s="129"/>
+      <c r="A41" s="128"/>
+      <c r="B41" s="128"/>
       <c r="C41" t="s">
         <v>67</v>
       </c>
@@ -15588,8 +15631,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="129"/>
-      <c r="B42" s="130"/>
+      <c r="A42" s="128"/>
+      <c r="B42" s="129"/>
       <c r="C42" s="4" t="s">
         <v>68</v>
       </c>
@@ -15610,10 +15653,10 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="131" t="s">
+      <c r="A43" s="130" t="s">
         <v>245</v>
       </c>
-      <c r="B43" s="131" t="s">
+      <c r="B43" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -15636,8 +15679,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="131"/>
-      <c r="B44" s="131"/>
+      <c r="A44" s="130"/>
+      <c r="B44" s="130"/>
       <c r="C44" t="s">
         <v>67</v>
       </c>
@@ -15658,8 +15701,8 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="131"/>
-      <c r="B45" s="132"/>
+      <c r="A45" s="130"/>
+      <c r="B45" s="131"/>
       <c r="C45" s="4" t="s">
         <v>68</v>
       </c>
@@ -15680,10 +15723,10 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="131" t="s">
+      <c r="A46" s="130" t="s">
         <v>246</v>
       </c>
-      <c r="B46" s="131" t="s">
+      <c r="B46" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -15706,8 +15749,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="131"/>
-      <c r="B47" s="131"/>
+      <c r="A47" s="130"/>
+      <c r="B47" s="130"/>
       <c r="C47" t="s">
         <v>67</v>
       </c>
@@ -15728,8 +15771,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="131"/>
-      <c r="B48" s="132"/>
+      <c r="A48" s="130"/>
+      <c r="B48" s="131"/>
       <c r="C48" s="4" t="s">
         <v>68</v>
       </c>
@@ -15750,10 +15793,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="131" t="s">
+      <c r="A49" s="130" t="s">
         <v>247</v>
       </c>
-      <c r="B49" s="131" t="s">
+      <c r="B49" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -15776,8 +15819,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="131"/>
-      <c r="B50" s="131"/>
+      <c r="A50" s="130"/>
+      <c r="B50" s="130"/>
       <c r="C50" t="s">
         <v>67</v>
       </c>
@@ -15798,8 +15841,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="131"/>
-      <c r="B51" s="132"/>
+      <c r="A51" s="130"/>
+      <c r="B51" s="131"/>
       <c r="C51" s="4" t="s">
         <v>68</v>
       </c>
@@ -15820,10 +15863,10 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="131" t="s">
+      <c r="A52" s="130" t="s">
         <v>248</v>
       </c>
-      <c r="B52" s="131" t="s">
+      <c r="B52" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -15846,8 +15889,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="131"/>
-      <c r="B53" s="131"/>
+      <c r="A53" s="130"/>
+      <c r="B53" s="130"/>
       <c r="C53" t="s">
         <v>67</v>
       </c>
@@ -15868,8 +15911,8 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="131"/>
-      <c r="B54" s="132"/>
+      <c r="A54" s="130"/>
+      <c r="B54" s="131"/>
       <c r="C54" s="4" t="s">
         <v>68</v>
       </c>
@@ -15890,10 +15933,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="131" t="s">
+      <c r="A55" s="130" t="s">
         <v>249</v>
       </c>
-      <c r="B55" s="131" t="s">
+      <c r="B55" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -15916,8 +15959,8 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="131"/>
-      <c r="B56" s="131"/>
+      <c r="A56" s="130"/>
+      <c r="B56" s="130"/>
       <c r="C56" t="s">
         <v>67</v>
       </c>
@@ -15938,8 +15981,8 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="131"/>
-      <c r="B57" s="132"/>
+      <c r="A57" s="130"/>
+      <c r="B57" s="131"/>
       <c r="C57" s="4" t="s">
         <v>68</v>
       </c>
@@ -15960,10 +16003,10 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="129" t="s">
+      <c r="A58" s="128" t="s">
         <v>172</v>
       </c>
-      <c r="B58" s="130" t="s">
+      <c r="B58" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -15986,8 +16029,8 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="129"/>
-      <c r="B59" s="129"/>
+      <c r="A59" s="128"/>
+      <c r="B59" s="128"/>
       <c r="C59" t="s">
         <v>67</v>
       </c>
@@ -16008,8 +16051,8 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="129"/>
-      <c r="B60" s="129"/>
+      <c r="A60" s="128"/>
+      <c r="B60" s="128"/>
       <c r="C60" s="4" t="s">
         <v>68</v>
       </c>
@@ -16030,10 +16073,10 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="129" t="s">
+      <c r="A61" s="128" t="s">
         <v>172</v>
       </c>
-      <c r="B61" s="130" t="s">
+      <c r="B61" s="129" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -16056,8 +16099,8 @@
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="129"/>
-      <c r="B62" s="129"/>
+      <c r="A62" s="128"/>
+      <c r="B62" s="128"/>
       <c r="C62" t="s">
         <v>67</v>
       </c>
@@ -16078,8 +16121,8 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="129"/>
-      <c r="B63" s="129"/>
+      <c r="A63" s="128"/>
+      <c r="B63" s="128"/>
       <c r="C63" s="4" t="s">
         <v>68</v>
       </c>
@@ -16100,10 +16143,10 @@
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="129" t="s">
+      <c r="A64" s="128" t="s">
         <v>250</v>
       </c>
-      <c r="B64" s="130" t="s">
+      <c r="B64" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -16126,8 +16169,8 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="129"/>
-      <c r="B65" s="129"/>
+      <c r="A65" s="128"/>
+      <c r="B65" s="128"/>
       <c r="C65" t="s">
         <v>67</v>
       </c>
@@ -16148,10 +16191,10 @@
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="129" t="s">
+      <c r="A66" s="128" t="s">
         <v>255</v>
       </c>
-      <c r="B66" s="130" t="s">
+      <c r="B66" s="129" t="s">
         <v>28</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -16174,8 +16217,8 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="129"/>
-      <c r="B67" s="129"/>
+      <c r="A67" s="128"/>
+      <c r="B67" s="128"/>
       <c r="C67" t="s">
         <v>67</v>
       </c>
@@ -16196,10 +16239,10 @@
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="131" t="s">
+      <c r="A68" s="130" t="s">
         <v>172</v>
       </c>
-      <c r="B68" s="131" t="s">
+      <c r="B68" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="12" t="s">
@@ -16222,8 +16265,8 @@
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="131"/>
-      <c r="B69" s="131"/>
+      <c r="A69" s="130"/>
+      <c r="B69" s="130"/>
       <c r="C69" s="11" t="s">
         <v>67</v>
       </c>
@@ -16244,8 +16287,8 @@
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="131"/>
-      <c r="B70" s="131"/>
+      <c r="A70" s="130"/>
+      <c r="B70" s="130"/>
       <c r="C70" s="12" t="s">
         <v>68</v>
       </c>
@@ -16266,10 +16309,10 @@
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="131" t="s">
+      <c r="A71" s="130" t="s">
         <v>172</v>
       </c>
-      <c r="B71" s="132" t="s">
+      <c r="B71" s="131" t="s">
         <v>17</v>
       </c>
       <c r="C71" s="12" t="s">
@@ -16292,8 +16335,8 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="131"/>
-      <c r="B72" s="131"/>
+      <c r="A72" s="130"/>
+      <c r="B72" s="130"/>
       <c r="C72" s="11" t="s">
         <v>67</v>
       </c>
@@ -16314,8 +16357,8 @@
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="131"/>
-      <c r="B73" s="131"/>
+      <c r="A73" s="130"/>
+      <c r="B73" s="130"/>
       <c r="C73" s="12" t="s">
         <v>68</v>
       </c>
@@ -16336,10 +16379,10 @@
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="131" t="s">
+      <c r="A74" s="130" t="s">
         <v>250</v>
       </c>
-      <c r="B74" s="131" t="s">
+      <c r="B74" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="12" t="s">
@@ -16362,8 +16405,8 @@
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="131"/>
-      <c r="B75" s="131"/>
+      <c r="A75" s="130"/>
+      <c r="B75" s="130"/>
       <c r="C75" s="11" t="s">
         <v>67</v>
       </c>
@@ -16384,10 +16427,10 @@
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="131" t="s">
+      <c r="A76" s="130" t="s">
         <v>255</v>
       </c>
-      <c r="B76" s="131" t="s">
+      <c r="B76" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C76" s="12" t="s">
@@ -16410,8 +16453,8 @@
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="131"/>
-      <c r="B77" s="131"/>
+      <c r="A77" s="130"/>
+      <c r="B77" s="130"/>
       <c r="C77" s="11" t="s">
         <v>67</v>
       </c>
@@ -16866,8 +16909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -17278,7 +17321,8 @@
         <v>0</v>
       </c>
       <c r="C29" s="14">
-        <v>0.12</v>
+        <f>'Baseline year demographics'!C24*(1-'Baseline year demographics'!C22)</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="D29" s="19">
         <v>0.19</v>
@@ -17292,7 +17336,8 @@
         <v>0</v>
       </c>
       <c r="C30" s="14">
-        <v>0.05</v>
+        <f>'Baseline year demographics'!C25*(1-'Baseline year demographics'!C22)</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="D30" s="19">
         <v>0.14000000000000001</v>
@@ -17306,7 +17351,8 @@
         <v>0</v>
       </c>
       <c r="C31" s="14">
-        <v>0.8</v>
+        <f>'Baseline year demographics'!C23*(1-'Baseline year demographics'!C22)</f>
+        <v>0.55999999999999994</v>
       </c>
       <c r="D31" s="19">
         <v>0.75</v>

</xml_diff>

<commit_message>
Fixes for getting women populations to function
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37340" yWindow="-20080" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-37340" yWindow="-20080" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="13" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,9 @@
     <sheet name="Interventions family planning" sheetId="34" r:id="rId19"/>
     <sheet name="Interventions target population" sheetId="21" r:id="rId20"/>
     <sheet name="Program dependencies" sheetId="40" r:id="rId21"/>
-    <sheet name="Program areas" sheetId="36" r:id="rId22"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId23"/>
-    <sheet name="Population risk areas" sheetId="41" r:id="rId24"/>
+    <sheet name="Program risk areas" sheetId="36" r:id="rId22"/>
+    <sheet name="Population risk areas" sheetId="43" r:id="rId23"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId24"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -597,54 +597,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% at risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% at risk from malaria</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C13" authorId="1">
       <text>
         <r>
@@ -670,6 +622,54 @@
       </text>
     </comment>
     <comment ref="D13" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -3949,7 +3949,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="257">
   <si>
     <t>year</t>
   </si>
@@ -4635,9 +4635,6 @@
     <t>fraction SAM to MAM</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Birth outcomes</t>
   </si>
   <si>
@@ -4720,6 +4717,9 @@
   </si>
   <si>
     <t>RR interval</t>
+  </si>
+  <si>
+    <t>Age group</t>
   </si>
 </sst>
 </file>
@@ -8020,7 +8020,7 @@
     </row>
     <row r="15" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C15" s="69">
         <v>0.2</v>
@@ -10407,10 +10407,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10516,16 +10516,16 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="D6" s="36">
-        <v>0.15</v>
+      <c r="C6" s="9">
+        <v>0.23</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.23</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -10538,10 +10538,10 @@
       <c r="B7" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="36">
-        <v>1</v>
-      </c>
-      <c r="D7" s="36">
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="9">
@@ -10553,7 +10553,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -10590,21 +10590,21 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
       </c>
       <c r="C10" s="36">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="D10" s="36">
-        <v>0.35</v>
-      </c>
-      <c r="E10" s="36">
-        <v>0</v>
-      </c>
-      <c r="F10" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
         <v>0</v>
       </c>
     </row>
@@ -10612,24 +10612,22 @@
       <c r="B11" t="s">
         <v>52</v>
       </c>
-      <c r="C11">
-        <f>'Baseline year demographics'!$C$9</f>
-        <v>0.1</v>
-      </c>
-      <c r="D11">
-        <f>'Baseline year demographics'!$C$9</f>
-        <v>0.1</v>
-      </c>
-      <c r="E11" s="36">
-        <v>0</v>
-      </c>
-      <c r="F11" s="36">
-        <v>0</v>
+      <c r="C11" s="36">
+        <v>1</v>
+      </c>
+      <c r="D11" s="36">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4" t="s">
-        <v>80</v>
+      <c r="A12" t="s">
+        <v>123</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
@@ -10663,6 +10661,45 @@
         <v>0</v>
       </c>
       <c r="F13" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="36">
+        <v>0.35</v>
+      </c>
+      <c r="D14" s="36">
+        <v>0.35</v>
+      </c>
+      <c r="E14" s="36">
+        <v>0</v>
+      </c>
+      <c r="F14" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <f>'Baseline year demographics'!$C$9</f>
+        <v>0.1</v>
+      </c>
+      <c r="D15">
+        <f>'Baseline year demographics'!$C$9</f>
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="36">
+        <v>0</v>
+      </c>
+      <c r="F15" s="36">
         <v>0</v>
       </c>
     </row>
@@ -10680,17 +10717,20 @@
   </sheetPr>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="56.5" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -13079,7 +13119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -13729,7 +13769,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C1" sqref="C1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15740,7 +15780,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15755,10 +15795,10 @@
         <v>209</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -15958,7 +15998,7 @@
         <v>131</v>
       </c>
       <c r="B32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -16046,7 +16086,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16075,10 +16115,10 @@
         <v>210</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>234</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>235</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>36</v>
@@ -16087,17 +16127,15 @@
         <v>219</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>228</v>
-      </c>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
@@ -16374,7 +16412,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -16388,7 +16426,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>140</v>
       </c>
@@ -16402,7 +16440,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>76</v>
       </c>
@@ -16410,7 +16448,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>141</v>
       </c>
@@ -16418,7 +16456,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>155</v>
       </c>
@@ -16426,7 +16464,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>156</v>
       </c>
@@ -16434,7 +16472,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
@@ -16442,12 +16480,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="K40" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -16456,11 +16491,297 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" s="47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" s="47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" t="s">
+        <v>171</v>
+      </c>
+      <c r="J6" s="47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J7" s="47"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" s="47"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" t="s">
+        <v>171</v>
+      </c>
+      <c r="J9" s="47"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="47"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17093,18 +17414,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -18869,21 +19178,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>238</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="115" t="s">
         <v>240</v>
-      </c>
-      <c r="B2" s="115" t="s">
-        <v>241</v>
       </c>
       <c r="C2" s="111">
         <v>0.15</v>
@@ -18891,7 +19200,7 @@
     </row>
     <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B3" s="110" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="111">
         <v>0.03</v>
@@ -18899,7 +19208,7 @@
     </row>
     <row r="4" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B4" s="110" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="111">
         <v>0</v>
@@ -18907,7 +19216,7 @@
     </row>
     <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.15">
       <c r="B5" s="112" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C5" s="111">
         <v>0.19</v>
@@ -18915,7 +19224,7 @@
     </row>
     <row r="6" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B6" s="112" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="111">
         <v>0.39</v>
@@ -18923,7 +19232,7 @@
     </row>
     <row r="7" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B7" s="112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" s="111">
         <v>0.19</v>
@@ -18931,7 +19240,7 @@
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B8" s="113" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="111">
         <v>1E-3</v>
@@ -18939,7 +19248,7 @@
     </row>
     <row r="9" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B9" s="113" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" s="111">
         <v>7.0000000000000001E-3</v>
@@ -18947,7 +19256,7 @@
     </row>
     <row r="10" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B10" s="113" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C10" s="111">
         <v>0.04</v>
@@ -18958,10 +19267,10 @@
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="109" t="s">
+        <v>249</v>
+      </c>
+      <c r="B12" s="114" t="s">
         <v>250</v>
-      </c>
-      <c r="B12" s="114" t="s">
-        <v>251</v>
       </c>
       <c r="C12" s="111">
         <v>0.34</v>
@@ -18969,7 +19278,7 @@
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B13" s="114" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C13" s="111">
         <v>0.05</v>
@@ -18977,7 +19286,7 @@
     </row>
     <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B14" s="114" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C14" s="111">
         <v>7.0000000000000007E-2</v>
@@ -18985,7 +19294,7 @@
     </row>
     <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B15" s="114" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C15" s="111">
         <v>0.55000000000000004</v>
@@ -19001,8 +19310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19297,10 +19606,10 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B23" s="116" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C23" s="117">
         <v>1</v>
@@ -19318,7 +19627,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="116" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C24" s="117">
         <v>1</v>
@@ -19336,7 +19645,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="116" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C25" s="117">
         <v>1</v>
@@ -19354,7 +19663,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="119" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C26" s="117">
         <v>1</v>
@@ -19372,7 +19681,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C27" s="117">
         <v>1</v>
@@ -19390,7 +19699,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="119" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C28" s="117">
         <v>1</v>
@@ -19408,7 +19717,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="120" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C29" s="117">
         <v>1</v>
@@ -19426,7 +19735,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="120" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C30" s="117">
         <v>1</v>
@@ -19444,7 +19753,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="120" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C31" s="117">
         <v>1</v>
@@ -19485,10 +19794,10 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B35" s="122" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C35" s="117">
         <v>1</v>
@@ -19506,7 +19815,7 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="122" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C36" s="117">
         <v>1</v>
@@ -19524,7 +19833,7 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="122" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" s="117">
         <v>1</v>
@@ -19542,7 +19851,7 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C38" s="117">
         <v>1</v>

</xml_diff>

<commit_message>
Discerning between ages targeted and ages impacted by programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="13" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -34,11 +34,12 @@
     <sheet name="Programs for PW" sheetId="45" r:id="rId20"/>
     <sheet name="Programs birth age" sheetId="46" r:id="rId21"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId22"/>
-    <sheet name="Program dependencies" sheetId="40" r:id="rId23"/>
-    <sheet name="Program risk areas" sheetId="36" r:id="rId24"/>
-    <sheet name="Population risk areas" sheetId="43" r:id="rId25"/>
-    <sheet name="Programs cost and coverage" sheetId="20" r:id="rId26"/>
-    <sheet name="Programs to include" sheetId="44" r:id="rId27"/>
+    <sheet name="Programs impacted population" sheetId="47" r:id="rId23"/>
+    <sheet name="Program dependencies" sheetId="40" r:id="rId24"/>
+    <sheet name="Program risk areas" sheetId="36" r:id="rId25"/>
+    <sheet name="Population risk areas" sheetId="43" r:id="rId26"/>
+    <sheet name="Programs cost and coverage" sheetId="20" r:id="rId27"/>
+    <sheet name="Programs to include" sheetId="44" r:id="rId28"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -3148,7 +3149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="269">
   <si>
     <t>year</t>
   </si>
@@ -5035,7 +5036,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5236,6 +5237,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5246,6 +5250,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7276,7 +7290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -8190,7 +8204,7 @@
       <c r="A2" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="125" t="s">
         <v>73</v>
       </c>
       <c r="C2" t="s">
@@ -8213,7 +8227,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="124"/>
+      <c r="B3" s="125"/>
       <c r="C3" t="s">
         <v>154</v>
       </c>
@@ -8235,7 +8249,7 @@
       <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="124"/>
+      <c r="B4" s="125"/>
       <c r="C4" t="s">
         <v>164</v>
       </c>
@@ -8262,7 +8276,7 @@
       <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="125" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8285,7 +8299,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="124"/>
+      <c r="B6" s="125"/>
       <c r="C6" t="s">
         <v>154</v>
       </c>
@@ -8306,7 +8320,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="124"/>
+      <c r="B7" s="125"/>
       <c r="C7" t="s">
         <v>164</v>
       </c>
@@ -8332,7 +8346,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="125" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8355,7 +8369,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="124"/>
+      <c r="B9" s="125"/>
       <c r="C9" t="s">
         <v>154</v>
       </c>
@@ -8376,7 +8390,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="124"/>
+      <c r="B10" s="125"/>
       <c r="C10" t="s">
         <v>164</v>
       </c>
@@ -8401,7 +8415,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="125" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8424,7 +8438,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="124"/>
+      <c r="B12" s="125"/>
       <c r="C12" t="s">
         <v>154</v>
       </c>
@@ -8445,7 +8459,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="124"/>
+      <c r="B13" s="125"/>
       <c r="C13" t="s">
         <v>164</v>
       </c>
@@ -8469,7 +8483,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="125" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8492,7 +8506,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="124"/>
+      <c r="B15" s="125"/>
       <c r="C15" t="s">
         <v>154</v>
       </c>
@@ -8513,7 +8527,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="124"/>
+      <c r="B16" s="125"/>
       <c r="C16" t="s">
         <v>164</v>
       </c>
@@ -8569,7 +8583,7 @@
       <c r="A19" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="124" t="s">
+      <c r="B19" s="125" t="s">
         <v>73</v>
       </c>
       <c r="C19" t="s">
@@ -8592,7 +8606,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="124"/>
+      <c r="B20" s="125"/>
       <c r="C20" t="s">
         <v>154</v>
       </c>
@@ -8613,7 +8627,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="124"/>
+      <c r="B21" s="125"/>
       <c r="C21" t="s">
         <v>164</v>
       </c>
@@ -8639,7 +8653,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="124" t="s">
+      <c r="B22" s="125" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8662,7 +8676,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="124"/>
+      <c r="B23" s="125"/>
       <c r="C23" t="s">
         <v>154</v>
       </c>
@@ -8683,7 +8697,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="124"/>
+      <c r="B24" s="125"/>
       <c r="C24" t="s">
         <v>164</v>
       </c>
@@ -8709,7 +8723,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="124" t="s">
+      <c r="B25" s="125" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8732,7 +8746,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="124"/>
+      <c r="B26" s="125"/>
       <c r="C26" t="s">
         <v>154</v>
       </c>
@@ -8753,7 +8767,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="124"/>
+      <c r="B27" s="125"/>
       <c r="C27" t="s">
         <v>164</v>
       </c>
@@ -8779,7 +8793,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="124" t="s">
+      <c r="B28" s="125" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -8802,7 +8816,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="124"/>
+      <c r="B29" s="125"/>
       <c r="C29" t="s">
         <v>154</v>
       </c>
@@ -8823,7 +8837,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="124"/>
+      <c r="B30" s="125"/>
       <c r="C30" t="s">
         <v>164</v>
       </c>
@@ -8849,7 +8863,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="125" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -8872,7 +8886,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="124"/>
+      <c r="B32" s="125"/>
       <c r="C32" t="s">
         <v>154</v>
       </c>
@@ -8893,7 +8907,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="124"/>
+      <c r="B33" s="125"/>
       <c r="C33" t="s">
         <v>164</v>
       </c>
@@ -8945,7 +8959,7 @@
       <c r="A36" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="125" t="s">
         <v>73</v>
       </c>
       <c r="C36" t="s">
@@ -8968,7 +8982,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="124"/>
+      <c r="B37" s="125"/>
       <c r="C37" t="s">
         <v>154</v>
       </c>
@@ -8989,7 +9003,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="124"/>
+      <c r="B38" s="125"/>
       <c r="C38" t="s">
         <v>164</v>
       </c>
@@ -9010,7 +9024,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="124" t="s">
+      <c r="B39" s="125" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9033,7 +9047,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="124"/>
+      <c r="B40" s="125"/>
       <c r="C40" t="s">
         <v>154</v>
       </c>
@@ -9054,7 +9068,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="124"/>
+      <c r="B41" s="125"/>
       <c r="C41" t="s">
         <v>164</v>
       </c>
@@ -9075,7 +9089,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="124" t="s">
+      <c r="B42" s="125" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9098,7 +9112,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="124"/>
+      <c r="B43" s="125"/>
       <c r="C43" t="s">
         <v>154</v>
       </c>
@@ -9119,7 +9133,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="124"/>
+      <c r="B44" s="125"/>
       <c r="C44" t="s">
         <v>164</v>
       </c>
@@ -9140,7 +9154,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="124" t="s">
+      <c r="B45" s="125" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9163,7 +9177,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="124"/>
+      <c r="B46" s="125"/>
       <c r="C46" t="s">
         <v>154</v>
       </c>
@@ -9184,7 +9198,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="124"/>
+      <c r="B47" s="125"/>
       <c r="C47" t="s">
         <v>164</v>
       </c>
@@ -9205,7 +9219,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="124" t="s">
+      <c r="B48" s="125" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9228,7 +9242,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="124"/>
+      <c r="B49" s="125"/>
       <c r="C49" t="s">
         <v>154</v>
       </c>
@@ -9249,7 +9263,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="124"/>
+      <c r="B50" s="125"/>
       <c r="C50" t="s">
         <v>164</v>
       </c>
@@ -10108,7 +10122,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11657,8 +11671,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13970,8 +13984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14452,19 +14466,19 @@
       <c r="C11" s="120">
         <v>0</v>
       </c>
-      <c r="D11" s="127">
+      <c r="D11" s="128">
         <f>'Baseline year demographics'!$C8</f>
         <v>0.36</v>
       </c>
-      <c r="E11" s="127">
+      <c r="E11" s="128">
         <f>'Baseline year demographics'!$C8</f>
         <v>0.36</v>
       </c>
-      <c r="F11" s="127">
+      <c r="F11" s="128">
         <f>'Baseline year demographics'!$C8</f>
         <v>0.36</v>
       </c>
-      <c r="G11" s="127">
+      <c r="G11" s="128">
         <f>'Baseline year demographics'!$C8</f>
         <v>0.36</v>
       </c>
@@ -15568,16 +15582,16 @@
       <c r="K36" s="45">
         <v>0</v>
       </c>
-      <c r="L36" s="122">
-        <v>1</v>
-      </c>
-      <c r="M36" s="122">
-        <v>1</v>
-      </c>
-      <c r="N36" s="122">
-        <v>1</v>
-      </c>
-      <c r="O36" s="122">
+      <c r="L36" s="123">
+        <v>1</v>
+      </c>
+      <c r="M36" s="123">
+        <v>1</v>
+      </c>
+      <c r="N36" s="123">
+        <v>1</v>
+      </c>
+      <c r="O36" s="123">
         <v>1</v>
       </c>
     </row>
@@ -16088,7 +16102,6 @@
         <v>78</v>
       </c>
       <c r="C49" s="32">
-        <f>'Baseline year demographics'!$C9</f>
         <v>0.1</v>
       </c>
       <c r="D49" s="32">
@@ -16145,8 +16158,7 @@
         <v>144</v>
       </c>
       <c r="C50" s="120">
-        <f>E50</f>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="D50" s="120">
         <v>0</v>
@@ -16201,8 +16213,7 @@
         <v>145</v>
       </c>
       <c r="C51" s="120">
-        <f>E51</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D51" s="120">
         <v>0</v>
@@ -16257,8 +16268,7 @@
         <v>146</v>
       </c>
       <c r="C52" s="120">
-        <f>E52</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D52" s="120">
         <v>0</v>
@@ -16360,11 +16370,2433 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="45">
+        <v>1</v>
+      </c>
+      <c r="D2" s="45">
+        <v>1</v>
+      </c>
+      <c r="E2" s="45">
+        <v>0</v>
+      </c>
+      <c r="F2" s="45">
+        <v>0</v>
+      </c>
+      <c r="G2" s="45">
+        <v>0</v>
+      </c>
+      <c r="H2" s="45">
+        <v>1</v>
+      </c>
+      <c r="I2" s="45">
+        <v>1</v>
+      </c>
+      <c r="J2" s="45">
+        <v>1</v>
+      </c>
+      <c r="K2" s="45">
+        <v>1</v>
+      </c>
+      <c r="L2" s="45">
+        <v>0</v>
+      </c>
+      <c r="M2" s="45">
+        <v>0</v>
+      </c>
+      <c r="N2" s="45">
+        <v>0</v>
+      </c>
+      <c r="O2" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="10"/>
+      <c r="B3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="45">
+        <v>0</v>
+      </c>
+      <c r="D3" s="45">
+        <v>0</v>
+      </c>
+      <c r="E3" s="45">
+        <v>1</v>
+      </c>
+      <c r="F3" s="45">
+        <v>1</v>
+      </c>
+      <c r="G3" s="45">
+        <v>1</v>
+      </c>
+      <c r="H3" s="45">
+        <v>0</v>
+      </c>
+      <c r="I3" s="45">
+        <v>0</v>
+      </c>
+      <c r="J3" s="45">
+        <v>0</v>
+      </c>
+      <c r="K3" s="45">
+        <v>0</v>
+      </c>
+      <c r="L3" s="45">
+        <v>0</v>
+      </c>
+      <c r="M3" s="45">
+        <v>0</v>
+      </c>
+      <c r="N3" s="45">
+        <v>0</v>
+      </c>
+      <c r="O3" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="45">
+        <v>0</v>
+      </c>
+      <c r="D4" s="45">
+        <v>0</v>
+      </c>
+      <c r="E4" s="45">
+        <v>1</v>
+      </c>
+      <c r="F4" s="45">
+        <v>1</v>
+      </c>
+      <c r="G4" s="45">
+        <v>1</v>
+      </c>
+      <c r="H4" s="45">
+        <v>0</v>
+      </c>
+      <c r="I4" s="45">
+        <v>0</v>
+      </c>
+      <c r="J4" s="45">
+        <v>0</v>
+      </c>
+      <c r="K4" s="45">
+        <v>0</v>
+      </c>
+      <c r="L4" s="45">
+        <v>0</v>
+      </c>
+      <c r="M4" s="45">
+        <v>0</v>
+      </c>
+      <c r="N4" s="45">
+        <v>0</v>
+      </c>
+      <c r="O4" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0</v>
+      </c>
+      <c r="D5" s="45">
+        <v>0</v>
+      </c>
+      <c r="E5" s="45">
+        <v>1</v>
+      </c>
+      <c r="F5" s="45">
+        <v>1</v>
+      </c>
+      <c r="G5" s="45">
+        <v>0</v>
+      </c>
+      <c r="H5" s="45">
+        <v>0</v>
+      </c>
+      <c r="I5" s="45">
+        <v>0</v>
+      </c>
+      <c r="J5" s="45">
+        <v>0</v>
+      </c>
+      <c r="K5" s="45">
+        <v>0</v>
+      </c>
+      <c r="L5" s="45">
+        <v>0</v>
+      </c>
+      <c r="M5" s="45">
+        <v>0</v>
+      </c>
+      <c r="N5" s="45">
+        <v>0</v>
+      </c>
+      <c r="O5" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="45">
+        <v>0</v>
+      </c>
+      <c r="D6" s="45">
+        <v>0</v>
+      </c>
+      <c r="E6" s="45">
+        <v>1</v>
+      </c>
+      <c r="F6" s="45">
+        <v>1</v>
+      </c>
+      <c r="G6" s="45">
+        <v>0</v>
+      </c>
+      <c r="H6" s="45">
+        <v>0</v>
+      </c>
+      <c r="I6" s="45">
+        <v>0</v>
+      </c>
+      <c r="J6" s="45">
+        <v>0</v>
+      </c>
+      <c r="K6" s="45">
+        <v>0</v>
+      </c>
+      <c r="L6" s="45">
+        <v>0</v>
+      </c>
+      <c r="M6" s="45">
+        <v>0</v>
+      </c>
+      <c r="N6" s="45">
+        <v>0</v>
+      </c>
+      <c r="O6" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="45">
+        <v>0</v>
+      </c>
+      <c r="D7" s="45">
+        <v>0</v>
+      </c>
+      <c r="E7" s="45">
+        <v>1</v>
+      </c>
+      <c r="F7" s="45">
+        <v>1</v>
+      </c>
+      <c r="G7" s="45">
+        <v>0</v>
+      </c>
+      <c r="H7" s="45">
+        <v>0</v>
+      </c>
+      <c r="I7" s="45">
+        <v>0</v>
+      </c>
+      <c r="J7" s="45">
+        <v>0</v>
+      </c>
+      <c r="K7" s="45">
+        <v>0</v>
+      </c>
+      <c r="L7" s="45">
+        <v>0</v>
+      </c>
+      <c r="M7" s="45">
+        <v>0</v>
+      </c>
+      <c r="N7" s="45">
+        <v>0</v>
+      </c>
+      <c r="O7" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="45">
+        <v>0</v>
+      </c>
+      <c r="D8" s="45">
+        <v>0</v>
+      </c>
+      <c r="E8" s="45">
+        <v>1</v>
+      </c>
+      <c r="F8" s="45">
+        <v>1</v>
+      </c>
+      <c r="G8" s="45">
+        <v>0</v>
+      </c>
+      <c r="H8" s="45">
+        <v>0</v>
+      </c>
+      <c r="I8" s="45">
+        <v>0</v>
+      </c>
+      <c r="J8" s="45">
+        <v>0</v>
+      </c>
+      <c r="K8" s="45">
+        <v>0</v>
+      </c>
+      <c r="L8" s="45">
+        <v>0</v>
+      </c>
+      <c r="M8" s="45">
+        <v>0</v>
+      </c>
+      <c r="N8" s="45">
+        <v>0</v>
+      </c>
+      <c r="O8" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="45">
+        <v>0</v>
+      </c>
+      <c r="D9" s="45">
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <v>1</v>
+      </c>
+      <c r="F9" s="45">
+        <v>1</v>
+      </c>
+      <c r="G9" s="45">
+        <v>1</v>
+      </c>
+      <c r="H9" s="45">
+        <v>0</v>
+      </c>
+      <c r="I9" s="45">
+        <v>0</v>
+      </c>
+      <c r="J9" s="45">
+        <v>0</v>
+      </c>
+      <c r="K9" s="45">
+        <v>0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0</v>
+      </c>
+      <c r="M9" s="45">
+        <v>0</v>
+      </c>
+      <c r="N9" s="45">
+        <v>0</v>
+      </c>
+      <c r="O9" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="45">
+        <v>0</v>
+      </c>
+      <c r="D10" s="45">
+        <v>0</v>
+      </c>
+      <c r="E10" s="45">
+        <v>1</v>
+      </c>
+      <c r="F10" s="45">
+        <v>1</v>
+      </c>
+      <c r="G10" s="45">
+        <v>1</v>
+      </c>
+      <c r="H10" s="45">
+        <v>0</v>
+      </c>
+      <c r="I10" s="45">
+        <v>0</v>
+      </c>
+      <c r="J10" s="45">
+        <v>0</v>
+      </c>
+      <c r="K10" s="45">
+        <v>0</v>
+      </c>
+      <c r="L10" s="45">
+        <v>0</v>
+      </c>
+      <c r="M10" s="45">
+        <v>0</v>
+      </c>
+      <c r="N10" s="45">
+        <v>0</v>
+      </c>
+      <c r="O10" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="122">
+        <v>0</v>
+      </c>
+      <c r="D11" s="122">
+        <v>1</v>
+      </c>
+      <c r="E11" s="45">
+        <v>1</v>
+      </c>
+      <c r="F11" s="45">
+        <v>1</v>
+      </c>
+      <c r="G11" s="122">
+        <v>1</v>
+      </c>
+      <c r="H11" s="45">
+        <v>0</v>
+      </c>
+      <c r="I11" s="45">
+        <v>0</v>
+      </c>
+      <c r="J11" s="45">
+        <v>0</v>
+      </c>
+      <c r="K11" s="45">
+        <v>0</v>
+      </c>
+      <c r="L11" s="45">
+        <v>0</v>
+      </c>
+      <c r="M11" s="45">
+        <v>0</v>
+      </c>
+      <c r="N11" s="45">
+        <v>0</v>
+      </c>
+      <c r="O11" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="122">
+        <v>0</v>
+      </c>
+      <c r="D12" s="122">
+        <v>1</v>
+      </c>
+      <c r="E12" s="122">
+        <v>1</v>
+      </c>
+      <c r="F12" s="122">
+        <v>1</v>
+      </c>
+      <c r="G12" s="122">
+        <v>1</v>
+      </c>
+      <c r="H12" s="45">
+        <v>0</v>
+      </c>
+      <c r="I12" s="45">
+        <v>0</v>
+      </c>
+      <c r="J12" s="45">
+        <v>0</v>
+      </c>
+      <c r="K12" s="45">
+        <v>0</v>
+      </c>
+      <c r="L12" s="45">
+        <v>0</v>
+      </c>
+      <c r="M12" s="45">
+        <v>0</v>
+      </c>
+      <c r="N12" s="45">
+        <v>0</v>
+      </c>
+      <c r="O12" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="122">
+        <v>0</v>
+      </c>
+      <c r="D13" s="122">
+        <v>1</v>
+      </c>
+      <c r="E13" s="122">
+        <v>1</v>
+      </c>
+      <c r="F13" s="122">
+        <v>1</v>
+      </c>
+      <c r="G13" s="122">
+        <v>1</v>
+      </c>
+      <c r="H13" s="45">
+        <v>0</v>
+      </c>
+      <c r="I13" s="45">
+        <v>0</v>
+      </c>
+      <c r="J13" s="45">
+        <v>0</v>
+      </c>
+      <c r="K13" s="45">
+        <v>0</v>
+      </c>
+      <c r="L13" s="45">
+        <v>0</v>
+      </c>
+      <c r="M13" s="45">
+        <v>0</v>
+      </c>
+      <c r="N13" s="45">
+        <v>0</v>
+      </c>
+      <c r="O13" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
+      <c r="K14" s="129"/>
+      <c r="L14" s="129"/>
+      <c r="M14" s="129"/>
+      <c r="N14" s="129"/>
+      <c r="O14" s="129"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="45">
+        <v>0</v>
+      </c>
+      <c r="D15" s="45">
+        <v>0</v>
+      </c>
+      <c r="E15" s="45">
+        <v>0</v>
+      </c>
+      <c r="F15" s="45">
+        <v>0</v>
+      </c>
+      <c r="G15" s="45">
+        <v>0</v>
+      </c>
+      <c r="H15" s="45">
+        <v>1</v>
+      </c>
+      <c r="I15" s="45">
+        <v>1</v>
+      </c>
+      <c r="J15" s="45">
+        <v>1</v>
+      </c>
+      <c r="K15" s="45">
+        <v>1</v>
+      </c>
+      <c r="L15" s="45">
+        <v>0</v>
+      </c>
+      <c r="M15" s="45">
+        <v>0</v>
+      </c>
+      <c r="N15" s="45">
+        <v>0</v>
+      </c>
+      <c r="O15" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="10"/>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="45">
+        <v>0</v>
+      </c>
+      <c r="D16" s="45">
+        <v>0</v>
+      </c>
+      <c r="E16" s="45">
+        <v>0</v>
+      </c>
+      <c r="F16" s="45">
+        <v>0</v>
+      </c>
+      <c r="G16" s="45">
+        <v>0</v>
+      </c>
+      <c r="H16" s="45">
+        <v>1</v>
+      </c>
+      <c r="I16" s="45">
+        <v>1</v>
+      </c>
+      <c r="J16" s="45">
+        <v>1</v>
+      </c>
+      <c r="K16" s="45">
+        <v>1</v>
+      </c>
+      <c r="L16" s="45">
+        <v>0</v>
+      </c>
+      <c r="M16" s="45">
+        <v>0</v>
+      </c>
+      <c r="N16" s="45">
+        <v>0</v>
+      </c>
+      <c r="O16" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="45">
+        <v>0</v>
+      </c>
+      <c r="D17" s="45">
+        <v>0</v>
+      </c>
+      <c r="E17" s="45">
+        <v>0</v>
+      </c>
+      <c r="F17" s="45">
+        <v>0</v>
+      </c>
+      <c r="G17" s="45">
+        <v>0</v>
+      </c>
+      <c r="H17" s="45">
+        <v>1</v>
+      </c>
+      <c r="I17" s="45">
+        <v>1</v>
+      </c>
+      <c r="J17" s="45">
+        <v>1</v>
+      </c>
+      <c r="K17" s="45">
+        <v>1</v>
+      </c>
+      <c r="L17" s="45">
+        <v>0</v>
+      </c>
+      <c r="M17" s="45">
+        <v>0</v>
+      </c>
+      <c r="N17" s="45">
+        <v>0</v>
+      </c>
+      <c r="O17" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="45">
+        <v>0</v>
+      </c>
+      <c r="D18" s="45">
+        <v>0</v>
+      </c>
+      <c r="E18" s="45">
+        <v>0</v>
+      </c>
+      <c r="F18" s="45">
+        <v>0</v>
+      </c>
+      <c r="G18" s="45">
+        <v>0</v>
+      </c>
+      <c r="H18" s="45">
+        <v>1</v>
+      </c>
+      <c r="I18" s="45">
+        <v>1</v>
+      </c>
+      <c r="J18" s="45">
+        <v>1</v>
+      </c>
+      <c r="K18" s="45">
+        <v>1</v>
+      </c>
+      <c r="L18" s="45">
+        <v>0</v>
+      </c>
+      <c r="M18" s="45">
+        <v>0</v>
+      </c>
+      <c r="N18" s="45">
+        <v>0</v>
+      </c>
+      <c r="O18" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="45">
+        <v>0</v>
+      </c>
+      <c r="D19" s="45">
+        <v>0</v>
+      </c>
+      <c r="E19" s="45">
+        <v>0</v>
+      </c>
+      <c r="F19" s="45">
+        <v>0</v>
+      </c>
+      <c r="G19" s="45">
+        <v>0</v>
+      </c>
+      <c r="H19" s="45">
+        <v>1</v>
+      </c>
+      <c r="I19" s="45">
+        <v>1</v>
+      </c>
+      <c r="J19" s="45">
+        <v>1</v>
+      </c>
+      <c r="K19" s="45">
+        <v>1</v>
+      </c>
+      <c r="L19" s="45">
+        <v>0</v>
+      </c>
+      <c r="M19" s="45">
+        <v>0</v>
+      </c>
+      <c r="N19" s="45">
+        <v>0</v>
+      </c>
+      <c r="O19" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="45">
+        <v>0</v>
+      </c>
+      <c r="D20" s="45">
+        <v>0</v>
+      </c>
+      <c r="E20" s="45">
+        <v>0</v>
+      </c>
+      <c r="F20" s="45">
+        <v>0</v>
+      </c>
+      <c r="G20" s="45">
+        <v>0</v>
+      </c>
+      <c r="H20" s="45">
+        <v>1</v>
+      </c>
+      <c r="I20" s="45">
+        <v>1</v>
+      </c>
+      <c r="J20" s="45">
+        <v>1</v>
+      </c>
+      <c r="K20" s="45">
+        <v>1</v>
+      </c>
+      <c r="L20" s="45">
+        <v>0</v>
+      </c>
+      <c r="M20" s="45">
+        <v>0</v>
+      </c>
+      <c r="N20" s="45">
+        <v>0</v>
+      </c>
+      <c r="O20" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="45">
+        <v>1</v>
+      </c>
+      <c r="D21" s="45">
+        <v>1</v>
+      </c>
+      <c r="E21" s="45">
+        <v>1</v>
+      </c>
+      <c r="F21" s="45">
+        <v>1</v>
+      </c>
+      <c r="G21" s="45">
+        <v>1</v>
+      </c>
+      <c r="H21" s="130">
+        <v>0</v>
+      </c>
+      <c r="I21" s="130">
+        <v>0</v>
+      </c>
+      <c r="J21" s="130">
+        <v>0</v>
+      </c>
+      <c r="K21" s="130">
+        <v>0</v>
+      </c>
+      <c r="L21" s="130">
+        <v>0</v>
+      </c>
+      <c r="M21" s="130">
+        <v>0</v>
+      </c>
+      <c r="N21" s="130">
+        <v>0</v>
+      </c>
+      <c r="O21" s="130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="45">
+        <v>1</v>
+      </c>
+      <c r="D22" s="45">
+        <v>1</v>
+      </c>
+      <c r="E22" s="45">
+        <v>1</v>
+      </c>
+      <c r="F22" s="45">
+        <v>1</v>
+      </c>
+      <c r="G22" s="45">
+        <v>1</v>
+      </c>
+      <c r="H22" s="130">
+        <v>0</v>
+      </c>
+      <c r="I22" s="130">
+        <v>0</v>
+      </c>
+      <c r="J22" s="130">
+        <v>0</v>
+      </c>
+      <c r="K22" s="130">
+        <v>0</v>
+      </c>
+      <c r="L22" s="130">
+        <v>0</v>
+      </c>
+      <c r="M22" s="130">
+        <v>0</v>
+      </c>
+      <c r="N22" s="130">
+        <v>0</v>
+      </c>
+      <c r="O22" s="130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="45">
+        <v>1</v>
+      </c>
+      <c r="D23" s="45">
+        <v>1</v>
+      </c>
+      <c r="E23" s="45">
+        <v>1</v>
+      </c>
+      <c r="F23" s="45">
+        <v>1</v>
+      </c>
+      <c r="G23" s="45">
+        <v>1</v>
+      </c>
+      <c r="H23" s="130">
+        <v>0</v>
+      </c>
+      <c r="I23" s="130">
+        <v>0</v>
+      </c>
+      <c r="J23" s="130">
+        <v>0</v>
+      </c>
+      <c r="K23" s="130">
+        <v>0</v>
+      </c>
+      <c r="L23" s="130">
+        <v>0</v>
+      </c>
+      <c r="M23" s="130">
+        <v>0</v>
+      </c>
+      <c r="N23" s="130">
+        <v>0</v>
+      </c>
+      <c r="O23" s="130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
+      <c r="K24" s="129"/>
+      <c r="L24" s="129"/>
+      <c r="M24" s="129"/>
+      <c r="N24" s="129"/>
+      <c r="O24" s="129"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="45">
+        <v>0</v>
+      </c>
+      <c r="D25" s="45">
+        <v>0</v>
+      </c>
+      <c r="E25" s="45">
+        <v>0</v>
+      </c>
+      <c r="F25" s="45">
+        <v>0</v>
+      </c>
+      <c r="G25" s="45">
+        <v>0</v>
+      </c>
+      <c r="H25" s="45">
+        <v>0</v>
+      </c>
+      <c r="I25" s="45">
+        <v>0</v>
+      </c>
+      <c r="J25" s="45">
+        <v>0</v>
+      </c>
+      <c r="K25" s="45">
+        <v>0</v>
+      </c>
+      <c r="L25" s="45">
+        <v>1</v>
+      </c>
+      <c r="M25" s="45">
+        <v>0</v>
+      </c>
+      <c r="N25" s="45">
+        <v>0</v>
+      </c>
+      <c r="O25" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="45">
+        <v>0</v>
+      </c>
+      <c r="D26" s="45">
+        <v>0</v>
+      </c>
+      <c r="E26" s="45">
+        <v>0</v>
+      </c>
+      <c r="F26" s="45">
+        <v>0</v>
+      </c>
+      <c r="G26" s="45">
+        <v>0</v>
+      </c>
+      <c r="H26" s="45">
+        <v>0</v>
+      </c>
+      <c r="I26" s="45">
+        <v>0</v>
+      </c>
+      <c r="J26" s="45">
+        <v>0</v>
+      </c>
+      <c r="K26" s="45">
+        <v>0</v>
+      </c>
+      <c r="L26" s="45">
+        <v>1</v>
+      </c>
+      <c r="M26" s="45">
+        <v>1</v>
+      </c>
+      <c r="N26" s="45">
+        <v>1</v>
+      </c>
+      <c r="O26" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="45">
+        <v>0</v>
+      </c>
+      <c r="D27" s="45">
+        <v>0</v>
+      </c>
+      <c r="E27" s="45">
+        <v>0</v>
+      </c>
+      <c r="F27" s="45">
+        <v>0</v>
+      </c>
+      <c r="G27" s="45">
+        <v>0</v>
+      </c>
+      <c r="H27" s="45">
+        <v>0</v>
+      </c>
+      <c r="I27" s="45">
+        <v>0</v>
+      </c>
+      <c r="J27" s="45">
+        <v>0</v>
+      </c>
+      <c r="K27" s="45">
+        <v>0</v>
+      </c>
+      <c r="L27" s="45">
+        <v>1</v>
+      </c>
+      <c r="M27" s="45">
+        <v>1</v>
+      </c>
+      <c r="N27" s="45">
+        <v>1</v>
+      </c>
+      <c r="O27" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="45">
+        <v>0</v>
+      </c>
+      <c r="D28" s="45">
+        <v>0</v>
+      </c>
+      <c r="E28" s="45">
+        <v>0</v>
+      </c>
+      <c r="F28" s="45">
+        <v>0</v>
+      </c>
+      <c r="G28" s="45">
+        <v>0</v>
+      </c>
+      <c r="H28" s="45">
+        <v>0</v>
+      </c>
+      <c r="I28" s="45">
+        <v>0</v>
+      </c>
+      <c r="J28" s="45">
+        <v>0</v>
+      </c>
+      <c r="K28" s="45">
+        <v>0</v>
+      </c>
+      <c r="L28" s="45">
+        <v>1</v>
+      </c>
+      <c r="M28" s="45">
+        <v>0</v>
+      </c>
+      <c r="N28" s="45">
+        <v>0</v>
+      </c>
+      <c r="O28" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="45">
+        <v>0</v>
+      </c>
+      <c r="D29" s="45">
+        <v>0</v>
+      </c>
+      <c r="E29" s="45">
+        <v>0</v>
+      </c>
+      <c r="F29" s="45">
+        <v>0</v>
+      </c>
+      <c r="G29" s="45">
+        <v>0</v>
+      </c>
+      <c r="H29" s="45">
+        <v>0</v>
+      </c>
+      <c r="I29" s="45">
+        <v>0</v>
+      </c>
+      <c r="J29" s="45">
+        <v>0</v>
+      </c>
+      <c r="K29" s="45">
+        <v>0</v>
+      </c>
+      <c r="L29" s="45">
+        <v>1</v>
+      </c>
+      <c r="M29" s="45">
+        <v>1</v>
+      </c>
+      <c r="N29" s="45">
+        <v>1</v>
+      </c>
+      <c r="O29" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="45">
+        <v>0</v>
+      </c>
+      <c r="D30" s="45">
+        <v>0</v>
+      </c>
+      <c r="E30" s="45">
+        <v>0</v>
+      </c>
+      <c r="F30" s="45">
+        <v>0</v>
+      </c>
+      <c r="G30" s="45">
+        <v>0</v>
+      </c>
+      <c r="H30" s="45">
+        <v>0</v>
+      </c>
+      <c r="I30" s="45">
+        <v>0</v>
+      </c>
+      <c r="J30" s="45">
+        <v>0</v>
+      </c>
+      <c r="K30" s="45">
+        <v>0</v>
+      </c>
+      <c r="L30" s="45">
+        <v>1</v>
+      </c>
+      <c r="M30" s="45">
+        <v>1</v>
+      </c>
+      <c r="N30" s="45">
+        <v>1</v>
+      </c>
+      <c r="O30" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="45">
+        <v>0</v>
+      </c>
+      <c r="D31" s="45">
+        <v>0</v>
+      </c>
+      <c r="E31" s="45">
+        <v>0</v>
+      </c>
+      <c r="F31" s="45">
+        <v>0</v>
+      </c>
+      <c r="G31" s="45">
+        <v>0</v>
+      </c>
+      <c r="H31" s="45">
+        <v>0</v>
+      </c>
+      <c r="I31" s="45">
+        <v>0</v>
+      </c>
+      <c r="J31" s="45">
+        <v>0</v>
+      </c>
+      <c r="K31" s="45">
+        <v>0</v>
+      </c>
+      <c r="L31" s="45">
+        <v>1</v>
+      </c>
+      <c r="M31" s="45">
+        <v>1</v>
+      </c>
+      <c r="N31" s="45">
+        <v>1</v>
+      </c>
+      <c r="O31" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="10"/>
+      <c r="B32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="45">
+        <v>0</v>
+      </c>
+      <c r="D32" s="45">
+        <v>0</v>
+      </c>
+      <c r="E32" s="45">
+        <v>0</v>
+      </c>
+      <c r="F32" s="45">
+        <v>0</v>
+      </c>
+      <c r="G32" s="45">
+        <v>0</v>
+      </c>
+      <c r="H32" s="45">
+        <v>0</v>
+      </c>
+      <c r="I32" s="45">
+        <v>0</v>
+      </c>
+      <c r="J32" s="45">
+        <v>0</v>
+      </c>
+      <c r="K32" s="45">
+        <v>0</v>
+      </c>
+      <c r="L32" s="45">
+        <v>1</v>
+      </c>
+      <c r="M32" s="45">
+        <v>0</v>
+      </c>
+      <c r="N32" s="45">
+        <v>0</v>
+      </c>
+      <c r="O32" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="45">
+        <v>0</v>
+      </c>
+      <c r="D33" s="45">
+        <v>0</v>
+      </c>
+      <c r="E33" s="45">
+        <v>0</v>
+      </c>
+      <c r="F33" s="45">
+        <v>0</v>
+      </c>
+      <c r="G33" s="45">
+        <v>0</v>
+      </c>
+      <c r="H33" s="45">
+        <v>0</v>
+      </c>
+      <c r="I33" s="45">
+        <v>0</v>
+      </c>
+      <c r="J33" s="45">
+        <v>0</v>
+      </c>
+      <c r="K33" s="45">
+        <v>0</v>
+      </c>
+      <c r="L33" s="45">
+        <v>1</v>
+      </c>
+      <c r="M33" s="45">
+        <v>1</v>
+      </c>
+      <c r="N33" s="45">
+        <v>1</v>
+      </c>
+      <c r="O33" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="45">
+        <v>0</v>
+      </c>
+      <c r="D34" s="45">
+        <v>0</v>
+      </c>
+      <c r="E34" s="45">
+        <v>0</v>
+      </c>
+      <c r="F34" s="45">
+        <v>0</v>
+      </c>
+      <c r="G34" s="45">
+        <v>0</v>
+      </c>
+      <c r="H34" s="45">
+        <v>0</v>
+      </c>
+      <c r="I34" s="45">
+        <v>0</v>
+      </c>
+      <c r="J34" s="45">
+        <v>0</v>
+      </c>
+      <c r="K34" s="45">
+        <v>0</v>
+      </c>
+      <c r="L34" s="45">
+        <v>1</v>
+      </c>
+      <c r="M34" s="45">
+        <v>1</v>
+      </c>
+      <c r="N34" s="45">
+        <v>1</v>
+      </c>
+      <c r="O34" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="45">
+        <v>0</v>
+      </c>
+      <c r="D35" s="45">
+        <v>0</v>
+      </c>
+      <c r="E35" s="45">
+        <v>0</v>
+      </c>
+      <c r="F35" s="45">
+        <v>0</v>
+      </c>
+      <c r="G35" s="45">
+        <v>0</v>
+      </c>
+      <c r="H35" s="45">
+        <v>0</v>
+      </c>
+      <c r="I35" s="45">
+        <v>0</v>
+      </c>
+      <c r="J35" s="45">
+        <v>0</v>
+      </c>
+      <c r="K35" s="45">
+        <v>0</v>
+      </c>
+      <c r="L35" s="45">
+        <v>1</v>
+      </c>
+      <c r="M35" s="45">
+        <v>0</v>
+      </c>
+      <c r="N35" s="45">
+        <v>0</v>
+      </c>
+      <c r="O35" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="45">
+        <v>0</v>
+      </c>
+      <c r="D36" s="45">
+        <v>0</v>
+      </c>
+      <c r="E36" s="45">
+        <v>0</v>
+      </c>
+      <c r="F36" s="45">
+        <v>0</v>
+      </c>
+      <c r="G36" s="45">
+        <v>0</v>
+      </c>
+      <c r="H36" s="45">
+        <v>0</v>
+      </c>
+      <c r="I36" s="45">
+        <v>0</v>
+      </c>
+      <c r="J36" s="45">
+        <v>0</v>
+      </c>
+      <c r="K36" s="45">
+        <v>0</v>
+      </c>
+      <c r="L36" s="45">
+        <v>1</v>
+      </c>
+      <c r="M36" s="45">
+        <v>1</v>
+      </c>
+      <c r="N36" s="45">
+        <v>1</v>
+      </c>
+      <c r="O36" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="45">
+        <v>0</v>
+      </c>
+      <c r="D37" s="45">
+        <v>0</v>
+      </c>
+      <c r="E37" s="45">
+        <v>0</v>
+      </c>
+      <c r="F37" s="45">
+        <v>0</v>
+      </c>
+      <c r="G37" s="45">
+        <v>0</v>
+      </c>
+      <c r="H37" s="45">
+        <v>0</v>
+      </c>
+      <c r="I37" s="45">
+        <v>0</v>
+      </c>
+      <c r="J37" s="45">
+        <v>0</v>
+      </c>
+      <c r="K37" s="45">
+        <v>0</v>
+      </c>
+      <c r="L37" s="45">
+        <v>1</v>
+      </c>
+      <c r="M37" s="45">
+        <v>1</v>
+      </c>
+      <c r="N37" s="45">
+        <v>1</v>
+      </c>
+      <c r="O37" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="45">
+        <v>0</v>
+      </c>
+      <c r="D38" s="45">
+        <v>0</v>
+      </c>
+      <c r="E38" s="45">
+        <v>0</v>
+      </c>
+      <c r="F38" s="45">
+        <v>0</v>
+      </c>
+      <c r="G38" s="45">
+        <v>0</v>
+      </c>
+      <c r="H38" s="45">
+        <v>0</v>
+      </c>
+      <c r="I38" s="45">
+        <v>0</v>
+      </c>
+      <c r="J38" s="45">
+        <v>0</v>
+      </c>
+      <c r="K38" s="45">
+        <v>0</v>
+      </c>
+      <c r="L38" s="45">
+        <v>1</v>
+      </c>
+      <c r="M38" s="45">
+        <v>1</v>
+      </c>
+      <c r="N38" s="45">
+        <v>1</v>
+      </c>
+      <c r="O38" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="45">
+        <v>0</v>
+      </c>
+      <c r="D39" s="45">
+        <v>0</v>
+      </c>
+      <c r="E39" s="45">
+        <v>0</v>
+      </c>
+      <c r="F39" s="45">
+        <v>0</v>
+      </c>
+      <c r="G39" s="45">
+        <v>0</v>
+      </c>
+      <c r="H39" s="45">
+        <v>0</v>
+      </c>
+      <c r="I39" s="45">
+        <v>0</v>
+      </c>
+      <c r="J39" s="45">
+        <v>0</v>
+      </c>
+      <c r="K39" s="45">
+        <v>0</v>
+      </c>
+      <c r="L39" s="130">
+        <v>1</v>
+      </c>
+      <c r="M39" s="130">
+        <v>1</v>
+      </c>
+      <c r="N39" s="130">
+        <v>1</v>
+      </c>
+      <c r="O39" s="130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C40" s="45">
+        <v>0</v>
+      </c>
+      <c r="D40" s="45">
+        <v>0</v>
+      </c>
+      <c r="E40" s="45">
+        <v>0</v>
+      </c>
+      <c r="F40" s="45">
+        <v>0</v>
+      </c>
+      <c r="G40" s="45">
+        <v>0</v>
+      </c>
+      <c r="H40" s="45">
+        <v>0</v>
+      </c>
+      <c r="I40" s="45">
+        <v>0</v>
+      </c>
+      <c r="J40" s="45">
+        <v>0</v>
+      </c>
+      <c r="K40" s="45">
+        <v>0</v>
+      </c>
+      <c r="L40" s="45">
+        <v>1</v>
+      </c>
+      <c r="M40" s="45">
+        <v>1</v>
+      </c>
+      <c r="N40" s="45">
+        <v>1</v>
+      </c>
+      <c r="O40" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="12"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="131"/>
+      <c r="F41" s="131"/>
+      <c r="G41" s="131"/>
+      <c r="H41" s="131"/>
+      <c r="I41" s="131"/>
+      <c r="J41" s="129"/>
+      <c r="K41" s="129"/>
+      <c r="L41" s="129"/>
+      <c r="M41" s="129"/>
+      <c r="N41" s="129"/>
+      <c r="O41" s="129"/>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>257</v>
+      </c>
+      <c r="C42" s="45">
+        <v>1</v>
+      </c>
+      <c r="D42" s="45">
+        <v>1</v>
+      </c>
+      <c r="E42" s="45">
+        <v>1</v>
+      </c>
+      <c r="F42" s="45">
+        <v>1</v>
+      </c>
+      <c r="G42" s="45">
+        <v>1</v>
+      </c>
+      <c r="H42" s="45">
+        <v>1</v>
+      </c>
+      <c r="I42" s="45">
+        <v>1</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>1</v>
+      </c>
+      <c r="L42" s="45">
+        <v>1</v>
+      </c>
+      <c r="M42" s="45">
+        <v>1</v>
+      </c>
+      <c r="N42" s="45">
+        <v>1</v>
+      </c>
+      <c r="O42" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" t="s">
+        <v>258</v>
+      </c>
+      <c r="C43" s="45">
+        <v>1</v>
+      </c>
+      <c r="D43" s="45">
+        <v>1</v>
+      </c>
+      <c r="E43" s="45">
+        <v>1</v>
+      </c>
+      <c r="F43" s="45">
+        <v>1</v>
+      </c>
+      <c r="G43" s="45">
+        <v>1</v>
+      </c>
+      <c r="H43" s="45">
+        <v>1</v>
+      </c>
+      <c r="I43" s="45">
+        <v>1</v>
+      </c>
+      <c r="J43" s="45">
+        <v>1</v>
+      </c>
+      <c r="K43" s="45">
+        <v>1</v>
+      </c>
+      <c r="L43" s="45">
+        <v>1</v>
+      </c>
+      <c r="M43" s="45">
+        <v>1</v>
+      </c>
+      <c r="N43" s="45">
+        <v>1</v>
+      </c>
+      <c r="O43" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C44" s="45">
+        <v>1</v>
+      </c>
+      <c r="D44" s="45">
+        <v>1</v>
+      </c>
+      <c r="E44" s="45">
+        <v>1</v>
+      </c>
+      <c r="F44" s="45">
+        <v>1</v>
+      </c>
+      <c r="G44" s="45">
+        <v>1</v>
+      </c>
+      <c r="H44" s="45">
+        <v>1</v>
+      </c>
+      <c r="I44" s="45">
+        <v>1</v>
+      </c>
+      <c r="J44" s="45">
+        <v>1</v>
+      </c>
+      <c r="K44" s="45">
+        <v>1</v>
+      </c>
+      <c r="L44" s="45">
+        <v>1</v>
+      </c>
+      <c r="M44" s="45">
+        <v>1</v>
+      </c>
+      <c r="N44" s="45">
+        <v>1</v>
+      </c>
+      <c r="O44" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" t="s">
+        <v>260</v>
+      </c>
+      <c r="C45" s="45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="45">
+        <v>1</v>
+      </c>
+      <c r="G45" s="45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="45">
+        <v>1</v>
+      </c>
+      <c r="I45" s="45">
+        <v>1</v>
+      </c>
+      <c r="J45" s="45">
+        <v>1</v>
+      </c>
+      <c r="K45" s="45">
+        <v>1</v>
+      </c>
+      <c r="L45" s="45">
+        <v>1</v>
+      </c>
+      <c r="M45" s="45">
+        <v>1</v>
+      </c>
+      <c r="N45" s="45">
+        <v>1</v>
+      </c>
+      <c r="O45" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" t="s">
+        <v>261</v>
+      </c>
+      <c r="C46" s="45">
+        <v>1</v>
+      </c>
+      <c r="D46" s="45">
+        <v>1</v>
+      </c>
+      <c r="E46" s="45">
+        <v>1</v>
+      </c>
+      <c r="F46" s="45">
+        <v>1</v>
+      </c>
+      <c r="G46" s="45">
+        <v>1</v>
+      </c>
+      <c r="H46" s="45">
+        <v>1</v>
+      </c>
+      <c r="I46" s="45">
+        <v>1</v>
+      </c>
+      <c r="J46" s="45">
+        <v>1</v>
+      </c>
+      <c r="K46" s="45">
+        <v>1</v>
+      </c>
+      <c r="L46" s="45">
+        <v>1</v>
+      </c>
+      <c r="M46" s="45">
+        <v>1</v>
+      </c>
+      <c r="N46" s="45">
+        <v>1</v>
+      </c>
+      <c r="O46" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" t="s">
+        <v>262</v>
+      </c>
+      <c r="C47" s="45">
+        <v>1</v>
+      </c>
+      <c r="D47" s="45">
+        <v>1</v>
+      </c>
+      <c r="E47" s="45">
+        <v>1</v>
+      </c>
+      <c r="F47" s="45">
+        <v>1</v>
+      </c>
+      <c r="G47" s="45">
+        <v>1</v>
+      </c>
+      <c r="H47" s="45">
+        <v>0</v>
+      </c>
+      <c r="I47" s="45">
+        <v>0</v>
+      </c>
+      <c r="J47" s="45">
+        <v>0</v>
+      </c>
+      <c r="K47" s="45">
+        <v>0</v>
+      </c>
+      <c r="L47" s="45">
+        <v>0</v>
+      </c>
+      <c r="M47" s="45">
+        <v>0</v>
+      </c>
+      <c r="N47" s="45">
+        <v>0</v>
+      </c>
+      <c r="O47" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" t="s">
+        <v>263</v>
+      </c>
+      <c r="C48" s="45">
+        <v>1</v>
+      </c>
+      <c r="D48" s="45">
+        <v>1</v>
+      </c>
+      <c r="E48" s="45">
+        <v>1</v>
+      </c>
+      <c r="F48" s="45">
+        <v>1</v>
+      </c>
+      <c r="G48" s="45">
+        <v>1</v>
+      </c>
+      <c r="H48" s="45">
+        <v>0</v>
+      </c>
+      <c r="I48" s="45">
+        <v>0</v>
+      </c>
+      <c r="J48" s="45">
+        <v>0</v>
+      </c>
+      <c r="K48" s="45">
+        <v>0</v>
+      </c>
+      <c r="L48" s="45">
+        <v>0</v>
+      </c>
+      <c r="M48" s="45">
+        <v>0</v>
+      </c>
+      <c r="N48" s="45">
+        <v>0</v>
+      </c>
+      <c r="O48" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C49" s="45">
+        <v>0</v>
+      </c>
+      <c r="D49" s="45">
+        <v>0</v>
+      </c>
+      <c r="E49" s="45">
+        <v>0</v>
+      </c>
+      <c r="F49" s="45">
+        <v>0</v>
+      </c>
+      <c r="G49" s="45">
+        <v>0</v>
+      </c>
+      <c r="H49" s="45">
+        <v>1</v>
+      </c>
+      <c r="I49" s="45">
+        <v>1</v>
+      </c>
+      <c r="J49" s="45">
+        <v>1</v>
+      </c>
+      <c r="K49" s="45">
+        <v>1</v>
+      </c>
+      <c r="L49" s="45">
+        <v>0</v>
+      </c>
+      <c r="M49" s="45">
+        <v>0</v>
+      </c>
+      <c r="N49" s="45">
+        <v>0</v>
+      </c>
+      <c r="O49" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="45">
+        <v>0</v>
+      </c>
+      <c r="D50" s="45">
+        <v>0</v>
+      </c>
+      <c r="E50" s="45">
+        <v>0</v>
+      </c>
+      <c r="F50" s="45">
+        <v>0</v>
+      </c>
+      <c r="G50" s="45">
+        <v>0</v>
+      </c>
+      <c r="H50" s="45">
+        <v>1</v>
+      </c>
+      <c r="I50" s="45">
+        <v>1</v>
+      </c>
+      <c r="J50" s="45">
+        <v>1</v>
+      </c>
+      <c r="K50" s="45">
+        <v>1</v>
+      </c>
+      <c r="L50" s="45">
+        <v>0</v>
+      </c>
+      <c r="M50" s="45">
+        <v>0</v>
+      </c>
+      <c r="N50" s="45">
+        <v>0</v>
+      </c>
+      <c r="O50" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" s="45">
+        <v>0</v>
+      </c>
+      <c r="D51" s="45">
+        <v>0</v>
+      </c>
+      <c r="E51" s="45">
+        <v>0</v>
+      </c>
+      <c r="F51" s="45">
+        <v>0</v>
+      </c>
+      <c r="G51" s="45">
+        <v>0</v>
+      </c>
+      <c r="H51" s="45">
+        <v>1</v>
+      </c>
+      <c r="I51" s="45">
+        <v>1</v>
+      </c>
+      <c r="J51" s="45">
+        <v>1</v>
+      </c>
+      <c r="K51" s="45">
+        <v>1</v>
+      </c>
+      <c r="L51" s="45">
+        <v>0</v>
+      </c>
+      <c r="M51" s="45">
+        <v>0</v>
+      </c>
+      <c r="N51" s="45">
+        <v>0</v>
+      </c>
+      <c r="O51" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="11"/>
+      <c r="B52" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="130">
+        <v>1</v>
+      </c>
+      <c r="D52" s="130">
+        <v>1</v>
+      </c>
+      <c r="E52" s="130">
+        <v>1</v>
+      </c>
+      <c r="F52" s="130">
+        <v>1</v>
+      </c>
+      <c r="G52" s="130">
+        <v>1</v>
+      </c>
+      <c r="H52" s="130">
+        <v>1</v>
+      </c>
+      <c r="I52" s="130">
+        <v>1</v>
+      </c>
+      <c r="J52" s="130">
+        <v>1</v>
+      </c>
+      <c r="K52" s="130">
+        <v>1</v>
+      </c>
+      <c r="L52" s="130">
+        <v>1</v>
+      </c>
+      <c r="M52" s="130">
+        <v>1</v>
+      </c>
+      <c r="N52" s="130">
+        <v>1</v>
+      </c>
+      <c r="O52" s="130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B53" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="122">
+        <v>1</v>
+      </c>
+      <c r="D53" s="122">
+        <v>0</v>
+      </c>
+      <c r="E53" s="132">
+        <v>1</v>
+      </c>
+      <c r="F53" s="132">
+        <v>1</v>
+      </c>
+      <c r="G53" s="132">
+        <v>1</v>
+      </c>
+      <c r="H53" s="132">
+        <v>1</v>
+      </c>
+      <c r="I53" s="132">
+        <v>1</v>
+      </c>
+      <c r="J53" s="132">
+        <v>1</v>
+      </c>
+      <c r="K53" s="132">
+        <v>1</v>
+      </c>
+      <c r="L53" s="132">
+        <v>1</v>
+      </c>
+      <c r="M53" s="132">
+        <v>1</v>
+      </c>
+      <c r="N53" s="132">
+        <v>1</v>
+      </c>
+      <c r="O53" s="132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="122">
+        <v>1</v>
+      </c>
+      <c r="D54" s="122">
+        <v>0</v>
+      </c>
+      <c r="E54" s="122">
+        <v>1</v>
+      </c>
+      <c r="F54" s="122">
+        <v>1</v>
+      </c>
+      <c r="G54" s="122">
+        <v>1</v>
+      </c>
+      <c r="H54" s="122">
+        <v>1</v>
+      </c>
+      <c r="I54" s="122">
+        <v>1</v>
+      </c>
+      <c r="J54" s="122">
+        <v>1</v>
+      </c>
+      <c r="K54" s="122">
+        <v>1</v>
+      </c>
+      <c r="L54" s="122">
+        <v>1</v>
+      </c>
+      <c r="M54" s="122">
+        <v>1</v>
+      </c>
+      <c r="N54" s="122">
+        <v>1</v>
+      </c>
+      <c r="O54" s="122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="122">
+        <v>1</v>
+      </c>
+      <c r="D55" s="122">
+        <v>0</v>
+      </c>
+      <c r="E55" s="122">
+        <v>1</v>
+      </c>
+      <c r="F55" s="122">
+        <v>1</v>
+      </c>
+      <c r="G55" s="122">
+        <v>1</v>
+      </c>
+      <c r="H55" s="122">
+        <v>1</v>
+      </c>
+      <c r="I55" s="122">
+        <v>1</v>
+      </c>
+      <c r="J55" s="122">
+        <v>1</v>
+      </c>
+      <c r="K55" s="122">
+        <v>1</v>
+      </c>
+      <c r="L55" s="122">
+        <v>1</v>
+      </c>
+      <c r="M55" s="122">
+        <v>1</v>
+      </c>
+      <c r="N55" s="122">
+        <v>1</v>
+      </c>
+      <c r="O55" s="122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="32">
+        <v>1</v>
+      </c>
+      <c r="F56" s="32">
+        <v>1</v>
+      </c>
+      <c r="G56" s="32">
+        <v>1</v>
+      </c>
+      <c r="H56" s="32">
+        <v>1</v>
+      </c>
+      <c r="I56" s="32">
+        <v>1</v>
+      </c>
+      <c r="J56" s="32">
+        <v>1</v>
+      </c>
+      <c r="K56" s="32">
+        <v>1</v>
+      </c>
+      <c r="L56" s="32">
+        <v>1</v>
+      </c>
+      <c r="M56" s="32">
+        <v>1</v>
+      </c>
+      <c r="N56" s="32">
+        <v>1</v>
+      </c>
+      <c r="O56" s="32">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16665,12 +19097,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17184,7 +19616,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A52" s="125" t="s">
+      <c r="A52" s="126" t="s">
         <v>161</v>
       </c>
       <c r="B52" t="s">
@@ -17195,7 +19627,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A53" s="125" t="s">
+      <c r="A53" s="126" t="s">
         <v>162</v>
       </c>
       <c r="B53" t="s">
@@ -17206,7 +19638,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A54" s="125" t="s">
+      <c r="A54" s="126" t="s">
         <v>163</v>
       </c>
       <c r="B54" t="s">
@@ -17221,7 +19653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -17509,12 +19941,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17554,7 +19986,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="124" t="s">
         <v>267</v>
       </c>
       <c r="B3" s="91">
@@ -18279,12 +20711,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B41"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18510,17 +20942,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="126" t="s">
+      <c r="A28" s="127" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="126" t="s">
+      <c r="A29" s="127" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="126" t="s">
+      <c r="A30" s="127" t="s">
         <v>80</v>
       </c>
     </row>
@@ -18693,17 +21125,17 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="125" t="s">
+      <c r="A52" s="126" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="125" t="s">
+      <c r="A53" s="126" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="125" t="s">
+      <c r="A54" s="126" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for BF update
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="-60" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="22" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3149,7 +3149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="269">
   <si>
     <t>year</t>
   </si>
@@ -9308,6 +9308,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9318,11 +9323,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9333,7 +9333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
+    <sheetView zoomScale="178" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -20723,8 +20723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20745,391 +20745,250 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>267</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B4" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>185</v>
       </c>
-      <c r="B6" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B7" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B8" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B9" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>124</v>
       </c>
-      <c r="B10" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>132</v>
       </c>
-      <c r="B11" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
-      <c r="B12" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>133</v>
       </c>
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>126</v>
       </c>
-      <c r="B14" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>134</v>
       </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
-      <c r="B16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>131</v>
       </c>
-      <c r="B17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>121</v>
       </c>
-      <c r="B18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>129</v>
       </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>122</v>
       </c>
-      <c r="B20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>120</v>
       </c>
-      <c r="B22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>128</v>
       </c>
-      <c r="B23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>119</v>
       </c>
-      <c r="B24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="126" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="126" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="126" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>135</v>
       </c>
-      <c r="B34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>138</v>
       </c>
-      <c r="B35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>262</v>
       </c>
-      <c r="B36" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B37" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B41" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>261</v>
       </c>
-      <c r="B45" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>260</v>
       </c>
-      <c r="B46" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>259</v>
       </c>
-      <c r="B47" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>257</v>
-      </c>
-      <c r="B48" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>258</v>
       </c>
-      <c r="B49" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>263</v>
       </c>
-      <c r="B50" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="B51" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Removed external links in workbook
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="22" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="21" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -9308,11 +9308,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9323,6 +9318,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -19953,8 +19953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20574,7 +20574,7 @@
       </c>
       <c r="D42" s="19">
         <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
-        <v>0.10046400000000001</v>
+        <v>10.046400000000002</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -20589,7 +20589,7 @@
       </c>
       <c r="D43" s="19">
         <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
-        <v>0.19933477199999997</v>
+        <v>19.933477200000002</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -20723,7 +20723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -22085,7 +22085,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22175,24 +22175,24 @@
         <v>147</v>
       </c>
       <c r="B5" s="46">
-        <f>Distributions!C10/100 * 2.6</f>
-        <v>3.9000000000000003E-3</v>
+        <f>Distributions!C10 * 2.6</f>
+        <v>0.39</v>
       </c>
       <c r="C5" s="46">
-        <f>Distributions!D10/100 * 2.6</f>
-        <v>3.9000000000000003E-3</v>
+        <f>Distributions!D10 * 2.6</f>
+        <v>0.39</v>
       </c>
       <c r="D5" s="46">
-        <f>Distributions!E10/100 * 2.6</f>
-        <v>3.3540000000000006E-3</v>
+        <f>Distributions!E10 * 2.6</f>
+        <v>0.33540000000000003</v>
       </c>
       <c r="E5" s="46">
-        <f>Distributions!F10/100 * 2.6</f>
-        <v>2.8600000000000001E-3</v>
+        <f>Distributions!F10 * 2.6</f>
+        <v>0.28600000000000003</v>
       </c>
       <c r="F5" s="46">
-        <f>Distributions!G10/100 * 2.6</f>
-        <v>2.7299999999999998E-3</v>
+        <f>Distributions!G10 * 2.6</f>
+        <v>0.27300000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -22200,24 +22200,24 @@
         <v>148</v>
       </c>
       <c r="B6" s="46">
-        <f>Distributions!C11/100 * 2.6</f>
-        <v>1.274E-3</v>
+        <f>Distributions!C11 * 2.6</f>
+        <v>0.12740000000000001</v>
       </c>
       <c r="C6" s="46">
-        <f>Distributions!D11/100 * 2.6</f>
-        <v>1.274E-3</v>
+        <f>Distributions!D11 * 2.6</f>
+        <v>0.12740000000000001</v>
       </c>
       <c r="D6" s="46">
-        <f>Distributions!E11/100 * 2.6</f>
-        <v>1.3780000000000001E-3</v>
+        <f>Distributions!E11 * 2.6</f>
+        <v>0.13780000000000001</v>
       </c>
       <c r="E6" s="46">
-        <f>Distributions!F11/100 * 2.6</f>
-        <v>1.0659999999999999E-3</v>
+        <f>Distributions!F11 * 2.6</f>
+        <v>0.10659999999999999</v>
       </c>
       <c r="F6" s="46">
-        <f>Distributions!G11/100 * 2.6</f>
-        <v>5.4600000000000004E-4</v>
+        <f>Distributions!G11 * 2.6</f>
+        <v>5.4600000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -22581,7 +22581,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updates to Bangladesh workbook
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="23" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="23" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,13 @@
     <sheet name="Program risk areas" sheetId="36" r:id="rId25"/>
     <sheet name="Population risk areas" sheetId="43" r:id="rId26"/>
     <sheet name="Programs cost and coverage" sheetId="20" r:id="rId27"/>
-    <sheet name="Reference programs" sheetId="48" r:id="rId28"/>
-    <sheet name="Programs to include" sheetId="44" r:id="rId29"/>
+    <sheet name="Programs annual spending" sheetId="49" r:id="rId28"/>
+    <sheet name="Reference programs" sheetId="48" r:id="rId29"/>
+    <sheet name="Programs to include" sheetId="44" r:id="rId30"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId31"/>
+  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -2439,6 +2443,54 @@
 </comments>
 </file>
 
+<file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D1465BC3-7A72-4A4A-932E-23AE61C586FF}">
+      <text>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="12"/>
+            <color rgb="FF7F7F7F"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This is the calibration year and uses baseline coverage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
@@ -2819,6 +2871,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Nick:
 Any breastfeeding. Other categories don't matter for this age upwards as relative risks are the same.</t>
@@ -3150,7 +3203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -3961,6 +4014,15 @@
   <si>
     <t>Calculated in model</t>
   </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Spending</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
 </sst>
 </file>
 
@@ -3972,7 +4034,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4095,6 +4157,22 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -5263,13 +5341,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="725">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7091,6 +7169,351 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Baseline year demographics"/>
+      <sheetName val="Demographic projections"/>
+      <sheetName val="Causes of death"/>
+      <sheetName val="Incidence of conditions"/>
+      <sheetName val="Prevalence of anaemia"/>
+      <sheetName val="Distributions"/>
+      <sheetName val="Distribution births"/>
+      <sheetName val="Birth outcomes &amp; risks"/>
+      <sheetName val="Relative risks"/>
+      <sheetName val="Odds ratios"/>
+      <sheetName val="IYCF package odds ratios"/>
+      <sheetName val="IYCF packages"/>
+      <sheetName val="IYCF cost &amp; coverage"/>
+      <sheetName val="Appropriate breastfeeding"/>
+      <sheetName val="Programs birth outcomes"/>
+      <sheetName val="Programs anemia"/>
+      <sheetName val="Programs wasting"/>
+      <sheetName val="Programs for children"/>
+      <sheetName val="Programs family planning"/>
+      <sheetName val="Programs for PW"/>
+      <sheetName val="Programs birth age"/>
+      <sheetName val="Programs target population"/>
+      <sheetName val="Programs impacted population"/>
+      <sheetName val="Program dependencies"/>
+      <sheetName val="Program risk areas"/>
+      <sheetName val="Population risk areas"/>
+      <sheetName val="Programs annual scale-up"/>
+      <sheetName val="Programs annual spending"/>
+      <sheetName val="Programs cost and coverage"/>
+      <sheetName val="Reference programs"/>
+      <sheetName val="Programs to include"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="C2">
+            <v>2016</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Balanced energy-protein supplementation</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Birth age program</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Calcium supplementation</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Cash transfers</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Family Planning</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>IFA fortification of maize</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>IFA fortification of rice</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>IFA fortification of wheat flour</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>IFAS not poor: community</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>IFAS not poor: community (malaria area)</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>IFAS not poor: hospital</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>IFAS not poor: hospital (malaria area)</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>IFAS not poor: retailer</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>IFAS not poor: retailer (malaria area)</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>IFAS not poor: school</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>IFAS not poor: school (malaria area)</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>IFAS poor: community</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>IFAS poor: community (malaria area)</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>IFAS poor: hospital</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>IFAS poor: hospital (malaria area)</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>IFAS poor: school</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>IFAS poor: school (malaria area)</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>IPTp</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>Iron and folic acid supplementation for pregnant women</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>Iron and iodine fortification of salt</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>Iron fortification of maize</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>Iron fortification of rice</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Iron fortification of wheat flour</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>Long-lasting insecticide-treated bednets</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>Mg for eclampsia</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>Mg for pre-eclampsia</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>Multiple micronutrient supplementation</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>Multiple micronutrient supplementation (malaria area)</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>Oral rehydration salts</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>Public provision of complementary foods</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>Public provision of complementary foods with iron</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Public provision of complementary foods with iron (malaria area)</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>Sprinkles</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>Sprinkles (malaria area)</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>Treatment of MAM</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>Treatment of SAM</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>Vitamin A supplementation</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>WASH: Handwashing</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>WASH: Hygenic disposal</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>WASH: Improved sanitation</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>WASH: Improved water source</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>WASH: Piped water</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>Zinc for treatment + ORS</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>Zinc supplementation</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>IYCF 1</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>IYCF 2</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>IYCF 3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8329,7 +8752,7 @@
       <c r="A2" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="136" t="s">
         <v>73</v>
       </c>
       <c r="C2" t="s">
@@ -8352,7 +8775,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="132"/>
+      <c r="B3" s="136"/>
       <c r="C3" t="s">
         <v>154</v>
       </c>
@@ -8374,7 +8797,7 @@
       <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="132"/>
+      <c r="B4" s="136"/>
       <c r="C4" t="s">
         <v>164</v>
       </c>
@@ -8401,7 +8824,7 @@
       <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="132" t="s">
+      <c r="B5" s="136" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8424,7 +8847,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="132"/>
+      <c r="B6" s="136"/>
       <c r="C6" t="s">
         <v>154</v>
       </c>
@@ -8445,7 +8868,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="132"/>
+      <c r="B7" s="136"/>
       <c r="C7" t="s">
         <v>164</v>
       </c>
@@ -8471,7 +8894,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="136" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8494,7 +8917,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="132"/>
+      <c r="B9" s="136"/>
       <c r="C9" t="s">
         <v>154</v>
       </c>
@@ -8515,7 +8938,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="132"/>
+      <c r="B10" s="136"/>
       <c r="C10" t="s">
         <v>164</v>
       </c>
@@ -8540,7 +8963,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="136" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8563,7 +8986,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="132"/>
+      <c r="B12" s="136"/>
       <c r="C12" t="s">
         <v>154</v>
       </c>
@@ -8584,7 +9007,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="132"/>
+      <c r="B13" s="136"/>
       <c r="C13" t="s">
         <v>164</v>
       </c>
@@ -8608,7 +9031,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="136" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8631,7 +9054,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="132"/>
+      <c r="B15" s="136"/>
       <c r="C15" t="s">
         <v>154</v>
       </c>
@@ -8652,7 +9075,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="132"/>
+      <c r="B16" s="136"/>
       <c r="C16" t="s">
         <v>164</v>
       </c>
@@ -8708,7 +9131,7 @@
       <c r="A19" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="132" t="s">
+      <c r="B19" s="136" t="s">
         <v>73</v>
       </c>
       <c r="C19" t="s">
@@ -8731,7 +9154,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="132"/>
+      <c r="B20" s="136"/>
       <c r="C20" t="s">
         <v>154</v>
       </c>
@@ -8752,7 +9175,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="132"/>
+      <c r="B21" s="136"/>
       <c r="C21" t="s">
         <v>164</v>
       </c>
@@ -8778,7 +9201,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="132" t="s">
+      <c r="B22" s="136" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8801,7 +9224,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="132"/>
+      <c r="B23" s="136"/>
       <c r="C23" t="s">
         <v>154</v>
       </c>
@@ -8822,7 +9245,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="132"/>
+      <c r="B24" s="136"/>
       <c r="C24" t="s">
         <v>164</v>
       </c>
@@ -8848,7 +9271,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="132" t="s">
+      <c r="B25" s="136" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8871,7 +9294,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="132"/>
+      <c r="B26" s="136"/>
       <c r="C26" t="s">
         <v>154</v>
       </c>
@@ -8892,7 +9315,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="132"/>
+      <c r="B27" s="136"/>
       <c r="C27" t="s">
         <v>164</v>
       </c>
@@ -8918,7 +9341,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="132" t="s">
+      <c r="B28" s="136" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -8941,7 +9364,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="132"/>
+      <c r="B29" s="136"/>
       <c r="C29" t="s">
         <v>154</v>
       </c>
@@ -8962,7 +9385,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="132"/>
+      <c r="B30" s="136"/>
       <c r="C30" t="s">
         <v>164</v>
       </c>
@@ -8988,7 +9411,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="132" t="s">
+      <c r="B31" s="136" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9011,7 +9434,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="132"/>
+      <c r="B32" s="136"/>
       <c r="C32" t="s">
         <v>154</v>
       </c>
@@ -9032,7 +9455,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="132"/>
+      <c r="B33" s="136"/>
       <c r="C33" t="s">
         <v>164</v>
       </c>
@@ -9084,7 +9507,7 @@
       <c r="A36" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="132" t="s">
+      <c r="B36" s="136" t="s">
         <v>73</v>
       </c>
       <c r="C36" t="s">
@@ -9107,7 +9530,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="132"/>
+      <c r="B37" s="136"/>
       <c r="C37" t="s">
         <v>154</v>
       </c>
@@ -9128,7 +9551,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="132"/>
+      <c r="B38" s="136"/>
       <c r="C38" t="s">
         <v>164</v>
       </c>
@@ -9149,7 +9572,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="132" t="s">
+      <c r="B39" s="136" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9172,7 +9595,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="132"/>
+      <c r="B40" s="136"/>
       <c r="C40" t="s">
         <v>154</v>
       </c>
@@ -9193,7 +9616,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="132"/>
+      <c r="B41" s="136"/>
       <c r="C41" t="s">
         <v>164</v>
       </c>
@@ -9214,7 +9637,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="132" t="s">
+      <c r="B42" s="136" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9237,7 +9660,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="132"/>
+      <c r="B43" s="136"/>
       <c r="C43" t="s">
         <v>154</v>
       </c>
@@ -9258,7 +9681,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="132"/>
+      <c r="B44" s="136"/>
       <c r="C44" t="s">
         <v>164</v>
       </c>
@@ -9279,7 +9702,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="132" t="s">
+      <c r="B45" s="136" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9302,7 +9725,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="132"/>
+      <c r="B46" s="136"/>
       <c r="C46" t="s">
         <v>154</v>
       </c>
@@ -9323,7 +9746,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="132"/>
+      <c r="B47" s="136"/>
       <c r="C47" t="s">
         <v>164</v>
       </c>
@@ -9344,7 +9767,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="132" t="s">
+      <c r="B48" s="136" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9367,7 +9790,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="132"/>
+      <c r="B49" s="136"/>
       <c r="C49" t="s">
         <v>154</v>
       </c>
@@ -9388,7 +9811,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="132"/>
+      <c r="B50" s="136"/>
       <c r="C50" t="s">
         <v>164</v>
       </c>
@@ -9433,11 +9856,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9448,6 +9866,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -20078,7 +20501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -20830,7 +21253,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="134" t="s">
+      <c r="A52" s="133" t="s">
         <v>161</v>
       </c>
       <c r="B52" s="71">
@@ -20844,10 +21267,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="135" t="s">
+      <c r="A53" s="134" t="s">
         <v>162</v>
       </c>
-      <c r="B53" s="136">
+      <c r="B53" s="135">
         <v>0</v>
       </c>
       <c r="C53">
@@ -20858,10 +21281,10 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="135" t="s">
+      <c r="A54" s="134" t="s">
         <v>163</v>
       </c>
-      <c r="B54" s="136">
+      <c r="B54" s="135">
         <v>0</v>
       </c>
       <c r="C54">
@@ -20882,6 +21305,1182 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34C1B36-2F1D-8141-8AE0-24B0DA699162}">
+  <dimension ref="A1:Y107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="99">
+        <f>'[1]Baseline year demographics'!$C2+1</f>
+        <v>2017</v>
+      </c>
+      <c r="D1" s="99">
+        <f>C1+1</f>
+        <v>2018</v>
+      </c>
+      <c r="E1" s="99">
+        <f t="shared" ref="E1:P1" si="0">D1+1</f>
+        <v>2019</v>
+      </c>
+      <c r="F1" s="99">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="G1" s="99">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="H1" s="99">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="I1" s="99">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="J1" s="99">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="K1" s="99">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="L1" s="99">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="M1" s="99">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="N1" s="99">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="O1" s="99">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="P1" s="99">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A2" t="str">
+        <f>'[1]Programs to include'!A2</f>
+        <v>Balanced energy-protein supplementation</v>
+      </c>
+      <c r="B2" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>Balanced energy-protein supplementation</v>
+      </c>
+      <c r="B3" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f>'[1]Programs to include'!A3</f>
+        <v>Birth age program</v>
+      </c>
+      <c r="B4" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A5" t="str">
+        <f>A4</f>
+        <v>Birth age program</v>
+      </c>
+      <c r="B5" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>'[1]Programs to include'!A4</f>
+        <v>Calcium supplementation</v>
+      </c>
+      <c r="B6" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>A6</f>
+        <v>Calcium supplementation</v>
+      </c>
+      <c r="B7" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" s="35"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A8" t="str">
+        <f>'[1]Programs to include'!A5</f>
+        <v>Cash transfers</v>
+      </c>
+      <c r="B8" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="35"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A9" t="str">
+        <f>A8</f>
+        <v>Cash transfers</v>
+      </c>
+      <c r="B9" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="35"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A10" t="str">
+        <f>'[1]Programs to include'!A6</f>
+        <v>Family Planning</v>
+      </c>
+      <c r="B10" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="35"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A11" t="str">
+        <f>A10</f>
+        <v>Family Planning</v>
+      </c>
+      <c r="B11" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" s="35"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A12" t="str">
+        <f>'[1]Programs to include'!A7</f>
+        <v>IFA fortification of maize</v>
+      </c>
+      <c r="B12" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" s="35"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A13" t="str">
+        <f>A12</f>
+        <v>IFA fortification of maize</v>
+      </c>
+      <c r="B13" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="35"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A14" t="str">
+        <f>'[1]Programs to include'!A8</f>
+        <v>IFA fortification of rice</v>
+      </c>
+      <c r="B14" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C14" s="35"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A15" t="str">
+        <f>A14</f>
+        <v>IFA fortification of rice</v>
+      </c>
+      <c r="B15" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" s="35"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A16" t="str">
+        <f>'[1]Programs to include'!A9</f>
+        <v>IFA fortification of wheat flour</v>
+      </c>
+      <c r="B16" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="35"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="str">
+        <f>A16</f>
+        <v>IFA fortification of wheat flour</v>
+      </c>
+      <c r="B17" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" s="35"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="str">
+        <f>'[1]Programs to include'!A10</f>
+        <v>IFAS not poor: community</v>
+      </c>
+      <c r="B18" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C18" s="35"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" t="str">
+        <f>A18</f>
+        <v>IFAS not poor: community</v>
+      </c>
+      <c r="B19" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="35"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" t="str">
+        <f>'[1]Programs to include'!A11</f>
+        <v>IFAS not poor: community (malaria area)</v>
+      </c>
+      <c r="B20" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="35"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" t="str">
+        <f>A20</f>
+        <v>IFAS not poor: community (malaria area)</v>
+      </c>
+      <c r="B21" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="35"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" t="str">
+        <f>'[1]Programs to include'!A12</f>
+        <v>IFAS not poor: hospital</v>
+      </c>
+      <c r="B22" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C22" s="35"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="str">
+        <f>A22</f>
+        <v>IFAS not poor: hospital</v>
+      </c>
+      <c r="B23" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C23" s="35"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="str">
+        <f>'[1]Programs to include'!A13</f>
+        <v>IFAS not poor: hospital (malaria area)</v>
+      </c>
+      <c r="B24" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" s="35"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="str">
+        <f>A24</f>
+        <v>IFAS not poor: hospital (malaria area)</v>
+      </c>
+      <c r="B25" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C25" s="35"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="str">
+        <f>'[1]Programs to include'!A14</f>
+        <v>IFAS not poor: retailer</v>
+      </c>
+      <c r="B26" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C26" s="35"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="str">
+        <f>A26</f>
+        <v>IFAS not poor: retailer</v>
+      </c>
+      <c r="B27" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="35"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="str">
+        <f>'[1]Programs to include'!A15</f>
+        <v>IFAS not poor: retailer (malaria area)</v>
+      </c>
+      <c r="B28" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="35"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="str">
+        <f>A28</f>
+        <v>IFAS not poor: retailer (malaria area)</v>
+      </c>
+      <c r="B29" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="35"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" t="str">
+        <f>'[1]Programs to include'!A16</f>
+        <v>IFAS not poor: school</v>
+      </c>
+      <c r="B30" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="35"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" t="str">
+        <f>A30</f>
+        <v>IFAS not poor: school</v>
+      </c>
+      <c r="B31" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" s="35"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="str">
+        <f>'[1]Programs to include'!A17</f>
+        <v>IFAS not poor: school (malaria area)</v>
+      </c>
+      <c r="B32" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="35"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" t="str">
+        <f>A32</f>
+        <v>IFAS not poor: school (malaria area)</v>
+      </c>
+      <c r="B33" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C33" s="35"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" t="str">
+        <f>'[1]Programs to include'!A18</f>
+        <v>IFAS poor: community</v>
+      </c>
+      <c r="B34" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C34" s="35"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="str">
+        <f>A34</f>
+        <v>IFAS poor: community</v>
+      </c>
+      <c r="B35" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C35" s="35"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" t="str">
+        <f>'[1]Programs to include'!A19</f>
+        <v>IFAS poor: community (malaria area)</v>
+      </c>
+      <c r="B36" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C36" s="35"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="str">
+        <f>A36</f>
+        <v>IFAS poor: community (malaria area)</v>
+      </c>
+      <c r="B37" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C37" s="35"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="str">
+        <f>'[1]Programs to include'!A20</f>
+        <v>IFAS poor: hospital</v>
+      </c>
+      <c r="B38" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C38" s="35"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" t="str">
+        <f>A38</f>
+        <v>IFAS poor: hospital</v>
+      </c>
+      <c r="B39" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C39" s="35"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="str">
+        <f>'[1]Programs to include'!A21</f>
+        <v>IFAS poor: hospital (malaria area)</v>
+      </c>
+      <c r="B40" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C40" s="35"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="str">
+        <f>A40</f>
+        <v>IFAS poor: hospital (malaria area)</v>
+      </c>
+      <c r="B41" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" s="35"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="str">
+        <f>'[1]Programs to include'!A22</f>
+        <v>IFAS poor: school</v>
+      </c>
+      <c r="B42" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C42" s="35"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" t="str">
+        <f>A42</f>
+        <v>IFAS poor: school</v>
+      </c>
+      <c r="B43" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C43" s="35"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="str">
+        <f>'[1]Programs to include'!A23</f>
+        <v>IFAS poor: school (malaria area)</v>
+      </c>
+      <c r="B44" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C44" s="35"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" t="str">
+        <f>A44</f>
+        <v>IFAS poor: school (malaria area)</v>
+      </c>
+      <c r="B45" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C45" s="35"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" t="str">
+        <f>'[1]Programs to include'!A24</f>
+        <v>IPTp</v>
+      </c>
+      <c r="B46" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" s="35"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" t="str">
+        <f>A46</f>
+        <v>IPTp</v>
+      </c>
+      <c r="B47" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C47" s="35"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" t="str">
+        <f>'[1]Programs to include'!A25</f>
+        <v>Iron and folic acid supplementation for pregnant women</v>
+      </c>
+      <c r="B48" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C48" s="35"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" t="str">
+        <f>A48</f>
+        <v>Iron and folic acid supplementation for pregnant women</v>
+      </c>
+      <c r="B49" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C49" s="35"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" t="str">
+        <f>'[1]Programs to include'!A26</f>
+        <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+      </c>
+      <c r="B50" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50" s="35"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" t="str">
+        <f>A50</f>
+        <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+      </c>
+      <c r="B51" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C51" s="35"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" t="str">
+        <f>'[1]Programs to include'!A27</f>
+        <v>Iron and iodine fortification of salt</v>
+      </c>
+      <c r="B52" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C52" s="35"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" t="str">
+        <f>A52</f>
+        <v>Iron and iodine fortification of salt</v>
+      </c>
+      <c r="B53" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C53" s="35"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" t="str">
+        <f>'[1]Programs to include'!A28</f>
+        <v>Iron fortification of maize</v>
+      </c>
+      <c r="B54" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C54" s="35"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A55" t="str">
+        <f>A54</f>
+        <v>Iron fortification of maize</v>
+      </c>
+      <c r="B55" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C55" s="35"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" t="str">
+        <f>'[1]Programs to include'!A29</f>
+        <v>Iron fortification of rice</v>
+      </c>
+      <c r="B56" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C56" s="35"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A57" t="str">
+        <f>A56</f>
+        <v>Iron fortification of rice</v>
+      </c>
+      <c r="B57" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" s="35"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A58" t="str">
+        <f>'[1]Programs to include'!A30</f>
+        <v>Iron fortification of wheat flour</v>
+      </c>
+      <c r="B58" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C58" s="35"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" t="str">
+        <f>A58</f>
+        <v>Iron fortification of wheat flour</v>
+      </c>
+      <c r="B59" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C59" s="35"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A60" t="str">
+        <f>'[1]Programs to include'!A31</f>
+        <v>Long-lasting insecticide-treated bednets</v>
+      </c>
+      <c r="B60" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="35"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A61" t="str">
+        <f>A60</f>
+        <v>Long-lasting insecticide-treated bednets</v>
+      </c>
+      <c r="B61" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C61" s="35"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" t="str">
+        <f>'[1]Programs to include'!A32</f>
+        <v>Mg for eclampsia</v>
+      </c>
+      <c r="B62" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C62" s="35"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A63" t="str">
+        <f>A62</f>
+        <v>Mg for eclampsia</v>
+      </c>
+      <c r="B63" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C63" s="35"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A64" t="str">
+        <f>'[1]Programs to include'!A33</f>
+        <v>Mg for pre-eclampsia</v>
+      </c>
+      <c r="B64" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C64" s="35"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" t="str">
+        <f>A64</f>
+        <v>Mg for pre-eclampsia</v>
+      </c>
+      <c r="B65" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C65" s="35"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A66" t="str">
+        <f>'[1]Programs to include'!A34</f>
+        <v>Multiple micronutrient supplementation</v>
+      </c>
+      <c r="B66" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A67" t="str">
+        <f>A66</f>
+        <v>Multiple micronutrient supplementation</v>
+      </c>
+      <c r="B67" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C67" s="35"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A68" t="str">
+        <f>'[1]Programs to include'!A35</f>
+        <v>Multiple micronutrient supplementation (malaria area)</v>
+      </c>
+      <c r="B68" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C68" s="35"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" t="str">
+        <f>A68</f>
+        <v>Multiple micronutrient supplementation (malaria area)</v>
+      </c>
+      <c r="B69" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C69" s="35"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A70" t="str">
+        <f>'[1]Programs to include'!A36</f>
+        <v>Oral rehydration salts</v>
+      </c>
+      <c r="B70" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C70" s="35"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" t="str">
+        <f>A70</f>
+        <v>Oral rehydration salts</v>
+      </c>
+      <c r="B71" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C71" s="35"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" t="str">
+        <f>'[1]Programs to include'!A37</f>
+        <v>Public provision of complementary foods</v>
+      </c>
+      <c r="B72" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C72" s="35"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" t="str">
+        <f>A72</f>
+        <v>Public provision of complementary foods</v>
+      </c>
+      <c r="B73" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C73" s="35"/>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A74" t="str">
+        <f>'[1]Programs to include'!A38</f>
+        <v>Public provision of complementary foods with iron</v>
+      </c>
+      <c r="B74" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C74" s="35"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A75" t="str">
+        <f>A74</f>
+        <v>Public provision of complementary foods with iron</v>
+      </c>
+      <c r="B75" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C75" s="35"/>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A76" t="str">
+        <f>'[1]Programs to include'!A39</f>
+        <v>Public provision of complementary foods with iron (malaria area)</v>
+      </c>
+      <c r="B76" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A77" t="str">
+        <f>A76</f>
+        <v>Public provision of complementary foods with iron (malaria area)</v>
+      </c>
+      <c r="B77" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C77" s="35"/>
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A78" t="str">
+        <f>'[1]Programs to include'!A40</f>
+        <v>Sprinkles</v>
+      </c>
+      <c r="B78" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" s="35"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A79" t="str">
+        <f>A78</f>
+        <v>Sprinkles</v>
+      </c>
+      <c r="B79" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C79" s="35"/>
+      <c r="D79">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A80" t="str">
+        <f>'[1]Programs to include'!A41</f>
+        <v>Sprinkles (malaria area)</v>
+      </c>
+      <c r="B80" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C80" s="35"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A81" t="str">
+        <f>A80</f>
+        <v>Sprinkles (malaria area)</v>
+      </c>
+      <c r="B81" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="35"/>
+      <c r="D81">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A82" t="str">
+        <f>'[1]Programs to include'!A42</f>
+        <v>Treatment of MAM</v>
+      </c>
+      <c r="B82" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C82" s="35"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A83" t="str">
+        <f>A82</f>
+        <v>Treatment of MAM</v>
+      </c>
+      <c r="B83" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C83" s="35"/>
+      <c r="D83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A84" t="str">
+        <f>'[1]Programs to include'!A43</f>
+        <v>Treatment of SAM</v>
+      </c>
+      <c r="B84" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C84" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A85" t="str">
+        <f>A84</f>
+        <v>Treatment of SAM</v>
+      </c>
+      <c r="B85" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C85" s="35"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A86" t="str">
+        <f>'[1]Programs to include'!A44</f>
+        <v>Vitamin A supplementation</v>
+      </c>
+      <c r="B86" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C86" s="35"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A87" t="str">
+        <f>A86</f>
+        <v>Vitamin A supplementation</v>
+      </c>
+      <c r="B87" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C87" s="35"/>
+      <c r="D87">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A88" t="str">
+        <f>'[1]Programs to include'!A45</f>
+        <v>WASH: Handwashing</v>
+      </c>
+      <c r="B88" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C88" s="35"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A89" t="str">
+        <f>A88</f>
+        <v>WASH: Handwashing</v>
+      </c>
+      <c r="B89" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C89" s="35"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A90" t="str">
+        <f>'[1]Programs to include'!A46</f>
+        <v>WASH: Hygenic disposal</v>
+      </c>
+      <c r="B90" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C90" s="35"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A91" t="str">
+        <f>A90</f>
+        <v>WASH: Hygenic disposal</v>
+      </c>
+      <c r="B91" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A92" t="str">
+        <f>'[1]Programs to include'!A47</f>
+        <v>WASH: Improved sanitation</v>
+      </c>
+      <c r="B92" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C92" s="35"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A93" t="str">
+        <f>A92</f>
+        <v>WASH: Improved sanitation</v>
+      </c>
+      <c r="B93" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="35"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A94" t="str">
+        <f>'[1]Programs to include'!A48</f>
+        <v>WASH: Improved water source</v>
+      </c>
+      <c r="B94" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C94" s="35"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A95" t="str">
+        <f>A94</f>
+        <v>WASH: Improved water source</v>
+      </c>
+      <c r="B95" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C95" s="35"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A96" t="str">
+        <f>'[1]Programs to include'!A49</f>
+        <v>WASH: Piped water</v>
+      </c>
+      <c r="B96" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="35"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A97" t="str">
+        <f>A96</f>
+        <v>WASH: Piped water</v>
+      </c>
+      <c r="B97" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C97" s="35"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A98" t="str">
+        <f>'[1]Programs to include'!A50</f>
+        <v>Zinc for treatment + ORS</v>
+      </c>
+      <c r="B98" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C98" s="35"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A99" t="str">
+        <f>A98</f>
+        <v>Zinc for treatment + ORS</v>
+      </c>
+      <c r="B99" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C99" s="35"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A100" t="str">
+        <f>'[1]Programs to include'!A51</f>
+        <v>Zinc supplementation</v>
+      </c>
+      <c r="B100" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C100" s="35"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A101" t="str">
+        <f>A100</f>
+        <v>Zinc supplementation</v>
+      </c>
+      <c r="B101" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C101" s="35"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A102" t="str">
+        <f>'[1]Programs to include'!A52</f>
+        <v>IYCF 1</v>
+      </c>
+      <c r="B102" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C102" s="35"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A103" t="str">
+        <f>A102</f>
+        <v>IYCF 1</v>
+      </c>
+      <c r="B103" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C103" s="35"/>
+      <c r="D103">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A104" t="str">
+        <f>'[1]Programs to include'!A53</f>
+        <v>IYCF 2</v>
+      </c>
+      <c r="B104" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C104" s="35"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A105" t="str">
+        <f>A104</f>
+        <v>IYCF 2</v>
+      </c>
+      <c r="B105" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C105" s="35"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A106" t="str">
+        <f>'[1]Programs to include'!A54</f>
+        <v>IYCF 3</v>
+      </c>
+      <c r="B106" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="C106" s="35"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A107" t="str">
+        <f>A106</f>
+        <v>IYCF 3</v>
+      </c>
+      <c r="B107" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="C107" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD8166B-8704-DF4E-9AA8-4565893AE0CB}">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -20897,12 +22496,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="132" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="132" t="s">
         <v>119</v>
       </c>
     </row>
@@ -20934,446 +22533,6 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>258</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:B54"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="70" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="126" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="126" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="126" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>135</v>
-      </c>
-      <c r="B34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>262</v>
-      </c>
-      <c r="B36" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>261</v>
-      </c>
-      <c r="B45" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>260</v>
-      </c>
-      <c r="B46" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>259</v>
-      </c>
-      <c r="B47" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
-        <v>257</v>
-      </c>
-      <c r="B48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>258</v>
-      </c>
-      <c r="B49" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>263</v>
-      </c>
-      <c r="B50" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B51" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="125" t="s">
-        <v>161</v>
-      </c>
-      <c r="B52" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="125" t="s">
-        <v>162</v>
-      </c>
-      <c r="B53" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="125" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -22300,6 +23459,449 @@
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="126" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="126" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="126" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>262</v>
+      </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>260</v>
+      </c>
+      <c r="B46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>259</v>
+      </c>
+      <c r="B47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>257</v>
+      </c>
+      <c r="B48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>258</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>263</v>
+      </c>
+      <c r="B50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" s="125" t="s">
+        <v>161</v>
+      </c>
+      <c r="B52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" s="125" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" s="125" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates for time-dependent coverages
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="23" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3300" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="15" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -12227,8 +12227,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14540,8 +14540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16139,16 +16139,20 @@
         <v>0</v>
       </c>
       <c r="L36" s="123">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.6</v>
       </c>
       <c r="M36" s="123">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.6</v>
       </c>
       <c r="N36" s="123">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.6</v>
       </c>
       <c r="O36" s="123">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -20501,8 +20505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22485,10 +22489,13 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
@@ -23469,8 +23476,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23491,7 +23498,7 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23499,7 +23506,7 @@
       <c r="A3" s="70" t="s">
         <v>267</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23507,7 +23514,7 @@
       <c r="A4" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23515,7 +23522,7 @@
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23523,7 +23530,7 @@
       <c r="A6" t="s">
         <v>185</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23531,7 +23538,7 @@
       <c r="A7" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23539,7 +23546,7 @@
       <c r="A8" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23547,7 +23554,7 @@
       <c r="A9" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23555,7 +23562,7 @@
       <c r="A10" t="s">
         <v>124</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23563,7 +23570,7 @@
       <c r="A11" t="s">
         <v>132</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23571,7 +23578,7 @@
       <c r="A12" t="s">
         <v>125</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23579,7 +23586,7 @@
       <c r="A13" t="s">
         <v>133</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23587,7 +23594,7 @@
       <c r="A14" t="s">
         <v>126</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23595,7 +23602,7 @@
       <c r="A15" t="s">
         <v>134</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23603,7 +23610,7 @@
       <c r="A16" t="s">
         <v>123</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23611,7 +23618,7 @@
       <c r="A17" t="s">
         <v>131</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23619,7 +23626,7 @@
       <c r="A18" t="s">
         <v>121</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23627,7 +23634,7 @@
       <c r="A19" t="s">
         <v>129</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23635,7 +23642,7 @@
       <c r="A20" t="s">
         <v>122</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23643,7 +23650,7 @@
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23651,7 +23658,7 @@
       <c r="A22" t="s">
         <v>120</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23659,7 +23666,7 @@
       <c r="A23" t="s">
         <v>128</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23667,7 +23674,7 @@
       <c r="A24" t="s">
         <v>119</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23675,7 +23682,7 @@
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23683,7 +23690,7 @@
       <c r="A26" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="132" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23691,7 +23698,7 @@
       <c r="A27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="132" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated OR & modes for IYCF packages
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36580" yWindow="-20580" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="17" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="-20360" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -5165,7 +5165,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5395,6 +5395,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="725">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -8413,8 +8414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="139" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8461,18 +8462,18 @@
         <v>152</v>
       </c>
       <c r="D2" s="54">
-        <v>1.85</v>
+        <v>1</v>
       </c>
       <c r="E2" s="54">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G2" s="54">
-        <v>1.01</v>
-      </c>
-      <c r="H2" s="56">
+        <v>1</v>
+      </c>
+      <c r="H2" s="54">
         <v>1</v>
       </c>
     </row>
@@ -8482,18 +8483,18 @@
         <v>153</v>
       </c>
       <c r="D3" s="54">
-        <v>1.9</v>
+        <v>1</v>
       </c>
       <c r="E3" s="54">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="F3" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G3" s="54">
-        <v>1.01</v>
-      </c>
-      <c r="H3" s="56">
+        <v>1</v>
+      </c>
+      <c r="H3" s="54">
         <v>1</v>
       </c>
       <c r="J3" s="54"/>
@@ -8504,23 +8505,18 @@
         <v>163</v>
       </c>
       <c r="D4" s="54">
-        <f>D17^(1/2)</f>
-        <v>1.0246950765959599</v>
+        <v>1</v>
       </c>
       <c r="E4" s="54">
-        <f>E17^(1/3)</f>
-        <v>1.0163963568148535</v>
+        <v>1</v>
       </c>
       <c r="F4" s="54">
-        <f>F17^(1/4)</f>
-        <v>1.0122722344290394</v>
+        <v>1</v>
       </c>
       <c r="G4" s="54">
-        <f t="shared" ref="G4:H4" si="0">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H4" s="54">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J4" s="54"/>
@@ -8533,7 +8529,7 @@
         <v>152</v>
       </c>
       <c r="D5" s="54">
-        <v>2.0299999999999998</v>
+        <v>5.16</v>
       </c>
       <c r="E5" s="54">
         <v>1</v>
@@ -8554,7 +8550,7 @@
         <v>153</v>
       </c>
       <c r="D6" s="54">
-        <v>2.17</v>
+        <v>5.16</v>
       </c>
       <c r="E6" s="54">
         <v>1</v>
@@ -8575,23 +8571,18 @@
         <v>163</v>
       </c>
       <c r="D7" s="54">
-        <f>D17^(1/2)</f>
-        <v>1.0246950765959599</v>
+        <v>1</v>
       </c>
       <c r="E7" s="54">
-        <f>E17^(1/3)</f>
-        <v>1.0163963568148535</v>
+        <v>1</v>
       </c>
       <c r="F7" s="54">
-        <f>F17^(1/4)</f>
-        <v>1.0122722344290394</v>
+        <v>1</v>
       </c>
       <c r="G7" s="54">
-        <f t="shared" ref="G7:H7" si="1">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H7" s="54">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8606,7 +8597,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="54">
-        <v>1.5</v>
+        <v>5.16</v>
       </c>
       <c r="F8" s="54">
         <v>1</v>
@@ -8627,7 +8618,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="54">
-        <v>1.5</v>
+        <v>5.16</v>
       </c>
       <c r="F9" s="54">
         <v>1</v>
@@ -8648,19 +8639,15 @@
         <v>1</v>
       </c>
       <c r="E10" s="54">
-        <f>E17^(1/3)</f>
-        <v>1.0163963568148535</v>
+        <v>1</v>
       </c>
       <c r="F10" s="54">
-        <f>F17^(1/4)</f>
-        <v>1.0122722344290394</v>
+        <v>1</v>
       </c>
       <c r="G10" s="54">
-        <f t="shared" ref="G10:H10" si="2">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H10" s="54">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -8678,7 +8665,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="54">
-        <v>1.1499999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="G11" s="54">
         <v>1</v>
@@ -8699,7 +8686,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="54">
-        <v>1.1499999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="G12" s="54">
         <v>1</v>
@@ -8720,15 +8707,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="54">
-        <f>F17^(1/4)</f>
-        <v>1.0122722344290394</v>
+        <v>1</v>
       </c>
       <c r="G13" s="54">
-        <f t="shared" ref="G13:H13" si="3">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H13" s="54">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -8749,7 +8733,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="54">
-        <v>1.1499999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="H14" s="56">
         <v>1</v>
@@ -8770,7 +8754,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="54">
-        <v>1.1000000000000001</v>
+        <v>1.82</v>
       </c>
       <c r="H15" s="56">
         <v>1</v>
@@ -8791,11 +8775,9 @@
         <v>1</v>
       </c>
       <c r="G16" s="54">
-        <f t="shared" ref="G16:H16" si="4">G17^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H16" s="54">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8846,10 +8828,10 @@
         <v>1</v>
       </c>
       <c r="F19" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G19" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H19" s="54">
         <v>1</v>
@@ -8867,10 +8849,10 @@
         <v>1</v>
       </c>
       <c r="F20" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G20" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H20" s="54">
         <v>1</v>
@@ -8882,23 +8864,18 @@
         <v>163</v>
       </c>
       <c r="D21" s="54">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E21" s="54">
-        <f t="shared" ref="E21:H21" si="5">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F21" s="54">
-        <f t="shared" si="5"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G21" s="54">
-        <f t="shared" si="5"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H21" s="54">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -8916,10 +8893,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G22" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H22" s="54">
         <v>1</v>
@@ -8937,10 +8914,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G23" s="54">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="H23" s="54">
         <v>1</v>
@@ -8952,23 +8929,18 @@
         <v>163</v>
       </c>
       <c r="D24" s="54">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E24" s="54">
-        <f t="shared" ref="E24:H24" si="6">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F24" s="54">
-        <f t="shared" si="6"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G24" s="54">
-        <f t="shared" si="6"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H24" s="54">
-        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -8986,10 +8958,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="54">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="54">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H25" s="54">
         <v>1</v>
@@ -9007,10 +8979,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="54">
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="G26" s="54">
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="H26" s="54">
         <v>1</v>
@@ -9022,23 +8994,18 @@
         <v>163</v>
       </c>
       <c r="D27" s="54">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E27" s="54">
-        <f t="shared" ref="E27:H27" si="7">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F27" s="54">
-        <f t="shared" si="7"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G27" s="54">
-        <f t="shared" si="7"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H27" s="54">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -9056,10 +9023,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="54">
-        <v>2</v>
+        <v>1.82</v>
       </c>
       <c r="G28" s="54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="54">
         <v>1</v>
@@ -9077,10 +9044,10 @@
         <v>1</v>
       </c>
       <c r="F29" s="54">
-        <v>1.9</v>
+        <v>1.82</v>
       </c>
       <c r="G29" s="54">
-        <v>1.9</v>
+        <v>1</v>
       </c>
       <c r="H29" s="54">
         <v>1</v>
@@ -9092,23 +9059,18 @@
         <v>163</v>
       </c>
       <c r="D30" s="54">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E30" s="54">
-        <f t="shared" ref="E30:H30" si="8">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F30" s="54">
-        <f t="shared" si="8"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G30" s="54">
-        <f t="shared" si="8"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H30" s="54">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -9129,7 +9091,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="54">
-        <v>2</v>
+        <v>1.82</v>
       </c>
       <c r="H31" s="54">
         <v>1</v>
@@ -9150,7 +9112,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="54">
-        <v>1.9</v>
+        <v>1.82</v>
       </c>
       <c r="H32" s="54">
         <v>1</v>
@@ -9162,23 +9124,18 @@
         <v>163</v>
       </c>
       <c r="D33" s="54">
-        <f>D34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="E33" s="54">
-        <f t="shared" ref="E33:H33" si="9">E34^(1/5)</f>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="F33" s="54">
-        <f t="shared" si="9"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="G33" s="54">
-        <f t="shared" si="9"/>
-        <v>1.0098057976734853</v>
+        <v>1</v>
       </c>
       <c r="H33" s="54">
-        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -9222,10 +9179,10 @@
         <v>1</v>
       </c>
       <c r="F36" s="54">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G36" s="54">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H36" s="54">
         <v>1</v>
@@ -9243,10 +9200,10 @@
         <v>1</v>
       </c>
       <c r="F37" s="54">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G37" s="54">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H37" s="54">
         <v>1</v>
@@ -9264,10 +9221,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G38" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H38" s="54">
         <v>1</v>
@@ -9329,10 +9286,10 @@
         <v>1</v>
       </c>
       <c r="F41" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G41" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H41" s="54">
         <v>1</v>
@@ -9394,10 +9351,10 @@
         <v>1</v>
       </c>
       <c r="F44" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G44" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H44" s="54">
         <v>1</v>
@@ -9459,10 +9416,10 @@
         <v>1</v>
       </c>
       <c r="F47" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G47" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H47" s="54">
         <v>1</v>
@@ -9527,7 +9484,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="54">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H50" s="54">
         <v>1</v>
@@ -9584,7 +9541,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="178" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9618,12 +9575,8 @@
       <c r="B2" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="76" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="76" t="s">
-        <v>164</v>
-      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
       <c r="E2" s="77"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -9632,7 +9585,9 @@
         <v>6</v>
       </c>
       <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
+      <c r="D3" s="137" t="s">
+        <v>164</v>
+      </c>
       <c r="E3" s="80"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -9641,7 +9596,9 @@
         <v>7</v>
       </c>
       <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
+      <c r="D4" s="137" t="s">
+        <v>164</v>
+      </c>
       <c r="E4" s="80"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -9650,7 +9607,9 @@
         <v>8</v>
       </c>
       <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
+      <c r="D5" s="134" t="s">
+        <v>164</v>
+      </c>
       <c r="E5" s="80"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -9659,7 +9618,9 @@
         <v>9</v>
       </c>
       <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
+      <c r="D6" s="134" t="s">
+        <v>164</v>
+      </c>
       <c r="E6" s="80"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -9687,12 +9648,8 @@
       <c r="B10" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="79" t="s">
-        <v>164</v>
-      </c>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
       <c r="E10" s="80"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -19363,7 +19320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26:I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated saturation coverage to 95%
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="-20360" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1972,30 +1972,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the fraction of the population eating these staples and belongs here.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="D8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000005000000}">
       <text>
         <r>
@@ -2242,7 +2218,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -2251,12 +2227,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-fictional</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>fictional</t>
         </r>
       </text>
     </comment>
@@ -2281,30 +2266,6 @@
           </rPr>
           <t xml:space="preserve">
 orton Copenhagen Consensus 2008</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the fraction of the population eating these staples and belongs here.</t>
         </r>
       </text>
     </comment>
@@ -3227,7 +3188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -5392,10 +5353,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="725">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -8455,7 +8416,7 @@
       <c r="A2" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="137" t="s">
         <v>72</v>
       </c>
       <c r="C2" t="s">
@@ -8478,7 +8439,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="136"/>
+      <c r="B3" s="137"/>
       <c r="C3" t="s">
         <v>153</v>
       </c>
@@ -8500,7 +8461,7 @@
       <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="136"/>
+      <c r="B4" s="137"/>
       <c r="C4" t="s">
         <v>163</v>
       </c>
@@ -8522,7 +8483,7 @@
       <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="137" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -8545,7 +8506,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="136"/>
+      <c r="B6" s="137"/>
       <c r="C6" t="s">
         <v>153</v>
       </c>
@@ -8566,7 +8527,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="136"/>
+      <c r="B7" s="137"/>
       <c r="C7" t="s">
         <v>163</v>
       </c>
@@ -8587,7 +8548,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="137" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -8610,7 +8571,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="136"/>
+      <c r="B9" s="137"/>
       <c r="C9" t="s">
         <v>153</v>
       </c>
@@ -8631,7 +8592,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="136"/>
+      <c r="B10" s="137"/>
       <c r="C10" t="s">
         <v>163</v>
       </c>
@@ -8652,7 +8613,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="136" t="s">
+      <c r="B11" s="137" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -8675,7 +8636,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="136"/>
+      <c r="B12" s="137"/>
       <c r="C12" t="s">
         <v>153</v>
       </c>
@@ -8696,7 +8657,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="136"/>
+      <c r="B13" s="137"/>
       <c r="C13" t="s">
         <v>163</v>
       </c>
@@ -8717,7 +8678,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="136" t="s">
+      <c r="B14" s="137" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -8740,7 +8701,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="136"/>
+      <c r="B15" s="137"/>
       <c r="C15" t="s">
         <v>153</v>
       </c>
@@ -8761,7 +8722,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="136"/>
+      <c r="B16" s="137"/>
       <c r="C16" t="s">
         <v>163</v>
       </c>
@@ -8815,7 +8776,7 @@
       <c r="A19" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="B19" s="136" t="s">
+      <c r="B19" s="137" t="s">
         <v>72</v>
       </c>
       <c r="C19" t="s">
@@ -8838,7 +8799,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="136"/>
+      <c r="B20" s="137"/>
       <c r="C20" t="s">
         <v>153</v>
       </c>
@@ -8859,7 +8820,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="136"/>
+      <c r="B21" s="137"/>
       <c r="C21" t="s">
         <v>163</v>
       </c>
@@ -8880,7 +8841,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="136" t="s">
+      <c r="B22" s="137" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8903,7 +8864,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="136"/>
+      <c r="B23" s="137"/>
       <c r="C23" t="s">
         <v>153</v>
       </c>
@@ -8924,7 +8885,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="136"/>
+      <c r="B24" s="137"/>
       <c r="C24" t="s">
         <v>163</v>
       </c>
@@ -8945,7 +8906,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="136" t="s">
+      <c r="B25" s="137" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8968,7 +8929,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="136"/>
+      <c r="B26" s="137"/>
       <c r="C26" t="s">
         <v>153</v>
       </c>
@@ -8989,7 +8950,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="136"/>
+      <c r="B27" s="137"/>
       <c r="C27" t="s">
         <v>163</v>
       </c>
@@ -9010,7 +8971,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="136" t="s">
+      <c r="B28" s="137" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -9033,7 +8994,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="136"/>
+      <c r="B29" s="137"/>
       <c r="C29" t="s">
         <v>153</v>
       </c>
@@ -9054,7 +9015,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="136"/>
+      <c r="B30" s="137"/>
       <c r="C30" t="s">
         <v>163</v>
       </c>
@@ -9075,7 +9036,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="136" t="s">
+      <c r="B31" s="137" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -9098,7 +9059,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="136"/>
+      <c r="B32" s="137"/>
       <c r="C32" t="s">
         <v>153</v>
       </c>
@@ -9119,7 +9080,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="136"/>
+      <c r="B33" s="137"/>
       <c r="C33" t="s">
         <v>163</v>
       </c>
@@ -9166,7 +9127,7 @@
       <c r="A36" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B36" s="136" t="s">
+      <c r="B36" s="137" t="s">
         <v>72</v>
       </c>
       <c r="C36" t="s">
@@ -9189,7 +9150,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="136"/>
+      <c r="B37" s="137"/>
       <c r="C37" t="s">
         <v>153</v>
       </c>
@@ -9210,7 +9171,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="136"/>
+      <c r="B38" s="137"/>
       <c r="C38" t="s">
         <v>163</v>
       </c>
@@ -9231,7 +9192,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="136" t="s">
+      <c r="B39" s="137" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -9254,7 +9215,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="136"/>
+      <c r="B40" s="137"/>
       <c r="C40" t="s">
         <v>153</v>
       </c>
@@ -9275,7 +9236,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="136"/>
+      <c r="B41" s="137"/>
       <c r="C41" t="s">
         <v>163</v>
       </c>
@@ -9296,7 +9257,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="136" t="s">
+      <c r="B42" s="137" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -9319,7 +9280,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="136"/>
+      <c r="B43" s="137"/>
       <c r="C43" t="s">
         <v>153</v>
       </c>
@@ -9340,7 +9301,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="136"/>
+      <c r="B44" s="137"/>
       <c r="C44" t="s">
         <v>163</v>
       </c>
@@ -9361,7 +9322,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="136" t="s">
+      <c r="B45" s="137" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -9384,7 +9345,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="136"/>
+      <c r="B46" s="137"/>
       <c r="C46" t="s">
         <v>153</v>
       </c>
@@ -9405,7 +9366,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="136"/>
+      <c r="B47" s="137"/>
       <c r="C47" t="s">
         <v>163</v>
       </c>
@@ -9426,7 +9387,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="136" t="s">
+      <c r="B48" s="137" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -9449,7 +9410,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="136"/>
+      <c r="B49" s="137"/>
       <c r="C49" t="s">
         <v>153</v>
       </c>
@@ -9470,7 +9431,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="136"/>
+      <c r="B50" s="137"/>
       <c r="C50" t="s">
         <v>163</v>
       </c>
@@ -9515,6 +9476,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9525,11 +9491,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9585,7 +9546,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="79"/>
-      <c r="D3" s="137" t="s">
+      <c r="D3" s="136" t="s">
         <v>164</v>
       </c>
       <c r="E3" s="80"/>
@@ -9596,7 +9557,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="79"/>
-      <c r="D4" s="137" t="s">
+      <c r="D4" s="136" t="s">
         <v>164</v>
       </c>
       <c r="E4" s="80"/>
@@ -14200,7 +14161,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20186,8 +20147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20220,7 +20181,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D2" s="14">
         <v>25</v>
@@ -20234,7 +20195,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D3" s="19">
         <v>0.8</v>
@@ -20249,7 +20210,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D4" s="19">
         <v>1</v>
@@ -20263,8 +20224,8 @@
       <c r="B5" s="14">
         <v>0</v>
       </c>
-      <c r="C5" s="13">
-        <v>0.85</v>
+      <c r="C5" s="14">
+        <v>0.95</v>
       </c>
       <c r="D5" s="19">
         <f>180</f>
@@ -20280,7 +20241,7 @@
         <v>0.5</v>
       </c>
       <c r="C6" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D6" s="19">
         <f>SUM('Programs family planning'!E2:E10)</f>
@@ -20296,7 +20257,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="14">
-        <v>0.05</v>
+        <v>0.95</v>
       </c>
       <c r="D7" s="19">
         <v>0.14000000000000001</v>
@@ -20311,7 +20272,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="14">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="D8" s="19">
         <v>0.75</v>
@@ -20326,7 +20287,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="14">
-        <v>0.12</v>
+        <v>0.95</v>
       </c>
       <c r="D9" s="19">
         <v>0.19</v>
@@ -20341,7 +20302,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D10" s="14">
         <v>0.73</v>
@@ -20355,7 +20316,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D11" s="14">
         <v>0.73</v>
@@ -20369,7 +20330,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D12" s="14">
         <v>1.78</v>
@@ -20383,7 +20344,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D13" s="14">
         <v>1.78</v>
@@ -20397,7 +20358,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D14" s="14">
         <v>0.24</v>
@@ -20411,7 +20372,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D15" s="14">
         <v>0.24</v>
@@ -20425,7 +20386,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D16" s="14">
         <v>0.55000000000000004</v>
@@ -20439,7 +20400,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D17" s="14">
         <v>0.55000000000000004</v>
@@ -20453,7 +20414,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D18" s="14">
         <v>0.73</v>
@@ -20467,7 +20428,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D19" s="14">
         <v>0.73</v>
@@ -20481,7 +20442,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D20" s="14">
         <v>1.78</v>
@@ -20495,7 +20456,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D21" s="14">
         <v>1.78</v>
@@ -20509,7 +20470,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D22" s="14">
         <v>0.55000000000000004</v>
@@ -20523,7 +20484,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D23" s="14">
         <v>0.55000000000000004</v>
@@ -20537,7 +20498,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D24" s="14">
         <v>2.06</v>
@@ -20550,8 +20511,8 @@
       <c r="B25" s="50">
         <v>0</v>
       </c>
-      <c r="C25" s="50">
-        <v>0.85</v>
+      <c r="C25" s="14">
+        <v>0.95</v>
       </c>
       <c r="D25" s="50">
         <v>1.78</v>
@@ -20566,7 +20527,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D26" s="14">
         <v>1.78</v>
@@ -20580,8 +20541,8 @@
       <c r="B27" s="14">
         <v>0</v>
       </c>
-      <c r="C27" s="13">
-        <v>0.85</v>
+      <c r="C27" s="14">
+        <v>0.95</v>
       </c>
       <c r="D27" s="19">
         <v>0.25</v>
@@ -20596,7 +20557,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="14">
-        <v>0.05</v>
+        <v>0.95</v>
       </c>
       <c r="D28" s="19">
         <v>0.13</v>
@@ -20611,7 +20572,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="14">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="D29" s="19">
         <v>0.74</v>
@@ -20626,7 +20587,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="14">
-        <v>0.12</v>
+        <v>0.95</v>
       </c>
       <c r="D30" s="19">
         <v>0.18</v>
@@ -20641,7 +20602,7 @@
         <v>0.2</v>
       </c>
       <c r="C31" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D31" s="19">
         <v>2.61</v>
@@ -20655,7 +20616,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D32" s="31">
         <v>1</v>
@@ -20669,7 +20630,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D33" s="31">
         <v>1</v>
@@ -20682,8 +20643,8 @@
       <c r="B34" s="50">
         <v>0</v>
       </c>
-      <c r="C34" s="50">
-        <v>0.85</v>
+      <c r="C34" s="14">
+        <v>0.95</v>
       </c>
       <c r="D34" s="50">
         <v>2.99</v>
@@ -20698,7 +20659,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D35" s="14">
         <v>2.99</v>
@@ -20713,7 +20674,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D36" s="19">
         <v>1</v>
@@ -20728,7 +20689,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D37" s="14">
         <v>48</v>
@@ -20742,8 +20703,8 @@
       <c r="B38" s="49">
         <v>0</v>
       </c>
-      <c r="C38" s="49">
-        <v>0.85</v>
+      <c r="C38" s="14">
+        <v>0.95</v>
       </c>
       <c r="D38" s="92">
         <v>50</v>
@@ -20757,8 +20718,8 @@
       <c r="B39" s="31">
         <v>0</v>
       </c>
-      <c r="C39" s="31">
-        <v>0.85</v>
+      <c r="C39" s="14">
+        <v>0.95</v>
       </c>
       <c r="D39" s="19">
         <v>51</v>
@@ -20772,8 +20733,8 @@
       <c r="B40" s="49">
         <v>0</v>
       </c>
-      <c r="C40" s="49">
-        <v>0.85</v>
+      <c r="C40" s="14">
+        <v>0.95</v>
       </c>
       <c r="D40" s="92">
         <v>1</v>
@@ -20787,8 +20748,8 @@
       <c r="B41" s="31">
         <v>0</v>
       </c>
-      <c r="C41" s="31">
-        <v>0.85</v>
+      <c r="C41" s="14">
+        <v>0.95</v>
       </c>
       <c r="D41" s="19">
         <v>1</v>
@@ -20802,8 +20763,8 @@
       <c r="B42" s="14">
         <v>0</v>
       </c>
-      <c r="C42" s="13">
-        <v>0.85</v>
+      <c r="C42" s="14">
+        <v>0.95</v>
       </c>
       <c r="D42" s="19">
         <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
@@ -20817,8 +20778,8 @@
       <c r="B43" s="14">
         <v>0.61</v>
       </c>
-      <c r="C43" s="13">
-        <v>0.85</v>
+      <c r="C43" s="14">
+        <v>0.95</v>
       </c>
       <c r="D43" s="19">
         <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
@@ -20833,7 +20794,7 @@
         <v>0.621</v>
       </c>
       <c r="C44" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D44" s="14">
         <v>0.35</v>
@@ -20846,8 +20807,8 @@
       <c r="B45" s="91">
         <v>0.4</v>
       </c>
-      <c r="C45" s="13">
-        <v>0.85</v>
+      <c r="C45" s="14">
+        <v>0.95</v>
       </c>
       <c r="D45" s="19">
         <v>1</v>
@@ -20860,8 +20821,8 @@
       <c r="B46" s="91">
         <v>0.38700000000000001</v>
       </c>
-      <c r="C46" s="13">
-        <v>0.85</v>
+      <c r="C46" s="14">
+        <v>0.95</v>
       </c>
       <c r="D46" s="19">
         <v>2.8</v>
@@ -20874,8 +20835,8 @@
       <c r="B47" s="91">
         <v>0.69</v>
       </c>
-      <c r="C47" s="13">
-        <v>0.85</v>
+      <c r="C47" s="14">
+        <v>0.95</v>
       </c>
       <c r="D47" s="19">
         <v>50.26</v>
@@ -20888,8 +20849,8 @@
       <c r="B48" s="91">
         <v>0.84</v>
       </c>
-      <c r="C48" s="13">
-        <v>0.85</v>
+      <c r="C48" s="14">
+        <v>0.95</v>
       </c>
       <c r="D48" s="19">
         <v>36.1</v>
@@ -20902,8 +20863,8 @@
       <c r="B49" s="91">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C49" s="13">
-        <v>0.85</v>
+      <c r="C49" s="14">
+        <v>0.95</v>
       </c>
       <c r="D49" s="19">
         <v>231.85</v>
@@ -20917,7 +20878,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D50" s="19">
         <v>1.5</v>
@@ -20931,7 +20892,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D51" s="14">
         <v>1</v>
@@ -23136,8 +23097,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23166,9 +23127,7 @@
       <c r="A3" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B3" s="132"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Corrected fraction targeted by IFAS programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="-20160" windowWidth="24640" windowHeight="18760" xr2:uid="{A331D684-01C0-6143-BA95-869254A5E453}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -7505,6 +7506,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7947,6 +7951,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8378,6 +8383,7 @@
     <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9504,6 +9510,7 @@
     <sheetView zoomScale="178" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9719,6 +9726,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9919,6 +9927,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9996,6 +10005,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10300,6 +10310,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11759,6 +11770,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11850,6 +11862,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13054,6 +13067,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13258,6 +13272,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13910,6 +13925,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14086,6 +14102,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14160,9 +14177,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -15143,8 +15161,8 @@
         <v>0</v>
       </c>
       <c r="L23" s="27">
-        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)*'Baseline year demographics'!$C$7</f>
-        <v>7.9833599999999991E-2</v>
+        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>0.1469664</v>
       </c>
       <c r="M23" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)</f>
@@ -15191,8 +15209,8 @@
         <v>0</v>
       </c>
       <c r="L24" s="27">
-        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)*'Baseline year demographics'!$C$7</f>
-        <v>3.4214399999999999E-2</v>
+        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>6.2985600000000003E-2</v>
       </c>
       <c r="M24" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
@@ -15284,8 +15302,8 @@
         <v>0</v>
       </c>
       <c r="L26" s="27">
-        <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)*'Baseline year demographics'!$C$7</f>
-        <v>9.9348480000000017E-2</v>
+        <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>0.18289152000000003</v>
       </c>
       <c r="M26" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)</f>
@@ -15332,8 +15350,8 @@
         <v>0</v>
       </c>
       <c r="L27" s="27">
-        <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)*'Baseline year demographics'!$C$7</f>
-        <v>4.2577919999999998E-2</v>
+        <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>7.8382080000000007E-2</v>
       </c>
       <c r="M27" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)</f>
@@ -15380,8 +15398,8 @@
         <v>0</v>
       </c>
       <c r="L28" s="27">
-        <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)*'Baseline year demographics'!$C$7</f>
-        <v>6.0825600000000001E-2</v>
+        <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>0.11197440000000002</v>
       </c>
       <c r="M28" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
@@ -15474,8 +15492,8 @@
         <v>0</v>
       </c>
       <c r="L30" s="27">
-        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)*'Baseline year demographics'!$C$7</f>
-        <v>8.8703999999999988E-3</v>
+        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>1.63296E-2</v>
       </c>
       <c r="M30" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)</f>
@@ -15522,20 +15540,20 @@
         <v>0</v>
       </c>
       <c r="L31" s="27">
-        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)*'Baseline year demographics'!$C$7</f>
-        <v>3.8015999999999992E-3</v>
+        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>6.9983999999999992E-3</v>
       </c>
       <c r="M31" s="27">
-        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>9.7199999999999995E-2</v>
+        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)</f>
+        <v>1.0799999999999999E-2</v>
       </c>
       <c r="N31" s="27">
-        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>9.7199999999999995E-2</v>
+        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)</f>
+        <v>1.0799999999999999E-2</v>
       </c>
       <c r="O31" s="27">
-        <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>9.7199999999999995E-2</v>
+        <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)</f>
+        <v>1.0799999999999999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15615,8 +15633,8 @@
         <v>0</v>
       </c>
       <c r="L33" s="27">
-        <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)*'Baseline year demographics'!$C$7</f>
-        <v>1.1038719999999998E-2</v>
+        <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>2.0321280000000001E-2</v>
       </c>
       <c r="M33" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)</f>
@@ -15663,8 +15681,8 @@
         <v>0</v>
       </c>
       <c r="L34" s="27">
-        <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)*'Baseline year demographics'!$C$7</f>
-        <v>4.7308799999999998E-3</v>
+        <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>8.7091200000000007E-3</v>
       </c>
       <c r="M34" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)</f>
@@ -15711,8 +15729,8 @@
         <v>0</v>
       </c>
       <c r="L35" s="27">
-        <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)*'Baseline year demographics'!$C$7</f>
-        <v>6.7583999999999986E-3</v>
+        <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
+        <v>1.2441599999999999E-2</v>
       </c>
       <c r="M35" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)</f>
@@ -16556,6 +16574,7 @@
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -18978,6 +18997,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19284,6 +19304,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26:I27"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19850,6 +19871,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -20147,9 +20169,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -20957,6 +20980,7 @@
     <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="A101" sqref="A101"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -22112,6 +22136,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -22176,6 +22201,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23100,6 +23126,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23536,6 +23563,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -23683,6 +23711,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -24032,6 +24061,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -24359,6 +24389,7 @@
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -24504,6 +24535,7 @@
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -25075,6 +25107,7 @@
     <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Removed dependencies on sprinkles
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="2200" yWindow="-20160" windowWidth="24640" windowHeight="18760" xr2:uid="{A331D684-01C0-6143-BA95-869254A5E453}"/>
+    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1805,6 +1804,126 @@
         </r>
       </text>
     </comment>
+    <comment ref="A69" authorId="1" shapeId="0" xr:uid="{8FF1E441-3BA0-844C-B7B8-11DFECE06F2E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Same effect as iron fortification</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A74" authorId="2" shapeId="0" xr:uid="{0178D8B6-FA21-F149-B1E0-1CD8A8ADD123}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+There is no unit cost for this to impact the budget.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A75" authorId="2" shapeId="0" xr:uid="{0ECE3856-BF67-5048-8528-F0A5D2B157B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+There is no unit cost for this to impact the budget.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A84" authorId="2" shapeId="0" xr:uid="{42139E10-19CD-534F-BFF9-B5DBCCC3E196}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A86" authorId="2" shapeId="0" xr:uid="{B47F5099-031E-624C-9E54-7FDF2CC319B8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -3189,7 +3308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -7506,9 +7625,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7951,7 +8067,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8383,7 +8498,6 @@
     <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9482,11 +9596,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -9497,6 +9606,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9510,7 +9624,6 @@
     <sheetView zoomScale="178" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9726,7 +9839,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9927,7 +10039,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10005,7 +10116,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10310,7 +10420,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11770,7 +11879,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11862,7 +11970,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13067,7 +13174,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13272,7 +13378,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13925,7 +14030,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14102,7 +14206,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14177,10 +14280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -16574,7 +16676,6 @@
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -18992,12 +19093,11 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19018,275 +19118,655 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>54</v>
+      <c r="A2" t="str">
+        <f>'Programs to include'!A2</f>
+        <v>Balanced energy-protein supplementation</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="62" t="s">
-        <v>184</v>
+      <c r="A3" t="str">
+        <f>'Programs to include'!A3</f>
+        <v>Birth age program</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f>'Programs to include'!A4</f>
+        <v>Calcium supplementation</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
-        <v>144</v>
+      <c r="A5" t="str">
+        <f>'Programs to include'!A5</f>
+        <v>Cash transfers</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
-        <v>145</v>
+      <c r="A6" t="str">
+        <f>'Programs to include'!A6</f>
+        <v>Family Planning</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
-        <v>143</v>
+      <c r="A7" t="str">
+        <f>'Programs to include'!A7</f>
+        <v>IFA fortification of maize</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>123</v>
+      <c r="A8" t="str">
+        <f>'Programs to include'!A8</f>
+        <v>IFA fortification of rice</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A9" t="str">
+        <f>'Programs to include'!A9</f>
+        <v>IFA fortification of wheat flour</v>
+      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>124</v>
+      <c r="A10" t="str">
+        <f>'Programs to include'!A10</f>
+        <v>IFAS not poor: community</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>132</v>
+      <c r="A11" t="str">
+        <f>'Programs to include'!A11</f>
+        <v>IFAS not poor: community (malaria area)</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>125</v>
+      <c r="A12" t="str">
+        <f>'Programs to include'!A12</f>
+        <v>IFAS not poor: hospital</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>133</v>
+      <c r="A13" t="str">
+        <f>'Programs to include'!A13</f>
+        <v>IFAS not poor: hospital (malaria area)</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>122</v>
+      <c r="A14" t="str">
+        <f>'Programs to include'!A14</f>
+        <v>IFAS not poor: retailer</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>130</v>
+      <c r="A15" t="str">
+        <f>'Programs to include'!A15</f>
+        <v>IFAS not poor: retailer (malaria area)</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>120</v>
+      <c r="A16" t="str">
+        <f>'Programs to include'!A16</f>
+        <v>IFAS not poor: school</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>128</v>
+      <c r="A17" t="str">
+        <f>'Programs to include'!A17</f>
+        <v>IFAS not poor: school (malaria area)</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>121</v>
+      <c r="A18" t="str">
+        <f>'Programs to include'!A18</f>
+        <v>IFAS poor: community</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>129</v>
+      <c r="A19" t="str">
+        <f>'Programs to include'!A19</f>
+        <v>IFAS poor: community (malaria area)</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>119</v>
+      <c r="A20" t="str">
+        <f>'Programs to include'!A20</f>
+        <v>IFAS poor: hospital</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>127</v>
+      <c r="A21" t="str">
+        <f>'Programs to include'!A21</f>
+        <v>IFAS poor: hospital (malaria area)</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+      <c r="A22" t="str">
+        <f>'Programs to include'!A22</f>
+        <v>IFAS poor: school</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="str">
+        <f>'Programs to include'!A23</f>
+        <v>IFAS poor: school (malaria area)</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="str">
+        <f>'Programs to include'!A24</f>
+        <v>IPTp</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="str">
+        <f>'Programs to include'!A25</f>
+        <v>Iron and folic acid supplementation for pregnant women</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="str">
+        <f>'Programs to include'!A26</f>
+        <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="str">
+        <f>'Programs to include'!A27</f>
+        <v>Iron and iodine fortification of salt</v>
+      </c>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="str">
+        <f>'Programs to include'!A28</f>
+        <v>Iron fortification of maize</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="str">
+        <f>'Programs to include'!A29</f>
+        <v>Iron fortification of rice</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" t="str">
+        <f>'Programs to include'!A30</f>
+        <v>Iron fortification of wheat flour</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" t="str">
+        <f>'Programs to include'!A31</f>
+        <v>Long-lasting insecticide-treated bednets</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="str">
+        <f>'Programs to include'!A32</f>
+        <v>Mg for eclampsia</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" t="str">
+        <f>'Programs to include'!A33</f>
+        <v>Mg for pre-eclampsia</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" t="str">
+        <f>'Programs to include'!A34</f>
+        <v>Multiple micronutrient supplementation</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="str">
+        <f>'Programs to include'!A35</f>
+        <v>Multiple micronutrient supplementation (malaria area)</v>
+      </c>
+      <c r="C35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" t="str">
+        <f>'Programs to include'!A36</f>
+        <v>Oral rehydration salts</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="str">
+        <f>'Programs to include'!A37</f>
+        <v>Public provision of complementary foods</v>
+      </c>
+      <c r="B37" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="str">
+        <f>'Programs to include'!A38</f>
+        <v>Public provision of complementary foods with iron</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" t="str">
+        <f>'Programs to include'!A39</f>
+        <v>Public provision of complementary foods with iron (malaria area)</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="str">
+        <f>'Programs to include'!A40</f>
+        <v>Sprinkles</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="str">
+        <f>'Programs to include'!A41</f>
+        <v>Sprinkles (malaria area)</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="str">
+        <f>'Programs to include'!A42</f>
+        <v>Treatment of MAM</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" t="str">
+        <f>'Programs to include'!A43</f>
+        <v>Treatment of SAM</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="str">
+        <f>'Programs to include'!A44</f>
+        <v>Vitamin A supplementation</v>
+      </c>
+      <c r="B44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" t="str">
+        <f>'Programs to include'!A45</f>
+        <v>WASH: Handwashing</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" t="str">
+        <f>'Programs to include'!A46</f>
+        <v>WASH: Hygenic disposal</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" t="str">
+        <f>'Programs to include'!A47</f>
+        <v>WASH: Improved sanitation</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" t="str">
+        <f>'Programs to include'!A48</f>
+        <v>WASH: Improved water source</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="str">
+        <f>'Programs to include'!A49</f>
+        <v>WASH: Piped water</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="str">
+        <f>'Programs to include'!A50</f>
+        <v>Zinc for treatment + ORS</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="str">
+        <f>'Programs to include'!A51</f>
+        <v>Zinc supplementation</v>
+      </c>
+      <c r="B51" s="4"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="str">
+        <f>'Programs to include'!A52</f>
+        <v>IYCF 1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="str">
+        <f>'Programs to include'!A53</f>
+        <v>IYCF 2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="str">
+        <f>'Programs to include'!A54</f>
+        <v>IYCF 3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <f>'Programs to include'!A64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A65" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A66" s="62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A67" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A68" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A69" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>130</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A85" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B85" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="4" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B86" t="s">
         <v>137</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C86" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A87" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B88" s="12" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A89" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B89" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="4" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A90" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B90" s="12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A91" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
         <v>137</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C93" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A94" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B94" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A95" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A96" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C96" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="4" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A97" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B97" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="30" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A98" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B98" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C98" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A99" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="4" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A100" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A101" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="4" t="s">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A102" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A103" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="4" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A104" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="4" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A105" s="4" t="s">
         <v>162</v>
       </c>
     </row>
@@ -19304,7 +19784,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26:I27"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19871,7 +20350,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -20172,7 +20650,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -20980,7 +21457,6 @@
     <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="A101" sqref="A101"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -22136,7 +22612,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -22201,7 +22676,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23126,7 +23600,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23563,7 +24036,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -23711,7 +24183,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -24061,7 +24532,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -24389,7 +24859,6 @@
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -24535,7 +25004,6 @@
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -25107,7 +25575,6 @@
     <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Ability to subset programs for optimisation based upon impact
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36880" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="21" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3308,7 +3308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -19095,7 +19095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
@@ -20648,7 +20648,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23597,8 +23597,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23627,7 +23627,9 @@
       <c r="A3" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="132"/>
+      <c r="B3" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Removed zinc supplementation direct impact on stunting (OR=1)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5380" yWindow="-20680" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2275,7 +2275,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -2284,12 +2284,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-fictional</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>fictional</t>
         </r>
       </text>
     </comment>
@@ -2963,7 +2972,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
-    <author>Janka Petravic</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
@@ -2991,27 +2999,79 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{B6F74FB5-0F52-2740-99BD-E2E0C841B7A4}">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LiST had 1.11 (0.9 for us), but removed impact due to very large impact.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{BA06A807-3581-A04E-8BD3-F953624B1017}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Janka Petravic:</t>
+          <t>LiST had 1.11 (0.9 for us), but removed impact due to very large impact.</t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-LiST: 1.11</t>
+</t>
         </r>
       </text>
     </comment>
@@ -3120,7 +3180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0900-000007000000}">
+    <comment ref="B18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0900-000007000000}">
       <text>
         <r>
           <rPr>
@@ -3144,7 +3204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0900-000008000000}">
+    <comment ref="B19" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0900-000008000000}">
       <text>
         <r>
           <rPr>
@@ -4025,7 +4085,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4189,6 +4249,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -7953,8 +8026,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8165,10 +8238,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -11856,7 +11929,7 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -18984,7 +19057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
@@ -20364,8 +20437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updated unit costs and bug fix
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="280" yWindow="-20920" windowWidth="35600" windowHeight="20580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37280" yWindow="-20860" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId32"/>
+    <externalReference r:id="rId33"/>
   </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1901,6 +1902,7 @@
     <author>Microsoft Office User</author>
     <author xml:space="preserve"> Janka Petravic</author>
     <author>Sam</author>
+    <author>Nick</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000001000000}">
@@ -1928,7 +1930,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000002000000}">
+    <comment ref="D5" authorId="1" shapeId="0" xr:uid="{A1E65624-DE3D-D14E-83C9-8C773DAC3361}">
       <text>
         <r>
           <rPr>
@@ -1952,7 +1954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000003000000}">
+    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{3E219A7C-659D-FF46-AE72-C054AE09773E}">
       <text>
         <r>
           <rPr>
@@ -1976,7 +1978,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000005000000}">
+    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{9EB5DC4C-B342-0248-A1E4-002D1787AD90}">
       <text>
         <r>
           <rPr>
@@ -2024,7 +2026,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000007000000}">
+    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{1DF64208-29DB-594C-8B3C-0E81C62C641F}">
       <text>
         <r>
           <rPr>
@@ -2072,7 +2074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000009000000}">
+    <comment ref="D14" authorId="1" shapeId="0" xr:uid="{65288BA2-E26E-CB41-B589-9D49AA5AA491}">
       <text>
         <r>
           <rPr>
@@ -2120,7 +2122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-00000B000000}">
+    <comment ref="D15" authorId="1" shapeId="0" xr:uid="{E0A94450-82D5-804F-80BE-A8E6FCB0B453}">
       <text>
         <r>
           <rPr>
@@ -2168,7 +2170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-00000D000000}">
+    <comment ref="D25" authorId="1" shapeId="0" xr:uid="{815B3481-9AAE-8240-969F-0169020E6771}">
       <text>
         <r>
           <rPr>
@@ -2249,7 +2251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000010000000}">
+    <comment ref="D27" authorId="1" shapeId="0" xr:uid="{7D532413-F852-4C4F-ACF4-7D68E50D583D}">
       <text>
         <r>
           <rPr>
@@ -2306,7 +2308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000013000000}">
+    <comment ref="D31" authorId="3" shapeId="0" xr:uid="{417E64AA-E4E5-0846-85A0-F5E6423A131A}">
       <text>
         <r>
           <rPr>
@@ -2330,7 +2332,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000014000000}">
+    <comment ref="D33" authorId="4" shapeId="0" xr:uid="{22579B08-B959-2E47-958D-B4ABF735A6AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BJOG. 2006 Feb;113(2):144-51.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D39" authorId="0" shapeId="0" xr:uid="{EA709C1A-7547-C246-A9CD-20DEA0F2AB21}">
       <text>
         <r>
           <rPr>
@@ -2355,13 +2381,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="D40" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000015000000}">
+    <comment ref="D40" authorId="1" shapeId="0" xr:uid="{11460982-48AC-0447-9BDC-CBD495A945F4}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -2370,16 +2396,25 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Horton CCC 2008: $0.9 -&gt; use $1 because of inflation</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Horton CCC 2008: $0.9 -&gt; use $1 because of inflation</t>
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000016000000}">
+    <comment ref="D42" authorId="1" shapeId="0" xr:uid="{2AED3EC0-27D2-3D4B-BE18-A29440CC0EB2}">
       <text>
         <r>
           <rPr>
@@ -2412,7 +2447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1A00-000017000000}">
+    <comment ref="D48" authorId="0" shapeId="0" xr:uid="{84B73750-3D6E-424A-918C-75383154C540}">
       <text>
         <r>
           <rPr>
@@ -4092,7 +4127,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4268,6 +4303,19 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -7453,6 +7501,158 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Baseline year demographics"/>
+      <sheetName val="Demographic projections"/>
+      <sheetName val="Causes of death"/>
+      <sheetName val="Incidence of conditions"/>
+      <sheetName val="Prevalence of anaemia"/>
+      <sheetName val="Distributions"/>
+      <sheetName val="Distribution births"/>
+      <sheetName val="Birth outcomes &amp; risks"/>
+      <sheetName val="Relative risks"/>
+      <sheetName val="Odds ratios"/>
+      <sheetName val="IYCF package odds ratios"/>
+      <sheetName val="IYCF packages"/>
+      <sheetName val="IYCF cost &amp; coverage"/>
+      <sheetName val="Appropriate breastfeeding"/>
+      <sheetName val="Programs birth outcomes"/>
+      <sheetName val="Programs anemia"/>
+      <sheetName val="Programs wasting"/>
+      <sheetName val="Programs for children"/>
+      <sheetName val="Programs family planning"/>
+      <sheetName val="Programs for PW"/>
+      <sheetName val="Programs birth age"/>
+      <sheetName val="Programs target population"/>
+      <sheetName val="Programs impacted population"/>
+      <sheetName val="Program dependencies"/>
+      <sheetName val="Program risk areas"/>
+      <sheetName val="Population risk areas"/>
+      <sheetName val="Programs cost and coverage"/>
+      <sheetName val="Programs annual spending"/>
+      <sheetName val="Reference programs"/>
+      <sheetName val="Programs to include"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="5">
+          <cell r="B5">
+            <v>0.39</v>
+          </cell>
+          <cell r="C5">
+            <v>0.39</v>
+          </cell>
+          <cell r="D5">
+            <v>0.33540000000000003</v>
+          </cell>
+          <cell r="E5">
+            <v>0.28600000000000003</v>
+          </cell>
+          <cell r="F5">
+            <v>0.27300000000000002</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0.12740000000000001</v>
+          </cell>
+          <cell r="C6">
+            <v>0.12740000000000001</v>
+          </cell>
+          <cell r="D6">
+            <v>0.13780000000000001</v>
+          </cell>
+          <cell r="E6">
+            <v>0.10659999999999999</v>
+          </cell>
+          <cell r="F6">
+            <v>5.4600000000000003E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18">
+        <row r="2">
+          <cell r="E2">
+            <v>7.1999999999999995E-2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="E3">
+            <v>3.7999999999999999E-2</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>0.16</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>0.126</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="E6">
+            <v>1.3999999999999999E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>0.40500000000000003</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>6.0000000000000001E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -13808,11 +14008,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -13823,6 +14018,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18492,8 +18692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19575,13 +19775,13 @@
         <v>0.20275200000000002</v>
       </c>
       <c r="M25" s="27">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="N25" s="27">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="O25" s="27">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -24687,8 +24887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24753,7 +24953,7 @@
         <v>0.95</v>
       </c>
       <c r="D4" s="19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -24784,7 +24984,7 @@
         <v>0.95</v>
       </c>
       <c r="D6" s="19">
-        <f>SUM('Programs family planning'!E2:E10)</f>
+        <f>SUM('[2]Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
       <c r="E6" s="62"/>
@@ -25159,7 +25359,7 @@
         <v>0.95</v>
       </c>
       <c r="D32" s="31">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -25173,7 +25373,7 @@
         <v>0.95</v>
       </c>
       <c r="D33" s="31">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -25217,7 +25417,7 @@
         <v>0.95</v>
       </c>
       <c r="D36" s="19">
-        <v>1</v>
+        <v>23.84</v>
       </c>
       <c r="E36" s="4"/>
     </row>
@@ -25307,8 +25507,8 @@
         <v>0.95</v>
       </c>
       <c r="D42" s="19">
-        <f>30*AVERAGE('Incidence of conditions'!B5:F5)</f>
-        <v>10.046400000000002</v>
+        <f>40*AVERAGE('[2]Incidence of conditions'!B5:F5)</f>
+        <v>13.395200000000003</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -25322,8 +25522,8 @@
         <v>0.95</v>
       </c>
       <c r="D43" s="19">
-        <f>179.97*AVERAGE('Incidence of conditions'!B6:F6)</f>
-        <v>19.933477200000002</v>
+        <f>90*AVERAGE('[2]Incidence of conditions'!B6:F6)</f>
+        <v>9.9684000000000008</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -25421,7 +25621,7 @@
         <v>0.95</v>
       </c>
       <c r="D50" s="19">
-        <v>1.5</v>
+        <v>5.53</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -25435,7 +25635,7 @@
         <v>0.95</v>
       </c>
       <c r="D51" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -26649,7 +26849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90087AAD-2450-AE43-8C0E-64315E9A418C}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -27147,7 +27347,7 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed birth age program from run
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37280" yWindow="-20860" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37280" yWindow="-20860" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3296,7 +3296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -24887,8 +24887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27347,8 +27347,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27377,9 +27377,7 @@
       <c r="A3" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B3" s="132"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Changed maternal mortality rate units
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37280" yWindow="-20860" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37420" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
     <author>Janka Petravic</author>
     <author>Ruth</author>
+    <author>Sam</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -74,7 +75,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -83,12 +84,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This is calculated, this is why it is grey -f formula should be in the input sheet</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is calculated, this is why it is grey -f formula should be in the input sheet</t>
         </r>
       </text>
     </comment>
@@ -149,27 +159,36 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{50B64CE5-C19E-7045-8799-38D8A3A6E19C}">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Sam:</t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-per 100,000 live births</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Per 1000 live births</t>
         </r>
       </text>
     </comment>
@@ -227,7 +246,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -236,12 +255,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Per 1000 live births</t>
         </r>
       </text>
     </comment>
@@ -251,7 +279,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -260,12 +288,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Per 1000 live births</t>
         </r>
       </text>
     </comment>
@@ -275,7 +312,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -284,12 +321,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Per 1000 live births</t>
         </r>
       </text>
     </comment>
@@ -3296,7 +3342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -7537,9 +7583,9 @@
       <sheetName val="Programs to include"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="5">
           <cell r="B5">
@@ -7576,20 +7622,20 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
       <sheetData sheetId="18">
         <row r="2">
           <cell r="E2">
@@ -7637,17 +7683,17 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7977,8 +8023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8130,7 +8176,8 @@
         <v>187</v>
       </c>
       <c r="C18" s="19">
-        <v>176</v>
+        <f>176/100</f>
+        <v>1.76</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17581,7 +17628,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18233,7 +18280,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18693,7 +18740,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21085,8 +21132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23508,7 +23555,7 @@
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24021,8 +24068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24588,7 +24635,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24888,7 +24935,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25694,8 +25741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34C1B36-2F1D-8141-8AE0-24B0DA699162}">
   <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25795,9 +25842,6 @@
         <v>271</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="D3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
@@ -27281,7 +27325,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27347,8 +27391,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27369,9 +27413,7 @@
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B2" s="132"/>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
@@ -27383,17 +27425,13 @@
       <c r="A4" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B4" s="132"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B5" s="132"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -27407,169 +27445,127 @@
       <c r="A7" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B7" s="132"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B8" s="132"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B9" s="132"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B10" s="132"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B11" s="132"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B12" s="132"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B13" s="132"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B14" s="132"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B15" s="132"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B16" s="132"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B17" s="132"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B18" s="132"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B19" s="132"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B20" s="132"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B21" s="132"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B22" s="132"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B23" s="132"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B24" s="132"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B25" s="132"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B26" s="132"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B27" s="132"/>
     </row>
     <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="126" t="s">
@@ -27590,177 +27586,133 @@
       <c r="A31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B31" s="132"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B32" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B32" s="132"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B33" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B33" s="132"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B34" s="132"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B35" s="132"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B36" s="132"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B37" s="132"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B38" s="132"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B39" s="132"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B40" s="132"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B41" s="132"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B42" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B42" s="132"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B43" s="132"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B44" s="132"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B45" s="132"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>259</v>
       </c>
-      <c r="B46" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B46" s="132"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>258</v>
       </c>
-      <c r="B47" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B47" s="132"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>256</v>
       </c>
-      <c r="B48" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B48" s="132"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>257</v>
       </c>
-      <c r="B49" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B49" s="132"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>262</v>
       </c>
-      <c r="B50" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B50" s="132"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B51" s="132"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B52" s="132"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="125" t="s">

</xml_diff>

<commit_message>
Changed output trackers to dictionaries, other clean-ups
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37420" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36540" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3342,7 +3342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -8023,7 +8023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -25742,7 +25742,7 @@
   <dimension ref="A1:Y107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25922,6 +25922,45 @@
         <v>271</v>
       </c>
       <c r="C11" s="35"/>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
@@ -26894,7 +26933,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27391,8 +27430,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27413,7 +27452,9 @@
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
@@ -27425,13 +27466,17 @@
       <c r="A4" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="132"/>
+      <c r="B4" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="132"/>
+      <c r="B5" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -27445,127 +27490,169 @@
       <c r="A7" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="132"/>
+      <c r="B7" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="132"/>
+      <c r="B8" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="132"/>
+      <c r="B10" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="132"/>
+      <c r="B12" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="132"/>
+      <c r="B13" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="132"/>
+      <c r="B14" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="132"/>
+      <c r="B15" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="132"/>
+      <c r="B16" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="132"/>
+      <c r="B17" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="132"/>
+      <c r="B18" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="132"/>
+      <c r="B19" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="132"/>
+      <c r="B20" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="132"/>
+      <c r="B21" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="132"/>
+      <c r="B22" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="132"/>
+      <c r="B23" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="132"/>
+      <c r="B24" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="132"/>
+      <c r="B25" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="132"/>
+      <c r="B26" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="132"/>
+      <c r="B27" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="126" t="s">
@@ -27586,133 +27673,177 @@
       <c r="A31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="132"/>
+      <c r="B31" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B32" s="132"/>
+      <c r="B32" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B33" s="132"/>
+      <c r="B33" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="132"/>
+      <c r="B34" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="132"/>
+      <c r="B35" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="132"/>
+      <c r="B36" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="132"/>
+      <c r="B37" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="132"/>
+      <c r="B38" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="132"/>
+      <c r="B39" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="132"/>
+      <c r="B40" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="132"/>
+      <c r="B41" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B42" s="132"/>
+      <c r="B42" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="132"/>
+      <c r="B43" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="132"/>
+      <c r="B44" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="132"/>
+      <c r="B45" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>259</v>
       </c>
-      <c r="B46" s="132"/>
+      <c r="B46" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>258</v>
       </c>
-      <c r="B47" s="132"/>
+      <c r="B47" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>256</v>
       </c>
-      <c r="B48" s="132"/>
+      <c r="B48" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>257</v>
       </c>
-      <c r="B49" s="132"/>
+      <c r="B49" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>262</v>
       </c>
-      <c r="B50" s="132"/>
+      <c r="B50" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="132"/>
+      <c r="B51" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="132"/>
+      <c r="B52" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="125" t="s">

</xml_diff>

<commit_message>
MAM & SAM outcomes
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36540" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -7399,11 +7399,11 @@
       <sheetName val="Programs to include"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5">
         <row r="3">
           <cell r="C3">
@@ -7517,31 +7517,31 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8466,7 +8466,7 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -14877,7 +14877,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18740,7 +18740,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21133,7 +21133,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23554,8 +23554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24069,7 +24069,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24935,7 +24935,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25922,45 +25922,6 @@
         <v>271</v>
       </c>
       <c r="C11" s="35"/>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
@@ -27430,8 +27391,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27658,16 +27619,19 @@
       <c r="A28" s="126" t="s">
         <v>80</v>
       </c>
+      <c r="B28" s="132"/>
     </row>
     <row r="29" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="126" t="s">
         <v>81</v>
       </c>
+      <c r="B29" s="132"/>
     </row>
     <row r="30" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="126" t="s">
         <v>79</v>
       </c>
+      <c r="B30" s="132"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">

</xml_diff>

<commit_message>
Using projected WRA population to get PW population and births
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,6 @@
     <sheet name="Reference programs" sheetId="48" r:id="rId30"/>
     <sheet name="Programs to include" sheetId="44" r:id="rId31"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId32"/>
-    <externalReference r:id="rId33"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -7361,344 +7357,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Baseline year demographics"/>
-      <sheetName val="Demographic projections"/>
-      <sheetName val="Annual prevalence"/>
-      <sheetName val="Causes of death"/>
-      <sheetName val="Incidence of conditions"/>
-      <sheetName val="Prevalence of anaemia"/>
-      <sheetName val="Distributions"/>
-      <sheetName val="Distribution births"/>
-      <sheetName val="Birth outcomes &amp; risks"/>
-      <sheetName val="Relative risks"/>
-      <sheetName val="Odds ratios"/>
-      <sheetName val="IYCF package odds ratios"/>
-      <sheetName val="IYCF packages"/>
-      <sheetName val="IYCF cost &amp; coverage"/>
-      <sheetName val="Appropriate breastfeeding"/>
-      <sheetName val="Programs birth outcomes"/>
-      <sheetName val="Programs anemia"/>
-      <sheetName val="Programs wasting"/>
-      <sheetName val="Programs for children"/>
-      <sheetName val="Programs family planning"/>
-      <sheetName val="Programs for PW"/>
-      <sheetName val="Programs birth age"/>
-      <sheetName val="Programs target population"/>
-      <sheetName val="Programs impacted population"/>
-      <sheetName val="Program dependencies"/>
-      <sheetName val="Program risk areas"/>
-      <sheetName val="Population risk areas"/>
-      <sheetName val="Programs annual scale-up"/>
-      <sheetName val="Programs annual spending"/>
-      <sheetName val="Reference programs"/>
-      <sheetName val="Programs cost and coverage"/>
-      <sheetName val="Programs to include"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="3">
-          <cell r="C3">
-            <v>0.05</v>
-          </cell>
-          <cell r="D3">
-            <v>0.05</v>
-          </cell>
-          <cell r="E3">
-            <v>0.31079999999999997</v>
-          </cell>
-          <cell r="F3">
-            <v>0.23100000000000001</v>
-          </cell>
-          <cell r="G3">
-            <v>0.17934</v>
-          </cell>
-          <cell r="H3">
-            <v>0.23580000000000001</v>
-          </cell>
-          <cell r="I3">
-            <v>0.23580000000000001</v>
-          </cell>
-          <cell r="J3">
-            <v>0.23580000000000001</v>
-          </cell>
-          <cell r="K3">
-            <v>0.23580000000000001</v>
-          </cell>
-          <cell r="L3">
-            <v>0.2238</v>
-          </cell>
-          <cell r="M3">
-            <v>0.2238</v>
-          </cell>
-          <cell r="N3">
-            <v>0.2238</v>
-          </cell>
-          <cell r="O3">
-            <v>0.2238</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="4">
-          <cell r="C4">
-            <v>0.10199999999999999</v>
-          </cell>
-          <cell r="D4">
-            <v>0.10199999999999999</v>
-          </cell>
-          <cell r="E4">
-            <v>0.14699999999999999</v>
-          </cell>
-          <cell r="F4">
-            <v>0.247</v>
-          </cell>
-          <cell r="G4">
-            <v>0.28100000000000003</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>3.7999999999999999E-2</v>
-          </cell>
-          <cell r="D5">
-            <v>3.7999999999999999E-2</v>
-          </cell>
-          <cell r="E5">
-            <v>4.9000000000000002E-2</v>
-          </cell>
-          <cell r="F5">
-            <v>0.13400000000000001</v>
-          </cell>
-          <cell r="G5">
-            <v>0.13300000000000001</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>0.15</v>
-          </cell>
-          <cell r="D10">
-            <v>0.15</v>
-          </cell>
-          <cell r="E10">
-            <v>0.129</v>
-          </cell>
-          <cell r="F10">
-            <v>0.11</v>
-          </cell>
-          <cell r="G10">
-            <v>0.105</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>4.9000000000000002E-2</v>
-          </cell>
-          <cell r="D11">
-            <v>4.9000000000000002E-2</v>
-          </cell>
-          <cell r="E11">
-            <v>5.2999999999999999E-2</v>
-          </cell>
-          <cell r="F11">
-            <v>4.0999999999999995E-2</v>
-          </cell>
-          <cell r="G11">
-            <v>2.1000000000000001E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Baseline year demographics"/>
-      <sheetName val="Demographic projections"/>
-      <sheetName val="Causes of death"/>
-      <sheetName val="Incidence of conditions"/>
-      <sheetName val="Prevalence of anaemia"/>
-      <sheetName val="Distributions"/>
-      <sheetName val="Distribution births"/>
-      <sheetName val="Birth outcomes &amp; risks"/>
-      <sheetName val="Relative risks"/>
-      <sheetName val="Odds ratios"/>
-      <sheetName val="IYCF package odds ratios"/>
-      <sheetName val="IYCF packages"/>
-      <sheetName val="IYCF cost &amp; coverage"/>
-      <sheetName val="Appropriate breastfeeding"/>
-      <sheetName val="Programs birth outcomes"/>
-      <sheetName val="Programs anemia"/>
-      <sheetName val="Programs wasting"/>
-      <sheetName val="Programs for children"/>
-      <sheetName val="Programs family planning"/>
-      <sheetName val="Programs for PW"/>
-      <sheetName val="Programs birth age"/>
-      <sheetName val="Programs target population"/>
-      <sheetName val="Programs impacted population"/>
-      <sheetName val="Program dependencies"/>
-      <sheetName val="Program risk areas"/>
-      <sheetName val="Population risk areas"/>
-      <sheetName val="Programs cost and coverage"/>
-      <sheetName val="Programs annual spending"/>
-      <sheetName val="Reference programs"/>
-      <sheetName val="Programs to include"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="5">
-          <cell r="B5">
-            <v>0.39</v>
-          </cell>
-          <cell r="C5">
-            <v>0.39</v>
-          </cell>
-          <cell r="D5">
-            <v>0.33540000000000003</v>
-          </cell>
-          <cell r="E5">
-            <v>0.28600000000000003</v>
-          </cell>
-          <cell r="F5">
-            <v>0.27300000000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>0.12740000000000001</v>
-          </cell>
-          <cell r="C6">
-            <v>0.12740000000000001</v>
-          </cell>
-          <cell r="D6">
-            <v>0.13780000000000001</v>
-          </cell>
-          <cell r="E6">
-            <v>0.10659999999999999</v>
-          </cell>
-          <cell r="F6">
-            <v>5.4600000000000003E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18">
-        <row r="2">
-          <cell r="E2">
-            <v>7.1999999999999995E-2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="E3">
-            <v>3.7999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="E4">
-            <v>0.16</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5">
-            <v>0.126</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>1.3999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7">
-            <v>0.40500000000000003</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>6.0000000000000001E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -23554,8 +23212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25031,7 +24689,7 @@
         <v>0.95</v>
       </c>
       <c r="D6" s="19">
-        <f>SUM('[2]Programs family planning'!E2:E10)</f>
+        <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
       <c r="E6" s="62"/>
@@ -25554,7 +25212,7 @@
         <v>0.95</v>
       </c>
       <c r="D42" s="19">
-        <f>40*AVERAGE('[2]Incidence of conditions'!B5:F5)</f>
+        <f>40*AVERAGE('Incidence of conditions'!B5:F5)</f>
         <v>13.395200000000003</v>
       </c>
     </row>
@@ -25569,7 +25227,7 @@
         <v>0.95</v>
       </c>
       <c r="D43" s="19">
-        <f>90*AVERAGE('[2]Incidence of conditions'!B6:F6)</f>
+        <f>90*AVERAGE('Incidence of conditions'!B6:F6)</f>
         <v>9.9684000000000008</v>
       </c>
     </row>
@@ -25742,7 +25400,7 @@
   <dimension ref="A1:Y107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25973,7 +25631,7 @@
       </c>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f>A16</f>
         <v>IFA fortification of wheat flour</v>
@@ -25983,7 +25641,7 @@
       </c>
       <c r="C17" s="35"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f>'Programs to include'!A10</f>
         <v>IFAS not poor: community</v>
@@ -25993,7 +25651,7 @@
       </c>
       <c r="C18" s="35"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f>A18</f>
         <v>IFAS not poor: community</v>
@@ -26002,8 +25660,11 @@
         <v>271</v>
       </c>
       <c r="C19" s="35"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f>'Programs to include'!A11</f>
         <v>IFAS not poor: community (malaria area)</v>
@@ -26013,7 +25674,7 @@
       </c>
       <c r="C20" s="35"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f>A20</f>
         <v>IFAS not poor: community (malaria area)</v>
@@ -26022,8 +25683,11 @@
         <v>271</v>
       </c>
       <c r="C21" s="35"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f>'Programs to include'!A12</f>
         <v>IFAS not poor: hospital</v>
@@ -26033,7 +25697,7 @@
       </c>
       <c r="C22" s="35"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>A22</f>
         <v>IFAS not poor: hospital</v>
@@ -26042,8 +25706,11 @@
         <v>271</v>
       </c>
       <c r="C23" s="35"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f>'Programs to include'!A13</f>
         <v>IFAS not poor: hospital (malaria area)</v>
@@ -26053,7 +25720,7 @@
       </c>
       <c r="C24" s="35"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f>A24</f>
         <v>IFAS not poor: hospital (malaria area)</v>
@@ -26062,8 +25729,11 @@
         <v>271</v>
       </c>
       <c r="C25" s="35"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="str">
         <f>'Programs to include'!A14</f>
         <v>IFAS not poor: retailer</v>
@@ -26073,7 +25743,7 @@
       </c>
       <c r="C26" s="35"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="str">
         <f>A26</f>
         <v>IFAS not poor: retailer</v>
@@ -26083,7 +25753,7 @@
       </c>
       <c r="C27" s="35"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="str">
         <f>'Programs to include'!A15</f>
         <v>IFAS not poor: retailer (malaria area)</v>
@@ -26093,7 +25763,7 @@
       </c>
       <c r="C28" s="35"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="str">
         <f>A28</f>
         <v>IFAS not poor: retailer (malaria area)</v>
@@ -26103,7 +25773,7 @@
       </c>
       <c r="C29" s="35"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="str">
         <f>'Programs to include'!A16</f>
         <v>IFAS not poor: school</v>
@@ -26113,7 +25783,7 @@
       </c>
       <c r="C30" s="35"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="str">
         <f>A30</f>
         <v>IFAS not poor: school</v>
@@ -26123,7 +25793,7 @@
       </c>
       <c r="C31" s="35"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="str">
         <f>'Programs to include'!A17</f>
         <v>IFAS not poor: school (malaria area)</v>
@@ -26942,39 +26612,39 @@
         <v>6</v>
       </c>
       <c r="C2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="D2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="E2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="F2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="G2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="H2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="I2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="J2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="K2" s="94">
-        <f>SUM([1]Distributions!$C$4:$C$5)</f>
+        <f>SUM(Distributions!$C$4:$C$5)</f>
         <v>0.13999999999999999</v>
       </c>
     </row>
@@ -26983,39 +26653,39 @@
         <v>7</v>
       </c>
       <c r="C3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="D3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="E3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="F3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="G3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="H3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="I3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="J3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="K3" s="94">
-        <f>SUM([1]Distributions!D$4:D$5)</f>
+        <f>SUM(Distributions!D$4:D$5)</f>
         <v>0.13999999999999999</v>
       </c>
     </row>
@@ -27024,39 +26694,39 @@
         <v>8</v>
       </c>
       <c r="C4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="D4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="E4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="F4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="G4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="H4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="I4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="J4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="K4" s="94">
-        <f>SUM([1]Distributions!E$4:E$5)</f>
+        <f>SUM(Distributions!E$4:E$5)</f>
         <v>0.19600000000000001</v>
       </c>
     </row>
@@ -27065,39 +26735,39 @@
         <v>9</v>
       </c>
       <c r="C5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="D5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="E5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="F5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="G5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="H5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="I5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="J5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
       <c r="K5" s="94">
-        <f>SUM([1]Distributions!F$4:F$5)</f>
+        <f>SUM(Distributions!F$4:F$5)</f>
         <v>0.38100000000000001</v>
       </c>
     </row>
@@ -27106,39 +26776,39 @@
         <v>10</v>
       </c>
       <c r="C6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="D6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="E6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="F6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="G6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="H6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="I6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="J6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
       <c r="K6" s="94">
-        <f>SUM([1]Distributions!G$4:G$5)</f>
+        <f>SUM(Distributions!G$4:G$5)</f>
         <v>0.41400000000000003</v>
       </c>
     </row>
@@ -27150,7 +26820,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="94">
-        <f>SUM([1]Distributions!C10:C11)</f>
+        <f>SUM(Distributions!C10:C11)</f>
         <v>0.19900000000000001</v>
       </c>
     </row>
@@ -27159,7 +26829,7 @@
         <v>7</v>
       </c>
       <c r="K9" s="94">
-        <f>SUM([1]Distributions!D10:D11)</f>
+        <f>SUM(Distributions!D10:D11)</f>
         <v>0.19900000000000001</v>
       </c>
     </row>
@@ -27168,7 +26838,7 @@
         <v>8</v>
       </c>
       <c r="K10" s="94">
-        <f>SUM([1]Distributions!E10:E11)</f>
+        <f>SUM(Distributions!E10:E11)</f>
         <v>0.182</v>
       </c>
     </row>
@@ -27177,7 +26847,7 @@
         <v>9</v>
       </c>
       <c r="K11" s="94">
-        <f>SUM([1]Distributions!F10:F11)</f>
+        <f>SUM(Distributions!F10:F11)</f>
         <v>0.151</v>
       </c>
     </row>
@@ -27186,7 +26856,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="94">
-        <f>SUM([1]Distributions!G10:G11)</f>
+        <f>SUM(Distributions!G10:G11)</f>
         <v>0.126</v>
       </c>
     </row>
@@ -27198,7 +26868,7 @@
         <v>6</v>
       </c>
       <c r="K14" s="94">
-        <f>'[1]Prevalence of anaemia'!C3</f>
+        <f>'Prevalence of anaemia'!C3</f>
         <v>0.05</v>
       </c>
     </row>
@@ -27207,7 +26877,7 @@
         <v>7</v>
       </c>
       <c r="K15" s="94">
-        <f>'[1]Prevalence of anaemia'!D3</f>
+        <f>'Prevalence of anaemia'!D3</f>
         <v>0.05</v>
       </c>
     </row>
@@ -27216,7 +26886,7 @@
         <v>8</v>
       </c>
       <c r="K16" s="94">
-        <f>'[1]Prevalence of anaemia'!E3</f>
+        <f>'Prevalence of anaemia'!E3</f>
         <v>0.31079999999999997</v>
       </c>
     </row>
@@ -27225,7 +26895,7 @@
         <v>9</v>
       </c>
       <c r="K17" s="94">
-        <f>'[1]Prevalence of anaemia'!F3</f>
+        <f>'Prevalence of anaemia'!F3</f>
         <v>0.23100000000000001</v>
       </c>
     </row>
@@ -27234,7 +26904,7 @@
         <v>10</v>
       </c>
       <c r="K18" s="94">
-        <f>'[1]Prevalence of anaemia'!G3</f>
+        <f>'Prevalence of anaemia'!G3</f>
         <v>0.17934</v>
       </c>
     </row>
@@ -27243,7 +26913,7 @@
         <v>114</v>
       </c>
       <c r="K19" s="94">
-        <f>'[1]Prevalence of anaemia'!H3</f>
+        <f>'Prevalence of anaemia'!H3</f>
         <v>0.23580000000000001</v>
       </c>
     </row>
@@ -27252,7 +26922,7 @@
         <v>115</v>
       </c>
       <c r="K20" s="94">
-        <f>'[1]Prevalence of anaemia'!I3</f>
+        <f>'Prevalence of anaemia'!I3</f>
         <v>0.23580000000000001</v>
       </c>
     </row>
@@ -27261,7 +26931,7 @@
         <v>116</v>
       </c>
       <c r="K21" s="94">
-        <f>'[1]Prevalence of anaemia'!J3</f>
+        <f>'Prevalence of anaemia'!J3</f>
         <v>0.23580000000000001</v>
       </c>
     </row>
@@ -27270,7 +26940,7 @@
         <v>117</v>
       </c>
       <c r="K22" s="94">
-        <f>'[1]Prevalence of anaemia'!K3</f>
+        <f>'Prevalence of anaemia'!K3</f>
         <v>0.23580000000000001</v>
       </c>
     </row>
@@ -27279,7 +26949,7 @@
         <v>110</v>
       </c>
       <c r="K23" s="94">
-        <f>'[1]Prevalence of anaemia'!L3</f>
+        <f>'Prevalence of anaemia'!L3</f>
         <v>0.2238</v>
       </c>
     </row>
@@ -27288,7 +26958,7 @@
         <v>111</v>
       </c>
       <c r="K24" s="94">
-        <f>'[1]Prevalence of anaemia'!M3</f>
+        <f>'Prevalence of anaemia'!M3</f>
         <v>0.2238</v>
       </c>
     </row>
@@ -27297,7 +26967,7 @@
         <v>112</v>
       </c>
       <c r="K25" s="94">
-        <f>'[1]Prevalence of anaemia'!N3</f>
+        <f>'Prevalence of anaemia'!N3</f>
         <v>0.2238</v>
       </c>
     </row>
@@ -27306,7 +26976,7 @@
         <v>113</v>
       </c>
       <c r="K26" s="94">
-        <f>'[1]Prevalence of anaemia'!O3</f>
+        <f>'Prevalence of anaemia'!O3</f>
         <v>0.2238</v>
       </c>
     </row>
@@ -27391,8 +27061,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Changed malaria area to 33%
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="17" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3338,7 +3338,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -7682,7 +7682,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7767,7 +7767,7 @@
         <v>66</v>
       </c>
       <c r="C9" s="19">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13713,6 +13713,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -13723,11 +13728,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18397,8 +18397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18698,11 +18698,11 @@
       </c>
       <c r="E7" s="27">
         <f>'Baseline year demographics'!C8*(1-'Baseline year demographics'!C9)</f>
-        <v>0.32400000000000001</v>
+        <v>0.24119999999999997</v>
       </c>
       <c r="F7" s="27">
         <f>'Baseline year demographics'!C8*(1-'Baseline year demographics'!C9)</f>
-        <v>0.32400000000000001</v>
+        <v>0.24119999999999997</v>
       </c>
       <c r="G7" s="27">
         <v>0</v>
@@ -18744,11 +18744,11 @@
       </c>
       <c r="E8" s="27">
         <f>'Baseline year demographics'!C8*'Baseline year demographics'!C9</f>
-        <v>3.5999999999999997E-2</v>
+        <v>0.1188</v>
       </c>
       <c r="F8" s="27">
         <f>'Baseline year demographics'!C8*'Baseline year demographics'!C9</f>
-        <v>3.5999999999999997E-2</v>
+        <v>0.1188</v>
       </c>
       <c r="G8" s="27">
         <v>0</v>
@@ -18790,15 +18790,15 @@
       </c>
       <c r="E9" s="27">
         <f>(1-'Baseline year demographics'!$C9)</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="F9" s="27">
         <f>(1-'Baseline year demographics'!$C9)</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="G9" s="27">
         <f>(1-'Baseline year demographics'!$C9)</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
@@ -18837,15 +18837,15 @@
       </c>
       <c r="E10" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="F10" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="G10" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="H10" s="3">
         <v>0</v>
@@ -19081,19 +19081,19 @@
       </c>
       <c r="H16" s="3">
         <f>1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="I16" s="3">
         <f>1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="J16" s="3">
         <f>1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="K16" s="3">
         <f>1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="L16" s="3">
         <v>0</v>
@@ -19129,19 +19129,19 @@
       </c>
       <c r="H17" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="I17" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="J17" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="K17" s="27">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
@@ -19177,19 +19177,19 @@
       </c>
       <c r="H18" s="32">
         <f xml:space="preserve"> 1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="I18" s="32">
         <f xml:space="preserve"> 1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="J18" s="32">
         <f xml:space="preserve"> 1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="K18" s="32">
         <f xml:space="preserve"> 1-'Baseline year demographics'!$C9</f>
-        <v>0.9</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="L18" s="3">
         <v>0</v>
@@ -19225,19 +19225,19 @@
       </c>
       <c r="H19" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="I19" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="J19" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="K19" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="L19" s="3">
         <v>0</v>
@@ -19273,19 +19273,19 @@
       </c>
       <c r="H20" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="I20" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="J20" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="K20" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="L20" s="3">
         <v>0</v>
@@ -19336,7 +19336,7 @@
       </c>
       <c r="L22" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*1*'Baseline year demographics'!$C$7</f>
-        <v>0.114048</v>
+        <v>8.4902399999999989E-2</v>
       </c>
       <c r="M22" s="27">
         <v>0</v>
@@ -19381,19 +19381,19 @@
       </c>
       <c r="L23" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>0.1469664</v>
+        <v>0.10940831999999998</v>
       </c>
       <c r="M23" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)</f>
-        <v>0.2268</v>
+        <v>0.16883999999999996</v>
       </c>
       <c r="N23" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)</f>
-        <v>0.2268</v>
+        <v>0.16883999999999996</v>
       </c>
       <c r="O23" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.7)</f>
-        <v>0.2268</v>
+        <v>0.16883999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19429,19 +19429,19 @@
       </c>
       <c r="L24" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>6.2985600000000003E-2</v>
+        <v>4.6889279999999998E-2</v>
       </c>
       <c r="M24" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>9.7199999999999995E-2</v>
+        <v>7.2359999999999994E-2</v>
       </c>
       <c r="N24" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>9.7199999999999995E-2</v>
+        <v>7.2359999999999994E-2</v>
       </c>
       <c r="O24" s="27">
         <f>'Baseline year demographics'!$C$8*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>9.7199999999999995E-2</v>
+        <v>7.2359999999999994E-2</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19477,7 +19477,7 @@
       </c>
       <c r="L25" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*1*'Baseline year demographics'!$C$7</f>
-        <v>0.20275200000000002</v>
+        <v>0.15093759999999998</v>
       </c>
       <c r="M25" s="27">
         <v>1E-3</v>
@@ -19522,19 +19522,19 @@
       </c>
       <c r="L26" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>0.18289152000000003</v>
+        <v>0.13615257599999997</v>
       </c>
       <c r="M26" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)</f>
-        <v>0.28224000000000005</v>
+        <v>0.21011199999999997</v>
       </c>
       <c r="N26" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)</f>
-        <v>0.28224000000000005</v>
+        <v>0.21011199999999997</v>
       </c>
       <c r="O26" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.49)</f>
-        <v>0.28224000000000005</v>
+        <v>0.21011199999999997</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19570,19 +19570,19 @@
       </c>
       <c r="L27" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>7.8382080000000007E-2</v>
+        <v>5.8351103999999994E-2</v>
       </c>
       <c r="M27" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)</f>
-        <v>0.12096000000000001</v>
+        <v>9.0047999999999989E-2</v>
       </c>
       <c r="N27" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)</f>
-        <v>0.12096000000000001</v>
+        <v>9.0047999999999989E-2</v>
       </c>
       <c r="O27" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.21)</f>
-        <v>0.12096000000000001</v>
+        <v>9.0047999999999989E-2</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19618,19 +19618,19 @@
       </c>
       <c r="L28" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>0.11197440000000002</v>
+        <v>8.3358719999999983E-2</v>
       </c>
       <c r="M28" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>0.17280000000000001</v>
+        <v>0.12863999999999998</v>
       </c>
       <c r="N28" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>0.17280000000000001</v>
+        <v>0.12863999999999998</v>
       </c>
       <c r="O28" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*(1-'Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>0.17280000000000001</v>
+        <v>0.12863999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19667,7 +19667,7 @@
       </c>
       <c r="L29" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*1*'Baseline year demographics'!$C$7</f>
-        <v>1.2671999999999998E-2</v>
+        <v>4.1817599999999996E-2</v>
       </c>
       <c r="M29" s="27">
         <v>0</v>
@@ -19712,19 +19712,19 @@
       </c>
       <c r="L30" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>1.63296E-2</v>
+        <v>5.388768E-2</v>
       </c>
       <c r="M30" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)</f>
-        <v>2.5199999999999997E-2</v>
+        <v>8.3159999999999998E-2</v>
       </c>
       <c r="N30" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)</f>
-        <v>2.5199999999999997E-2</v>
+        <v>8.3159999999999998E-2</v>
       </c>
       <c r="O30" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.7)</f>
-        <v>2.5199999999999997E-2</v>
+        <v>8.3159999999999998E-2</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19760,19 +19760,19 @@
       </c>
       <c r="L31" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>6.9983999999999992E-3</v>
+        <v>2.3094719999999999E-2</v>
       </c>
       <c r="M31" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>1.0799999999999999E-2</v>
+        <v>3.5639999999999998E-2</v>
       </c>
       <c r="N31" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>1.0799999999999999E-2</v>
+        <v>3.5639999999999998E-2</v>
       </c>
       <c r="O31" s="27">
         <f>'Baseline year demographics'!$C$8*('Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>1.0799999999999999E-2</v>
+        <v>3.5639999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19808,7 +19808,7 @@
       </c>
       <c r="L32" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*1*'Baseline year demographics'!$C$7</f>
-        <v>2.2527999999999999E-2</v>
+        <v>7.4342400000000003E-2</v>
       </c>
       <c r="M32" s="27">
         <v>0</v>
@@ -19853,19 +19853,19 @@
       </c>
       <c r="L33" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>2.0321280000000001E-2</v>
+        <v>6.7060224000000015E-2</v>
       </c>
       <c r="M33" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)</f>
-        <v>3.1359999999999999E-2</v>
+        <v>0.10348800000000001</v>
       </c>
       <c r="N33" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)</f>
-        <v>3.1359999999999999E-2</v>
+        <v>0.10348800000000001</v>
       </c>
       <c r="O33" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.49)</f>
-        <v>3.1359999999999999E-2</v>
+        <v>0.10348800000000001</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19901,19 +19901,19 @@
       </c>
       <c r="L34" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>8.7091200000000007E-3</v>
+        <v>2.8740096000000003E-2</v>
       </c>
       <c r="M34" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)</f>
-        <v>1.3440000000000001E-2</v>
+        <v>4.4352000000000003E-2</v>
       </c>
       <c r="N34" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)</f>
-        <v>1.3440000000000001E-2</v>
+        <v>4.4352000000000003E-2</v>
       </c>
       <c r="O34" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.21)</f>
-        <v>1.3440000000000001E-2</v>
+        <v>4.4352000000000003E-2</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19949,19 +19949,19 @@
       </c>
       <c r="L35" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)*(1-'Baseline year demographics'!$C$7)</f>
-        <v>1.2441599999999999E-2</v>
+        <v>4.1057280000000002E-2</v>
       </c>
       <c r="M35" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>1.9199999999999998E-2</v>
+        <v>6.336E-2</v>
       </c>
       <c r="N35" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>1.9199999999999998E-2</v>
+        <v>6.336E-2</v>
       </c>
       <c r="O35" s="27">
         <f>(1-'Baseline year demographics'!$C$8)*('Baseline year demographics'!$C$9)*(0.3)</f>
-        <v>1.9199999999999998E-2</v>
+        <v>6.336E-2</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -20523,51 +20523,51 @@
       </c>
       <c r="D49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="E49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="F49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="G49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="H49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="I49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="J49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="K49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="L49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="M49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="N49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="O49" s="32">
         <f>'Baseline year demographics'!$C9</f>
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="50" spans="1:15" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -24593,7 +24593,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25171,7 +25171,7 @@
       </c>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
@@ -27061,8 +27061,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27083,9 +27083,7 @@
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B2" s="132"/>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
@@ -27097,193 +27095,145 @@
       <c r="A4" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B4" s="132"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B5" s="132"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B6" s="132"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B7" s="132"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B8" s="132"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B9" s="132"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B10" s="132"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B11" s="132"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B12" s="132"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B13" s="132"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B14" s="132"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B15" s="132"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B16" s="132"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B17" s="132"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B18" s="132"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B19" s="132"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B20" s="132"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B21" s="132"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B22" s="132"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B23" s="132"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B24" s="132"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B25" s="132"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B26" s="132"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B27" s="132"/>
     </row>
     <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="126" t="s">
@@ -27307,73 +27257,55 @@
       <c r="A31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B31" s="132"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B32" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B32" s="132"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B33" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B33" s="132"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B34" s="132"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B35" s="132"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B36" s="132"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B37" s="132"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B38" s="132"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B39" s="132"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
@@ -27387,9 +27319,7 @@
       <c r="A41" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B41" s="132"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
@@ -27403,9 +27333,7 @@
       <c r="A43" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B43" s="132"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
@@ -27419,65 +27347,49 @@
       <c r="A45" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B45" s="132"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>259</v>
       </c>
-      <c r="B46" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B46" s="132"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>258</v>
       </c>
-      <c r="B47" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B47" s="132"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>256</v>
       </c>
-      <c r="B48" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B48" s="132"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>257</v>
       </c>
-      <c r="B49" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B49" s="132"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>262</v>
       </c>
-      <c r="B50" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B50" s="132"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B51" s="132"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="132" t="s">
-        <v>164</v>
-      </c>
+      <c r="B52" s="132"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="125" t="s">

</xml_diff>

<commit_message>
Added programs back in
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="17" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3338,7 +3338,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -18397,7 +18397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
@@ -27061,8 +27061,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27083,7 +27083,9 @@
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
@@ -27095,145 +27097,193 @@
       <c r="A4" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="132"/>
+      <c r="B4" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="132"/>
+      <c r="B5" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="132"/>
+      <c r="B6" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="132"/>
+      <c r="B7" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="132"/>
+      <c r="B8" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="132"/>
+      <c r="B10" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="132"/>
+      <c r="B12" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="132"/>
+      <c r="B13" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="132"/>
+      <c r="B14" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="132"/>
+      <c r="B15" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="132"/>
+      <c r="B16" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="132"/>
+      <c r="B17" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="132"/>
+      <c r="B18" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="132"/>
+      <c r="B19" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="132"/>
+      <c r="B20" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="132"/>
+      <c r="B21" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="132"/>
+      <c r="B22" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="132"/>
+      <c r="B23" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="132"/>
+      <c r="B24" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="132"/>
+      <c r="B25" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="132"/>
+      <c r="B26" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="132"/>
+      <c r="B27" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="28" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="126" t="s">
@@ -27257,55 +27307,73 @@
       <c r="A31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="132"/>
+      <c r="B31" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B32" s="132"/>
+      <c r="B32" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B33" s="132"/>
+      <c r="B33" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="132"/>
+      <c r="B34" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="132"/>
+      <c r="B35" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="132"/>
+      <c r="B36" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="132"/>
+      <c r="B37" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="132"/>
+      <c r="B38" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="132"/>
+      <c r="B39" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
@@ -27319,7 +27387,9 @@
       <c r="A41" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="132"/>
+      <c r="B41" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
@@ -27333,7 +27403,9 @@
       <c r="A43" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="132"/>
+      <c r="B43" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
@@ -27347,49 +27419,65 @@
       <c r="A45" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="132"/>
+      <c r="B45" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>259</v>
       </c>
-      <c r="B46" s="132"/>
+      <c r="B46" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>258</v>
       </c>
-      <c r="B47" s="132"/>
+      <c r="B47" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>256</v>
       </c>
-      <c r="B48" s="132"/>
+      <c r="B48" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>257</v>
       </c>
-      <c r="B49" s="132"/>
+      <c r="B49" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>262</v>
       </c>
-      <c r="B50" s="132"/>
+      <c r="B50" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="132"/>
+      <c r="B51" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="132"/>
+      <c r="B52" s="132" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="125" t="s">

</xml_diff>

<commit_message>
Update to zinc aff frac
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Nov/InputForCode_Bangladesh.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Nov/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E306C62B-D47E-AA41-9829-8018E1A4808F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36560" yWindow="-21140" windowWidth="35600" windowHeight="20580" tabRatio="500" firstSheet="7" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1433,7 +1434,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -1442,12 +1443,54 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-rac zinc deficient</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>frac zinc deficient</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D46" authorId="0" shapeId="0" xr:uid="{4791A64F-56B2-644F-9D9D-6669F82A1C20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>frac zinc deficient</t>
         </r>
       </text>
     </comment>
@@ -12265,7 +12308,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13796,6 +13839,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -13806,11 +13854,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -16167,8 +16210,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17210,19 +17253,19 @@
         <v>101</v>
       </c>
       <c r="D46" s="12">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E46" s="12">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F46" s="12">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G46" s="12">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H46" s="12">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
@@ -18480,7 +18523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -20875,7 +20918,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23297,7 +23340,7 @@
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23811,7 +23854,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24677,7 +24720,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25483,8 +25526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34C1B36-2F1D-8141-8AE0-24B0DA699162}">
   <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27146,7 +27189,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>